<commit_message>
Finalized and sourced Capacitor values for all filters
</commit_message>
<xml_diff>
--- a/Documents/BOM.xlsx
+++ b/Documents/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ECE_Projects\Music_Visualizer\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64C711DE-A04F-4857-97B7-C743A9FA9575}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB3DF128-8D54-45D9-BE9D-7D6FC360A007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{1F4A7036-4694-4970-BB5D-7CBECC831452}"/>
   </bookViews>
@@ -41,20 +41,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="90">
   <si>
     <t>Component</t>
   </si>
   <si>
-    <t>Link 1</t>
-  </si>
-  <si>
-    <t>Price 1</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
     <t>R1</t>
   </si>
   <si>
@@ -76,9 +67,6 @@
     <t>R4</t>
   </si>
   <si>
-    <t>90k costs $0.566</t>
-  </si>
-  <si>
     <t>R5</t>
   </si>
   <si>
@@ -121,9 +109,6 @@
     <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FBF52-118K?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWLYl8UX2zz89Y%3D</t>
   </si>
   <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FBF52-124K?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWLa%252BsgMfUiG2c%3D</t>
-  </si>
-  <si>
     <t>R10</t>
   </si>
   <si>
@@ -133,9 +118,6 @@
     <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FBF52-63K4?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWLcQ8fVKU%252BU94%3D</t>
   </si>
   <si>
-    <t>62.2k costs $0.718</t>
-  </si>
-  <si>
     <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FTE52-62K?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWLQBQPreYQV54%3D</t>
   </si>
   <si>
@@ -145,9 +127,6 @@
     <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FBF52-66K5?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWLQvEIp9Ucnpc%3D</t>
   </si>
   <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FBF52-133K?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWLiEQg4%252BXaLek%3D</t>
-  </si>
-  <si>
     <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FBF52-45K3?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWLZQJ76omWcBk%3D</t>
   </si>
   <si>
@@ -196,9 +175,6 @@
     <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FBF52-162K?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWLuQHAVLCqkm8%3D</t>
   </si>
   <si>
-    <t>https://www.mouser.ca/c/passive-components/resistors/through-hole-resistors/metal-film-resistors/?resistance=402%20kOhms&amp;tolerance=1%20%25&amp;instock=y&amp;sort=pricing</t>
-  </si>
-  <si>
     <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FRF52-78K7?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWLpw24GLtACaE%3D</t>
   </si>
   <si>
@@ -229,9 +205,6 @@
     <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FRF52-2K87?qs=sGAEpiMZZMsPqMdJzcrNwsMt%252BTupSSYjJQ%2FQGxQHoP8%3D</t>
   </si>
   <si>
-    <t>95k costs over $1.00</t>
-  </si>
-  <si>
     <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FBF52-95K3?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWL08Z1ESWg%252BHo%3D</t>
   </si>
   <si>
@@ -256,13 +229,88 @@
     <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FRF52-19K6?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWLYCnE65764HQ%3D</t>
   </si>
   <si>
-    <t>10.6k costs $0.276</t>
-  </si>
-  <si>
     <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FRF52-10K5?qs=sGAEpiMZZMsPqMdJzcrNwsMt%252BTupSSYjSfrSYPK%2FjDA%3D</t>
   </si>
   <si>
     <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FBF52-309K?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWLIiIIHbDRC1U%3D</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Ideal Value (nF)</t>
+  </si>
+  <si>
+    <t>Implemented Value (nF)</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/KEMET/R82EC2470AA60J?qs=Jv4FAWB%252B0HZ7iV08qIayRQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/KEMET/R82EC2270DQ50J?qs=Jv4FAWB%252B0HZvsaU83gp7aA%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/KEMET/R82IC2750DQ50J?qs=Jv4FAWB%252B0Hay7Xg1QVvwZA%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/KEMET/R82EC1680AA50J?qs=Jv4FAWB%252B0HYqZ5SSAUehwg%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Panasonic/ECW-HA3C243J?qs=Qtr4Kn8gT99qCmDlHSUg%2FA%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/KEMET/R82EC1470AA50J?qs=Jv4FAWB%252B0HbarvYaCHIS7Q%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/KEMET/R82EC1330JE50J?qs=Jv4FAWB%252B0HaKxYy7WO79fg%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Panasonic/ECW-HA3C622H?qs=alij%252Bcw9eGAgau2Xq4ECcg%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Panasonic/ECW-HA3C162J4?qs=Qtr4Kn8gT992Q7YG%2Ff1p5g%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/KEMET/R82EC1100Z350J?qs=lDWqi%2FyC4HJfno26FHExPA%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Panasonic/ECW-HA3C302J4?qs=Qtr4Kn8gT9%252BZ4p5F1qsqKA%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FBF52-402K?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWL8Ad6fBGB2S0%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Panasonic/ECW-HA3C133J?qs=Qtr4Kn8gT99ASgbewS4Hog%3D%3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Link </t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FBF52-137K?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWLIshtPH5zdIw%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FBF52-37K4?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWLdLZun4bPFoQ%3D</t>
   </si>
 </sst>
 </file>
@@ -272,7 +320,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -292,6 +340,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -650,10 +704,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F8295C8-65E6-45FB-87E8-3A2215DAA9D2}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -669,27 +723,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>1</v>
+        <v>86</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>3</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>84.6</v>
@@ -698,19 +750,19 @@
         <v>84.5</v>
       </c>
       <c r="D2">
-        <f>100*ABS(B2-C2)/B2</f>
+        <f t="shared" ref="D2:D7" si="0">100*ABS(B2-C2)/B2</f>
         <v>0.11820330969266468</v>
       </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="2">
+      <c r="E2" s="2">
         <v>0.152</v>
+      </c>
+      <c r="F2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>160</v>
@@ -719,19 +771,19 @@
         <v>160</v>
       </c>
       <c r="D3">
-        <f>100*ABS(B3-C3)/B3</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="2">
+      <c r="E3" s="2">
         <v>0.16600000000000001</v>
+      </c>
+      <c r="F3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>169</v>
@@ -740,19 +792,19 @@
         <v>169</v>
       </c>
       <c r="D4">
-        <f>100*ABS(B4-C4)/B4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="2">
+      <c r="E4" s="2">
         <v>0.16600000000000001</v>
+      </c>
+      <c r="F4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>90</v>
@@ -761,22 +813,19 @@
         <v>90.9</v>
       </c>
       <c r="D5">
-        <f>100*ABS(B5-C5)/B5</f>
+        <f t="shared" si="0"/>
         <v>1.0000000000000062</v>
       </c>
-      <c r="E5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0.13800000000000001</v>
-      </c>
-      <c r="G5" t="s">
-        <v>11</v>
+      <c r="E5" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="F5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>37</v>
@@ -785,19 +834,19 @@
         <v>37.4</v>
       </c>
       <c r="D6">
-        <f>100*ABS(B6-C6)/B6</f>
+        <f t="shared" si="0"/>
         <v>1.0810810810810771</v>
       </c>
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0.13800000000000001</v>
+      <c r="E6" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>405</v>
@@ -806,19 +855,19 @@
         <v>402</v>
       </c>
       <c r="D7">
-        <f>100*ABS(B7-C7)/B7</f>
+        <f t="shared" si="0"/>
         <v>0.7407407407407407</v>
       </c>
-      <c r="E7" t="s">
-        <v>51</v>
-      </c>
-      <c r="F7" s="2">
+      <c r="E7" s="2">
         <v>0.152</v>
+      </c>
+      <c r="F7" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <v>86.7</v>
@@ -827,19 +876,19 @@
         <v>86.6</v>
       </c>
       <c r="D8">
-        <f t="shared" ref="D8:D10" si="0">100*ABS(B8-C8)/B8</f>
+        <f t="shared" ref="D8:D10" si="1">100*ABS(B8-C8)/B8</f>
         <v>0.11534025374856807</v>
       </c>
-      <c r="E8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="2">
-        <v>0.13800000000000001</v>
+      <c r="E8" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B9">
         <v>35.6</v>
@@ -848,19 +897,19 @@
         <v>35.700000000000003</v>
       </c>
       <c r="D9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.28089887640449834</v>
       </c>
-      <c r="E9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="2">
+      <c r="E9" s="2">
         <v>0.152</v>
+      </c>
+      <c r="F9" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B10">
         <v>390</v>
@@ -869,30 +918,162 @@
         <v>390</v>
       </c>
       <c r="D10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="2">
+      <c r="E10" s="2">
         <v>0.152</v>
       </c>
+      <c r="F10" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>64</v>
+      </c>
       <c r="D11">
         <f>SUM(D2:D10)</f>
         <v>3.3362642616675551</v>
       </c>
+      <c r="E11" s="2">
+        <f>SUM(E2:E10)</f>
+        <v>1.3539999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14">
+        <v>47</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.373</v>
+      </c>
+      <c r="F14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15">
+        <v>47</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.373</v>
+      </c>
+      <c r="F15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16">
+        <v>27</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.35899999999999999</v>
+      </c>
+      <c r="F16" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17">
+        <v>27</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.35899999999999999</v>
+      </c>
+      <c r="F17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18">
+        <v>75</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.82799999999999996</v>
+      </c>
+      <c r="F18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19">
+        <v>75</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.82799999999999996</v>
+      </c>
+      <c r="F19" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" s="2">
+        <f>SUM(E14:E19)</f>
+        <v>3.1199999999999997</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>64</v>
+      </c>
+      <c r="E22" s="2">
+        <f>E11+E20</f>
+        <v>4.4739999999999993</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9015A39E-4C3F-4E48-B877-A44E11CEB1FD}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1:G1048576"/>
@@ -911,27 +1092,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>1</v>
+        <v>86</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>3</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>111</v>
@@ -943,16 +1122,16 @@
         <f>100*ABS(B2-C2)/B2</f>
         <v>0</v>
       </c>
-      <c r="E2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0.13800000000000001</v>
+      <c r="E2" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>90.7</v>
@@ -964,16 +1143,16 @@
         <f t="shared" ref="D3:D11" si="0">100*ABS(B3-C3)/B3</f>
         <v>0.22050716648291382</v>
       </c>
-      <c r="E3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0.13800000000000001</v>
+      <c r="E3" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>163</v>
@@ -985,16 +1164,16 @@
         <f t="shared" si="0"/>
         <v>0.61349693251533743</v>
       </c>
-      <c r="E4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F4" s="2">
+      <c r="E4" s="2">
         <v>0.16600000000000001</v>
+      </c>
+      <c r="F4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>118</v>
@@ -1006,16 +1185,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0.13800000000000001</v>
+      <c r="E5" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>63.5</v>
@@ -1027,16 +1206,16 @@
         <f t="shared" si="0"/>
         <v>0.15748031496063217</v>
       </c>
-      <c r="E6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0.13800000000000001</v>
+      <c r="E6" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="F6" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>62.2</v>
@@ -1048,19 +1227,16 @@
         <f t="shared" si="0"/>
         <v>0.32154340836013318</v>
       </c>
-      <c r="E7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="2">
-        <v>0.13800000000000001</v>
-      </c>
-      <c r="G7" t="s">
-        <v>30</v>
+      <c r="E7" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="F7" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <v>312</v>
@@ -1072,16 +1248,16 @@
         <f t="shared" si="0"/>
         <v>0.96153846153846156</v>
       </c>
-      <c r="E8" t="s">
-        <v>73</v>
-      </c>
-      <c r="F8" s="2">
-        <v>0.13800000000000001</v>
+      <c r="E8" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="F8" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B9">
         <v>67.599999999999994</v>
@@ -1093,16 +1269,16 @@
         <f t="shared" si="0"/>
         <v>0.59171597633136941</v>
       </c>
-      <c r="E9" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" s="2">
+      <c r="E9" s="2">
         <v>0.152</v>
+      </c>
+      <c r="F9" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B10">
         <v>66.2</v>
@@ -1114,16 +1290,16 @@
         <f t="shared" si="0"/>
         <v>0.45317220543806214</v>
       </c>
-      <c r="E10" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="2">
-        <v>0.13800000000000001</v>
+      <c r="E10" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="F10" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B11">
         <v>332</v>
@@ -1135,22 +1311,153 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E11" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" s="2">
+      <c r="E11" s="2">
         <v>0.16600000000000001</v>
       </c>
+      <c r="F11" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>64</v>
+      </c>
       <c r="D12">
         <f>SUM(D2:D11)</f>
         <v>3.3194544656269094</v>
       </c>
+      <c r="E12" s="2">
+        <f>SUM(E2:E11)</f>
+        <v>1.4500000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15">
+        <v>13</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="F15" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16">
+        <v>13</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="F16" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17">
+        <v>6.8</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.33100000000000002</v>
+      </c>
+      <c r="F17" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18">
+        <v>6.8</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.33100000000000002</v>
+      </c>
+      <c r="F18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19">
+        <v>24</v>
+      </c>
+      <c r="E19" s="2">
+        <v>1.48</v>
+      </c>
+      <c r="F19" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20">
+        <v>24</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1.48</v>
+      </c>
+      <c r="F20" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>64</v>
+      </c>
+      <c r="E21" s="2">
+        <f>SUM(E15:E20)</f>
+        <v>5.9220000000000006</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>64</v>
+      </c>
+      <c r="E23" s="2">
+        <f>E12+E21</f>
+        <v>7.3720000000000008</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E5" r:id="rId1" xr:uid="{7C4A873B-76ED-4822-8A83-F29474C12A63}"/>
+    <hyperlink ref="F5" r:id="rId1" xr:uid="{7C4A873B-76ED-4822-8A83-F29474C12A63}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1158,7 +1465,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA94F869-6CDA-42B7-B92B-C65898560124}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1:G1048576"/>
@@ -1177,27 +1484,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>1</v>
+        <v>86</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>3</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>135</v>
@@ -1206,19 +1511,19 @@
         <v>137</v>
       </c>
       <c r="D2">
-        <f>100*ABS(B2-C2)/B2</f>
+        <f t="shared" ref="D2:D10" si="0">100*ABS(B2-C2)/B2</f>
         <v>1.4814814814814814</v>
       </c>
-      <c r="E2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0.13800000000000001</v>
+      <c r="E2" s="2">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="F2" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>45.1</v>
@@ -1227,19 +1532,19 @@
         <v>45.3</v>
       </c>
       <c r="D3">
-        <f>100*ABS(B3-C3)/B3</f>
+        <f t="shared" si="0"/>
         <v>0.44345898004433643</v>
       </c>
-      <c r="E3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0.13800000000000001</v>
+      <c r="E3" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="F3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>271</v>
@@ -1248,19 +1553,19 @@
         <v>270</v>
       </c>
       <c r="D4">
-        <f>100*ABS(B4-C4)/B4</f>
+        <f t="shared" si="0"/>
         <v>0.36900369003690037</v>
       </c>
-      <c r="E4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0.13800000000000001</v>
+      <c r="E4" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="F4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>142</v>
@@ -1269,19 +1574,19 @@
         <v>143</v>
       </c>
       <c r="D5">
-        <f>100*ABS(B5-C5)/B5</f>
+        <f t="shared" si="0"/>
         <v>0.70422535211267601</v>
       </c>
-      <c r="E5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0.13800000000000001</v>
+      <c r="E5" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="F5" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>19.2</v>
@@ -1290,19 +1595,19 @@
         <v>19.2</v>
       </c>
       <c r="D6">
-        <f>100*ABS(B6-C6)/B6</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" s="2">
+      <c r="E6" s="2">
         <v>0.152</v>
+      </c>
+      <c r="F6" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>595</v>
@@ -1311,19 +1616,19 @@
         <v>600</v>
       </c>
       <c r="D7">
-        <f>100*ABS(B7-C7)/B7</f>
+        <f t="shared" si="0"/>
         <v>0.84033613445378152</v>
       </c>
-      <c r="E7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F7" s="2">
+      <c r="E7" s="2">
         <v>0.152</v>
+      </c>
+      <c r="F7" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <v>139</v>
@@ -1332,19 +1637,19 @@
         <v>140</v>
       </c>
       <c r="D8">
-        <f>100*ABS(B8-C8)/B8</f>
+        <f t="shared" si="0"/>
         <v>0.71942446043165464</v>
       </c>
-      <c r="E8" t="s">
-        <v>40</v>
-      </c>
-      <c r="F8" s="2">
+      <c r="E8" s="2">
         <v>0.16600000000000001</v>
+      </c>
+      <c r="F8" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B9">
         <v>18.899999999999999</v>
@@ -1353,19 +1658,19 @@
         <v>19</v>
       </c>
       <c r="D9">
-        <f>100*ABS(B9-C9)/B9</f>
+        <f t="shared" si="0"/>
         <v>0.52910052910053662</v>
       </c>
-      <c r="E9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F9" s="2">
-        <v>0.13800000000000001</v>
+      <c r="E9" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="F9" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B10">
         <v>583</v>
@@ -1374,20 +1679,150 @@
         <v>576</v>
       </c>
       <c r="D10">
-        <f>100*ABS(B10-C10)/B10</f>
+        <f t="shared" si="0"/>
         <v>1.2006861063464838</v>
       </c>
-      <c r="E10" t="s">
-        <v>42</v>
-      </c>
-      <c r="F10" s="2">
-        <v>0.13800000000000001</v>
+      <c r="E10" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="F10" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>64</v>
+      </c>
       <c r="D11">
         <f>SUM(D2:D10)</f>
         <v>6.2877167340078506</v>
+      </c>
+      <c r="E11" s="2">
+        <f>SUM(E2:E10)</f>
+        <v>1.3260000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14">
+        <v>4.7</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="F14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15">
+        <v>4.7</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="F15" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16">
+        <v>3.3</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.317</v>
+      </c>
+      <c r="F16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17">
+        <v>3.3</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.317</v>
+      </c>
+      <c r="F17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18">
+        <v>6.2</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="F18" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19">
+        <v>6.2</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="F19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" s="2">
+        <f>SUM(E14:E19)</f>
+        <v>3.202</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>64</v>
+      </c>
+      <c r="E22" s="2">
+        <f>E11+E20</f>
+        <v>4.5280000000000005</v>
       </c>
     </row>
   </sheetData>
@@ -1397,7 +1832,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99571FDB-D382-46BD-933E-AF5B2116BB53}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1:G1048576"/>
@@ -1416,27 +1851,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>1</v>
+        <v>86</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>3</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>99.7</v>
@@ -1448,16 +1881,16 @@
         <f>100*ABS(B2-C2)/B2</f>
         <v>0.30090270812437026</v>
       </c>
-      <c r="E2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0.13800000000000001</v>
+      <c r="E2" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="F2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>99.2</v>
@@ -1469,16 +1902,16 @@
         <f>100*ABS(B3-C3)/B3</f>
         <v>0.80645161290322287</v>
       </c>
-      <c r="E3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0.13800000000000001</v>
+      <c r="E3" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="F3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>65.8</v>
@@ -1490,16 +1923,16 @@
         <f>100*ABS(B4-C4)/B4</f>
         <v>1.063829787234047</v>
       </c>
-      <c r="E4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0.13800000000000001</v>
+      <c r="E4" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="F4" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>33.200000000000003</v>
@@ -1511,16 +1944,16 @@
         <f>100*ABS(B5-C5)/B5</f>
         <v>0</v>
       </c>
-      <c r="E5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F5" s="2">
+      <c r="E5" s="2">
         <v>0.16600000000000001</v>
+      </c>
+      <c r="F5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>55.9</v>
@@ -1532,16 +1965,16 @@
         <f>100*ABS(B6-C6)/B6</f>
         <v>0.17889087656529773</v>
       </c>
-      <c r="E6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F6" s="2">
+      <c r="E6" s="2">
         <v>0.152</v>
+      </c>
+      <c r="F6" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>48.6</v>
@@ -1553,16 +1986,16 @@
         <f t="shared" ref="D7:D11" si="0">100*ABS(B7-C7)/B7</f>
         <v>0.2057613168724309</v>
       </c>
-      <c r="E7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F7" s="2">
+      <c r="E7" s="2">
         <v>0.16600000000000001</v>
+      </c>
+      <c r="F7" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <v>271</v>
@@ -1574,16 +2007,16 @@
         <f t="shared" si="0"/>
         <v>0.36900369003690037</v>
       </c>
-      <c r="E8" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8" s="2">
-        <v>0.13800000000000001</v>
+      <c r="E8" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="F8" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B9">
         <v>67</v>
@@ -1595,16 +2028,16 @@
         <f t="shared" si="0"/>
         <v>0.74626865671641796</v>
       </c>
-      <c r="E9" t="s">
-        <v>47</v>
-      </c>
-      <c r="F9" s="2">
+      <c r="E9" s="2">
         <v>0.16600000000000001</v>
+      </c>
+      <c r="F9" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B10">
         <v>58.2</v>
@@ -1616,16 +2049,16 @@
         <f t="shared" si="0"/>
         <v>1.0309278350515487</v>
       </c>
-      <c r="E10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F10" s="2">
-        <v>0.13800000000000001</v>
+      <c r="E10" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="F10" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B11">
         <v>325</v>
@@ -1637,17 +2070,147 @@
         <f t="shared" si="0"/>
         <v>0.30769230769230771</v>
       </c>
-      <c r="E11" t="s">
-        <v>49</v>
-      </c>
-      <c r="F11" s="2">
+      <c r="E11" s="2">
         <v>0.16600000000000001</v>
       </c>
+      <c r="F11" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>64</v>
+      </c>
       <c r="D12">
         <f>SUM(D2:D11)</f>
         <v>5.0097287911965429</v>
+      </c>
+      <c r="E12" s="2">
+        <f>SUM(E2:E11)</f>
+        <v>1.5059999999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15">
+        <v>1.6</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1.04</v>
+      </c>
+      <c r="F15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16">
+        <v>1.6</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1.04</v>
+      </c>
+      <c r="F16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.152</v>
+      </c>
+      <c r="F17" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.152</v>
+      </c>
+      <c r="F18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="E19" s="2">
+        <v>1.01</v>
+      </c>
+      <c r="F19" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1.01</v>
+      </c>
+      <c r="F20" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>64</v>
+      </c>
+      <c r="E21" s="2">
+        <f>SUM(E15:E20)</f>
+        <v>4.4039999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>64</v>
+      </c>
+      <c r="E23" s="2">
+        <f>E12+E21</f>
+        <v>5.91</v>
       </c>
     </row>
   </sheetData>
@@ -1657,7 +2220,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FA0D483-C574-49A8-A0EA-072A18CA1F90}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1:G1048576"/>
@@ -1676,27 +2239,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>1</v>
+        <v>86</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>3</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>79.5</v>
@@ -1708,16 +2269,16 @@
         <f>100*ABS(B2-C2)/B2</f>
         <v>1.0062893081760971</v>
       </c>
-      <c r="E2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F2" s="2">
+      <c r="E2" s="2">
         <v>0.16600000000000001</v>
+      </c>
+      <c r="F2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>26.5</v>
@@ -1729,16 +2290,16 @@
         <f>100*ABS(B3-C3)/B3</f>
         <v>0.75471698113207275</v>
       </c>
-      <c r="E3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0.13800000000000001</v>
+      <c r="E3" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="F3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>159</v>
@@ -1750,16 +2311,16 @@
         <f t="shared" ref="D4:D10" si="0">100*ABS(B4-C4)/B4</f>
         <v>0.62893081761006286</v>
       </c>
-      <c r="E4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="2">
+      <c r="E4" s="2">
         <v>0.16600000000000001</v>
+      </c>
+      <c r="F4" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>58.6</v>
@@ -1771,16 +2332,16 @@
         <f t="shared" si="0"/>
         <v>0.68259385665528771</v>
       </c>
-      <c r="E5" t="s">
-        <v>54</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0.13800000000000001</v>
+      <c r="E5" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="F5" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>7.94</v>
@@ -1792,16 +2353,16 @@
         <f t="shared" si="0"/>
         <v>0.88161209068010427</v>
       </c>
-      <c r="E6" t="s">
-        <v>55</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0.13800000000000001</v>
+      <c r="E6" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="F6" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>245</v>
@@ -1813,16 +2374,16 @@
         <f t="shared" si="0"/>
         <v>0.81632653061224492</v>
       </c>
-      <c r="E7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F7" s="2">
+      <c r="E7" s="2">
         <v>0.16600000000000001</v>
+      </c>
+      <c r="F7" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <v>108</v>
@@ -1834,16 +2395,16 @@
         <f t="shared" si="0"/>
         <v>0.92592592592592593</v>
       </c>
-      <c r="E8" t="s">
-        <v>57</v>
-      </c>
-      <c r="F8" s="2">
-        <v>0.13800000000000001</v>
+      <c r="E8" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="F8" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B9">
         <v>14.6</v>
@@ -1855,16 +2416,16 @@
         <f t="shared" si="0"/>
         <v>0.6849315068493127</v>
       </c>
-      <c r="E9" t="s">
-        <v>58</v>
-      </c>
-      <c r="F9" s="2">
-        <v>0.13800000000000001</v>
+      <c r="E9" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="F9" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B10">
         <v>452</v>
@@ -1876,17 +2437,147 @@
         <f t="shared" si="0"/>
         <v>0.22123893805309736</v>
       </c>
-      <c r="E10" t="s">
-        <v>59</v>
-      </c>
-      <c r="F10" s="2">
+      <c r="E10" s="2">
         <v>0.152</v>
       </c>
+      <c r="F10" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>64</v>
+      </c>
       <c r="D11">
         <f>SUM(D2:D10)</f>
         <v>6.6025659556942049</v>
+      </c>
+      <c r="E11" s="2">
+        <f>SUM(E2:E10)</f>
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.152</v>
+      </c>
+      <c r="F14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.152</v>
+      </c>
+      <c r="F15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.152</v>
+      </c>
+      <c r="F16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.152</v>
+      </c>
+      <c r="F17" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.152</v>
+      </c>
+      <c r="F18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.152</v>
+      </c>
+      <c r="F19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" s="2">
+        <f>SUM(E14:E19)</f>
+        <v>0.91200000000000003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>64</v>
+      </c>
+      <c r="E22" s="2">
+        <f>E11+E20</f>
+        <v>2.2520000000000002</v>
       </c>
     </row>
   </sheetData>
@@ -1896,7 +2587,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5443C8D0-3F9E-42A4-A7A9-47E7E9623942}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1:G1048576"/>
@@ -1915,27 +2606,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>1</v>
+        <v>86</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>3</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>79.5</v>
@@ -1944,19 +2633,19 @@
         <v>78.7</v>
       </c>
       <c r="D2">
-        <f>100*ABS(B2-C2)/B2</f>
+        <f t="shared" ref="D2:D10" si="0">100*ABS(B2-C2)/B2</f>
         <v>1.0062893081760971</v>
       </c>
-      <c r="E2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F2" s="2">
+      <c r="E2" s="2">
         <v>0.16600000000000001</v>
+      </c>
+      <c r="F2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>7.24</v>
@@ -1965,19 +2654,19 @@
         <v>7.3</v>
       </c>
       <c r="D3">
-        <f>100*ABS(B3-C3)/B3</f>
+        <f t="shared" si="0"/>
         <v>0.82872928176795035</v>
       </c>
-      <c r="E3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F3" s="2">
+      <c r="E3" s="2">
         <v>0.152</v>
+      </c>
+      <c r="F3" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>159</v>
@@ -1986,19 +2675,19 @@
         <v>160</v>
       </c>
       <c r="D4">
-        <f>100*ABS(B4-C4)/B4</f>
+        <f t="shared" si="0"/>
         <v>0.62893081761006286</v>
       </c>
-      <c r="E4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="2">
+      <c r="E4" s="2">
         <v>0.16600000000000001</v>
+      </c>
+      <c r="F4" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>66.599999999999994</v>
@@ -2007,19 +2696,19 @@
         <v>66.5</v>
       </c>
       <c r="D5">
-        <f>100*ABS(B5-C5)/B5</f>
+        <f t="shared" si="0"/>
         <v>0.15015015015014163</v>
       </c>
-      <c r="E5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0.13800000000000001</v>
+      <c r="E5" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="F5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>2.85</v>
@@ -2028,19 +2717,19 @@
         <v>2.87</v>
       </c>
       <c r="D6">
-        <f>100*ABS(B6-C6)/B6</f>
+        <f t="shared" si="0"/>
         <v>0.70175438596491291</v>
       </c>
-      <c r="E6" t="s">
-        <v>61</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0.13800000000000001</v>
+      <c r="E6" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="F6" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>271</v>
@@ -2049,19 +2738,19 @@
         <v>270</v>
       </c>
       <c r="D7">
-        <f>100*ABS(B7-C7)/B7</f>
+        <f t="shared" si="0"/>
         <v>0.36900369003690037</v>
       </c>
-      <c r="E7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F7" s="2">
-        <v>0.13800000000000001</v>
+      <c r="E7" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="F7" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <v>94.9</v>
@@ -2070,22 +2759,19 @@
         <v>95.3</v>
       </c>
       <c r="D8">
-        <f>100*ABS(B8-C8)/B8</f>
+        <f t="shared" si="0"/>
         <v>0.42149631190726178</v>
       </c>
-      <c r="E8" t="s">
-        <v>63</v>
-      </c>
-      <c r="F8" s="2">
-        <v>0.13800000000000001</v>
-      </c>
-      <c r="G8" t="s">
-        <v>62</v>
+      <c r="E8" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="F8" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B9">
         <v>4.0599999999999996</v>
@@ -2094,19 +2780,19 @@
         <v>4.0199999999999996</v>
       </c>
       <c r="D9">
-        <f>100*ABS(B9-C9)/B9</f>
+        <f t="shared" si="0"/>
         <v>0.98522167487684831</v>
       </c>
-      <c r="E9" t="s">
-        <v>64</v>
-      </c>
-      <c r="F9" s="2">
-        <v>0.13800000000000001</v>
+      <c r="E9" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="F9" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B10">
         <v>386</v>
@@ -2115,20 +2801,149 @@
         <v>383</v>
       </c>
       <c r="D10">
-        <f>100*ABS(B10-C10)/B10</f>
+        <f t="shared" si="0"/>
         <v>0.77720207253886009</v>
       </c>
-      <c r="E10" t="s">
-        <v>65</v>
-      </c>
-      <c r="F10" s="2">
-        <v>0.13800000000000001</v>
+      <c r="E10" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="F10" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>64</v>
+      </c>
       <c r="D11">
         <f>SUM(D2:D10)</f>
         <v>5.8687776930290356</v>
+      </c>
+      <c r="E11" s="2">
+        <f>SUM(E2:E10)</f>
+        <v>1.3119999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.152</v>
+      </c>
+      <c r="F14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.152</v>
+      </c>
+      <c r="F15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.152</v>
+      </c>
+      <c r="F16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.152</v>
+      </c>
+      <c r="F17" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.152</v>
+      </c>
+      <c r="F18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.152</v>
+      </c>
+      <c r="F19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" s="2">
+        <f>SUM(E14:E19)</f>
+        <v>0.91200000000000003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>64</v>
+      </c>
+      <c r="E22" s="2">
+        <f>E11+E20</f>
+        <v>2.2239999999999998</v>
       </c>
     </row>
   </sheetData>
@@ -2138,10 +2953,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{402F22C9-9046-40B7-9C8A-21A255598059}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2157,27 +2972,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>1</v>
+        <v>86</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>3</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>11.4</v>
@@ -2186,19 +2999,19 @@
         <v>11.5</v>
       </c>
       <c r="D2">
-        <f>100*ABS(B2-C2)/B2</f>
+        <f t="shared" ref="D2:D10" si="0">100*ABS(B2-C2)/B2</f>
         <v>0.87719298245613719</v>
       </c>
-      <c r="E2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0.13800000000000001</v>
+      <c r="E2" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="F2" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>48.8</v>
@@ -2207,19 +3020,19 @@
         <v>48.7</v>
       </c>
       <c r="D3">
-        <f>100*ABS(B3-C3)/B3</f>
+        <f t="shared" si="0"/>
         <v>0.20491803278687362</v>
       </c>
-      <c r="E3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F3" s="2">
+      <c r="E3" s="2">
         <v>0.16600000000000001</v>
+      </c>
+      <c r="F3" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>22.7</v>
@@ -2228,19 +3041,19 @@
         <v>22.6</v>
       </c>
       <c r="D4">
-        <f>100*ABS(B4-C4)/B4</f>
+        <f t="shared" si="0"/>
         <v>0.44052863436122408</v>
       </c>
-      <c r="E4" t="s">
-        <v>67</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0.13800000000000001</v>
+      <c r="E4" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="F4" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>8.02</v>
@@ -2249,19 +3062,19 @@
         <v>8.06</v>
       </c>
       <c r="D5">
-        <f>100*ABS(B5-C5)/B5</f>
+        <f t="shared" si="0"/>
         <v>0.49875311720699411</v>
       </c>
-      <c r="E5" t="s">
-        <v>68</v>
-      </c>
-      <c r="F5" s="2">
+      <c r="E5" s="2">
         <v>0.16600000000000001</v>
+      </c>
+      <c r="F5" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>4.3499999999999996</v>
@@ -2270,19 +3083,19 @@
         <v>4.32</v>
       </c>
       <c r="D6">
-        <f>100*ABS(B6-C6)/B6</f>
+        <f t="shared" si="0"/>
         <v>0.68965517241377849</v>
       </c>
-      <c r="E6" t="s">
-        <v>69</v>
-      </c>
-      <c r="F6" s="2">
+      <c r="E6" s="2">
         <v>0.16600000000000001</v>
+      </c>
+      <c r="F6" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>37</v>
@@ -2291,19 +3104,19 @@
         <v>37.4</v>
       </c>
       <c r="D7">
-        <f>100*ABS(B7-C7)/B7</f>
+        <f t="shared" si="0"/>
         <v>1.0810810810810771</v>
       </c>
-      <c r="E7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="2">
-        <v>0.13800000000000001</v>
+      <c r="E7" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="F7" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <v>19.600000000000001</v>
@@ -2312,19 +3125,19 @@
         <v>19.600000000000001</v>
       </c>
       <c r="D8">
-        <f>100*ABS(B8-C8)/B8</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E8" t="s">
-        <v>70</v>
-      </c>
-      <c r="F8" s="2">
+      <c r="E8" s="2">
         <v>0.17899999999999999</v>
+      </c>
+      <c r="F8" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B9">
         <v>10.6</v>
@@ -2333,22 +3146,19 @@
         <v>10.5</v>
       </c>
       <c r="D9">
-        <f>100*ABS(B9-C9)/B9</f>
+        <f t="shared" si="0"/>
         <v>0.94339622641509102</v>
       </c>
-      <c r="E9" t="s">
-        <v>72</v>
-      </c>
-      <c r="F9" s="2">
+      <c r="E9" s="2">
         <v>0.16600000000000001</v>
       </c>
-      <c r="G9" t="s">
-        <v>71</v>
+      <c r="F9" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B10">
         <v>90.5</v>
@@ -2357,20 +3167,149 @@
         <v>90.9</v>
       </c>
       <c r="D10">
-        <f>100*ABS(B10-C10)/B10</f>
+        <f t="shared" si="0"/>
         <v>0.44198895027624935</v>
       </c>
-      <c r="E10" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="2">
-        <v>0.13800000000000001</v>
+      <c r="E10" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="F10" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>64</v>
+      </c>
       <c r="D11">
         <f>SUM(D2:D10)</f>
         <v>5.177514196997425</v>
+      </c>
+      <c r="E11" s="2">
+        <f>SUM(E2:E10)</f>
+        <v>1.395</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.152</v>
+      </c>
+      <c r="F14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.152</v>
+      </c>
+      <c r="F15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.152</v>
+      </c>
+      <c r="F16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.152</v>
+      </c>
+      <c r="F17" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.152</v>
+      </c>
+      <c r="F18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.152</v>
+      </c>
+      <c r="F19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" s="2">
+        <f>SUM(E14:E19)</f>
+        <v>0.91200000000000003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>64</v>
+      </c>
+      <c r="E22" s="2">
+        <f>E11+E20</f>
+        <v>2.3069999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Replaced through-hole resistors and capacitors with SMD types, all resisotrs of Case Code (mm) 0603, most caps are Case Code (mm) 0603, a few are 1005, 1608, 2012 and 3216
</commit_message>
<xml_diff>
--- a/Documents/BOM.xlsx
+++ b/Documents/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ECE_Projects\Music_Visualizer\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB3DF128-8D54-45D9-BE9D-7D6FC360A007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CA6424E-C989-452F-8F6C-1B7447174F59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{1F4A7036-4694-4970-BB5D-7CBECC831452}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{1F4A7036-4694-4970-BB5D-7CBECC831452}"/>
   </bookViews>
   <sheets>
     <sheet name="Sub-Bass" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="88">
   <si>
     <t>Component</t>
   </si>
@@ -49,45 +49,27 @@
     <t>R1</t>
   </si>
   <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FBF52-84K5?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWL2kDhMAOIWaw%3D</t>
-  </si>
-  <si>
     <t>R2</t>
   </si>
   <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FRF52-160K?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWLKp1bNII2Nvk%3D</t>
-  </si>
-  <si>
     <t>R3</t>
   </si>
   <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FTE52-169K?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWLOoHSKHxivvo%3D</t>
-  </si>
-  <si>
     <t>R4</t>
   </si>
   <si>
     <t>R5</t>
   </si>
   <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FTE52-36K?qs=sGAEpiMZZMsPqMdJzcrNwvki5I7GwxKepnj5ARZ5vuI%3D</t>
-  </si>
-  <si>
     <t>R6</t>
   </si>
   <si>
     <t>R7</t>
   </si>
   <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FBF52-86K6?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWLD9ddB4j1Mdc%3D</t>
-  </si>
-  <si>
     <t>R8</t>
   </si>
   <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FTE52-35K7?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWLg0tDR7dwLc0%3D</t>
-  </si>
-  <si>
     <t>R9</t>
   </si>
   <si>
@@ -103,138 +85,9 @@
     <t>Implemented Value (kOhms)</t>
   </si>
   <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MF0207FRE52-100K?qs=sGAEpiMZZMsPqMdJzcrNwoMVoLRhO46JEYGHnzzlg66u8WN1bzgCIQ%3D%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FBF52-118K?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWLYl8UX2zz89Y%3D</t>
-  </si>
-  <si>
     <t>R10</t>
   </si>
   <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FRF52-332K?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWL%252BlV%252BSjquq%252B8%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FBF52-63K4?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWLcQ8fVKU%252BU94%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FTE52-62K?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWLQBQPreYQV54%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FBF52-90K9?qs=sGAEpiMZZMsPqMdJzcrNwhW0f6Ofw06mWwaWA39peqE%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FBF52-66K5?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWLQvEIp9Ucnpc%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FBF52-45K3?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWLZQJ76omWcBk%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-12FTF52-270K?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWLu7Jy6zdmiXU%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FBF52-143K?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWL6Fe7lsg%2FFzw%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FTE52-19K2?qs=xZ%2FP%252Ba9zWqaqn%252BDY6CDuyw%3D%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FTF52-600K?qs=sGAEpiMZZMsPqMdJzcrNwqpmsrDQJrmx3rHlUVuxZ%2FaYEY4oT6P4Yg%3D%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FTE52-140K?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWLgNLXyHZkbKU%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-12FTE52-19K?qs=sGAEpiMZZMsPqMdJzcrNwqpmsrDQJrmxlYYNIng8obZT75H5pLquCg%3D%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FBF52-576K?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWLcL5BVDOeExM%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-12FTF52-100K?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWL3GVOiMccmLA%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FBF52-33K2?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWLaU%252BtxKEo2c4%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FTE52-56K?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWLAXP5ldnKcZI%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FRF52-48K7?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWLdfj%252BeMU3vgI%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FTE52-66K5?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWLU%2FLs51ILg5E%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FBF52-57K6?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWLZc4q5SP8nCM%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FTE52-324K?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWLa%252Bd6RhdWolE%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FBF52-162K?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWLuQHAVLCqkm8%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FRF52-78K7?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWLpw24GLtACaE%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FBF52-26K7?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWLfMywfJ5hhJ4%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FBF52-59K?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWLUVGuYzHfdhA%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FBF52-7K87?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWLrQFfkSJN9iA%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FBF52-243K?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWLibTMlLr%252BMwQ%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FBF52-107K?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWLI5pDBNrCUBI%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FBF52-14K7?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWLHxO13joWOqI%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FTF52-453K?qs=sGAEpiMZZMsPqMdJzcrNwoMVoLRhO46JNTzoU4A7mPqrrcPWwVh6Ug%3D%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FTF52-7K3?qs=xZ%2FP%252Ba9zWqZg%2FHzponmImA%3D%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FRF52-2K87?qs=sGAEpiMZZMsPqMdJzcrNwsMt%252BTupSSYjJQ%2FQGxQHoP8%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FBF52-95K3?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWL08Z1ESWg%252BHo%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FBF52-4K02?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWLYpQNTL6%2FrRU%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FBF52-383K?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWLC4DDOXygom8%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FBF52-11K5?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWLmPex%252BRZRyHU%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FBF52-22K6?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWLheW65%252BIyBGU%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FRF52-8K06?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWLgHp6Ktvnuas%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FBF52-4K32?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWL904SEvVYEqM%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FRF52-19K6?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWLYCnE65764HQ%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FRF52-10K5?qs=sGAEpiMZZMsPqMdJzcrNwsMt%252BTupSSYjSfrSYPK%2FjDA%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FBF52-309K?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWLIiIIHbDRC1U%3D</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -262,55 +115,196 @@
     <t>C6</t>
   </si>
   <si>
-    <t>https://www.mouser.ca/ProductDetail/KEMET/R82EC2470AA60J?qs=Jv4FAWB%252B0HZ7iV08qIayRQ%3D%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/KEMET/R82EC2270DQ50J?qs=Jv4FAWB%252B0HZvsaU83gp7aA%3D%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/KEMET/R82IC2750DQ50J?qs=Jv4FAWB%252B0Hay7Xg1QVvwZA%3D%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/KEMET/R82EC1680AA50J?qs=Jv4FAWB%252B0HYqZ5SSAUehwg%3D%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/Panasonic/ECW-HA3C243J?qs=Qtr4Kn8gT99qCmDlHSUg%2FA%3D%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/KEMET/R82EC1470AA50J?qs=Jv4FAWB%252B0HbarvYaCHIS7Q%3D%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/KEMET/R82EC1330JE50J?qs=Jv4FAWB%252B0HaKxYy7WO79fg%3D%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/Panasonic/ECW-HA3C622H?qs=alij%252Bcw9eGAgau2Xq4ECcg%3D%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/Panasonic/ECW-HA3C162J4?qs=Qtr4Kn8gT992Q7YG%2Ff1p5g%3D%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/KEMET/R82EC1100Z350J?qs=lDWqi%2FyC4HJfno26FHExPA%3D%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/Panasonic/ECW-HA3C302J4?qs=Qtr4Kn8gT9%252BZ4p5F1qsqKA%3D%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FBF52-402K?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWL8Ad6fBGB2S0%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/Panasonic/ECW-HA3C133J?qs=Qtr4Kn8gT99ASgbewS4Hog%3D%3D</t>
-  </si>
-  <si>
     <t xml:space="preserve">Price </t>
   </si>
   <si>
     <t xml:space="preserve">Link </t>
   </si>
   <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FBF52-137K?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWLIshtPH5zdIw%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FBF52-37K4?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWLdLZun4bPFoQ%3D</t>
+    <t>https://www.mouser.ca/ProductDetail/Panasonic/ERJ-1GNF8452C?qs=nuXzIS8loXH90W30k0dNHQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/RC0201FR-0748K7L?qs=Q4gDqC5t5%2FBg%252BbTLyGfzlg%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/RC0201FR-0722K6L?qs=Q4gDqC5t5%2FDfKfQWyU4%252BiA%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/KOA-Speer/RK73H1HTTC8061F?qs=Dja1%252By9mYNKiO6TQkm%2F1Qw%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/RC0201FR-074K32L?qs=1s%252BlIcjv25vWx%252BqK4%252BbArw%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/RC0201FR-0737K4L?qs=1s%252BlIcjv25v1ASuLT00nyQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/RC0201FR-0719K6L?qs=Q4gDqC5t5%2FAXYnwJ%2F1LJ1w%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/RC0201FR-0710K7L?qs=LWWr1WFOkdGbwvvDW%252BwafA%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/KOA-Speer/RK73H1HTTC9092F?qs=K9FXhptayOvRgFqv3pmI9w%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/RC0201FR-0784K5L?qs=1s%252BlIcjv25t7dHWc8JnGTg%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/RC0201FR-07160KL?qs=NgbZBzc1CyGM1lealcn2TQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/RC0201FR-07169KL?qs=Q4gDqC5t5%2FBd%252B5gHVZ%2FcRA%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/RC0201FR-07402KL?qs=Q4gDqC5t5%2FDWgIVAW5QfCg%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Panasonic/ERJ-1GNF8662C?qs=nuXzIS8loXFlDwYbF78RCg%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Panasonic/ERJ-1GNF3572C?qs=nuXzIS8loXFaHLbgYRQyPw%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/RC0201FR-07110KL?qs=Q4gDqC5t5%2FAYMQb655YGSA%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/RC0201FR-07162KL?qs=Q4gDqC5t5%2FCzgdxtz4wrrA%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/RC0201FR-07118KL?qs=1s%252BlIcjv25uY2DxzYONL5w%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/RC0201FR-0763K4L?qs=1s%252BlIcjv25tcwt7EbFMNIQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/RC0201FR-0762KL?qs=T5Xi1deG72hwzuQVNbjwYA%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/RC0201FR-07309KL?qs=1s%252BlIcjv25t7XHsqr7bZEw%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/RC0201FR-0764R9L?qs=Q4gDqC5t5%2FDobIVFw2xGCg%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/RC0201FR-0766K5L?qs=1s%252BlIcjv25vToHi13h0JHg%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/RC0201FR-07332KL?qs=HhvughMb5%252BURbSQZhHaoLw%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/RC0201FR-07137KL?qs=1s%252BlIcjv25suoh06l3U6mg%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/RC0201FR-0745R3L?qs=1s%252BlIcjv25saSg5DxZFouA%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/RC0201FR-07270KL?qs=sxZXDnvRBEjqiXYlj%252BIzJA%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Panasonic/ERJ-1GNF1433C?qs=nuXzIS8loXHVPsmeBHcD%252BQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/RC0201FR-0719K1L?qs=1s%252BlIcjv25vfzjam%2FKVxpA%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/RC0201FR-07590KL?qs=Q4gDqC5t5%2FBLTR4MNkVktg%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Panasonic/ERJ-1GNF1403C?qs=nuXzIS8loXGdtW17oc3Kzw%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/RC0201FR-07576KL?qs=1s%252BlIcjv25t%2FGP%252B8%2FDjPGA%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/RC0201FR-07100KL?qs=H0f9D%252BN4ztJ6ZeeQPytEvw%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Panasonic/ERJ-1GNF3322C?qs=nuXzIS8loXHtnTwUK3SGyw%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/RC0201FR-0756KL?qs=sxZXDnvRBEj4gOv2%252BGTV5g%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/RC0201FR-0757K6L?qs=1s%252BlIcjv25uRlaWtBM4hww%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/RC0201FR-07324KL?qs=1s%252BlIcjv25ufPeVyPisNow%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/RC0201FR-0778K7L?qs=HhvughMb5%252BV89D4KqxZ6NQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/KOA-Speer/RK73H1HTTC2672F?qs=Dja1%252By9mYNIHc8loCF4sQQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/RC0201FR-0759KL?qs=Q4gDqC5t5%2FBHW0Rk%2FMhAYg%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/RC0201FR-077K87L?qs=Q4gDqC5t5%2FA%252BVn2QozfPPQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/RC0201FR-07243KL?qs=1s%252BlIcjv25u7f0t4i6xCgQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/RC0201FR-07107KL?qs=LWWr1WFOkdHH5Rp94xr4Iw%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/KOA-Speer/RK73H1HTTC1472F?qs=iMOwM72IGIthAR8zl912DA%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/RC0201FR-07453KL?qs=1s%252BlIcjv25sZ2i87AF%252BnmQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/RC0201FR-077K32L?qs=1s%252BlIcjv25uU326Z4WHoJw%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Vishay-Dale/CRCW02012K87FNED?qs=DyUWGjl%252BcVtI7guDtDR79g%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/RC0201FR-0795K3L?qs=Q4gDqC5t5%2FBLLeKdNYvlFQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/AC0201FR-074K02L?qs=NgbZBzc1CyFZdTchJUi9Lg%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/RC0201FR-07383KL?qs=Q4gDqC5t5%2FDHT%2FrVRi5gbA%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Murata-Electronics/GRM033R60J473JE19D?qs=2W5sgKM%2F371oABOEgqyRPQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Murata-Electronics/GRM31M7U1H753JA01L?qs=MY6wChARw2ziD9B8PoiLnw%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Murata-Electronics/GRM155R71A273JA01J?qs=QzBtWTOodeUtk%252B%2FBGtTKUw%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Murata-Electronics/GRM155R71E133JA61D?qs=IPQhFcwEUOjuw1uZ1gniBw%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Murata-Electronics/GRM033R61A682JA01D?qs=2W5sgKM%2F3702xblnCTl4Dw%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Kyocera-AVX/08051C243JAT2A?qs=TmFcSEGKcGVzRC3S3hofTg%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Murata-Electronics/GRM033R71A472JA01D?qs=2W5sgKM%2F370cXAKpGxiVIg%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Murata-Electronics/GRM033R71A332JA01D?qs=2W5sgKM%2F370phi8a2ERuFA%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Murata-Electronics/GRM2195C1H622JA01D?qs=3Vu9ppaVHS7Zec7lWvNffA%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Murata-Electronics/GRM1885C1H162JA01D?qs=2YjXvJr3xvj9dMpk%252BcTsdg%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Murata-Electronics/GRM0335C1E102JA01D?qs=jHkklCh7amiSnRIIKCexXw%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Murata-Electronics/GRM155R71H302JA01D?qs=IPQhFcwEUOge2e%252BWJcpNPw%3D%3D</t>
   </si>
 </sst>
 </file>
@@ -707,7 +701,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -723,19 +717,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>86</v>
+        <v>24</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>87</v>
+        <v>25</v>
       </c>
       <c r="G1" s="1"/>
     </row>
@@ -754,15 +748,15 @@
         <v>0.11820330969266468</v>
       </c>
       <c r="E2" s="2">
-        <v>0.152</v>
+        <v>0.16600000000000001</v>
       </c>
       <c r="F2" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>160</v>
@@ -778,12 +772,12 @@
         <v>0.16600000000000001</v>
       </c>
       <c r="F3" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>169</v>
@@ -799,12 +793,12 @@
         <v>0.16600000000000001</v>
       </c>
       <c r="F4" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>90</v>
@@ -820,12 +814,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>37</v>
@@ -841,12 +835,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F6" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>405</v>
@@ -859,15 +853,15 @@
         <v>0.7407407407407407</v>
       </c>
       <c r="E7" s="2">
-        <v>0.152</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F7" t="s">
-        <v>84</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>86.7</v>
@@ -880,15 +874,15 @@
         <v>0.11534025374856807</v>
       </c>
       <c r="E8" s="2">
-        <v>0.13800000000000001</v>
+        <v>0.16600000000000001</v>
       </c>
       <c r="F8" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>35.6</v>
@@ -901,15 +895,15 @@
         <v>0.28089887640449834</v>
       </c>
       <c r="E9" s="2">
-        <v>0.152</v>
+        <v>0.16600000000000001</v>
       </c>
       <c r="F9" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>390</v>
@@ -925,12 +919,12 @@
         <v>0.152</v>
       </c>
       <c r="F10" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>64</v>
+        <v>15</v>
       </c>
       <c r="D11">
         <f>SUM(D2:D10)</f>
@@ -938,7 +932,7 @@
       </c>
       <c r="E11" s="2">
         <f>SUM(E2:E10)</f>
-        <v>1.3539999999999999</v>
+        <v>1.3959999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -946,122 +940,122 @@
         <v>0</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>65</v>
+        <v>16</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>66</v>
+        <v>17</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>86</v>
+        <v>24</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>87</v>
+        <v>25</v>
       </c>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>67</v>
+        <v>18</v>
       </c>
       <c r="B14">
         <v>47</v>
       </c>
       <c r="E14" s="2">
-        <v>0.373</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F14" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>68</v>
+        <v>19</v>
       </c>
       <c r="B15">
         <v>47</v>
       </c>
       <c r="E15" s="2">
-        <v>0.373</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F15" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>69</v>
+        <v>20</v>
       </c>
       <c r="B16">
         <v>27</v>
       </c>
       <c r="E16" s="2">
-        <v>0.35899999999999999</v>
+        <v>0.152</v>
       </c>
       <c r="F16" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>70</v>
+        <v>21</v>
       </c>
       <c r="B17">
         <v>27</v>
       </c>
       <c r="E17" s="2">
-        <v>0.35899999999999999</v>
+        <v>0.152</v>
       </c>
       <c r="F17" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>71</v>
+        <v>22</v>
       </c>
       <c r="B18">
         <v>75</v>
       </c>
       <c r="E18" s="2">
-        <v>0.82799999999999996</v>
+        <v>0.75900000000000001</v>
       </c>
       <c r="F18" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>72</v>
+        <v>23</v>
       </c>
       <c r="B19">
         <v>75</v>
       </c>
       <c r="E19" s="2">
-        <v>0.82799999999999996</v>
+        <v>0.75900000000000001</v>
       </c>
       <c r="F19" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>64</v>
+        <v>15</v>
       </c>
       <c r="E20" s="2">
         <f>SUM(E14:E19)</f>
-        <v>3.1199999999999997</v>
+        <v>2.0979999999999999</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>64</v>
+        <v>15</v>
       </c>
       <c r="E22" s="2">
         <f>E11+E20</f>
-        <v>4.4739999999999993</v>
+        <v>3.4939999999999998</v>
       </c>
     </row>
   </sheetData>
@@ -1076,7 +1070,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="E19" sqref="E19:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1092,19 +1086,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>86</v>
+        <v>24</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>87</v>
+        <v>25</v>
       </c>
       <c r="G1" s="1"/>
     </row>
@@ -1116,22 +1110,22 @@
         <v>111</v>
       </c>
       <c r="C2">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D2">
         <f>100*ABS(B2-C2)/B2</f>
-        <v>0</v>
+        <v>0.90090090090090091</v>
       </c>
       <c r="E2" s="2">
         <v>0.13800000000000001</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>90.7</v>
@@ -1147,12 +1141,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>163</v>
@@ -1165,15 +1159,15 @@
         <v>0.61349693251533743</v>
       </c>
       <c r="E4" s="2">
-        <v>0.16600000000000001</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>118</v>
@@ -1189,12 +1183,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>63.5</v>
@@ -1210,12 +1204,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F6" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>62.2</v>
@@ -1231,12 +1225,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F7" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>312</v>
@@ -1252,12 +1246,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F8" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>67.599999999999994</v>
@@ -1270,15 +1264,15 @@
         <v>0.59171597633136941</v>
       </c>
       <c r="E9" s="2">
-        <v>0.152</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F9" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>66.2</v>
@@ -1294,12 +1288,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F10" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B11">
         <v>332</v>
@@ -1312,23 +1306,23 @@
         <v>0</v>
       </c>
       <c r="E11" s="2">
-        <v>0.16600000000000001</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F11" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>64</v>
+        <v>15</v>
       </c>
       <c r="D12">
         <f>SUM(D2:D11)</f>
-        <v>3.3194544656269094</v>
+        <v>4.2203553665278104</v>
       </c>
       <c r="E12" s="2">
         <f>SUM(E2:E11)</f>
-        <v>1.4500000000000002</v>
+        <v>1.38</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1336,129 +1330,126 @@
         <v>0</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>65</v>
+        <v>16</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>66</v>
+        <v>17</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>86</v>
+        <v>24</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>87</v>
+        <v>25</v>
       </c>
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>67</v>
+        <v>18</v>
       </c>
       <c r="B15">
         <v>13</v>
       </c>
       <c r="E15" s="2">
-        <v>1.1499999999999999</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F15" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>68</v>
+        <v>19</v>
       </c>
       <c r="B16">
         <v>13</v>
       </c>
       <c r="E16" s="2">
-        <v>1.1499999999999999</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F16" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>69</v>
+        <v>20</v>
       </c>
       <c r="B17">
         <v>6.8</v>
       </c>
       <c r="E17" s="2">
-        <v>0.33100000000000002</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F17" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>70</v>
+        <v>21</v>
       </c>
       <c r="B18">
         <v>6.8</v>
       </c>
       <c r="E18" s="2">
-        <v>0.33100000000000002</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F18" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>71</v>
+        <v>22</v>
       </c>
       <c r="B19">
         <v>24</v>
       </c>
       <c r="E19" s="2">
-        <v>1.48</v>
+        <v>0.45500000000000002</v>
       </c>
       <c r="F19" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>72</v>
+        <v>23</v>
       </c>
       <c r="B20">
         <v>24</v>
       </c>
       <c r="E20" s="2">
-        <v>1.48</v>
+        <v>0.45500000000000002</v>
       </c>
       <c r="F20" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>64</v>
+        <v>15</v>
       </c>
       <c r="E21" s="2">
         <f>SUM(E15:E20)</f>
-        <v>5.9220000000000006</v>
+        <v>1.4620000000000002</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>64</v>
+        <v>15</v>
       </c>
       <c r="E23" s="2">
         <f>E12+E21</f>
-        <v>7.3720000000000008</v>
+        <v>2.8420000000000001</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="F5" r:id="rId1" xr:uid="{7C4A873B-76ED-4822-8A83-F29474C12A63}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1468,7 +1459,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="E18" sqref="E18:E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1484,19 +1475,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>86</v>
+        <v>24</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>87</v>
+        <v>25</v>
       </c>
       <c r="G1" s="1"/>
     </row>
@@ -1518,12 +1509,12 @@
         <v>0.16600000000000001</v>
       </c>
       <c r="F2" t="s">
-        <v>88</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>45.1</v>
@@ -1539,12 +1530,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F3" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>271</v>
@@ -1560,12 +1551,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F4" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>142</v>
@@ -1578,57 +1569,57 @@
         <v>0.70422535211267601</v>
       </c>
       <c r="E5" s="2">
-        <v>0.13800000000000001</v>
+        <v>0.16600000000000001</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>19.2</v>
       </c>
       <c r="C6">
-        <v>19.2</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.52083333333332227</v>
       </c>
       <c r="E6" s="2">
-        <v>0.152</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F6" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>595</v>
       </c>
       <c r="C7">
-        <v>600</v>
+        <v>590</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
         <v>0.84033613445378152</v>
       </c>
       <c r="E7" s="2">
-        <v>0.152</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F7" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>139</v>
@@ -1644,33 +1635,33 @@
         <v>0.16600000000000001</v>
       </c>
       <c r="F8" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>18.899999999999999</v>
       </c>
       <c r="C9">
-        <v>19</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>0.52910052910053662</v>
+        <v>1.0582010582010732</v>
       </c>
       <c r="E9" s="2">
         <v>0.13800000000000001</v>
       </c>
       <c r="F9" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>583</v>
@@ -1683,23 +1674,23 @@
         <v>1.2006861063464838</v>
       </c>
       <c r="E10" s="2">
-        <v>0.13800000000000001</v>
+        <v>0.16600000000000001</v>
       </c>
       <c r="F10" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>64</v>
+        <v>15</v>
       </c>
       <c r="D11">
         <f>SUM(D2:D10)</f>
-        <v>6.2877167340078506</v>
+        <v>7.3376505964417094</v>
       </c>
       <c r="E11" s="2">
         <f>SUM(E2:E10)</f>
-        <v>1.3260000000000001</v>
+        <v>1.3540000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1707,122 +1698,122 @@
         <v>0</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>65</v>
+        <v>16</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>66</v>
+        <v>17</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>86</v>
+        <v>24</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>87</v>
+        <v>25</v>
       </c>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>67</v>
+        <v>18</v>
       </c>
       <c r="B14">
         <v>4.7</v>
       </c>
       <c r="E14" s="2">
-        <v>0.28999999999999998</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F14" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>68</v>
+        <v>19</v>
       </c>
       <c r="B15">
         <v>4.7</v>
       </c>
       <c r="E15" s="2">
-        <v>0.28999999999999998</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F15" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>69</v>
+        <v>20</v>
       </c>
       <c r="B16">
         <v>3.3</v>
       </c>
       <c r="E16" s="2">
-        <v>0.317</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F16" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>70</v>
+        <v>21</v>
       </c>
       <c r="B17">
         <v>3.3</v>
       </c>
       <c r="E17" s="2">
-        <v>0.317</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F17" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>71</v>
+        <v>22</v>
       </c>
       <c r="B18">
         <v>6.2</v>
       </c>
       <c r="E18" s="2">
-        <v>0.99399999999999999</v>
+        <v>0.42799999999999999</v>
       </c>
       <c r="F18" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>72</v>
+        <v>23</v>
       </c>
       <c r="B19">
         <v>6.2</v>
       </c>
       <c r="E19" s="2">
-        <v>0.99399999999999999</v>
+        <v>0.42799999999999999</v>
       </c>
       <c r="F19" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>64</v>
+        <v>15</v>
       </c>
       <c r="E20" s="2">
         <f>SUM(E14:E19)</f>
-        <v>3.202</v>
+        <v>1.4079999999999999</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>64</v>
+        <v>15</v>
       </c>
       <c r="E22" s="2">
         <f>E11+E20</f>
-        <v>4.5280000000000005</v>
+        <v>2.762</v>
       </c>
     </row>
   </sheetData>
@@ -1835,7 +1826,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="E17" sqref="E17:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1851,19 +1842,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>86</v>
+        <v>24</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>87</v>
+        <v>25</v>
       </c>
       <c r="G1" s="1"/>
     </row>
@@ -1885,12 +1876,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F2" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>99.2</v>
@@ -1906,12 +1897,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F3" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>65.8</v>
@@ -1927,12 +1918,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F4" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>33.200000000000003</v>
@@ -1948,12 +1939,12 @@
         <v>0.16600000000000001</v>
       </c>
       <c r="F5" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>55.9</v>
@@ -1966,15 +1957,15 @@
         <v>0.17889087656529773</v>
       </c>
       <c r="E6" s="2">
-        <v>0.152</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F6" t="s">
-        <v>38</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>48.6</v>
@@ -1987,15 +1978,15 @@
         <v>0.2057613168724309</v>
       </c>
       <c r="E7" s="2">
-        <v>0.16600000000000001</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F7" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>271</v>
@@ -2011,12 +2002,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F8" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>67</v>
@@ -2029,15 +2020,15 @@
         <v>0.74626865671641796</v>
       </c>
       <c r="E9" s="2">
-        <v>0.16600000000000001</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F9" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>58.2</v>
@@ -2053,12 +2044,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F10" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B11">
         <v>325</v>
@@ -2071,15 +2062,15 @@
         <v>0.30769230769230771</v>
       </c>
       <c r="E11" s="2">
-        <v>0.16600000000000001</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F11" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>64</v>
+        <v>15</v>
       </c>
       <c r="D12">
         <f>SUM(D2:D11)</f>
@@ -2087,7 +2078,7 @@
       </c>
       <c r="E12" s="2">
         <f>SUM(E2:E11)</f>
-        <v>1.5059999999999998</v>
+        <v>1.4079999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2095,122 +2086,122 @@
         <v>0</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>65</v>
+        <v>16</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>66</v>
+        <v>17</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>86</v>
+        <v>24</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>87</v>
+        <v>25</v>
       </c>
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>67</v>
+        <v>18</v>
       </c>
       <c r="B15">
         <v>1.6</v>
       </c>
       <c r="E15" s="2">
-        <v>1.04</v>
+        <v>0.17899999999999999</v>
       </c>
       <c r="F15" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>68</v>
+        <v>19</v>
       </c>
       <c r="B16">
         <v>1.6</v>
       </c>
       <c r="E16" s="2">
-        <v>1.04</v>
+        <v>0.17899999999999999</v>
       </c>
       <c r="F16" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>69</v>
+        <v>20</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="E17" s="2">
-        <v>0.152</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F17" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>70</v>
+        <v>21</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="E18" s="2">
-        <v>0.152</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F18" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>71</v>
+        <v>22</v>
       </c>
       <c r="B19">
         <v>3</v>
       </c>
       <c r="E19" s="2">
-        <v>1.01</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F19" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>72</v>
+        <v>23</v>
       </c>
       <c r="B20">
         <v>3</v>
       </c>
       <c r="E20" s="2">
-        <v>1.01</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F20" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>64</v>
+        <v>15</v>
       </c>
       <c r="E21" s="2">
         <f>SUM(E15:E20)</f>
-        <v>4.4039999999999999</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>64</v>
+        <v>15</v>
       </c>
       <c r="E23" s="2">
         <f>E12+E21</f>
-        <v>5.91</v>
+        <v>2.3180000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -2223,7 +2214,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="E14" sqref="E14:F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2239,19 +2230,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>86</v>
+        <v>24</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>87</v>
+        <v>25</v>
       </c>
       <c r="G1" s="1"/>
     </row>
@@ -2270,15 +2261,15 @@
         <v>1.0062893081760971</v>
       </c>
       <c r="E2" s="2">
-        <v>0.16600000000000001</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F2" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>26.5</v>
@@ -2291,15 +2282,15 @@
         <v>0.75471698113207275</v>
       </c>
       <c r="E3" s="2">
-        <v>0.13800000000000001</v>
+        <v>0.16600000000000001</v>
       </c>
       <c r="F3" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>159</v>
@@ -2312,15 +2303,15 @@
         <v>0.62893081761006286</v>
       </c>
       <c r="E4" s="2">
-        <v>0.16600000000000001</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F4" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>58.6</v>
@@ -2336,12 +2327,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F5" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>7.94</v>
@@ -2357,12 +2348,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F6" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>245</v>
@@ -2375,15 +2366,15 @@
         <v>0.81632653061224492</v>
       </c>
       <c r="E7" s="2">
-        <v>0.16600000000000001</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F7" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>108</v>
@@ -2399,12 +2390,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F8" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>14.6</v>
@@ -2420,12 +2411,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F9" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>452</v>
@@ -2438,15 +2429,15 @@
         <v>0.22123893805309736</v>
       </c>
       <c r="E10" s="2">
-        <v>0.152</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F10" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>64</v>
+        <v>15</v>
       </c>
       <c r="D11">
         <f>SUM(D2:D10)</f>
@@ -2454,7 +2445,7 @@
       </c>
       <c r="E11" s="2">
         <f>SUM(E2:E10)</f>
-        <v>1.34</v>
+        <v>1.27</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2462,122 +2453,122 @@
         <v>0</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>65</v>
+        <v>16</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>66</v>
+        <v>17</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>86</v>
+        <v>24</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>87</v>
+        <v>25</v>
       </c>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>67</v>
+        <v>18</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="E14" s="2">
-        <v>0.152</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F14" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>68</v>
+        <v>19</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="E15" s="2">
-        <v>0.152</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F15" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>69</v>
+        <v>20</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="E16" s="2">
-        <v>0.152</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F16" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>70</v>
+        <v>21</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="E17" s="2">
-        <v>0.152</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F17" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>71</v>
+        <v>22</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="E18" s="2">
-        <v>0.152</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F18" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>72</v>
+        <v>23</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="E19" s="2">
-        <v>0.152</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F19" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>64</v>
+        <v>15</v>
       </c>
       <c r="E20" s="2">
         <f>SUM(E14:E19)</f>
-        <v>0.91200000000000003</v>
+        <v>0.82800000000000007</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>64</v>
+        <v>15</v>
       </c>
       <c r="E22" s="2">
         <f>E11+E20</f>
-        <v>2.2520000000000002</v>
+        <v>2.0979999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -2590,7 +2581,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="E14" sqref="E14:F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2606,19 +2597,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>86</v>
+        <v>24</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>87</v>
+        <v>25</v>
       </c>
       <c r="G1" s="1"/>
     </row>
@@ -2637,36 +2628,36 @@
         <v>1.0062893081760971</v>
       </c>
       <c r="E2" s="2">
-        <v>0.16600000000000001</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F2" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>7.24</v>
       </c>
       <c r="C3">
-        <v>7.3</v>
+        <v>7.32</v>
       </c>
       <c r="D3">
         <f t="shared" si="0"/>
-        <v>0.82872928176795035</v>
+        <v>1.1049723756906087</v>
       </c>
       <c r="E3" s="2">
-        <v>0.152</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F3" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>159</v>
@@ -2682,12 +2673,12 @@
         <v>0.16600000000000001</v>
       </c>
       <c r="F4" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>66.599999999999994</v>
@@ -2703,12 +2694,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F5" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>2.85</v>
@@ -2721,15 +2712,15 @@
         <v>0.70175438596491291</v>
       </c>
       <c r="E6" s="2">
-        <v>0.13800000000000001</v>
+        <v>0.16600000000000001</v>
       </c>
       <c r="F6" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>271</v>
@@ -2745,12 +2736,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F7" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>94.9</v>
@@ -2766,12 +2757,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F8" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>4.0599999999999996</v>
@@ -2787,12 +2778,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F9" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>386</v>
@@ -2807,21 +2798,21 @@
       <c r="E10" s="2">
         <v>0.13800000000000001</v>
       </c>
-      <c r="F10" t="s">
-        <v>56</v>
+      <c r="F10" s="3" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>64</v>
+        <v>15</v>
       </c>
       <c r="D11">
         <f>SUM(D2:D10)</f>
-        <v>5.8687776930290356</v>
+        <v>6.1450207869516928</v>
       </c>
       <c r="E11" s="2">
         <f>SUM(E2:E10)</f>
-        <v>1.3119999999999998</v>
+        <v>1.298</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2829,124 +2820,127 @@
         <v>0</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>65</v>
+        <v>16</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>66</v>
+        <v>17</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>86</v>
+        <v>24</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>87</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>67</v>
+        <v>18</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="E14" s="2">
-        <v>0.152</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F14" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>68</v>
+        <v>19</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="E15" s="2">
-        <v>0.152</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F15" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>69</v>
+        <v>20</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="E16" s="2">
-        <v>0.152</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F16" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>70</v>
+        <v>21</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="E17" s="2">
-        <v>0.152</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F17" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>71</v>
+        <v>22</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="E18" s="2">
-        <v>0.152</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F18" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>72</v>
+        <v>23</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="E19" s="2">
-        <v>0.152</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F19" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>64</v>
+        <v>15</v>
       </c>
       <c r="E20" s="2">
         <f>SUM(E14:E19)</f>
-        <v>0.91200000000000003</v>
+        <v>0.82800000000000007</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>64</v>
+        <v>15</v>
       </c>
       <c r="E22" s="2">
         <f>E11+E20</f>
-        <v>2.2239999999999998</v>
+        <v>2.1260000000000003</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F10" r:id="rId1" xr:uid="{F4013F7B-2BF5-48F6-B2FD-018004F8799F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2956,7 +2950,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2972,19 +2966,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>86</v>
+        <v>24</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>87</v>
+        <v>25</v>
       </c>
       <c r="G1" s="1"/>
     </row>
@@ -3003,15 +2997,15 @@
         <v>0.87719298245613719</v>
       </c>
       <c r="E2" s="2">
-        <v>0.13800000000000001</v>
+        <v>0.16600000000000001</v>
       </c>
       <c r="F2" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>48.8</v>
@@ -3024,15 +3018,15 @@
         <v>0.20491803278687362</v>
       </c>
       <c r="E3" s="2">
-        <v>0.16600000000000001</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F3" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>22.7</v>
@@ -3048,12 +3042,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F4" t="s">
-        <v>58</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>8.02</v>
@@ -3066,15 +3060,15 @@
         <v>0.49875311720699411</v>
       </c>
       <c r="E5" s="2">
-        <v>0.16600000000000001</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F5" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>4.3499999999999996</v>
@@ -3087,15 +3081,15 @@
         <v>0.68965517241377849</v>
       </c>
       <c r="E6" s="2">
-        <v>0.16600000000000001</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F6" t="s">
-        <v>60</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>37</v>
@@ -3111,12 +3105,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F7" t="s">
-        <v>89</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>19.600000000000001</v>
@@ -3129,36 +3123,36 @@
         <v>0</v>
       </c>
       <c r="E8" s="2">
-        <v>0.17899999999999999</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F8" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>10.6</v>
       </c>
       <c r="C9">
-        <v>10.5</v>
+        <v>10.7</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
         <v>0.94339622641509102</v>
       </c>
       <c r="E9" s="2">
-        <v>0.16600000000000001</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F9" t="s">
-        <v>62</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>90.5</v>
@@ -3174,12 +3168,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F10" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>64</v>
+        <v>15</v>
       </c>
       <c r="D11">
         <f>SUM(D2:D10)</f>
@@ -3187,7 +3181,7 @@
       </c>
       <c r="E11" s="2">
         <f>SUM(E2:E10)</f>
-        <v>1.395</v>
+        <v>1.27</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3195,121 +3189,118 @@
         <v>0</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>65</v>
+        <v>16</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>66</v>
+        <v>17</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>86</v>
+        <v>24</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>87</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>67</v>
+        <v>18</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="E14" s="2">
-        <v>0.152</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F14" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>68</v>
+        <v>19</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="E15" s="2">
-        <v>0.152</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F15" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>69</v>
+        <v>20</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="E16" s="2">
-        <v>0.152</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F16" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>70</v>
+        <v>21</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="E17" s="2">
-        <v>0.152</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F17" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>71</v>
+        <v>22</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="E18" s="2">
-        <v>0.152</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F18" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>72</v>
+        <v>23</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="E19" s="2">
-        <v>0.152</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F19" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>64</v>
-      </c>
-      <c r="E20" s="2">
-        <f>SUM(E14:E19)</f>
-        <v>0.91200000000000003</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="E20" s="2"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>64</v>
+        <v>15</v>
       </c>
       <c r="E22" s="2">
         <f>E11+E20</f>
-        <v>2.3069999999999999</v>
+        <v>1.27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Case code (mm) and datasheet links for all resistors and capacitors in Sub-bass and Bass filters in the BOM excel file
</commit_message>
<xml_diff>
--- a/Documents/BOM.xlsx
+++ b/Documents/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ECE_Projects\Music_Visualizer\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CA6424E-C989-452F-8F6C-1B7447174F59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9D97B15-C5C5-43AF-8C5B-6D610BF8BDB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{1F4A7036-4694-4970-BB5D-7CBECC831452}"/>
+    <workbookView xWindow="-3720" yWindow="1776" windowWidth="8856" windowHeight="4800" activeTab="1" xr2:uid="{1F4A7036-4694-4970-BB5D-7CBECC831452}"/>
   </bookViews>
   <sheets>
     <sheet name="Sub-Bass" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="102">
   <si>
     <t>Component</t>
   </si>
@@ -73,9 +73,6 @@
     <t>R9</t>
   </si>
   <si>
-    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FTE52-390K?qs=sGAEpiMZZMsPqMdJzcrNwiweiCzxKzWLe1tTBDHIIqQ%3D</t>
-  </si>
-  <si>
     <t>Percentage Diff</t>
   </si>
   <si>
@@ -305,6 +302,51 @@
   </si>
   <si>
     <t>https://www.mouser.ca/ProductDetail/Murata-Electronics/GRM155R71H302JA01D?qs=IPQhFcwEUOge2e%252BWJcpNPw%3D%3D</t>
+  </si>
+  <si>
+    <t>Case Code (mm)</t>
+  </si>
+  <si>
+    <t>Datasheet</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf</t>
+  </si>
+  <si>
+    <t>0603</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/datasheet/2/219/RK73H-1825326.pdf</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/datasheet/2/315/AOA0000C304-1149620.pdf</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/KOA-Speer/RK73H1HTTC3903F?qs=sGAEpiMZZMvdGkrng054t%252BxQCaKQW4HiYbuNpmvjLME%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/datasheet/2/281/1/GRM033R60J473JE19_01A-1981825.pdf</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/datasheet/2/281/1/GRM155R71A273JA01_02A-1983900.pdf</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/datasheet/2/281/1/GRM31M7U1H753JA01_01A-1987984.pdf</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/datasheet/2/447/PYu_AC_51_RoHS_L_7-1714230.pdf</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/datasheet/2/281/murata_03052018_GRM_Series_1-1310166.pdf</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/datasheet/2/281/1/GRM033R61A682JA01_01A-1981870.pdf</t>
+  </si>
+  <si>
+    <t>2012</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/datasheet/2/40/X7RDielectric-777024.pdf</t>
   </si>
 </sst>
 </file>
@@ -375,12 +417,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -698,10 +746,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F8295C8-65E6-45FB-87E8-3A2215DAA9D2}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="G2" sqref="G2:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -710,30 +758,37 @@
     <col min="2" max="2" width="18.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="76.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="D1" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -751,10 +806,16 @@
         <v>0.16600000000000001</v>
       </c>
       <c r="F2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -772,10 +833,16 @@
         <v>0.16600000000000001</v>
       </c>
       <c r="F3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -793,10 +860,16 @@
         <v>0.16600000000000001</v>
       </c>
       <c r="F4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -814,10 +887,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -835,10 +914,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -856,10 +941,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -877,10 +968,16 @@
         <v>0.16600000000000001</v>
       </c>
       <c r="F8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -898,10 +995,16 @@
         <v>0.16600000000000001</v>
       </c>
       <c r="F9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -919,12 +1022,18 @@
         <v>0.152</v>
       </c>
       <c r="F10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11">
         <f>SUM(D2:D10)</f>
@@ -935,30 +1044,35 @@
         <v>1.3959999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>17</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>18</v>
       </c>
       <c r="B14">
         <v>47</v>
@@ -967,12 +1081,18 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F14" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15">
         <v>47</v>
@@ -981,12 +1101,18 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16">
         <v>27</v>
@@ -995,12 +1121,18 @@
         <v>0.152</v>
       </c>
       <c r="F16" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+      <c r="G16" s="6">
+        <v>1005</v>
+      </c>
+      <c r="H16" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B17">
         <v>27</v>
@@ -1009,12 +1141,18 @@
         <v>0.152</v>
       </c>
       <c r="F17" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+      <c r="G17" s="6">
+        <v>1005</v>
+      </c>
+      <c r="H17" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18">
         <v>75</v>
@@ -1023,12 +1161,18 @@
         <v>0.75900000000000001</v>
       </c>
       <c r="F18" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+      <c r="G18" s="6">
+        <v>3216</v>
+      </c>
+      <c r="H18" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19">
         <v>75</v>
@@ -1037,21 +1181,27 @@
         <v>0.75900000000000001</v>
       </c>
       <c r="F19" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+      <c r="G19" s="6">
+        <v>3216</v>
+      </c>
+      <c r="H19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E20" s="2">
         <f>SUM(E14:E19)</f>
         <v>2.0979999999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E22" s="2">
         <f>E11+E20</f>
@@ -1062,15 +1212,18 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="G2:G3" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9015A39E-4C3F-4E48-B877-A44E11CEB1FD}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19:E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1079,30 +1232,37 @@
     <col min="2" max="2" width="18.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="D1" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1120,10 +1280,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1141,10 +1307,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1162,10 +1334,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1183,10 +1361,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1204,10 +1388,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1225,10 +1415,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1246,10 +1442,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1267,10 +1469,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1288,12 +1496,18 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11">
         <v>332</v>
@@ -1309,12 +1523,18 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D12">
         <f>SUM(D2:D11)</f>
@@ -1325,30 +1545,35 @@
         <v>1.38</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>17</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>18</v>
       </c>
       <c r="B15">
         <v>13</v>
@@ -1357,12 +1582,18 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F15" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+      <c r="G15" s="6">
+        <v>1005</v>
+      </c>
+      <c r="H15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16">
         <v>13</v>
@@ -1371,12 +1602,18 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F16" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+      <c r="G16" s="6">
+        <v>1005</v>
+      </c>
+      <c r="H16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17">
         <v>6.8</v>
@@ -1385,12 +1622,18 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F17" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H17" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B18">
         <v>6.8</v>
@@ -1399,12 +1642,18 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F18" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H18" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B19">
         <v>24</v>
@@ -1413,12 +1662,18 @@
         <v>0.45500000000000002</v>
       </c>
       <c r="F19" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="H19" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20">
         <v>24</v>
@@ -1427,21 +1682,27 @@
         <v>0.45500000000000002</v>
       </c>
       <c r="F20" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="H20" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E21" s="2">
         <f>SUM(E15:E20)</f>
         <v>1.4620000000000002</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E23" s="2">
         <f>E12+E21</f>
@@ -1475,19 +1736,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="D1" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="G1" s="1"/>
     </row>
@@ -1509,7 +1770,7 @@
         <v>0.16600000000000001</v>
       </c>
       <c r="F2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -1530,7 +1791,7 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -1551,7 +1812,7 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -1572,7 +1833,7 @@
         <v>0.16600000000000001</v>
       </c>
       <c r="F5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1593,7 +1854,7 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1614,7 +1875,7 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -1635,7 +1896,7 @@
         <v>0.16600000000000001</v>
       </c>
       <c r="F8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -1656,7 +1917,7 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -1677,12 +1938,12 @@
         <v>0.16600000000000001</v>
       </c>
       <c r="F10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11">
         <f>SUM(D2:D10)</f>
@@ -1698,25 +1959,25 @@
         <v>0</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="D13" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14">
         <v>4.7</v>
@@ -1725,12 +1986,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15">
         <v>4.7</v>
@@ -1739,12 +2000,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16">
         <v>3.3</v>
@@ -1753,12 +2014,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B17">
         <v>3.3</v>
@@ -1767,12 +2028,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18">
         <v>6.2</v>
@@ -1781,12 +2042,12 @@
         <v>0.42799999999999999</v>
       </c>
       <c r="F18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19">
         <v>6.2</v>
@@ -1795,12 +2056,12 @@
         <v>0.42799999999999999</v>
       </c>
       <c r="F19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E20" s="2">
         <f>SUM(E14:E19)</f>
@@ -1809,7 +2070,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E22" s="2">
         <f>E11+E20</f>
@@ -1842,19 +2103,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="D1" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="G1" s="1"/>
     </row>
@@ -1876,7 +2137,7 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -1897,7 +2158,7 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -1918,7 +2179,7 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -1939,7 +2200,7 @@
         <v>0.16600000000000001</v>
       </c>
       <c r="F5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1960,7 +2221,7 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1981,7 +2242,7 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -2002,7 +2263,7 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -2023,7 +2284,7 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -2044,12 +2305,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11">
         <v>325</v>
@@ -2065,12 +2326,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D12">
         <f>SUM(D2:D11)</f>
@@ -2086,25 +2347,25 @@
         <v>0</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="D14" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15">
         <v>1.6</v>
@@ -2113,12 +2374,12 @@
         <v>0.17899999999999999</v>
       </c>
       <c r="F15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16">
         <v>1.6</v>
@@ -2127,12 +2388,12 @@
         <v>0.17899999999999999</v>
       </c>
       <c r="F16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -2141,12 +2402,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -2155,12 +2416,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B19">
         <v>3</v>
@@ -2169,12 +2430,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20">
         <v>3</v>
@@ -2183,12 +2444,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E21" s="2">
         <f>SUM(E15:E20)</f>
@@ -2197,7 +2458,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E23" s="2">
         <f>E12+E21</f>
@@ -2230,19 +2491,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="D1" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="G1" s="1"/>
     </row>
@@ -2264,7 +2525,7 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -2285,7 +2546,7 @@
         <v>0.16600000000000001</v>
       </c>
       <c r="F3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -2306,7 +2567,7 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -2327,7 +2588,7 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -2348,7 +2609,7 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -2369,7 +2630,7 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -2390,7 +2651,7 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -2411,7 +2672,7 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -2432,12 +2693,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11">
         <f>SUM(D2:D10)</f>
@@ -2453,25 +2714,25 @@
         <v>0</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="D13" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -2480,12 +2741,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -2494,12 +2755,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -2508,12 +2769,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -2522,12 +2783,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -2536,12 +2797,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -2550,12 +2811,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E20" s="2">
         <f>SUM(E14:E19)</f>
@@ -2564,7 +2825,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E22" s="2">
         <f>E11+E20</f>
@@ -2597,19 +2858,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="D1" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="G1" s="1"/>
     </row>
@@ -2631,7 +2892,7 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -2652,7 +2913,7 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -2673,7 +2934,7 @@
         <v>0.16600000000000001</v>
       </c>
       <c r="F4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -2694,7 +2955,7 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -2715,7 +2976,7 @@
         <v>0.16600000000000001</v>
       </c>
       <c r="F6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -2736,7 +2997,7 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -2757,7 +3018,7 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -2778,7 +3039,7 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -2799,12 +3060,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11">
         <f>SUM(D2:D10)</f>
@@ -2820,24 +3081,24 @@
         <v>0</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="D13" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -2846,12 +3107,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -2860,12 +3121,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -2874,12 +3135,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -2888,12 +3149,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -2902,12 +3163,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -2916,12 +3177,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E20" s="2">
         <f>SUM(E14:E19)</f>
@@ -2930,7 +3191,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E22" s="2">
         <f>E11+E20</f>
@@ -2949,7 +3210,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{402F22C9-9046-40B7-9C8A-21A255598059}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
@@ -2966,19 +3227,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="D1" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="G1" s="1"/>
     </row>
@@ -3000,7 +3261,7 @@
         <v>0.16600000000000001</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -3021,7 +3282,7 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -3042,7 +3303,7 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -3063,7 +3324,7 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -3084,7 +3345,7 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -3105,7 +3366,7 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -3126,7 +3387,7 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -3147,7 +3408,7 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -3168,12 +3429,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11">
         <f>SUM(D2:D10)</f>
@@ -3189,24 +3450,24 @@
         <v>0</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="D13" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -3215,12 +3476,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -3229,12 +3490,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -3243,12 +3504,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -3257,12 +3518,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -3271,12 +3532,12 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -3285,18 +3546,18 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E20" s="2"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E22" s="2">
         <f>E11+E20</f>

</xml_diff>

<commit_message>
Added Case code (mm) and datasheet links for all resistors and capacitors in the remaining filters
</commit_message>
<xml_diff>
--- a/Documents/BOM.xlsx
+++ b/Documents/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ECE_Projects\Music_Visualizer\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9D97B15-C5C5-43AF-8C5B-6D610BF8BDB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B79F74-99C3-44E8-89B3-56572B01DCEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3720" yWindow="1776" windowWidth="8856" windowHeight="4800" activeTab="1" xr2:uid="{1F4A7036-4694-4970-BB5D-7CBECC831452}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{1F4A7036-4694-4970-BB5D-7CBECC831452}"/>
   </bookViews>
   <sheets>
     <sheet name="Sub-Bass" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="148">
   <si>
     <t>Component</t>
   </si>
@@ -118,9 +118,6 @@
     <t xml:space="preserve">Link </t>
   </si>
   <si>
-    <t>https://www.mouser.ca/ProductDetail/Panasonic/ERJ-1GNF8452C?qs=nuXzIS8loXH90W30k0dNHQ%3D%3D</t>
-  </si>
-  <si>
     <t>https://www.mouser.ca/ProductDetail/YAGEO/RC0201FR-0748K7L?qs=Q4gDqC5t5%2FBg%252BbTLyGfzlg%3D%3D</t>
   </si>
   <si>
@@ -347,6 +344,147 @@
   </si>
   <si>
     <t>https://www.mouser.ca/datasheet/2/40/X7RDielectric-777024.pdf</t>
+  </si>
+  <si>
+    <t> RC0201FR-07137KL Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t> RC0201FR-0745R3L Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t> RC0201FR-07270KL Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>ERJ-1GNF1433C Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>RC0201FR-0719K1L Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>RC0201FR-07590KL Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>ERJ-1GNF1403C Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>RC0201FR-07576KL Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t> GRM033R71A472JA01D Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>GRM033R71A332JA01D Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>GRM2195C1H622JA01D Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>RC0201FR-07100KL Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>RC0201FR-0766K5L Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>ERJ-1GNF3322C Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>RC0201FR-0756KL Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>RC0201FR-0748K7L Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>RC0201FR-07270KL Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>RC0201FR-0757K6L Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>RC0201FR-07324KL Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>1005</t>
+  </si>
+  <si>
+    <t>1608</t>
+  </si>
+  <si>
+    <t>GRM1885C1H162JA01D Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>GRM0335C1E102JA01D Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>GRM155R71H302JA01D Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>RC0201FR-0778K7L Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>RK73H1HTTC2672F Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>RC0201FR-07160KL Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>RC0201FR-0759KL Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>RC0201FR-077K87L Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>RC0201FR-07243KL Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>RC0201FR-07107KL Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>RK73H1HTTC1472F Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>RC0201FR-07453KL Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>RC0201FR-077K32L Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>CRCW02012K87FNED Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>RC0201FR-0795K3L Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>AC0201FR-074K02L Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>RC0201FR-07383KL Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/RC0805FR-0711K5L?qs=8Y8p%252BasKcI6PCsTI4Jd5ZA%3D%3D</t>
+  </si>
+  <si>
+    <t>RC0805FR-0711K5L Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>RC0201FR-0722K6L Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>RK73H1HTTC8061F Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>RC0201FR-074K32L Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>RC0201FR-0737K4L Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>RC0201FR-0719K6L Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>RC0201FR-0710K7L Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>RK73H1HTTC9092F Datasheet (PDF)</t>
   </si>
 </sst>
 </file>
@@ -417,7 +555,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -429,6 +567,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -782,10 +924,10 @@
         <v>24</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -806,13 +948,13 @@
         <v>0.16600000000000001</v>
       </c>
       <c r="F2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -833,13 +975,13 @@
         <v>0.16600000000000001</v>
       </c>
       <c r="F3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -860,13 +1002,13 @@
         <v>0.16600000000000001</v>
       </c>
       <c r="F4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -887,13 +1029,13 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G5" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H5" t="s">
         <v>90</v>
-      </c>
-      <c r="H5" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -914,13 +1056,13 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -941,13 +1083,13 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -968,13 +1110,13 @@
         <v>0.16600000000000001</v>
       </c>
       <c r="F8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -995,13 +1137,13 @@
         <v>0.16600000000000001</v>
       </c>
       <c r="F9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -1022,13 +1164,13 @@
         <v>0.152</v>
       </c>
       <c r="F10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G10" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H10" t="s">
         <v>90</v>
-      </c>
-      <c r="H10" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -1064,10 +1206,10 @@
         <v>24</v>
       </c>
       <c r="G13" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H13" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -1081,13 +1223,13 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -1101,13 +1243,13 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -1121,13 +1263,13 @@
         <v>0.152</v>
       </c>
       <c r="F16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G16" s="6">
         <v>1005</v>
       </c>
       <c r="H16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -1141,13 +1283,13 @@
         <v>0.152</v>
       </c>
       <c r="F17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G17" s="6">
         <v>1005</v>
       </c>
       <c r="H17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -1161,13 +1303,13 @@
         <v>0.75900000000000001</v>
       </c>
       <c r="F18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G18" s="6">
         <v>3216</v>
       </c>
       <c r="H18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -1181,13 +1323,13 @@
         <v>0.75900000000000001</v>
       </c>
       <c r="F19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G19" s="6">
         <v>3216</v>
       </c>
       <c r="H19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
@@ -1222,8 +1364,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9015A39E-4C3F-4E48-B877-A44E11CEB1FD}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1256,10 +1398,10 @@
         <v>24</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -1280,13 +1422,13 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -1307,13 +1449,13 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G3" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H3" t="s">
         <v>90</v>
-      </c>
-      <c r="H3" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -1334,13 +1476,13 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -1361,13 +1503,13 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -1388,13 +1530,13 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -1415,13 +1557,13 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -1442,13 +1584,13 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -1469,13 +1611,13 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -1496,13 +1638,13 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -1523,13 +1665,13 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -1565,10 +1707,10 @@
         <v>24</v>
       </c>
       <c r="G14" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H14" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -1582,13 +1724,13 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G15" s="6">
         <v>1005</v>
       </c>
       <c r="H15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -1602,13 +1744,13 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G16" s="6">
         <v>1005</v>
       </c>
       <c r="H16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -1622,13 +1764,13 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -1642,13 +1784,13 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -1662,13 +1804,13 @@
         <v>0.45500000000000002</v>
       </c>
       <c r="F19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G19" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="H19" t="s">
         <v>100</v>
-      </c>
-      <c r="H19" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
@@ -1682,13 +1824,13 @@
         <v>0.45500000000000002</v>
       </c>
       <c r="F20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G20" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="H20" t="s">
         <v>100</v>
-      </c>
-      <c r="H20" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
@@ -1717,10 +1859,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA94F869-6CDA-42B7-B92B-C65898560124}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18:E19"/>
+      <selection activeCell="G2" sqref="G2:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1729,9 +1871,11 @@
     <col min="2" max="2" width="18.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1750,9 +1894,14 @@
       <c r="F1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1770,10 +1919,16 @@
         <v>0.16600000000000001</v>
       </c>
       <c r="F2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1791,10 +1946,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1812,10 +1973,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1833,10 +2000,16 @@
         <v>0.16600000000000001</v>
       </c>
       <c r="F5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1854,10 +2027,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1875,10 +2054,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1896,10 +2081,16 @@
         <v>0.16600000000000001</v>
       </c>
       <c r="F8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1917,10 +2108,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1938,10 +2135,16 @@
         <v>0.16600000000000001</v>
       </c>
       <c r="F10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1954,7 +2157,7 @@
         <v>1.3540000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
@@ -1973,9 +2176,14 @@
       <c r="F13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G13" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1986,10 +2194,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F14" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -2000,10 +2214,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F15" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -2014,10 +2234,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F16" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -2028,10 +2254,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F17" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -2042,10 +2274,16 @@
         <v>0.42799999999999999</v>
       </c>
       <c r="F18" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -2056,10 +2294,16 @@
         <v>0.42799999999999999</v>
       </c>
       <c r="F19" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -2068,7 +2312,7 @@
         <v>1.4079999999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -2078,16 +2322,34 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{4DE652F3-1F5B-4436-A817-9DE7874D9570}"/>
+    <hyperlink ref="H3" r:id="rId2" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{1D69C91E-2295-4DE4-9667-EFC807D4553A}"/>
+    <hyperlink ref="H4" r:id="rId3" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{B411CA90-460B-4438-ABD8-8DE3874A8A80}"/>
+    <hyperlink ref="H5" r:id="rId4" display="https://www.mouser.ca/datasheet/2/315/AOA0000C304-1149620.pdf" xr:uid="{DD020D11-16C9-4C8A-9832-65686C7B0499}"/>
+    <hyperlink ref="H6" r:id="rId5" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{AA0F14C7-7B55-4324-9B5F-60D7972B8547}"/>
+    <hyperlink ref="H7" r:id="rId6" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{82D1DB7D-3A65-4297-B4FD-851043099BCA}"/>
+    <hyperlink ref="H8" r:id="rId7" display="https://www.mouser.ca/datasheet/2/315/AOA0000C304-1149620.pdf" xr:uid="{487F0D3E-A39C-46CD-810B-4CE7DE49E19B}"/>
+    <hyperlink ref="H9" r:id="rId8" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{98FAC4BA-2337-4A21-8DB6-D896610BEC1F}"/>
+    <hyperlink ref="H10" r:id="rId9" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{6BD02177-0FF5-4475-84F2-5A43B298DCB4}"/>
+    <hyperlink ref="H14" r:id="rId10" display="https://www.mouser.ca/datasheet/2/281/1/GRM033R71A472JA01_01A-1981970.pdf" xr:uid="{35A57E51-8CDA-4B99-90C5-790DE5F718F1}"/>
+    <hyperlink ref="H15" r:id="rId11" display="https://www.mouser.ca/datasheet/2/281/1/GRM033R71A472JA01_01A-1981970.pdf" xr:uid="{EC4F301A-1953-4D86-8E6C-059DEA3473D4}"/>
+    <hyperlink ref="H16" r:id="rId12" display="https://www.mouser.ca/datasheet/2/281/1/GRM033R71A332JA01_01A-1981937.pdf" xr:uid="{B2A34AA9-10D4-4758-AB1F-B46D78054155}"/>
+    <hyperlink ref="H17" r:id="rId13" display="https://www.mouser.ca/datasheet/2/281/1/GRM033R71A332JA01_01A-1981937.pdf" xr:uid="{0D533E40-688F-4751-AADC-F2611DFE2BA8}"/>
+    <hyperlink ref="H18" r:id="rId14" display="https://www.mouser.ca/datasheet/2/281/1/GRM2195C1H622JA01_01A-1986260.pdf" xr:uid="{5BA28F4C-4F6F-44D0-9CBA-CBD75DA1C1E2}"/>
+    <hyperlink ref="H19" r:id="rId15" display="https://www.mouser.ca/datasheet/2/281/1/GRM2195C1H622JA01_01A-1986260.pdf" xr:uid="{03E24CAC-25B3-4AA5-8DF6-098C9761C8A9}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99571FDB-D382-46BD-933E-AF5B2116BB53}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17:F18"/>
+      <selection activeCell="G2" sqref="G2:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2096,9 +2358,11 @@
     <col min="2" max="2" width="18.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2117,9 +2381,14 @@
       <c r="F1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2137,10 +2406,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2158,10 +2433,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2179,10 +2460,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2200,10 +2487,16 @@
         <v>0.16600000000000001</v>
       </c>
       <c r="F5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2221,10 +2514,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -2242,10 +2541,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2263,10 +2568,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -2284,10 +2595,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -2305,10 +2622,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -2326,10 +2649,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -2342,7 +2671,7 @@
         <v>1.4079999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
@@ -2361,9 +2690,14 @@
       <c r="F14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G14" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -2374,10 +2708,16 @@
         <v>0.17899999999999999</v>
       </c>
       <c r="F15" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -2388,10 +2728,16 @@
         <v>0.17899999999999999</v>
       </c>
       <c r="F16" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -2402,10 +2748,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F17" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -2416,10 +2768,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F18" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -2430,10 +2788,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F19" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -2444,10 +2808,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F20" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -2456,7 +2826,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>14</v>
       </c>
@@ -2466,16 +2836,34 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{2070C4A0-EA03-493A-8C1C-B23170BCC1E8}"/>
+    <hyperlink ref="H3" r:id="rId2" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{169E0BB1-F2D0-4719-93ED-9BD4E5AF3154}"/>
+    <hyperlink ref="H4" r:id="rId3" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{760DC3DA-5B57-466A-8544-70DEFA94D5BD}"/>
+    <hyperlink ref="H5" r:id="rId4" display="https://www.mouser.ca/datasheet/2/315/AOA0000C304-1149620.pdf" xr:uid="{D7A4154D-72EF-4737-B65B-C3FB2547D8CE}"/>
+    <hyperlink ref="H6" r:id="rId5" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{0E45FA3E-67A9-4FED-B81E-7B2E5D705B1D}"/>
+    <hyperlink ref="H7" r:id="rId6" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{66E06D70-2652-48C0-AF52-D2A01A1A4DCA}"/>
+    <hyperlink ref="H8" r:id="rId7" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{1CB75236-99A0-4775-B0F0-91CFE35848E0}"/>
+    <hyperlink ref="H9" r:id="rId8" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{7E9D0B52-74E6-4B31-A1CF-AD4D3B46A2AF}"/>
+    <hyperlink ref="H10" r:id="rId9" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{F8CE49A9-8B91-46C0-98C3-3F59D7D68BF8}"/>
+    <hyperlink ref="H11" r:id="rId10" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{E3C4F7E6-4B60-4763-9C6B-1FC33F65DFCC}"/>
+    <hyperlink ref="H15" r:id="rId11" display="https://www.mouser.ca/datasheet/2/281/1/GRM1885C1H162JA01_01A-1984769.pdf" xr:uid="{C9713A7A-5A83-4C36-A74F-05CAB403C3BD}"/>
+    <hyperlink ref="H16" r:id="rId12" display="https://www.mouser.ca/datasheet/2/281/1/GRM1885C1H162JA01_01A-1984769.pdf" xr:uid="{85B50FEE-D8DF-43D8-AA40-5F4EA2162223}"/>
+    <hyperlink ref="H17" r:id="rId13" display="https://www.mouser.ca/datasheet/2/281/1/GRM0335C1E102JA01_01A-1980306.pdf" xr:uid="{1D28022C-6C8B-48C1-A73C-F70BFBEEB6CF}"/>
+    <hyperlink ref="H18" r:id="rId14" display="https://www.mouser.ca/datasheet/2/281/1/GRM0335C1E102JA01_01A-1980306.pdf" xr:uid="{9B696EDC-9D2A-488F-9A9F-F86299C1D1A2}"/>
+    <hyperlink ref="H19" r:id="rId15" display="https://www.mouser.ca/datasheet/2/281/murata_03052018_GRM_Series_1-1310166.pdf" xr:uid="{17A7D9F4-25A0-468F-991B-283239A5FBAB}"/>
+    <hyperlink ref="H20" r:id="rId16" display="https://www.mouser.ca/datasheet/2/281/murata_03052018_GRM_Series_1-1310166.pdf" xr:uid="{D2B6F0B9-42C9-4D37-8282-9B3B79C61C76}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FA0D483-C574-49A8-A0EA-072A18CA1F90}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14:F19"/>
+      <selection activeCell="G14" sqref="G14:H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2484,9 +2872,11 @@
     <col min="2" max="2" width="18.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2505,9 +2895,14 @@
       <c r="F1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2525,10 +2920,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2546,10 +2947,16 @@
         <v>0.16600000000000001</v>
       </c>
       <c r="F3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2567,10 +2974,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2588,10 +3001,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2609,10 +3028,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -2630,10 +3055,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2651,10 +3082,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F8" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -2672,10 +3109,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F9" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -2693,10 +3136,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F10" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -2709,7 +3158,7 @@
         <v>1.27</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
@@ -2728,9 +3177,14 @@
       <c r="F13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G13" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -2741,10 +3195,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F14" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -2755,10 +3215,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F15" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -2769,10 +3235,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F16" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -2783,10 +3255,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F17" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -2797,10 +3275,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F18" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -2811,10 +3295,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F19" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -2823,7 +3313,7 @@
         <v>0.82800000000000007</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -2833,16 +3323,33 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{97F6D0C8-9CA6-4CF8-A167-21AD100E905E}"/>
+    <hyperlink ref="H3" r:id="rId2" display="https://www.mouser.ca/datasheet/2/219/RK73H-1825326.pdf" xr:uid="{EDA77192-FD7B-4584-9002-41FB7A94B1F9}"/>
+    <hyperlink ref="H4" r:id="rId3" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{A80D054D-09DD-4EE5-81F2-B2C353E03480}"/>
+    <hyperlink ref="H5" r:id="rId4" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{1E90B038-A93D-40F4-ADEE-76ABC348D447}"/>
+    <hyperlink ref="H6" r:id="rId5" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{2FFA81D4-4714-4BA6-9298-9DE903BCCC14}"/>
+    <hyperlink ref="H7" r:id="rId6" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{E9746157-BF15-40DE-8953-4511F788F25E}"/>
+    <hyperlink ref="H8" r:id="rId7" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{80D8A026-BD85-4593-BDCA-D35CC7955A7A}"/>
+    <hyperlink ref="H9" r:id="rId8" display="https://www.mouser.ca/datasheet/2/219/RK73H-1825326.pdf" xr:uid="{03F27F37-5052-4AF9-9D4C-F2961179D91A}"/>
+    <hyperlink ref="H10" r:id="rId9" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{8FD6CA09-DCB3-41DA-8DE1-B02105868272}"/>
+    <hyperlink ref="H14" r:id="rId10" display="https://www.mouser.ca/datasheet/2/281/1/GRM0335C1E102JA01_01A-1980306.pdf" xr:uid="{7AC3D20B-3B7C-41B4-B623-90F82F9C3D45}"/>
+    <hyperlink ref="H15" r:id="rId11" display="https://www.mouser.ca/datasheet/2/281/1/GRM0335C1E102JA01_01A-1980306.pdf" xr:uid="{6F39723A-852C-410B-A489-14E114356808}"/>
+    <hyperlink ref="H16" r:id="rId12" display="https://www.mouser.ca/datasheet/2/281/1/GRM0335C1E102JA01_01A-1980306.pdf" xr:uid="{2D321C2B-805C-4EA0-8536-400E7F6CA0EC}"/>
+    <hyperlink ref="H17" r:id="rId13" display="https://www.mouser.ca/datasheet/2/281/1/GRM0335C1E102JA01_01A-1980306.pdf" xr:uid="{2B6C6400-F70B-4442-BAC7-EDA288798CF9}"/>
+    <hyperlink ref="H18" r:id="rId14" display="https://www.mouser.ca/datasheet/2/281/1/GRM0335C1E102JA01_01A-1980306.pdf" xr:uid="{6E758FF1-8C0E-41C4-A752-D7209F374CBF}"/>
+    <hyperlink ref="H19" r:id="rId15" display="https://www.mouser.ca/datasheet/2/281/1/GRM0335C1E102JA01_01A-1980306.pdf" xr:uid="{516BFA38-786B-40D0-AE2F-E710249CCD53}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5443C8D0-3F9E-42A4-A7A9-47E7E9623942}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14:F19"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2851,9 +3358,11 @@
     <col min="2" max="2" width="18.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2872,9 +3381,14 @@
       <c r="F1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2892,10 +3406,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2913,10 +3433,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2934,10 +3460,16 @@
         <v>0.16600000000000001</v>
       </c>
       <c r="F4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2955,10 +3487,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2976,10 +3514,16 @@
         <v>0.16600000000000001</v>
       </c>
       <c r="F6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -2997,10 +3541,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -3018,10 +3568,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -3039,10 +3595,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F9" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -3060,10 +3622,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -3076,7 +3644,7 @@
         <v>1.298</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
@@ -3095,8 +3663,14 @@
       <c r="F13" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G13" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -3107,10 +3681,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F14" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -3121,10 +3701,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F15" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -3135,10 +3721,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F16" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -3149,10 +3741,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F17" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -3163,10 +3761,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F18" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -3177,10 +3781,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F19" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -3189,7 +3799,7 @@
         <v>0.82800000000000007</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -3201,6 +3811,21 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F10" r:id="rId1" xr:uid="{F4013F7B-2BF5-48F6-B2FD-018004F8799F}"/>
+    <hyperlink ref="H2" r:id="rId2" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{315DF4CA-987E-49DA-9194-A69CE44982AD}"/>
+    <hyperlink ref="H3" r:id="rId3" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{8966099E-C335-4CEE-9617-F87C6CD0B964}"/>
+    <hyperlink ref="H4" r:id="rId4" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{26B86C37-03C1-4492-BFF9-E640717F888A}"/>
+    <hyperlink ref="H5" r:id="rId5" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{2BDFA139-8F2D-4142-B742-165D0206B9CD}"/>
+    <hyperlink ref="H6" r:id="rId6" display="https://www.mouser.ca/datasheet/2/427/crcw0201e3-1761851.pdf" xr:uid="{D578B8C5-F0ED-4BCA-B2C7-EAEC1F534951}"/>
+    <hyperlink ref="H7" r:id="rId7" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{CD7462DD-C19A-40DB-BD3B-4F7998BED0C3}"/>
+    <hyperlink ref="H8" r:id="rId8" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{0C40AFBB-DDCF-4D55-97A6-2C3134155A6F}"/>
+    <hyperlink ref="H9" r:id="rId9" display="https://www.mouser.ca/datasheet/2/447/PYu_AC_51_RoHS_L_7-1714230.pdf" xr:uid="{F8B599C5-9D25-4B1B-BA72-D273B4BE0454}"/>
+    <hyperlink ref="H10" r:id="rId10" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{C0B7CCBC-31F1-4DD9-89D0-3D51C380E9C1}"/>
+    <hyperlink ref="H14" r:id="rId11" display="https://www.mouser.ca/datasheet/2/281/1/GRM0335C1E102JA01_01A-1980306.pdf" xr:uid="{9F08F217-7677-4ECE-9F1C-FF522AC33351}"/>
+    <hyperlink ref="H15" r:id="rId12" display="https://www.mouser.ca/datasheet/2/281/1/GRM0335C1E102JA01_01A-1980306.pdf" xr:uid="{943449AA-3A2F-4D0C-8E09-1F273BF1E8CF}"/>
+    <hyperlink ref="H16" r:id="rId13" display="https://www.mouser.ca/datasheet/2/281/1/GRM0335C1E102JA01_01A-1980306.pdf" xr:uid="{DFF66894-889F-43FD-A2C1-B9C4C47585CC}"/>
+    <hyperlink ref="H17" r:id="rId14" display="https://www.mouser.ca/datasheet/2/281/1/GRM0335C1E102JA01_01A-1980306.pdf" xr:uid="{E0FC5CDE-6431-4D42-9AD7-0CE77467B52C}"/>
+    <hyperlink ref="H18" r:id="rId15" display="https://www.mouser.ca/datasheet/2/281/1/GRM0335C1E102JA01_01A-1980306.pdf" xr:uid="{E5C76637-62FD-479E-98F7-4BF37102E1EA}"/>
+    <hyperlink ref="H19" r:id="rId16" display="https://www.mouser.ca/datasheet/2/281/1/GRM0335C1E102JA01_01A-1980306.pdf" xr:uid="{BC0822AC-58FB-4B65-A268-AFA977D295B2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3208,10 +3833,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{402F22C9-9046-40B7-9C8A-21A255598059}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3220,9 +3845,11 @@
     <col min="2" max="2" width="18.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3241,9 +3868,14 @@
       <c r="F1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -3261,10 +3893,16 @@
         <v>0.16600000000000001</v>
       </c>
       <c r="F2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>139</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -3282,10 +3920,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -3303,10 +3947,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -3324,10 +3974,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -3345,10 +4001,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -3366,10 +4028,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -3387,10 +4055,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -3408,10 +4082,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -3429,10 +4109,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -3444,8 +4130,12 @@
         <f>SUM(E2:E10)</f>
         <v>1.27</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H11" s="8"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H12" s="8"/>
+    </row>
+    <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
@@ -3464,8 +4154,14 @@
       <c r="F13" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G13" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -3476,10 +4172,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F14" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -3490,10 +4192,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F15" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -3504,10 +4212,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F16" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -3518,10 +4232,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F17" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -3532,10 +4252,16 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F18" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -3546,16 +4272,22 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F19" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>14</v>
       </c>
       <c r="E20" s="2"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -3565,6 +4297,23 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H14" r:id="rId1" display="https://www.mouser.ca/datasheet/2/281/1/GRM0335C1E102JA01_01A-1980306.pdf" xr:uid="{7BF7240F-1FAB-40B4-A685-F895D3B519F4}"/>
+    <hyperlink ref="H15" r:id="rId2" display="https://www.mouser.ca/datasheet/2/281/1/GRM0335C1E102JA01_01A-1980306.pdf" xr:uid="{15FF3824-8D00-46BF-9219-36FE857EBB08}"/>
+    <hyperlink ref="H16" r:id="rId3" display="https://www.mouser.ca/datasheet/2/281/1/GRM0335C1E102JA01_01A-1980306.pdf" xr:uid="{8E4EF360-6DF2-4C4B-837B-70BD632C2482}"/>
+    <hyperlink ref="H17" r:id="rId4" display="https://www.mouser.ca/datasheet/2/281/1/GRM0335C1E102JA01_01A-1980306.pdf" xr:uid="{51D2A29B-752C-4EE0-99AB-432A7713C414}"/>
+    <hyperlink ref="H18" r:id="rId5" display="https://www.mouser.ca/datasheet/2/281/1/GRM0335C1E102JA01_01A-1980306.pdf" xr:uid="{DA3FFB80-65BB-4EA9-9171-2018C41BE53D}"/>
+    <hyperlink ref="H19" r:id="rId6" display="https://www.mouser.ca/datasheet/2/281/1/GRM0335C1E102JA01_01A-1980306.pdf" xr:uid="{21CA3543-89F8-4C44-A591-1FE3922E51C4}"/>
+    <hyperlink ref="H2" r:id="rId7" display="https://www.mouser.ca/datasheet/2/447/Yageo_03_18_2021_PYu_RC_Group_51_RoHS_L_11-2199992.pdf" xr:uid="{AE8F117C-6067-4C73-9452-10A484F668FE}"/>
+    <hyperlink ref="H3" r:id="rId8" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{613CF69F-4176-4DBA-9F93-95DA1E47CC2B}"/>
+    <hyperlink ref="H4" r:id="rId9" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{B167F338-8C26-451A-A64D-4BDBE7592C89}"/>
+    <hyperlink ref="H5" r:id="rId10" display="https://www.mouser.ca/datasheet/2/219/RK73H-1825326.pdf" xr:uid="{DCBA1493-E1B4-4D03-8715-0EA6F287F128}"/>
+    <hyperlink ref="H6" r:id="rId11" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{A2964043-D1F9-49AF-964E-FEE626CA0525}"/>
+    <hyperlink ref="H7" r:id="rId12" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{2584D0CF-B221-4C29-BC31-50CA7F8A068E}"/>
+    <hyperlink ref="H8" r:id="rId13" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{280EACF1-CDDF-4E0A-B9E8-4107A27AA717}"/>
+    <hyperlink ref="H9" r:id="rId14" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{C8F69D6C-125E-42F2-B7CB-D347382A9A89}"/>
+    <hyperlink ref="H10" r:id="rId15" display="https://www.mouser.ca/datasheet/2/219/RK73H-1825326.pdf" xr:uid="{BE602546-C6F9-468E-87AC-0357C5023458}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added passive components of all filters on one sheet it Bom, component number reflects its ordering in the schematic
</commit_message>
<xml_diff>
--- a/Documents/BOM.xlsx
+++ b/Documents/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ECE_Projects\Music_Visualizer\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B79F74-99C3-44E8-89B3-56572B01DCEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5446767D-79C0-4394-ABF0-110E36039F3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{1F4A7036-4694-4970-BB5D-7CBECC831452}"/>
+    <workbookView xWindow="53115" yWindow="3015" windowWidth="8850" windowHeight="6000" firstSheet="3" activeTab="7" xr2:uid="{1F4A7036-4694-4970-BB5D-7CBECC831452}"/>
   </bookViews>
   <sheets>
     <sheet name="Sub-Bass" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="UpperMid" sheetId="5" r:id="rId5"/>
     <sheet name="Presence" sheetId="6" r:id="rId6"/>
     <sheet name="Brilliance" sheetId="7" r:id="rId7"/>
+    <sheet name="All Filters" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="241">
   <si>
     <t>Component</t>
   </si>
@@ -485,6 +486,285 @@
   </si>
   <si>
     <t>RK73H1HTTC9092F Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>Value (kOhms)</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>R14</t>
+  </si>
+  <si>
+    <t>R15</t>
+  </si>
+  <si>
+    <t>R16</t>
+  </si>
+  <si>
+    <t>R17</t>
+  </si>
+  <si>
+    <t>R18</t>
+  </si>
+  <si>
+    <t>R19</t>
+  </si>
+  <si>
+    <t>R20</t>
+  </si>
+  <si>
+    <t>R21</t>
+  </si>
+  <si>
+    <t>R22</t>
+  </si>
+  <si>
+    <t>R23</t>
+  </si>
+  <si>
+    <t>R24</t>
+  </si>
+  <si>
+    <t>R25</t>
+  </si>
+  <si>
+    <t>R26</t>
+  </si>
+  <si>
+    <t>R27</t>
+  </si>
+  <si>
+    <t>R28</t>
+  </si>
+  <si>
+    <t>R29</t>
+  </si>
+  <si>
+    <t>R30</t>
+  </si>
+  <si>
+    <t>R31</t>
+  </si>
+  <si>
+    <t>R32</t>
+  </si>
+  <si>
+    <t>R33</t>
+  </si>
+  <si>
+    <t>R34</t>
+  </si>
+  <si>
+    <t>R35</t>
+  </si>
+  <si>
+    <t>R36</t>
+  </si>
+  <si>
+    <t>R37</t>
+  </si>
+  <si>
+    <t>R38</t>
+  </si>
+  <si>
+    <t>R39</t>
+  </si>
+  <si>
+    <t>R40</t>
+  </si>
+  <si>
+    <t>R41</t>
+  </si>
+  <si>
+    <t>R42</t>
+  </si>
+  <si>
+    <t>R43</t>
+  </si>
+  <si>
+    <t>R44</t>
+  </si>
+  <si>
+    <t>R45</t>
+  </si>
+  <si>
+    <t>R46</t>
+  </si>
+  <si>
+    <t>R47</t>
+  </si>
+  <si>
+    <t>R48</t>
+  </si>
+  <si>
+    <t>R49</t>
+  </si>
+  <si>
+    <t>R50</t>
+  </si>
+  <si>
+    <t>R51</t>
+  </si>
+  <si>
+    <t>R52</t>
+  </si>
+  <si>
+    <t>R53</t>
+  </si>
+  <si>
+    <t>R54</t>
+  </si>
+  <si>
+    <t>R55</t>
+  </si>
+  <si>
+    <t>R56</t>
+  </si>
+  <si>
+    <t>R57</t>
+  </si>
+  <si>
+    <t>R58</t>
+  </si>
+  <si>
+    <t>R59</t>
+  </si>
+  <si>
+    <t>R60</t>
+  </si>
+  <si>
+    <t>R61</t>
+  </si>
+  <si>
+    <t>R62</t>
+  </si>
+  <si>
+    <t>R63</t>
+  </si>
+  <si>
+    <t>R64</t>
+  </si>
+  <si>
+    <t>R65</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>C9</t>
+  </si>
+  <si>
+    <t>C10</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>C13</t>
+  </si>
+  <si>
+    <t>C14</t>
+  </si>
+  <si>
+    <t>C15</t>
+  </si>
+  <si>
+    <t>C16</t>
+  </si>
+  <si>
+    <t>C17</t>
+  </si>
+  <si>
+    <t>C18</t>
+  </si>
+  <si>
+    <t>C19</t>
+  </si>
+  <si>
+    <t>C20</t>
+  </si>
+  <si>
+    <t>C21</t>
+  </si>
+  <si>
+    <t>C22</t>
+  </si>
+  <si>
+    <t>C23</t>
+  </si>
+  <si>
+    <t>C24</t>
+  </si>
+  <si>
+    <t>C25</t>
+  </si>
+  <si>
+    <t>C26</t>
+  </si>
+  <si>
+    <t>C27</t>
+  </si>
+  <si>
+    <t>C28</t>
+  </si>
+  <si>
+    <t>C29</t>
+  </si>
+  <si>
+    <t>C30</t>
+  </si>
+  <si>
+    <t>C31</t>
+  </si>
+  <si>
+    <t>C32</t>
+  </si>
+  <si>
+    <t>C33</t>
+  </si>
+  <si>
+    <t>C34</t>
+  </si>
+  <si>
+    <t>C35</t>
+  </si>
+  <si>
+    <t>C36</t>
+  </si>
+  <si>
+    <t>C37</t>
+  </si>
+  <si>
+    <t>C38</t>
+  </si>
+  <si>
+    <t>C39</t>
+  </si>
+  <si>
+    <t>C40</t>
+  </si>
+  <si>
+    <t>C41</t>
+  </si>
+  <si>
+    <t>C42</t>
+  </si>
+  <si>
+    <t>v</t>
   </si>
 </sst>
 </file>
@@ -533,7 +813,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -550,12 +830,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="mediumDashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="mediumDashed">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -571,6 +869,30 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -891,7 +1213,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G9"/>
+      <selection activeCell="E14" sqref="E14:H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1365,7 +1687,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1862,7 +2184,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G10"/>
+      <selection activeCell="E14" sqref="E14:H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2190,8 +2512,8 @@
       <c r="B14">
         <v>4.7</v>
       </c>
-      <c r="E14" s="2">
-        <v>0.13800000000000001</v>
+      <c r="E14" s="2" t="s">
+        <v>240</v>
       </c>
       <c r="F14" t="s">
         <v>80</v>
@@ -2309,7 +2631,7 @@
       </c>
       <c r="E20" s="2">
         <f>SUM(E14:E19)</f>
-        <v>1.4079999999999999</v>
+        <v>1.27</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
@@ -2318,7 +2640,7 @@
       </c>
       <c r="E22" s="2">
         <f>E11+E20</f>
-        <v>2.762</v>
+        <v>2.6240000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -2349,7 +2671,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G10"/>
+      <selection activeCell="E15" sqref="E15:H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2863,7 +3185,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14:H19"/>
+      <selection activeCell="E14" sqref="E14:H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3349,7 +3671,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="E2" sqref="E2:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3835,8 +4157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{402F22C9-9046-40B7-9C8A-21A255598059}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4316,4 +4638,2265 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5E7DEB4-5FFB-4F8D-963A-C08EFBE9A2C1}">
+  <dimension ref="A1:F108"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="F111" sqref="F111"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="76.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>84.5</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>160</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="D3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>169</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="D4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>90.9</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>37.4</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>402</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>86.6</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="D8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>35.700000000000003</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="D9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="9">
+        <v>390</v>
+      </c>
+      <c r="C10" s="10">
+        <v>0.152</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>110</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>149</v>
+      </c>
+      <c r="B12">
+        <v>90.9</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>150</v>
+      </c>
+      <c r="B13">
+        <v>162</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F13" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>151</v>
+      </c>
+      <c r="B14">
+        <v>118</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>152</v>
+      </c>
+      <c r="B15">
+        <v>63.4</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>153</v>
+      </c>
+      <c r="B16">
+        <v>62</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>154</v>
+      </c>
+      <c r="B17">
+        <v>309</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D17" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F17" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>155</v>
+      </c>
+      <c r="B18">
+        <v>68</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D18" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F18" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>156</v>
+      </c>
+      <c r="B19">
+        <v>66.5</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D19" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F19" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="B20" s="9">
+        <v>332</v>
+      </c>
+      <c r="C20" s="10">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>158</v>
+      </c>
+      <c r="B21">
+        <v>137</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="D21" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>159</v>
+      </c>
+      <c r="B22">
+        <v>45.3</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>160</v>
+      </c>
+      <c r="B23">
+        <v>270</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D23" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>161</v>
+      </c>
+      <c r="B24">
+        <v>143</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="D24" t="s">
+        <v>51</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>162</v>
+      </c>
+      <c r="B25">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D25" t="s">
+        <v>52</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>163</v>
+      </c>
+      <c r="B26">
+        <v>590</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D26" t="s">
+        <v>53</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>164</v>
+      </c>
+      <c r="B27">
+        <v>140</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="D27" t="s">
+        <v>54</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>165</v>
+      </c>
+      <c r="B28">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D28" t="s">
+        <v>52</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="B29" s="9">
+        <v>576</v>
+      </c>
+      <c r="C29" s="10">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>167</v>
+      </c>
+      <c r="B30">
+        <v>100</v>
+      </c>
+      <c r="C30" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D30" t="s">
+        <v>56</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>168</v>
+      </c>
+      <c r="B31">
+        <v>100</v>
+      </c>
+      <c r="C31" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D31" t="s">
+        <v>56</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>169</v>
+      </c>
+      <c r="B32">
+        <v>66.5</v>
+      </c>
+      <c r="C32" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D32" t="s">
+        <v>46</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>170</v>
+      </c>
+      <c r="B33">
+        <v>33.200000000000003</v>
+      </c>
+      <c r="C33" s="2">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="D33" t="s">
+        <v>57</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>171</v>
+      </c>
+      <c r="B34">
+        <v>56</v>
+      </c>
+      <c r="C34" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D34" t="s">
+        <v>58</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>172</v>
+      </c>
+      <c r="B35">
+        <v>48.7</v>
+      </c>
+      <c r="C35" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D35" t="s">
+        <v>25</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>173</v>
+      </c>
+      <c r="B36">
+        <v>270</v>
+      </c>
+      <c r="C36" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D36" t="s">
+        <v>50</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>174</v>
+      </c>
+      <c r="B37">
+        <v>66.5</v>
+      </c>
+      <c r="C37" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D37" t="s">
+        <v>46</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>175</v>
+      </c>
+      <c r="B38">
+        <v>57.6</v>
+      </c>
+      <c r="C38" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D38" t="s">
+        <v>59</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="B39" s="9">
+        <v>324</v>
+      </c>
+      <c r="C39" s="10">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="F39" s="12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>177</v>
+      </c>
+      <c r="B40">
+        <v>78.7</v>
+      </c>
+      <c r="C40" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D40" t="s">
+        <v>61</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>178</v>
+      </c>
+      <c r="B41">
+        <v>26.7</v>
+      </c>
+      <c r="C41" s="2">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="D41" t="s">
+        <v>62</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>179</v>
+      </c>
+      <c r="B42">
+        <v>160</v>
+      </c>
+      <c r="C42" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D42" t="s">
+        <v>34</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>180</v>
+      </c>
+      <c r="B43">
+        <v>59</v>
+      </c>
+      <c r="C43" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D43" t="s">
+        <v>63</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>181</v>
+      </c>
+      <c r="B44">
+        <v>7.87</v>
+      </c>
+      <c r="C44" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D44" t="s">
+        <v>64</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>182</v>
+      </c>
+      <c r="B45">
+        <v>243</v>
+      </c>
+      <c r="C45" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D45" t="s">
+        <v>65</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>183</v>
+      </c>
+      <c r="B46">
+        <v>107</v>
+      </c>
+      <c r="C46" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D46" t="s">
+        <v>66</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>184</v>
+      </c>
+      <c r="B47">
+        <v>14.7</v>
+      </c>
+      <c r="C47" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D47" t="s">
+        <v>67</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="B48" s="9">
+        <v>453</v>
+      </c>
+      <c r="C48" s="10">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D48" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="E48" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="F48" s="12" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>186</v>
+      </c>
+      <c r="B49">
+        <v>78.7</v>
+      </c>
+      <c r="C49" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D49" t="s">
+        <v>61</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>187</v>
+      </c>
+      <c r="B50">
+        <v>7.32</v>
+      </c>
+      <c r="C50" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D50" t="s">
+        <v>69</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>188</v>
+      </c>
+      <c r="B51">
+        <v>160</v>
+      </c>
+      <c r="C51" s="2">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="D51" t="s">
+        <v>34</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>189</v>
+      </c>
+      <c r="B52">
+        <v>66.5</v>
+      </c>
+      <c r="C52" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D52" t="s">
+        <v>46</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>190</v>
+      </c>
+      <c r="B53">
+        <v>2.87</v>
+      </c>
+      <c r="C53" s="2">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="D53" t="s">
+        <v>70</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>191</v>
+      </c>
+      <c r="B54">
+        <v>270</v>
+      </c>
+      <c r="C54" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D54" t="s">
+        <v>50</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>192</v>
+      </c>
+      <c r="B55">
+        <v>95.3</v>
+      </c>
+      <c r="C55" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D55" t="s">
+        <v>71</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>193</v>
+      </c>
+      <c r="B56">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="C56" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D56" t="s">
+        <v>72</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="B57" s="9">
+        <v>383</v>
+      </c>
+      <c r="C57" s="10">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D57" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="E57" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="F57" s="12" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>195</v>
+      </c>
+      <c r="B58">
+        <v>11.5</v>
+      </c>
+      <c r="C58" s="2">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="D58" t="s">
+        <v>139</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="F58" s="7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>196</v>
+      </c>
+      <c r="B59">
+        <v>48.7</v>
+      </c>
+      <c r="C59" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D59" t="s">
+        <v>25</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>197</v>
+      </c>
+      <c r="B60">
+        <v>22.6</v>
+      </c>
+      <c r="C60" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D60" t="s">
+        <v>26</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>198</v>
+      </c>
+      <c r="B61">
+        <v>8.06</v>
+      </c>
+      <c r="C61" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D61" t="s">
+        <v>27</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>199</v>
+      </c>
+      <c r="B62">
+        <v>4.32</v>
+      </c>
+      <c r="C62" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D62" t="s">
+        <v>28</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>200</v>
+      </c>
+      <c r="B63">
+        <v>37.4</v>
+      </c>
+      <c r="C63" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D63" t="s">
+        <v>29</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>201</v>
+      </c>
+      <c r="B64">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="C64" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D64" t="s">
+        <v>30</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>202</v>
+      </c>
+      <c r="B65">
+        <v>10.7</v>
+      </c>
+      <c r="C65" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D65" t="s">
+        <v>31</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="B66" s="9">
+        <v>90.9</v>
+      </c>
+      <c r="C66" s="10">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D66" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E66" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="F66" s="12" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>17</v>
+      </c>
+      <c r="B67">
+        <v>47</v>
+      </c>
+      <c r="C67" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D67" t="s">
+        <v>74</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F67" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>18</v>
+      </c>
+      <c r="B68">
+        <v>47</v>
+      </c>
+      <c r="C68" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D68" t="s">
+        <v>74</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F68" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>19</v>
+      </c>
+      <c r="B69">
+        <v>27</v>
+      </c>
+      <c r="C69" s="2">
+        <v>0.152</v>
+      </c>
+      <c r="D69" t="s">
+        <v>76</v>
+      </c>
+      <c r="E69" s="6">
+        <v>1005</v>
+      </c>
+      <c r="F69" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>20</v>
+      </c>
+      <c r="B70">
+        <v>27</v>
+      </c>
+      <c r="C70" s="2">
+        <v>0.152</v>
+      </c>
+      <c r="D70" t="s">
+        <v>76</v>
+      </c>
+      <c r="E70" s="6">
+        <v>1005</v>
+      </c>
+      <c r="F70" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>21</v>
+      </c>
+      <c r="B71">
+        <v>75</v>
+      </c>
+      <c r="C71" s="2">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="D71" t="s">
+        <v>75</v>
+      </c>
+      <c r="E71" s="6">
+        <v>3216</v>
+      </c>
+      <c r="F71" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B72" s="9">
+        <v>75</v>
+      </c>
+      <c r="C72" s="10">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="D72" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="E72" s="13">
+        <v>3216</v>
+      </c>
+      <c r="F72" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A73" s="14" t="s">
+        <v>204</v>
+      </c>
+      <c r="B73">
+        <v>13</v>
+      </c>
+      <c r="C73" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D73" t="s">
+        <v>77</v>
+      </c>
+      <c r="E73" s="6">
+        <v>1005</v>
+      </c>
+      <c r="F73" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A74" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="B74">
+        <v>13</v>
+      </c>
+      <c r="C74" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D74" t="s">
+        <v>77</v>
+      </c>
+      <c r="E74" s="6">
+        <v>1005</v>
+      </c>
+      <c r="F74" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="B75">
+        <v>6.8</v>
+      </c>
+      <c r="C75" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D75" t="s">
+        <v>78</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F75" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A76" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="B76">
+        <v>6.8</v>
+      </c>
+      <c r="C76" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D76" t="s">
+        <v>78</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F76" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A77" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="B77">
+        <v>24</v>
+      </c>
+      <c r="C77" s="2">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="D77" t="s">
+        <v>79</v>
+      </c>
+      <c r="E77" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="F77" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A78" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="B78" s="9">
+        <v>24</v>
+      </c>
+      <c r="C78" s="10">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="D78" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="E78" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F78" s="9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A79" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="B79">
+        <v>4.7</v>
+      </c>
+      <c r="C79" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D79" t="s">
+        <v>80</v>
+      </c>
+      <c r="E79" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F79" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A80" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="B80">
+        <v>4.7</v>
+      </c>
+      <c r="C80" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D80" t="s">
+        <v>80</v>
+      </c>
+      <c r="E80" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F80" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A81" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="B81">
+        <v>3.3</v>
+      </c>
+      <c r="C81" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D81" t="s">
+        <v>81</v>
+      </c>
+      <c r="E81" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F81" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A82" s="14" t="s">
+        <v>213</v>
+      </c>
+      <c r="B82">
+        <v>3.3</v>
+      </c>
+      <c r="C82" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D82" t="s">
+        <v>81</v>
+      </c>
+      <c r="E82" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F82" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A83" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="B83">
+        <v>6.2</v>
+      </c>
+      <c r="C83" s="2">
+        <v>0.42799999999999999</v>
+      </c>
+      <c r="D83" t="s">
+        <v>82</v>
+      </c>
+      <c r="E83" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="F83" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A84" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="B84" s="9">
+        <v>6.2</v>
+      </c>
+      <c r="C84" s="10">
+        <v>0.42799999999999999</v>
+      </c>
+      <c r="D84" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="E84" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F84" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A85" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="B85">
+        <v>1.6</v>
+      </c>
+      <c r="C85" s="2">
+        <v>0.17899999999999999</v>
+      </c>
+      <c r="D85" t="s">
+        <v>83</v>
+      </c>
+      <c r="E85" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="F85" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A86" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="B86">
+        <v>1.6</v>
+      </c>
+      <c r="C86" s="2">
+        <v>0.17899999999999999</v>
+      </c>
+      <c r="D86" t="s">
+        <v>83</v>
+      </c>
+      <c r="E86" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="F86" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A87" s="14" t="s">
+        <v>218</v>
+      </c>
+      <c r="B87">
+        <v>1</v>
+      </c>
+      <c r="C87" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D87" t="s">
+        <v>84</v>
+      </c>
+      <c r="E87" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F87" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A88" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="B88">
+        <v>1</v>
+      </c>
+      <c r="C88" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D88" t="s">
+        <v>84</v>
+      </c>
+      <c r="E88" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F88" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A89" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="B89">
+        <v>3</v>
+      </c>
+      <c r="C89" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D89" t="s">
+        <v>85</v>
+      </c>
+      <c r="E89" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="F89" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A90" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="B90" s="9">
+        <v>3</v>
+      </c>
+      <c r="C90" s="10">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D90" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="E90" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="F90" s="12" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A91" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="B91">
+        <v>1</v>
+      </c>
+      <c r="C91" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D91" t="s">
+        <v>84</v>
+      </c>
+      <c r="E91" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F91" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A92" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="B92">
+        <v>1</v>
+      </c>
+      <c r="C92" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D92" t="s">
+        <v>84</v>
+      </c>
+      <c r="E92" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F92" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A93" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="B93">
+        <v>1</v>
+      </c>
+      <c r="C93" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D93" t="s">
+        <v>84</v>
+      </c>
+      <c r="E93" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F93" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A94" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="B94">
+        <v>1</v>
+      </c>
+      <c r="C94" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D94" t="s">
+        <v>84</v>
+      </c>
+      <c r="E94" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F94" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A95" s="14" t="s">
+        <v>226</v>
+      </c>
+      <c r="B95">
+        <v>1</v>
+      </c>
+      <c r="C95" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D95" t="s">
+        <v>84</v>
+      </c>
+      <c r="E95" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F95" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A96" s="15" t="s">
+        <v>227</v>
+      </c>
+      <c r="B96" s="9">
+        <v>1</v>
+      </c>
+      <c r="C96" s="10">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D96" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="E96" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="F96" s="12" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A97" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="B97" s="21">
+        <v>1</v>
+      </c>
+      <c r="C97" s="22">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D97" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="E97" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="F97" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A98" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="B98" s="16">
+        <v>1</v>
+      </c>
+      <c r="C98" s="17">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D98" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="E98" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="F98" s="19" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A99" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="B99" s="16">
+        <v>1</v>
+      </c>
+      <c r="C99" s="17">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D99" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="E99" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="F99" s="19" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A100" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="B100" s="16">
+        <v>1</v>
+      </c>
+      <c r="C100" s="17">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D100" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="E100" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="F100" s="19" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A101" s="14" t="s">
+        <v>232</v>
+      </c>
+      <c r="B101" s="16">
+        <v>1</v>
+      </c>
+      <c r="C101" s="17">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D101" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="E101" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="F101" s="19" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A102" s="15" t="s">
+        <v>233</v>
+      </c>
+      <c r="B102" s="9">
+        <v>1</v>
+      </c>
+      <c r="C102" s="10">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D102" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="E102" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="F102" s="12" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A103" s="14" t="s">
+        <v>234</v>
+      </c>
+      <c r="B103">
+        <v>1</v>
+      </c>
+      <c r="C103" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D103" t="s">
+        <v>84</v>
+      </c>
+      <c r="E103" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F103" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A104" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="B104">
+        <v>1</v>
+      </c>
+      <c r="C104" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D104" t="s">
+        <v>84</v>
+      </c>
+      <c r="E104" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F104" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A105" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="B105">
+        <v>1</v>
+      </c>
+      <c r="C105" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D105" t="s">
+        <v>84</v>
+      </c>
+      <c r="E105" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F105" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A106" s="14" t="s">
+        <v>237</v>
+      </c>
+      <c r="B106">
+        <v>1</v>
+      </c>
+      <c r="C106" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D106" t="s">
+        <v>84</v>
+      </c>
+      <c r="E106" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F106" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A107" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="B107">
+        <v>1</v>
+      </c>
+      <c r="C107" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D107" t="s">
+        <v>84</v>
+      </c>
+      <c r="E107" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F107" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A108" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="B108" s="9">
+        <v>1</v>
+      </c>
+      <c r="C108" s="10">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D108" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="E108" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="F108" s="12" t="s">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="F21" r:id="rId1" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{FD9529E3-40C1-4269-9308-A90EB6F99C44}"/>
+    <hyperlink ref="F22" r:id="rId2" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{AF05A996-0EA5-4A4B-99F7-B6218120F0B8}"/>
+    <hyperlink ref="F23" r:id="rId3" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{03494045-2A4B-4002-BCA7-A755F9571329}"/>
+    <hyperlink ref="F24" r:id="rId4" display="https://www.mouser.ca/datasheet/2/315/AOA0000C304-1149620.pdf" xr:uid="{1580B869-2B3E-42DF-8069-E44C33CA85C2}"/>
+    <hyperlink ref="F25" r:id="rId5" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{A8FA7F70-6CB8-4768-ABB5-466F8167C5A7}"/>
+    <hyperlink ref="F26" r:id="rId6" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{DC681EA6-2B6F-4E11-8A32-81603563F94B}"/>
+    <hyperlink ref="F27" r:id="rId7" display="https://www.mouser.ca/datasheet/2/315/AOA0000C304-1149620.pdf" xr:uid="{E7F0B69F-60DF-4D2B-9E43-6B59777DA5FD}"/>
+    <hyperlink ref="F28" r:id="rId8" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{E5ED0D8F-8C7D-4331-831A-271744B441C5}"/>
+    <hyperlink ref="F29" r:id="rId9" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{C3A4D775-79FF-4016-B072-489F8EBE84B3}"/>
+    <hyperlink ref="F30" r:id="rId10" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{0EB2A5DD-EAE6-47E0-968A-67833B7174C3}"/>
+    <hyperlink ref="F31" r:id="rId11" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{6A4FDB44-6AE2-4E6C-9A5E-24CA09F1AA5A}"/>
+    <hyperlink ref="F32" r:id="rId12" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{E40727DA-99E0-4ACB-884A-DFF96FAFF28D}"/>
+    <hyperlink ref="F33" r:id="rId13" display="https://www.mouser.ca/datasheet/2/315/AOA0000C304-1149620.pdf" xr:uid="{3DD78109-2D56-4234-87B5-B042D8C23DA7}"/>
+    <hyperlink ref="F34" r:id="rId14" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{BBC48974-2854-4BD3-8BDA-DE947C368567}"/>
+    <hyperlink ref="F35" r:id="rId15" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{4E281739-3835-4BCF-9C7B-3CF2BDC4091A}"/>
+    <hyperlink ref="F36" r:id="rId16" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{11DDB7B4-80D4-497F-82B9-9B2BAB3CD932}"/>
+    <hyperlink ref="F37" r:id="rId17" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{27DDB5EE-0D1C-4E88-B32C-F94E0DBC8FA1}"/>
+    <hyperlink ref="F38" r:id="rId18" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{F8A9305C-C834-41F3-9CD9-E4FDAF19645D}"/>
+    <hyperlink ref="F39" r:id="rId19" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{F35710BE-87B5-4075-86F7-6837FF96F463}"/>
+    <hyperlink ref="F40" r:id="rId20" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{259AC562-7AB1-4886-9772-DA6728CAA8F6}"/>
+    <hyperlink ref="F41" r:id="rId21" display="https://www.mouser.ca/datasheet/2/219/RK73H-1825326.pdf" xr:uid="{723422E5-45DA-4E6D-AC15-9C08A292A2F0}"/>
+    <hyperlink ref="F42" r:id="rId22" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{FC52CC8E-EB24-4AAA-BB26-93DB08110EF8}"/>
+    <hyperlink ref="F43" r:id="rId23" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{96AE4BE9-98D8-40FE-B6B7-65F6D96C864A}"/>
+    <hyperlink ref="F44" r:id="rId24" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{E0359093-3924-49AF-8716-D2DCEEA99753}"/>
+    <hyperlink ref="F45" r:id="rId25" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{921E3894-7975-45A3-9C86-901A1CA13EDD}"/>
+    <hyperlink ref="F46" r:id="rId26" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{E612FF43-23ED-4F85-8330-CD975D7D919B}"/>
+    <hyperlink ref="F47" r:id="rId27" display="https://www.mouser.ca/datasheet/2/219/RK73H-1825326.pdf" xr:uid="{19611E56-8A88-4C73-BA9F-BF7EECC2D3D9}"/>
+    <hyperlink ref="F48" r:id="rId28" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{3135B02F-24BA-41E2-BD1A-495B96BE4D42}"/>
+    <hyperlink ref="D57" r:id="rId29" xr:uid="{64FC0717-8FFD-444E-BA6B-296024B6CC9E}"/>
+    <hyperlink ref="F49" r:id="rId30" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{D4CC2860-DDC1-49B9-9D01-92DBE6D7AF86}"/>
+    <hyperlink ref="F50" r:id="rId31" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{61C95871-9315-42D6-9353-F7A3506CBA38}"/>
+    <hyperlink ref="F51" r:id="rId32" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{3F7E1927-1003-453C-9DF8-53C3552F065F}"/>
+    <hyperlink ref="F52" r:id="rId33" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{33F699B4-86AF-4F0D-A232-F64B5251B610}"/>
+    <hyperlink ref="F53" r:id="rId34" display="https://www.mouser.ca/datasheet/2/427/crcw0201e3-1761851.pdf" xr:uid="{17871B00-FD6D-40F3-A699-9428A7EF17EB}"/>
+    <hyperlink ref="F54" r:id="rId35" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{C079597D-30CA-4045-A9E5-BD13A759F493}"/>
+    <hyperlink ref="F55" r:id="rId36" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{7E31A499-E499-4ED6-BB06-D806B68FD9B5}"/>
+    <hyperlink ref="F56" r:id="rId37" display="https://www.mouser.ca/datasheet/2/447/PYu_AC_51_RoHS_L_7-1714230.pdf" xr:uid="{368312DA-E0A7-4CD5-A292-0FA831C3F947}"/>
+    <hyperlink ref="F57" r:id="rId38" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{FB2CBCEB-B200-4B83-B265-7A61CE61968D}"/>
+    <hyperlink ref="F58" r:id="rId39" display="https://www.mouser.ca/datasheet/2/447/Yageo_03_18_2021_PYu_RC_Group_51_RoHS_L_11-2199992.pdf" xr:uid="{1B45DEBB-2050-44B6-897A-59BDA4F2A593}"/>
+    <hyperlink ref="F59" r:id="rId40" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{F90094AE-1100-4160-831D-6E72766A9AA8}"/>
+    <hyperlink ref="F60" r:id="rId41" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{8D4347FF-3E40-4580-847E-F13E96530DFA}"/>
+    <hyperlink ref="F61" r:id="rId42" display="https://www.mouser.ca/datasheet/2/219/RK73H-1825326.pdf" xr:uid="{C9DE6C51-B5C7-4F5B-8A67-86A8D88F4522}"/>
+    <hyperlink ref="F62" r:id="rId43" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{BAC11EE4-036C-423F-BDB4-A5B9F78DA9BC}"/>
+    <hyperlink ref="F63" r:id="rId44" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{4DDCF0D7-DE2B-40A7-B359-20DAC1834571}"/>
+    <hyperlink ref="F64" r:id="rId45" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{1EFCB2B0-E9F8-4323-A5BA-2B341C09475A}"/>
+    <hyperlink ref="F65" r:id="rId46" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{BC58F616-EBC9-4F89-83CF-0E8584509D82}"/>
+    <hyperlink ref="F66" r:id="rId47" display="https://www.mouser.ca/datasheet/2/219/RK73H-1825326.pdf" xr:uid="{BBA32F4A-DD55-48F6-B98F-679FC061CEA4}"/>
+    <hyperlink ref="F79" r:id="rId48" display="https://www.mouser.ca/datasheet/2/281/1/GRM033R71A472JA01_01A-1981970.pdf" xr:uid="{82657021-7BC3-4AE0-9ADF-24E04368E8DC}"/>
+    <hyperlink ref="F80" r:id="rId49" display="https://www.mouser.ca/datasheet/2/281/1/GRM033R71A472JA01_01A-1981970.pdf" xr:uid="{8AB0CD5B-CA31-4243-9C1B-F61A8A9D7EC7}"/>
+    <hyperlink ref="F81" r:id="rId50" display="https://www.mouser.ca/datasheet/2/281/1/GRM033R71A332JA01_01A-1981937.pdf" xr:uid="{6E17525F-EB48-4E44-819F-5F55C7DFF933}"/>
+    <hyperlink ref="F82" r:id="rId51" display="https://www.mouser.ca/datasheet/2/281/1/GRM033R71A332JA01_01A-1981937.pdf" xr:uid="{2B101EFC-C080-4B09-BEBF-9670A5BCCE89}"/>
+    <hyperlink ref="F83" r:id="rId52" display="https://www.mouser.ca/datasheet/2/281/1/GRM2195C1H622JA01_01A-1986260.pdf" xr:uid="{22989E17-FB72-4044-886F-62F815E6EF93}"/>
+    <hyperlink ref="F84" r:id="rId53" display="https://www.mouser.ca/datasheet/2/281/1/GRM2195C1H622JA01_01A-1986260.pdf" xr:uid="{AE57E836-E1A9-4AF8-A7A1-17522A066637}"/>
+    <hyperlink ref="F85" r:id="rId54" display="https://www.mouser.ca/datasheet/2/281/1/GRM1885C1H162JA01_01A-1984769.pdf" xr:uid="{E09052E6-7EF4-4D90-B782-51CD15C9584E}"/>
+    <hyperlink ref="F86" r:id="rId55" display="https://www.mouser.ca/datasheet/2/281/1/GRM1885C1H162JA01_01A-1984769.pdf" xr:uid="{AEB327D0-99F1-4BE0-9C88-FA576634E701}"/>
+    <hyperlink ref="F87" r:id="rId56" display="https://www.mouser.ca/datasheet/2/281/1/GRM0335C1E102JA01_01A-1980306.pdf" xr:uid="{F89248B6-20D9-4A57-B97F-95AF3F433B33}"/>
+    <hyperlink ref="F88" r:id="rId57" display="https://www.mouser.ca/datasheet/2/281/1/GRM0335C1E102JA01_01A-1980306.pdf" xr:uid="{4E4C871E-37CD-4FFF-A930-A5D6F50A73D6}"/>
+    <hyperlink ref="F89" r:id="rId58" display="https://www.mouser.ca/datasheet/2/281/murata_03052018_GRM_Series_1-1310166.pdf" xr:uid="{98275737-0377-4222-95D6-74E1F965F237}"/>
+    <hyperlink ref="F90" r:id="rId59" display="https://www.mouser.ca/datasheet/2/281/murata_03052018_GRM_Series_1-1310166.pdf" xr:uid="{D3C2EF5A-9F49-41A5-B814-9F41CD309FEF}"/>
+    <hyperlink ref="F91" r:id="rId60" display="https://www.mouser.ca/datasheet/2/281/1/GRM0335C1E102JA01_01A-1980306.pdf" xr:uid="{E4FBADA0-23E7-4837-A876-DF7EA6ABE130}"/>
+    <hyperlink ref="F92" r:id="rId61" display="https://www.mouser.ca/datasheet/2/281/1/GRM0335C1E102JA01_01A-1980306.pdf" xr:uid="{AC47177C-1C42-4C73-90C2-BD4520BE83A5}"/>
+    <hyperlink ref="F93" r:id="rId62" display="https://www.mouser.ca/datasheet/2/281/1/GRM0335C1E102JA01_01A-1980306.pdf" xr:uid="{876FD6FF-9DBC-4296-8238-F86FED83B892}"/>
+    <hyperlink ref="F94" r:id="rId63" display="https://www.mouser.ca/datasheet/2/281/1/GRM0335C1E102JA01_01A-1980306.pdf" xr:uid="{BA8711E3-DA63-4499-A590-982649526B6A}"/>
+    <hyperlink ref="F95" r:id="rId64" display="https://www.mouser.ca/datasheet/2/281/1/GRM0335C1E102JA01_01A-1980306.pdf" xr:uid="{1CFF6C58-623D-434C-BEDA-E6E2C9893FBB}"/>
+    <hyperlink ref="F96" r:id="rId65" display="https://www.mouser.ca/datasheet/2/281/1/GRM0335C1E102JA01_01A-1980306.pdf" xr:uid="{6370957B-1692-4246-BB90-D5F8062AFD9F}"/>
+    <hyperlink ref="F97" r:id="rId66" display="https://www.mouser.ca/datasheet/2/281/1/GRM0335C1E102JA01_01A-1980306.pdf" xr:uid="{F2B11D76-492C-4B14-927F-D6264CA34676}"/>
+    <hyperlink ref="F98" r:id="rId67" display="https://www.mouser.ca/datasheet/2/281/1/GRM0335C1E102JA01_01A-1980306.pdf" xr:uid="{5455CA56-F191-4F9A-AA21-4D7CC4333AD4}"/>
+    <hyperlink ref="F99" r:id="rId68" display="https://www.mouser.ca/datasheet/2/281/1/GRM0335C1E102JA01_01A-1980306.pdf" xr:uid="{71679B2D-7E4C-4994-AA0C-AEC7F7C4E369}"/>
+    <hyperlink ref="F100" r:id="rId69" display="https://www.mouser.ca/datasheet/2/281/1/GRM0335C1E102JA01_01A-1980306.pdf" xr:uid="{EB87D4B6-EAE1-440B-9AE6-6DE3AC4C9DC7}"/>
+    <hyperlink ref="F101" r:id="rId70" display="https://www.mouser.ca/datasheet/2/281/1/GRM0335C1E102JA01_01A-1980306.pdf" xr:uid="{90AD138A-0AC7-433B-8A48-8F133ECA9564}"/>
+    <hyperlink ref="F102" r:id="rId71" display="https://www.mouser.ca/datasheet/2/281/1/GRM0335C1E102JA01_01A-1980306.pdf" xr:uid="{0E05E654-8FDA-444A-9078-41EEE131A875}"/>
+    <hyperlink ref="F103" r:id="rId72" display="https://www.mouser.ca/datasheet/2/281/1/GRM0335C1E102JA01_01A-1980306.pdf" xr:uid="{826DE407-2EFB-4288-87A2-1C9A2B46351D}"/>
+    <hyperlink ref="F104" r:id="rId73" display="https://www.mouser.ca/datasheet/2/281/1/GRM0335C1E102JA01_01A-1980306.pdf" xr:uid="{93AB788C-9E90-4932-BE9B-000C8F95CE8C}"/>
+    <hyperlink ref="F105" r:id="rId74" display="https://www.mouser.ca/datasheet/2/281/1/GRM0335C1E102JA01_01A-1980306.pdf" xr:uid="{2F527C91-C776-4E4A-90E1-AB1DD4DFAEDE}"/>
+    <hyperlink ref="F106" r:id="rId75" display="https://www.mouser.ca/datasheet/2/281/1/GRM0335C1E102JA01_01A-1980306.pdf" xr:uid="{71183E3C-1321-4C74-9C36-AF467F1E7694}"/>
+    <hyperlink ref="F107" r:id="rId76" display="https://www.mouser.ca/datasheet/2/281/1/GRM0335C1E102JA01_01A-1980306.pdf" xr:uid="{6107289D-2BCB-46B1-914E-5EA5AB170858}"/>
+    <hyperlink ref="F108" r:id="rId77" display="https://www.mouser.ca/datasheet/2/281/1/GRM0335C1E102JA01_01A-1980306.pdf" xr:uid="{E5DD7520-2C5E-4FF1-8071-DF8F821AA0D7}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId78"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Sourced all power circuitry
</commit_message>
<xml_diff>
--- a/Documents/BOM.xlsx
+++ b/Documents/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ECE_Projects\Music_Visualizer\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5446767D-79C0-4394-ABF0-110E36039F3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{219855FE-35BF-4243-B163-8CAE2E539364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="53115" yWindow="3015" windowWidth="8850" windowHeight="6000" firstSheet="3" activeTab="7" xr2:uid="{1F4A7036-4694-4970-BB5D-7CBECC831452}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{1F4A7036-4694-4970-BB5D-7CBECC831452}"/>
   </bookViews>
   <sheets>
     <sheet name="Sub-Bass" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Presence" sheetId="6" r:id="rId6"/>
     <sheet name="Brilliance" sheetId="7" r:id="rId7"/>
     <sheet name="All Filters" sheetId="8" r:id="rId8"/>
+    <sheet name="Power" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1074" uniqueCount="289">
   <si>
     <t>Component</t>
   </si>
@@ -765,6 +766,150 @@
   </si>
   <si>
     <t>v</t>
+  </si>
+  <si>
+    <t>Value /Purpose</t>
+  </si>
+  <si>
+    <t>PJ-070BH-SMT-TR</t>
+  </si>
+  <si>
+    <t>DC Power Jack</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/CUI-Devices/PJ-070BH-SMT-TR?qs=WyjlAZoYn52QG%252BaAz33LnQ%3D%3D</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>PJ-070BH-SMT-TR Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/onsemi/MC78L05ABDR2G?qs=%252B9%2Fcbd0IE0S6pmohSdZNkw%3D%3D</t>
+  </si>
+  <si>
+    <t>MC78L05ABDR2G</t>
+  </si>
+  <si>
+    <t>SOIC-8</t>
+  </si>
+  <si>
+    <t>MC78L05ABDR2G Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>MC79L05ACDR</t>
+  </si>
+  <si>
+    <t>Neg 5V Regulator</t>
+  </si>
+  <si>
+    <t>Pos 5V Regulator</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Texas-Instruments/MC79L05ACDR?qs=5BZzbFV4k2vE9gurfnXONg%3D%3D</t>
+  </si>
+  <si>
+    <t>MC79L05ACDR Datasheet</t>
+  </si>
+  <si>
+    <t>0.33uF</t>
+  </si>
+  <si>
+    <t>0.1uF</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Wurth-Elektronik/885012206074?qs=sGAEpiMZZMsh%252B1woXyUXj4jKQI6sNRw6hUfYRzIL2Qg%3D</t>
+  </si>
+  <si>
+    <t>885012206074 Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Samsung-Electro-Mechanics/CL21B104KACNNND?qs=sGAEpiMZZMsh%252B1woXyUXj9e2R%2FOkAO5oTPr84lvL%2FIA%3D</t>
+  </si>
+  <si>
+    <t>CL21B104KACNNND Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>Timer IC for Neg V</t>
+  </si>
+  <si>
+    <t>NE555DRG4</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Texas-Instruments/NE555DRG4?qs=rLYyFdxB%2FmreBHawQCpQ0Q%3D%3D</t>
+  </si>
+  <si>
+    <t>NE555DRG4 Datasheet</t>
+  </si>
+  <si>
+    <t>Ra</t>
+  </si>
+  <si>
+    <t>Rb</t>
+  </si>
+  <si>
+    <t>1kohm</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Welwyn-Components-TT-Electronics/ASC0402-1K0FT10?qs=sGAEpiMZZMtlubZbdhIBING1Nf%252BWA64mzV6yVEFyGxo%3D</t>
+  </si>
+  <si>
+    <t>ASC0402-1K0FT10 Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>10kohm</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/RC0402FR-1310KP?qs=sGAEpiMZZMtlubZbdhIBIAA5Rg%252BBqQHDc9Qj423b9VE%3D</t>
+  </si>
+  <si>
+    <t>RC0402FR-1310KP Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>Diode for Neg V</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Diodes-Incorporated/1N4001-T?qs=e%2FRqmsgwm9i%2FVrrtazegeg%3D%3D</t>
+  </si>
+  <si>
+    <t>DO-41</t>
+  </si>
+  <si>
+    <t>DO-42</t>
+  </si>
+  <si>
+    <t>DO-43</t>
+  </si>
+  <si>
+    <t>DO-44</t>
+  </si>
+  <si>
+    <t>1N4001-T Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>220uF</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Wurth-Elektronik/860020273009?qs=sGAEpiMZZMsh%252B1woXyUXj4jKQI6sNRw6c3%252BIcJMXhKw%3D</t>
+  </si>
+  <si>
+    <t>2.5 mm</t>
+  </si>
+  <si>
+    <t>860020273009 Datasheet (PDF)</t>
   </si>
 </sst>
 </file>
@@ -4644,8 +4789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5E7DEB4-5FFB-4F8D-963A-C08EFBE9A2C1}">
   <dimension ref="A1:F108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="F111" sqref="F111"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6899,4 +7044,422 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId78"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D76251E-3DCF-437B-AB0F-DECE015281CC}">
+  <dimension ref="A1:F19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C2">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="E2" t="s">
+        <v>245</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B3" t="s">
+        <v>253</v>
+      </c>
+      <c r="C3">
+        <v>0.60699999999999998</v>
+      </c>
+      <c r="D3" t="s">
+        <v>247</v>
+      </c>
+      <c r="E3" t="s">
+        <v>249</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>251</v>
+      </c>
+      <c r="B4" t="s">
+        <v>252</v>
+      </c>
+      <c r="C4">
+        <v>0.71799999999999997</v>
+      </c>
+      <c r="D4" t="s">
+        <v>254</v>
+      </c>
+      <c r="E4" t="s">
+        <v>249</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>256</v>
+      </c>
+      <c r="C5">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D5" t="s">
+        <v>258</v>
+      </c>
+      <c r="E5">
+        <v>1608</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>257</v>
+      </c>
+      <c r="C6">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D6" t="s">
+        <v>260</v>
+      </c>
+      <c r="E6">
+        <v>2012</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>256</v>
+      </c>
+      <c r="C7">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D7" t="s">
+        <v>258</v>
+      </c>
+      <c r="E7">
+        <v>1608</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>257</v>
+      </c>
+      <c r="C8">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D8" t="s">
+        <v>260</v>
+      </c>
+      <c r="E8">
+        <v>2012</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>263</v>
+      </c>
+      <c r="B9" t="s">
+        <v>262</v>
+      </c>
+      <c r="C9">
+        <v>0.52400000000000002</v>
+      </c>
+      <c r="D9" t="s">
+        <v>264</v>
+      </c>
+      <c r="E9" t="s">
+        <v>249</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>266</v>
+      </c>
+      <c r="B10" t="s">
+        <v>268</v>
+      </c>
+      <c r="C10">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D10" t="s">
+        <v>269</v>
+      </c>
+      <c r="E10">
+        <v>1005</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>267</v>
+      </c>
+      <c r="B11" t="s">
+        <v>271</v>
+      </c>
+      <c r="C11">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D11" t="s">
+        <v>272</v>
+      </c>
+      <c r="E11">
+        <v>1005</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>281</v>
+      </c>
+      <c r="B12" t="s">
+        <v>274</v>
+      </c>
+      <c r="C12">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="D12" t="s">
+        <v>275</v>
+      </c>
+      <c r="E12" t="s">
+        <v>276</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>282</v>
+      </c>
+      <c r="B13" t="s">
+        <v>274</v>
+      </c>
+      <c r="C13">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="D13" t="s">
+        <v>275</v>
+      </c>
+      <c r="E13" t="s">
+        <v>277</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>283</v>
+      </c>
+      <c r="B14" t="s">
+        <v>274</v>
+      </c>
+      <c r="C14">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="D14" t="s">
+        <v>275</v>
+      </c>
+      <c r="E14" t="s">
+        <v>278</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>284</v>
+      </c>
+      <c r="B15" t="s">
+        <v>274</v>
+      </c>
+      <c r="C15">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="D15" t="s">
+        <v>275</v>
+      </c>
+      <c r="E15" t="s">
+        <v>279</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>285</v>
+      </c>
+      <c r="C16">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="D16" t="s">
+        <v>286</v>
+      </c>
+      <c r="E16" t="s">
+        <v>287</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>285</v>
+      </c>
+      <c r="C17">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="D17" t="s">
+        <v>286</v>
+      </c>
+      <c r="E17" t="s">
+        <v>287</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>285</v>
+      </c>
+      <c r="C18">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="D18" t="s">
+        <v>286</v>
+      </c>
+      <c r="E18" t="s">
+        <v>287</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" t="s">
+        <v>285</v>
+      </c>
+      <c r="C19">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="D19" t="s">
+        <v>286</v>
+      </c>
+      <c r="E19" t="s">
+        <v>287</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>288</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{F7601112-5E1E-4D0E-BE31-9676A7D4FBFB}"/>
+    <hyperlink ref="F2" r:id="rId2" display="https://www.mouser.ca/datasheet/2/670/pj_070bh_smt_tr-1778782.pdf" xr:uid="{402328B1-ACA2-41C6-A714-3277512E8C2C}"/>
+    <hyperlink ref="F3" r:id="rId3" display="https://www.mouser.ca/datasheet/2/308/1/MC78L00A_D-2315651.pdf" xr:uid="{6F8E1E5A-793C-400E-9E7B-FD3CEFE42008}"/>
+    <hyperlink ref="F4" r:id="rId4" display="http://www.ti.com/general/docs/suppproductinfo.tsp?distId=26&amp;gotoUrl=http://www.ti.com/lit/gpn/mc79l" xr:uid="{218BC41D-9665-49ED-BE78-800B8B13E928}"/>
+    <hyperlink ref="F5" r:id="rId5" display="https://www.mouser.ca/datasheet/2/445/885012206074-1727575.pdf" xr:uid="{52890E42-E5EC-4144-B12A-ACE8949FCE71}"/>
+    <hyperlink ref="F7" r:id="rId6" display="https://www.mouser.ca/datasheet/2/445/885012206074-1727575.pdf" xr:uid="{D17B156E-38A1-43DA-837B-3E11B1A36780}"/>
+    <hyperlink ref="F6" r:id="rId7" display="https://www.mouser.ca/datasheet/2/585/MLCC-1837944.pdf" xr:uid="{B5E4DB07-AA26-45F7-8D12-2D1C7AA146A1}"/>
+    <hyperlink ref="F8" r:id="rId8" display="https://www.mouser.ca/datasheet/2/585/MLCC-1837944.pdf" xr:uid="{6CD6DD47-0D21-450D-8CB9-10ACFC0AF589}"/>
+    <hyperlink ref="F9" r:id="rId9" display="http://www.ti.com/general/docs/suppproductinfo.tsp?distId=26&amp;gotoUrl=http%3A%2F%2Fwww.ti.com%2Flit%2Fgpn%2Fne555" xr:uid="{FB2DF6E4-09A3-42A2-AEF8-9E2485A608FF}"/>
+    <hyperlink ref="F10" r:id="rId10" display="https://www.mouser.ca/datasheet/2/414/ttelectronics_ttrb_s_a0010037465_1-1991369.pdf" xr:uid="{0B5F64DC-CE67-4581-BCD5-C44893DE0ABC}"/>
+    <hyperlink ref="F11" r:id="rId11" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_51_RoHS_P_4-2944025.pdf" xr:uid="{02613C4F-AE1A-4770-BD64-FE47AE0E4520}"/>
+    <hyperlink ref="F12" r:id="rId12" display="https://www.diodes.com/assets/Datasheets/ds28002.pdf" xr:uid="{ACD05526-59A8-4F88-813B-254108DA8998}"/>
+    <hyperlink ref="F13:F15" r:id="rId13" display="https://www.diodes.com/assets/Datasheets/ds28002.pdf" xr:uid="{02F96806-947E-4B7D-B6C1-20D4DA35DC4D}"/>
+    <hyperlink ref="F16" r:id="rId14" display="https://www.mouser.ca/datasheet/2/445/860020273009-1725581.pdf" xr:uid="{9D448218-EE6C-4A4C-9E2F-39CD14500BF5}"/>
+    <hyperlink ref="F17:F19" r:id="rId15" display="https://www.mouser.ca/datasheet/2/445/860020273009-1725581.pdf" xr:uid="{4920975F-26D1-4DC7-A2F2-44F04D705761}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Sourced male and female audio inputs, selector switch and power button
</commit_message>
<xml_diff>
--- a/Documents/BOM.xlsx
+++ b/Documents/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ECE_Projects\Music_Visualizer\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{219855FE-35BF-4243-B163-8CAE2E539364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4D46BE6-532E-4BA7-BABA-FFF0FD696CE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{1F4A7036-4694-4970-BB5D-7CBECC831452}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="9" xr2:uid="{1F4A7036-4694-4970-BB5D-7CBECC831452}"/>
   </bookViews>
   <sheets>
     <sheet name="Sub-Bass" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="Brilliance" sheetId="7" r:id="rId7"/>
     <sheet name="All Filters" sheetId="8" r:id="rId8"/>
     <sheet name="Power" sheetId="9" r:id="rId9"/>
+    <sheet name="Audio Input" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1074" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1096" uniqueCount="305">
   <si>
     <t>Component</t>
   </si>
@@ -910,6 +911,54 @@
   </si>
   <si>
     <t>860020273009 Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>SP-3533-02</t>
+  </si>
+  <si>
+    <t>Male Jack</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/CUI-Devices/SP-3533-02?qs=%252BEew9%252B0nqrCkfyt%2FFhI%252B5A%3D%3D</t>
+  </si>
+  <si>
+    <t>SP-3533-02 Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>STX-3000</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Kycon/STX-3000?qs=kjZ2mQLP346Nbz1X9BOzfg%3D%3D</t>
+  </si>
+  <si>
+    <t>STX-3000 Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>Female Jack</t>
+  </si>
+  <si>
+    <t>OS102011MS2QN1</t>
+  </si>
+  <si>
+    <t>Slide Selector Switch</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/CK/OS102011MS2QN1?qs=WtljUlYws5RvQ1hEv876nQ%3D%3D</t>
+  </si>
+  <si>
+    <t>OS102011MS2QN1 Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>RA11131123</t>
+  </si>
+  <si>
+    <t>On/OFF switch</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/E-Switch/RA11131123?qs=QtyuwXswaQhc6OwdGDJDiQ%3D%3D</t>
+  </si>
+  <si>
+    <t>RA11131123 Datasheet (PDF)</t>
   </si>
 </sst>
 </file>
@@ -1827,6 +1876,120 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DDCAF3D-5C32-4D35-8B8A-81DDBAD115B7}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>289</v>
+      </c>
+      <c r="B2" t="s">
+        <v>290</v>
+      </c>
+      <c r="C2">
+        <v>2.98</v>
+      </c>
+      <c r="D2" t="s">
+        <v>291</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>293</v>
+      </c>
+      <c r="B3" t="s">
+        <v>296</v>
+      </c>
+      <c r="C3">
+        <v>1.02</v>
+      </c>
+      <c r="D3" t="s">
+        <v>294</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>297</v>
+      </c>
+      <c r="B4" t="s">
+        <v>298</v>
+      </c>
+      <c r="C4">
+        <v>0.53800000000000003</v>
+      </c>
+      <c r="D4" t="s">
+        <v>299</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>301</v>
+      </c>
+      <c r="B5" t="s">
+        <v>302</v>
+      </c>
+      <c r="C5">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="D5" t="s">
+        <v>303</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>304</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" display="https://www.mouser.ca/datasheet/2/670/sp_3533_02-1779105.pdf" xr:uid="{0BBD912E-C261-456C-88A9-FE678FAB28D2}"/>
+    <hyperlink ref="F3" r:id="rId2" display="https://www.mouser.ca/datasheet/2/222/STX3000-334650.pdf" xr:uid="{1ACD33CC-24A0-4994-8029-9014B522D898}"/>
+    <hyperlink ref="F4" r:id="rId3" display="https://www.mouser.ca/datasheet/2/60/os-1841429.pdf" xr:uid="{17ED7DCD-6C55-4839-A640-E17F4B8F5C87}"/>
+    <hyperlink ref="F5" r:id="rId4" display="https://www.mouser.ca/datasheet/2/140/ESCH_S_A0005379088_1-2548267.pdf" xr:uid="{6163F807-0B97-43B7-BFDF-6FED3C31E5D7}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9015A39E-4C3F-4E48-B877-A44E11CEB1FD}">
   <dimension ref="A1:H23"/>
@@ -7050,8 +7213,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D76251E-3DCF-437B-AB0F-DECE015281CC}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Updated Bom, Full Visualizer Circuit, and Circuit for establishing -5 volts
</commit_message>
<xml_diff>
--- a/Documents/BOM.xlsx
+++ b/Documents/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ECE_Projects\Music_Visualizer\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4D46BE6-532E-4BA7-BABA-FFF0FD696CE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B957C07-C0F7-4D18-9245-A48AC9359E9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="9" xr2:uid="{1F4A7036-4694-4970-BB5D-7CBECC831452}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="766" activeTab="4" xr2:uid="{1F4A7036-4694-4970-BB5D-7CBECC831452}"/>
   </bookViews>
   <sheets>
     <sheet name="Sub-Bass" sheetId="1" r:id="rId1"/>
@@ -21,8 +21,11 @@
     <sheet name="Presence" sheetId="6" r:id="rId6"/>
     <sheet name="Brilliance" sheetId="7" r:id="rId7"/>
     <sheet name="All Filters" sheetId="8" r:id="rId8"/>
-    <sheet name="Power" sheetId="9" r:id="rId9"/>
-    <sheet name="Audio Input" sheetId="10" r:id="rId10"/>
+    <sheet name="FilterAmps" sheetId="12" r:id="rId9"/>
+    <sheet name="PowerV1" sheetId="9" r:id="rId10"/>
+    <sheet name="PowerV2" sheetId="13" r:id="rId11"/>
+    <sheet name="Audio Input" sheetId="10" r:id="rId12"/>
+    <sheet name="LED" sheetId="11" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1096" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1257" uniqueCount="363">
   <si>
     <t>Component</t>
   </si>
@@ -959,6 +962,180 @@
   </si>
   <si>
     <t>RA11131123 Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>Multicolored LEDs</t>
+  </si>
+  <si>
+    <t>Volume Display</t>
+  </si>
+  <si>
+    <t>https://www.amazon.ca/gp/product/B07N2GVCYZ/ref=ppx_yo_dt_b_asin_title_o03_s00?ie=UTF8&amp;psc=1</t>
+  </si>
+  <si>
+    <t>LM3915</t>
+  </si>
+  <si>
+    <t>LED Driver</t>
+  </si>
+  <si>
+    <t>https://www.amazon.ca/gp/product/B0839884KH/ref=ppx_yo_dt_b_asin_title_o05_s00?ie=UTF8&amp;psc=1</t>
+  </si>
+  <si>
+    <t>https://www.electroschematics.com/wp-content/uploads/2010/02/LM3915.pdf</t>
+  </si>
+  <si>
+    <t>https://cdn-shop.adafruit.com/datasheets/WP7113SRD-D.pdf</t>
+  </si>
+  <si>
+    <t>220u</t>
+  </si>
+  <si>
+    <t>680ohm</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/RC0603FR-07680RL?qs=sGAEpiMZZMtlubZbdhIBIP1i7CT%2FCYQh9lCWD%252B01TEA%3D</t>
+  </si>
+  <si>
+    <t>RC0603FR-07680RL Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Bourns/PTV09A-4020F-A502?qs=Qzws7J6gxqxBJ1n21bU9RA%3D%3D</t>
+  </si>
+  <si>
+    <t>PTV09A-4020F-A502 Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>NCS333ASQ3T2G</t>
+  </si>
+  <si>
+    <t>Op-amp (voltage buffer)</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/onsemi/NCS333ASQ3T2G?qs=F5EMLAvA7ICve3AOVqAtkg%3D%3D</t>
+  </si>
+  <si>
+    <t>NCS333ASQ3T2G Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>SC-70-5</t>
+  </si>
+  <si>
+    <t>NCP161ASN350T1G</t>
+  </si>
+  <si>
+    <t>LDO 3.5V Regulator</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/onsemi/NCP161ASN350T1G?qs=vLWxofP3U2wUsLuPD6e2Og%3D%3D</t>
+  </si>
+  <si>
+    <t>SOT-23-5</t>
+  </si>
+  <si>
+    <t>NCP161ASN350T1G Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>Potentiometer</t>
+  </si>
+  <si>
+    <t>5k - LED Current Adjuster</t>
+  </si>
+  <si>
+    <t>5k - LED Rhi Adjuster</t>
+  </si>
+  <si>
+    <t>LM324DR2G</t>
+  </si>
+  <si>
+    <t>Filter Op amps</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/onsemi/LM324DR2G?qs=2OtswVQKCOEcq0L2uFhs6w%3D%3D</t>
+  </si>
+  <si>
+    <t>SOIC-14</t>
+  </si>
+  <si>
+    <t>LM324DR2G Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>Negative V Circuit</t>
+  </si>
+  <si>
+    <t>Negative V w Reg</t>
+  </si>
+  <si>
+    <t>10uF</t>
+  </si>
+  <si>
+    <t>100uF</t>
+  </si>
+  <si>
+    <t>0.002uF</t>
+  </si>
+  <si>
+    <t>20k</t>
+  </si>
+  <si>
+    <t>102k</t>
+  </si>
+  <si>
+    <t>1uF</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/KEMET/C0402C101K8RACAUTO?qs=sGAEpiMZZMsh%252B1woXyUXj5aDdx2Hq%2F9OG0FkqlIM%252BR0%3D</t>
+  </si>
+  <si>
+    <t>C0402C101K8RACAUTO Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Samsung-Electro-Mechanics/CL21A106MQFNNNE?qs=sGAEpiMZZMsh%252B1woXyUXj%252BV5GOLijFH83FB2x1Z8J88%3D</t>
+  </si>
+  <si>
+    <t>CL21A106MQFNNNE Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Wurth-Elektronik/860010372006?qs=sGAEpiMZZMsh%252B1woXyUXj4jKQI6sNRw6f7foC99ndMU%3D</t>
+  </si>
+  <si>
+    <t>T-H</t>
+  </si>
+  <si>
+    <t>860010372006 Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/CC0402KRX7R9BB202?qs=sGAEpiMZZMsh%252B1woXyUXj8PMfHfoZZHB4VPZkHtoXzE%3D</t>
+  </si>
+  <si>
+    <t>CC0402KRX7R9BB202 Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/RC0603FR-0720KL?qs=sGAEpiMZZMtlubZbdhIBIPpBVm91En7nVDpcdouZiz8%3D</t>
+  </si>
+  <si>
+    <t>RC0603FR-0720KL Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/AC0603FR-07102KL?qs=sGAEpiMZZMtlubZbdhIBIG07xJe44c5ATOIyMmimQ4I%3D</t>
+  </si>
+  <si>
+    <t>AC0603FR-07102KL Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Texas-Instruments/LT1054IPE4?qs=paYhMW8qfivWYjyBPd45bA%3D%3D</t>
+  </si>
+  <si>
+    <t>LT1054IPE4 Datasheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +5V Regulator</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -5V Conv &amp; Reg</t>
+  </si>
+  <si>
+    <t>LT1054IPE4</t>
   </si>
 </sst>
 </file>
@@ -1877,11 +2054,763 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D76251E-3DCF-437B-AB0F-DECE015281CC}">
+  <dimension ref="A1:F21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C2">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="E2" t="s">
+        <v>245</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B3" t="s">
+        <v>253</v>
+      </c>
+      <c r="C3">
+        <v>0.60699999999999998</v>
+      </c>
+      <c r="D3" t="s">
+        <v>247</v>
+      </c>
+      <c r="E3" t="s">
+        <v>249</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>251</v>
+      </c>
+      <c r="B4" t="s">
+        <v>252</v>
+      </c>
+      <c r="C4">
+        <v>0.71799999999999997</v>
+      </c>
+      <c r="D4" t="s">
+        <v>254</v>
+      </c>
+      <c r="E4" t="s">
+        <v>249</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>256</v>
+      </c>
+      <c r="C5">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D5" t="s">
+        <v>258</v>
+      </c>
+      <c r="E5">
+        <v>1608</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>257</v>
+      </c>
+      <c r="C6">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D6" t="s">
+        <v>260</v>
+      </c>
+      <c r="E6">
+        <v>2012</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>256</v>
+      </c>
+      <c r="C7">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D7" t="s">
+        <v>258</v>
+      </c>
+      <c r="E7">
+        <v>1608</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>257</v>
+      </c>
+      <c r="C8">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D8" t="s">
+        <v>260</v>
+      </c>
+      <c r="E8">
+        <v>2012</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>263</v>
+      </c>
+      <c r="B9" t="s">
+        <v>262</v>
+      </c>
+      <c r="C9">
+        <v>0.52400000000000002</v>
+      </c>
+      <c r="D9" t="s">
+        <v>264</v>
+      </c>
+      <c r="E9" t="s">
+        <v>249</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>266</v>
+      </c>
+      <c r="B10" t="s">
+        <v>268</v>
+      </c>
+      <c r="C10">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D10" t="s">
+        <v>269</v>
+      </c>
+      <c r="E10">
+        <v>1005</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>267</v>
+      </c>
+      <c r="B11" t="s">
+        <v>271</v>
+      </c>
+      <c r="C11">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D11" t="s">
+        <v>272</v>
+      </c>
+      <c r="E11">
+        <v>1005</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>281</v>
+      </c>
+      <c r="B12" t="s">
+        <v>274</v>
+      </c>
+      <c r="C12">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="D12" t="s">
+        <v>275</v>
+      </c>
+      <c r="E12" t="s">
+        <v>276</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>282</v>
+      </c>
+      <c r="B13" t="s">
+        <v>274</v>
+      </c>
+      <c r="C13">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="D13" t="s">
+        <v>275</v>
+      </c>
+      <c r="E13" t="s">
+        <v>277</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>283</v>
+      </c>
+      <c r="B14" t="s">
+        <v>274</v>
+      </c>
+      <c r="C14">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="D14" t="s">
+        <v>275</v>
+      </c>
+      <c r="E14" t="s">
+        <v>278</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>284</v>
+      </c>
+      <c r="B15" t="s">
+        <v>274</v>
+      </c>
+      <c r="C15">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="D15" t="s">
+        <v>275</v>
+      </c>
+      <c r="E15" t="s">
+        <v>279</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>285</v>
+      </c>
+      <c r="C16">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="D16" t="s">
+        <v>286</v>
+      </c>
+      <c r="E16" t="s">
+        <v>287</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>285</v>
+      </c>
+      <c r="C17">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="D17" t="s">
+        <v>286</v>
+      </c>
+      <c r="E17" t="s">
+        <v>287</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>285</v>
+      </c>
+      <c r="C18">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="D18" t="s">
+        <v>286</v>
+      </c>
+      <c r="E18" t="s">
+        <v>287</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" t="s">
+        <v>285</v>
+      </c>
+      <c r="C19">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="D19" t="s">
+        <v>286</v>
+      </c>
+      <c r="E19" t="s">
+        <v>287</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>337</v>
+      </c>
+      <c r="C20">
+        <f>SUM(C9:C19)</f>
+        <v>2.7879999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>338</v>
+      </c>
+      <c r="C21">
+        <f>SUM(C9:C19)+C4+C5+C6</f>
+        <v>3.7819999999999996</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{F7601112-5E1E-4D0E-BE31-9676A7D4FBFB}"/>
+    <hyperlink ref="F2" r:id="rId2" display="https://www.mouser.ca/datasheet/2/670/pj_070bh_smt_tr-1778782.pdf" xr:uid="{402328B1-ACA2-41C6-A714-3277512E8C2C}"/>
+    <hyperlink ref="F3" r:id="rId3" display="https://www.mouser.ca/datasheet/2/308/1/MC78L00A_D-2315651.pdf" xr:uid="{6F8E1E5A-793C-400E-9E7B-FD3CEFE42008}"/>
+    <hyperlink ref="F4" r:id="rId4" display="http://www.ti.com/general/docs/suppproductinfo.tsp?distId=26&amp;gotoUrl=http://www.ti.com/lit/gpn/mc79l" xr:uid="{218BC41D-9665-49ED-BE78-800B8B13E928}"/>
+    <hyperlink ref="F5" r:id="rId5" display="https://www.mouser.ca/datasheet/2/445/885012206074-1727575.pdf" xr:uid="{52890E42-E5EC-4144-B12A-ACE8949FCE71}"/>
+    <hyperlink ref="F7" r:id="rId6" display="https://www.mouser.ca/datasheet/2/445/885012206074-1727575.pdf" xr:uid="{D17B156E-38A1-43DA-837B-3E11B1A36780}"/>
+    <hyperlink ref="F6" r:id="rId7" display="https://www.mouser.ca/datasheet/2/585/MLCC-1837944.pdf" xr:uid="{B5E4DB07-AA26-45F7-8D12-2D1C7AA146A1}"/>
+    <hyperlink ref="F8" r:id="rId8" display="https://www.mouser.ca/datasheet/2/585/MLCC-1837944.pdf" xr:uid="{6CD6DD47-0D21-450D-8CB9-10ACFC0AF589}"/>
+    <hyperlink ref="F9" r:id="rId9" display="http://www.ti.com/general/docs/suppproductinfo.tsp?distId=26&amp;gotoUrl=http%3A%2F%2Fwww.ti.com%2Flit%2Fgpn%2Fne555" xr:uid="{FB2DF6E4-09A3-42A2-AEF8-9E2485A608FF}"/>
+    <hyperlink ref="F10" r:id="rId10" display="https://www.mouser.ca/datasheet/2/414/ttelectronics_ttrb_s_a0010037465_1-1991369.pdf" xr:uid="{0B5F64DC-CE67-4581-BCD5-C44893DE0ABC}"/>
+    <hyperlink ref="F11" r:id="rId11" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_51_RoHS_P_4-2944025.pdf" xr:uid="{02613C4F-AE1A-4770-BD64-FE47AE0E4520}"/>
+    <hyperlink ref="F12" r:id="rId12" display="https://www.diodes.com/assets/Datasheets/ds28002.pdf" xr:uid="{ACD05526-59A8-4F88-813B-254108DA8998}"/>
+    <hyperlink ref="F13:F15" r:id="rId13" display="https://www.diodes.com/assets/Datasheets/ds28002.pdf" xr:uid="{02F96806-947E-4B7D-B6C1-20D4DA35DC4D}"/>
+    <hyperlink ref="F16" r:id="rId14" display="https://www.mouser.ca/datasheet/2/445/860020273009-1725581.pdf" xr:uid="{9D448218-EE6C-4A4C-9E2F-39CD14500BF5}"/>
+    <hyperlink ref="F17:F19" r:id="rId15" display="https://www.mouser.ca/datasheet/2/445/860020273009-1725581.pdf" xr:uid="{4920975F-26D1-4DC7-A2F2-44F04D705761}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C595792-1ED3-4550-B2C6-F49A784AB9C0}">
+  <dimension ref="A1:F19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C2">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="E2" t="s">
+        <v>245</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B3" t="s">
+        <v>360</v>
+      </c>
+      <c r="C3">
+        <v>0.60699999999999998</v>
+      </c>
+      <c r="D3" t="s">
+        <v>247</v>
+      </c>
+      <c r="E3" t="s">
+        <v>249</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>362</v>
+      </c>
+      <c r="B4" t="s">
+        <v>361</v>
+      </c>
+      <c r="C4">
+        <v>3.81</v>
+      </c>
+      <c r="D4" t="s">
+        <v>358</v>
+      </c>
+      <c r="E4" t="s">
+        <v>350</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>256</v>
+      </c>
+      <c r="C5">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D5" t="s">
+        <v>258</v>
+      </c>
+      <c r="E5">
+        <v>1608</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>257</v>
+      </c>
+      <c r="C6">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D6" t="s">
+        <v>260</v>
+      </c>
+      <c r="E6">
+        <v>2012</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>344</v>
+      </c>
+      <c r="C7">
+        <v>0.11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>345</v>
+      </c>
+      <c r="E7">
+        <v>1005</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>344</v>
+      </c>
+      <c r="C8">
+        <v>0.11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>345</v>
+      </c>
+      <c r="E8">
+        <v>1005</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>339</v>
+      </c>
+      <c r="C9">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D9" t="s">
+        <v>347</v>
+      </c>
+      <c r="E9">
+        <v>2012</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>340</v>
+      </c>
+      <c r="C10">
+        <v>0.152</v>
+      </c>
+      <c r="D10" t="s">
+        <v>349</v>
+      </c>
+      <c r="E10" t="s">
+        <v>350</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>204</v>
+      </c>
+      <c r="B11" t="s">
+        <v>341</v>
+      </c>
+      <c r="C11">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D11" t="s">
+        <v>352</v>
+      </c>
+      <c r="E11">
+        <v>1005</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>342</v>
+      </c>
+      <c r="C12">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D12" t="s">
+        <v>354</v>
+      </c>
+      <c r="E12">
+        <v>1608</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>343</v>
+      </c>
+      <c r="C13">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D13" t="s">
+        <v>356</v>
+      </c>
+      <c r="E13">
+        <v>1608</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C14">
+        <f>SUM(C2:C13)</f>
+        <v>7.7969999999999997</v>
+      </c>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F19" s="3"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{CFF3DE83-5BAE-4804-8A55-854D18FC4CED}"/>
+    <hyperlink ref="F2" r:id="rId2" display="https://www.mouser.ca/datasheet/2/670/pj_070bh_smt_tr-1778782.pdf" xr:uid="{2B8C46C9-C49A-424B-B89F-66EA4B5C10F7}"/>
+    <hyperlink ref="F3" r:id="rId3" display="https://www.mouser.ca/datasheet/2/308/1/MC78L00A_D-2315651.pdf" xr:uid="{43449A74-1523-4758-8BBF-93FCE8715047}"/>
+    <hyperlink ref="F5" r:id="rId4" display="https://www.mouser.ca/datasheet/2/445/885012206074-1727575.pdf" xr:uid="{EBC70B85-FF91-416D-B612-46304B897B4E}"/>
+    <hyperlink ref="F6" r:id="rId5" display="https://www.mouser.ca/datasheet/2/585/MLCC-1837944.pdf" xr:uid="{D8D5728D-F054-483C-A177-2BEE9D8A376A}"/>
+    <hyperlink ref="F7" r:id="rId6" display="https://www.mouser.ca/datasheet/2/212/1/C0603X102K4RACAUTO-2933386.pdf" xr:uid="{C98FBE3A-22C1-4CF7-A5EE-579F267C6CDB}"/>
+    <hyperlink ref="F8" r:id="rId7" display="https://www.mouser.ca/datasheet/2/212/1/C0603X102K4RACAUTO-2933386.pdf" xr:uid="{412EA33E-F9D4-4F61-AB59-88704BA3C736}"/>
+    <hyperlink ref="F9" r:id="rId8" display="https://www.mouser.ca/datasheet/2/585/MLCC-1837944.pdf" xr:uid="{FEDC0B60-64E5-413A-890C-A929293CB610}"/>
+    <hyperlink ref="F10" r:id="rId9" display="https://www.mouser.ca/datasheet/2/445/860010372006-1725314.pdf" xr:uid="{DBA0956B-B8D9-4F30-93A7-E5D8C434E760}"/>
+    <hyperlink ref="F11" r:id="rId10" display="https://www.mouser.ca/datasheet/2/447/yago_s_a0003557223_1-2286436.pdf" xr:uid="{2BF698B5-2BBF-4440-9932-2433F49FF139}"/>
+    <hyperlink ref="F4" r:id="rId11" display="https://www.ti.com/general/docs/suppproductinfo.tsp?distId=26&amp;gotoUrl=https://www.ti.com/lit/gpn/lt1054" xr:uid="{3B0922DB-30FA-4D77-8674-D69A0BABD8CF}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DDCAF3D-5C32-4D35-8B8A-81DDBAD115B7}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1987,6 +2916,324 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{422FDBAB-416A-4921-A7D0-3405100F2A2C}">
+  <dimension ref="A1:F15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>305</v>
+      </c>
+      <c r="B2" t="s">
+        <v>306</v>
+      </c>
+      <c r="C2">
+        <v>16.59</v>
+      </c>
+      <c r="D2" t="s">
+        <v>307</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>308</v>
+      </c>
+      <c r="B3" t="s">
+        <v>309</v>
+      </c>
+      <c r="C3">
+        <v>22.67</v>
+      </c>
+      <c r="D3" t="s">
+        <v>310</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C4">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="E4" t="s">
+        <v>287</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>314</v>
+      </c>
+      <c r="C5">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D5" t="s">
+        <v>315</v>
+      </c>
+      <c r="E5">
+        <v>1608</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>314</v>
+      </c>
+      <c r="C6">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D6" t="s">
+        <v>315</v>
+      </c>
+      <c r="E6">
+        <v>1608</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>314</v>
+      </c>
+      <c r="C7">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D7" t="s">
+        <v>315</v>
+      </c>
+      <c r="E7">
+        <v>1608</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>314</v>
+      </c>
+      <c r="C8">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D8" t="s">
+        <v>315</v>
+      </c>
+      <c r="E8">
+        <v>1608</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>314</v>
+      </c>
+      <c r="C9">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D9" t="s">
+        <v>315</v>
+      </c>
+      <c r="E9">
+        <v>1608</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>314</v>
+      </c>
+      <c r="C10">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D10" t="s">
+        <v>315</v>
+      </c>
+      <c r="E10">
+        <v>1608</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>314</v>
+      </c>
+      <c r="C11">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D11" t="s">
+        <v>315</v>
+      </c>
+      <c r="E11">
+        <v>1608</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>329</v>
+      </c>
+      <c r="B12" t="s">
+        <v>330</v>
+      </c>
+      <c r="C12">
+        <v>1.38</v>
+      </c>
+      <c r="D12" t="s">
+        <v>317</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>319</v>
+      </c>
+      <c r="B13" t="s">
+        <v>320</v>
+      </c>
+      <c r="C13">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="D13" t="s">
+        <v>321</v>
+      </c>
+      <c r="E13" t="s">
+        <v>323</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>324</v>
+      </c>
+      <c r="B14" t="s">
+        <v>325</v>
+      </c>
+      <c r="C14">
+        <v>0.71799999999999997</v>
+      </c>
+      <c r="D14" t="s">
+        <v>326</v>
+      </c>
+      <c r="E14" t="s">
+        <v>327</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>329</v>
+      </c>
+      <c r="B15" t="s">
+        <v>331</v>
+      </c>
+      <c r="C15">
+        <v>1.38</v>
+      </c>
+      <c r="D15" t="s">
+        <v>317</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>318</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1" xr:uid="{4086144A-D13C-4CF7-B0A2-04DC9FD2E687}"/>
+    <hyperlink ref="F4" r:id="rId2" display="https://www.mouser.ca/datasheet/2/445/860020273009-1725581.pdf" xr:uid="{DF0F49A7-30B6-415A-AA6E-5F9F70F3E664}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{502E7D33-C429-41BF-8FAA-6D1BB65BAFC1}"/>
+    <hyperlink ref="F12" r:id="rId4" display="https://www.mouser.ca/datasheet/2/54/ptv09-777818.pdf" xr:uid="{BBF2E0E5-0197-4455-B910-736161147ECB}"/>
+    <hyperlink ref="F13" r:id="rId5" display="https://www.mouser.ca/datasheet/2/308/1/NCS333_D-2317376.pdf" xr:uid="{7C0CF1F9-6D8B-4838-AF4F-5E3806F151A2}"/>
+    <hyperlink ref="F14" r:id="rId6" display="https://www.mouser.ca/datasheet/2/308/1/NCP161_D-2316989.pdf" xr:uid="{7A98D1F1-404F-44D8-89D1-D9D1436D893F}"/>
+    <hyperlink ref="F15" r:id="rId7" display="https://www.mouser.ca/datasheet/2/54/ptv09-777818.pdf" xr:uid="{8236BBA3-E1C5-477D-B2F7-BBC0C6E41223}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -3492,7 +4739,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FA0D483-C574-49A8-A0EA-072A18CA1F90}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E14" sqref="E14:H19"/>
     </sheetView>
   </sheetViews>
@@ -4952,8 +6199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5E7DEB4-5FFB-4F8D-963A-C08EFBE9A2C1}">
   <dimension ref="A1:F108"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="A109" sqref="A109:A114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7210,17 +8457,18 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D76251E-3DCF-437B-AB0F-DECE015281CC}">
-  <dimension ref="A1:F19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F0F8697-67F6-479D-8A67-86E9F1D85B02}">
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -7244,385 +8492,132 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>242</v>
+      <c r="A2" s="14" t="s">
+        <v>332</v>
       </c>
       <c r="B2" t="s">
-        <v>243</v>
+        <v>333</v>
       </c>
       <c r="C2">
-        <v>2.1800000000000002</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>244</v>
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="D2" t="s">
+        <v>334</v>
       </c>
       <c r="E2" t="s">
-        <v>245</v>
+        <v>335</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>246</v>
+        <v>336</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>248</v>
+      <c r="A3" s="14" t="s">
+        <v>332</v>
       </c>
       <c r="B3" t="s">
-        <v>253</v>
+        <v>333</v>
       </c>
       <c r="C3">
-        <v>0.60699999999999998</v>
+        <v>0.75900000000000001</v>
       </c>
       <c r="D3" t="s">
-        <v>247</v>
+        <v>334</v>
       </c>
       <c r="E3" t="s">
-        <v>249</v>
+        <v>335</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>250</v>
+        <v>336</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>251</v>
+      <c r="A4" s="14" t="s">
+        <v>332</v>
       </c>
       <c r="B4" t="s">
-        <v>252</v>
+        <v>333</v>
       </c>
       <c r="C4">
-        <v>0.71799999999999997</v>
+        <v>0.75900000000000001</v>
       </c>
       <c r="D4" t="s">
-        <v>254</v>
+        <v>334</v>
       </c>
       <c r="E4" t="s">
-        <v>249</v>
+        <v>335</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>255</v>
+        <v>336</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>17</v>
+      <c r="A5" s="14" t="s">
+        <v>332</v>
       </c>
       <c r="B5" t="s">
-        <v>256</v>
+        <v>333</v>
       </c>
       <c r="C5">
-        <v>0.13800000000000001</v>
+        <v>0.75900000000000001</v>
       </c>
       <c r="D5" t="s">
-        <v>258</v>
-      </c>
-      <c r="E5">
-        <v>1608</v>
+        <v>334</v>
+      </c>
+      <c r="E5" t="s">
+        <v>335</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>259</v>
+        <v>336</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>18</v>
+      <c r="A6" s="14" t="s">
+        <v>332</v>
       </c>
       <c r="B6" t="s">
-        <v>257</v>
+        <v>333</v>
       </c>
       <c r="C6">
-        <v>0.13800000000000001</v>
+        <v>0.75900000000000001</v>
       </c>
       <c r="D6" t="s">
-        <v>260</v>
-      </c>
-      <c r="E6">
-        <v>2012</v>
+        <v>334</v>
+      </c>
+      <c r="E6" t="s">
+        <v>335</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>261</v>
+        <v>336</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>19</v>
+      <c r="A7" s="14" t="s">
+        <v>332</v>
       </c>
       <c r="B7" t="s">
-        <v>256</v>
+        <v>333</v>
       </c>
       <c r="C7">
-        <v>0.13800000000000001</v>
+        <v>0.75900000000000001</v>
       </c>
       <c r="D7" t="s">
-        <v>258</v>
-      </c>
-      <c r="E7">
-        <v>1608</v>
+        <v>334</v>
+      </c>
+      <c r="E7" t="s">
+        <v>335</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" t="s">
-        <v>257</v>
-      </c>
-      <c r="C8">
-        <v>0.13800000000000001</v>
-      </c>
-      <c r="D8" t="s">
-        <v>260</v>
-      </c>
-      <c r="E8">
-        <v>2012</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>263</v>
-      </c>
-      <c r="B9" t="s">
-        <v>262</v>
-      </c>
-      <c r="C9">
-        <v>0.52400000000000002</v>
-      </c>
-      <c r="D9" t="s">
-        <v>264</v>
-      </c>
-      <c r="E9" t="s">
-        <v>249</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>266</v>
-      </c>
-      <c r="B10" t="s">
-        <v>268</v>
-      </c>
-      <c r="C10">
-        <v>0.13800000000000001</v>
-      </c>
-      <c r="D10" t="s">
-        <v>269</v>
-      </c>
-      <c r="E10">
-        <v>1005</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>267</v>
-      </c>
-      <c r="B11" t="s">
-        <v>271</v>
-      </c>
-      <c r="C11">
-        <v>0.13800000000000001</v>
-      </c>
-      <c r="D11" t="s">
-        <v>272</v>
-      </c>
-      <c r="E11">
-        <v>1005</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>281</v>
-      </c>
-      <c r="B12" t="s">
-        <v>274</v>
-      </c>
-      <c r="C12">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="D12" t="s">
-        <v>275</v>
-      </c>
-      <c r="E12" t="s">
-        <v>276</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>282</v>
-      </c>
-      <c r="B13" t="s">
-        <v>274</v>
-      </c>
-      <c r="C13">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="D13" t="s">
-        <v>275</v>
-      </c>
-      <c r="E13" t="s">
-        <v>277</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>283</v>
-      </c>
-      <c r="B14" t="s">
-        <v>274</v>
-      </c>
-      <c r="C14">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="D14" t="s">
-        <v>275</v>
-      </c>
-      <c r="E14" t="s">
-        <v>278</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>284</v>
-      </c>
-      <c r="B15" t="s">
-        <v>274</v>
-      </c>
-      <c r="C15">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="D15" t="s">
-        <v>275</v>
-      </c>
-      <c r="E15" t="s">
-        <v>279</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" t="s">
-        <v>285</v>
-      </c>
-      <c r="C16">
-        <v>0.20699999999999999</v>
-      </c>
-      <c r="D16" t="s">
-        <v>286</v>
-      </c>
-      <c r="E16" t="s">
-        <v>287</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" t="s">
-        <v>285</v>
-      </c>
-      <c r="C17">
-        <v>0.20699999999999999</v>
-      </c>
-      <c r="D17" t="s">
-        <v>286</v>
-      </c>
-      <c r="E17" t="s">
-        <v>287</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" t="s">
-        <v>285</v>
-      </c>
-      <c r="C18">
-        <v>0.20699999999999999</v>
-      </c>
-      <c r="D18" t="s">
-        <v>286</v>
-      </c>
-      <c r="E18" t="s">
-        <v>287</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" t="s">
-        <v>285</v>
-      </c>
-      <c r="C19">
-        <v>0.20699999999999999</v>
-      </c>
-      <c r="D19" t="s">
-        <v>286</v>
-      </c>
-      <c r="E19" t="s">
-        <v>287</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>288</v>
+        <v>336</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{F7601112-5E1E-4D0E-BE31-9676A7D4FBFB}"/>
-    <hyperlink ref="F2" r:id="rId2" display="https://www.mouser.ca/datasheet/2/670/pj_070bh_smt_tr-1778782.pdf" xr:uid="{402328B1-ACA2-41C6-A714-3277512E8C2C}"/>
-    <hyperlink ref="F3" r:id="rId3" display="https://www.mouser.ca/datasheet/2/308/1/MC78L00A_D-2315651.pdf" xr:uid="{6F8E1E5A-793C-400E-9E7B-FD3CEFE42008}"/>
-    <hyperlink ref="F4" r:id="rId4" display="http://www.ti.com/general/docs/suppproductinfo.tsp?distId=26&amp;gotoUrl=http://www.ti.com/lit/gpn/mc79l" xr:uid="{218BC41D-9665-49ED-BE78-800B8B13E928}"/>
-    <hyperlink ref="F5" r:id="rId5" display="https://www.mouser.ca/datasheet/2/445/885012206074-1727575.pdf" xr:uid="{52890E42-E5EC-4144-B12A-ACE8949FCE71}"/>
-    <hyperlink ref="F7" r:id="rId6" display="https://www.mouser.ca/datasheet/2/445/885012206074-1727575.pdf" xr:uid="{D17B156E-38A1-43DA-837B-3E11B1A36780}"/>
-    <hyperlink ref="F6" r:id="rId7" display="https://www.mouser.ca/datasheet/2/585/MLCC-1837944.pdf" xr:uid="{B5E4DB07-AA26-45F7-8D12-2D1C7AA146A1}"/>
-    <hyperlink ref="F8" r:id="rId8" display="https://www.mouser.ca/datasheet/2/585/MLCC-1837944.pdf" xr:uid="{6CD6DD47-0D21-450D-8CB9-10ACFC0AF589}"/>
-    <hyperlink ref="F9" r:id="rId9" display="http://www.ti.com/general/docs/suppproductinfo.tsp?distId=26&amp;gotoUrl=http%3A%2F%2Fwww.ti.com%2Flit%2Fgpn%2Fne555" xr:uid="{FB2DF6E4-09A3-42A2-AEF8-9E2485A608FF}"/>
-    <hyperlink ref="F10" r:id="rId10" display="https://www.mouser.ca/datasheet/2/414/ttelectronics_ttrb_s_a0010037465_1-1991369.pdf" xr:uid="{0B5F64DC-CE67-4581-BCD5-C44893DE0ABC}"/>
-    <hyperlink ref="F11" r:id="rId11" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_51_RoHS_P_4-2944025.pdf" xr:uid="{02613C4F-AE1A-4770-BD64-FE47AE0E4520}"/>
-    <hyperlink ref="F12" r:id="rId12" display="https://www.diodes.com/assets/Datasheets/ds28002.pdf" xr:uid="{ACD05526-59A8-4F88-813B-254108DA8998}"/>
-    <hyperlink ref="F13:F15" r:id="rId13" display="https://www.diodes.com/assets/Datasheets/ds28002.pdf" xr:uid="{02F96806-947E-4B7D-B6C1-20D4DA35DC4D}"/>
-    <hyperlink ref="F16" r:id="rId14" display="https://www.mouser.ca/datasheet/2/445/860020273009-1725581.pdf" xr:uid="{9D448218-EE6C-4A4C-9E2F-39CD14500BF5}"/>
-    <hyperlink ref="F17:F19" r:id="rId15" display="https://www.mouser.ca/datasheet/2/445/860020273009-1725581.pdf" xr:uid="{4920975F-26D1-4DC7-A2F2-44F04D705761}"/>
+    <hyperlink ref="F2" r:id="rId1" display="https://www.mouser.ca/datasheet/2/308/1/LM324_D-2314880.pdf" xr:uid="{5738DCC6-A9AF-4BAB-9BBE-7D8F57A9641C}"/>
+    <hyperlink ref="F3:F7" r:id="rId2" display="https://www.mouser.ca/datasheet/2/308/1/LM324_D-2314880.pdf" xr:uid="{B27EA078-2732-42F6-BF1D-C143F533A3FB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId16"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finished power circuitry schematic and updated BOM
</commit_message>
<xml_diff>
--- a/Documents/BOM.xlsx
+++ b/Documents/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ECE_Projects\Music_Visualizer\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B957C07-C0F7-4D18-9245-A48AC9359E9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3757F595-FA8A-493A-B089-B7EA1EC898A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="766" activeTab="4" xr2:uid="{1F4A7036-4694-4970-BB5D-7CBECC831452}"/>
+    <workbookView xWindow="46200" yWindow="4140" windowWidth="13830" windowHeight="7170" tabRatio="824" firstSheet="4" activeTab="10" xr2:uid="{1F4A7036-4694-4970-BB5D-7CBECC831452}"/>
   </bookViews>
   <sheets>
     <sheet name="Sub-Bass" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,8 @@
     <sheet name="PowerV1" sheetId="9" r:id="rId10"/>
     <sheet name="PowerV2" sheetId="13" r:id="rId11"/>
     <sheet name="Audio Input" sheetId="10" r:id="rId12"/>
-    <sheet name="LED" sheetId="11" r:id="rId13"/>
+    <sheet name="Audio Input  V2" sheetId="14" r:id="rId13"/>
+    <sheet name="LED" sheetId="11" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1257" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1280" uniqueCount="368">
   <si>
     <t>Component</t>
   </si>
@@ -1136,6 +1137,21 @@
   </si>
   <si>
     <t>LT1054IPE4</t>
+  </si>
+  <si>
+    <t>Case Code (inches)</t>
+  </si>
+  <si>
+    <t>SJ-3523-SMT-TR</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/CUI-Devices/SJ-3523-SMT-TR?qs=WyjlAZoYn51zOHzJ3r4ZRA%3D%3D</t>
+  </si>
+  <si>
+    <t>SJ-3523-SMT-TR Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>MC78L05ACPRAG</t>
   </si>
 </sst>
 </file>
@@ -1584,7 +1600,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14:H19"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2493,8 +2509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C595792-1ED3-4550-B2C6-F49A784AB9C0}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2545,19 +2561,19 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>248</v>
+        <v>367</v>
       </c>
       <c r="B3" t="s">
         <v>360</v>
       </c>
       <c r="C3">
-        <v>0.60699999999999998</v>
+        <v>0.69</v>
       </c>
       <c r="D3" t="s">
         <v>247</v>
       </c>
       <c r="E3" t="s">
-        <v>249</v>
+        <v>350</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>250</v>
@@ -2766,7 +2782,7 @@
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C14">
         <f>SUM(C2:C13)</f>
-        <v>7.7969999999999997</v>
+        <v>7.88</v>
       </c>
       <c r="F14" s="3"/>
     </row>
@@ -2810,7 +2826,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection sqref="A1:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2920,6 +2936,119 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBB0EED6-7AEC-4823-91A2-5A66F8F096F2}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>289</v>
+      </c>
+      <c r="B2" t="s">
+        <v>290</v>
+      </c>
+      <c r="C2">
+        <v>2.98</v>
+      </c>
+      <c r="D2" t="s">
+        <v>291</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>364</v>
+      </c>
+      <c r="B3" t="s">
+        <v>296</v>
+      </c>
+      <c r="C3">
+        <v>1.19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>365</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>297</v>
+      </c>
+      <c r="B4" t="s">
+        <v>298</v>
+      </c>
+      <c r="C4">
+        <v>0.53800000000000003</v>
+      </c>
+      <c r="D4" t="s">
+        <v>299</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>301</v>
+      </c>
+      <c r="B5" t="s">
+        <v>302</v>
+      </c>
+      <c r="C5">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="D5" t="s">
+        <v>303</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>304</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" display="https://www.mouser.ca/datasheet/2/670/sp_3533_02-1779105.pdf" xr:uid="{64024244-CF4B-4410-93D1-8014F099D798}"/>
+    <hyperlink ref="F4" r:id="rId2" display="https://www.mouser.ca/datasheet/2/60/os-1841429.pdf" xr:uid="{358D795B-5584-405C-9659-E433776CC60B}"/>
+    <hyperlink ref="F5" r:id="rId3" display="https://www.mouser.ca/datasheet/2/140/ESCH_S_A0005379088_1-2548267.pdf" xr:uid="{72A05A94-118D-4533-B3B9-93B88199E5DB}"/>
+    <hyperlink ref="F3" r:id="rId4" display="https://www.mouser.ca/datasheet/2/670/sj_352x_smt-1779397.pdf" xr:uid="{D42553CD-8A54-404C-A56C-02200684FF6B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{422FDBAB-416A-4921-A7D0-3405100F2A2C}">
   <dimension ref="A1:F15"/>
   <sheetViews>
@@ -4739,7 +4868,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FA0D483-C574-49A8-A0EA-072A18CA1F90}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14:H19"/>
     </sheetView>
   </sheetViews>
@@ -6197,20 +6326,22 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5E7DEB4-5FFB-4F8D-963A-C08EFBE9A2C1}">
-  <dimension ref="A1:F108"/>
+  <dimension ref="A1:G108"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="A109" sqref="A109:A114"/>
+    <sheetView topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="D77" sqref="D77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="76.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6229,8 +6360,11 @@
       <c r="F1" s="4" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" s="1" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -6249,8 +6383,11 @@
       <c r="F2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -6269,8 +6406,11 @@
       <c r="F3" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -6289,8 +6429,11 @@
       <c r="F4" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -6309,8 +6452,11 @@
       <c r="F5" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G5">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -6329,8 +6475,11 @@
       <c r="F6" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G6">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -6349,8 +6498,11 @@
       <c r="F7" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G7">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -6369,8 +6521,11 @@
       <c r="F8" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G8">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -6389,8 +6544,11 @@
       <c r="F9" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G9">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
         <v>9</v>
       </c>
@@ -6409,8 +6567,11 @@
       <c r="F10" s="9" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G10">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -6430,7 +6591,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>149</v>
       </c>
@@ -6450,7 +6611,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>150</v>
       </c>
@@ -6470,7 +6631,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>151</v>
       </c>
@@ -6490,7 +6651,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>152</v>
       </c>
@@ -6510,7 +6671,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>153</v>
       </c>
@@ -7490,7 +7651,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>202</v>
       </c>
@@ -7510,7 +7671,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="9" t="s">
         <v>203</v>
       </c>
@@ -7530,7 +7691,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>17</v>
       </c>
@@ -7550,7 +7711,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>18</v>
       </c>
@@ -7570,7 +7731,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>19</v>
       </c>
@@ -7590,7 +7751,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>20</v>
       </c>
@@ -7610,7 +7771,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>21</v>
       </c>
@@ -7630,7 +7791,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="9" t="s">
         <v>22</v>
       </c>
@@ -7650,7 +7811,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="14" t="s">
         <v>204</v>
       </c>
@@ -7669,8 +7830,11 @@
       <c r="F73" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G73">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" s="14" t="s">
         <v>205</v>
       </c>
@@ -7689,8 +7853,11 @@
       <c r="F74" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G74">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" s="14" t="s">
         <v>206</v>
       </c>
@@ -7709,8 +7876,11 @@
       <c r="F75" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G75">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" s="14" t="s">
         <v>207</v>
       </c>
@@ -7729,8 +7899,11 @@
       <c r="F76" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G76">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" s="14" t="s">
         <v>208</v>
       </c>
@@ -7749,8 +7922,11 @@
       <c r="F77" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G77">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="15" t="s">
         <v>209</v>
       </c>
@@ -7769,8 +7945,11 @@
       <c r="F78" s="9" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G78">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" s="14" t="s">
         <v>210</v>
       </c>
@@ -7790,7 +7969,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" s="14" t="s">
         <v>211</v>
       </c>

</xml_diff>

<commit_message>
Completed and annotated Spectrum filters and power circuitry, and updated BOM
</commit_message>
<xml_diff>
--- a/Documents/BOM.xlsx
+++ b/Documents/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ECE_Projects\Music_Visualizer\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3757F595-FA8A-493A-B089-B7EA1EC898A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D92922C-D975-4A4F-B4FC-A34910A45881}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="46200" yWindow="4140" windowWidth="13830" windowHeight="7170" tabRatio="824" firstSheet="4" activeTab="10" xr2:uid="{1F4A7036-4694-4970-BB5D-7CBECC831452}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="824" activeTab="7" xr2:uid="{1F4A7036-4694-4970-BB5D-7CBECC831452}"/>
   </bookViews>
   <sheets>
     <sheet name="Sub-Bass" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="UpperMid" sheetId="5" r:id="rId5"/>
     <sheet name="Presence" sheetId="6" r:id="rId6"/>
     <sheet name="Brilliance" sheetId="7" r:id="rId7"/>
-    <sheet name="All Filters" sheetId="8" r:id="rId8"/>
+    <sheet name="AllPassives" sheetId="8" r:id="rId8"/>
     <sheet name="FilterAmps" sheetId="12" r:id="rId9"/>
     <sheet name="PowerV1" sheetId="9" r:id="rId10"/>
     <sheet name="PowerV2" sheetId="13" r:id="rId11"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1280" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1395" uniqueCount="412">
   <si>
     <t>Component</t>
   </si>
@@ -494,9 +494,6 @@
     <t>RK73H1HTTC9092F Datasheet (PDF)</t>
   </si>
   <si>
-    <t>Value (kOhms)</t>
-  </si>
-  <si>
     <t>R11</t>
   </si>
   <si>
@@ -1139,9 +1136,6 @@
     <t>LT1054IPE4</t>
   </si>
   <si>
-    <t>Case Code (inches)</t>
-  </si>
-  <si>
     <t>SJ-3523-SMT-TR</t>
   </si>
   <si>
@@ -1152,6 +1146,144 @@
   </si>
   <si>
     <t>MC78L05ACPRAG</t>
+  </si>
+  <si>
+    <t>Fitler</t>
+  </si>
+  <si>
+    <t>Sub-Bass</t>
+  </si>
+  <si>
+    <t>Bass</t>
+  </si>
+  <si>
+    <t>Low-Midrange</t>
+  </si>
+  <si>
+    <t>Midrange</t>
+  </si>
+  <si>
+    <t>Upper-Midrange</t>
+  </si>
+  <si>
+    <t>Presence</t>
+  </si>
+  <si>
+    <t>Brillliance</t>
+  </si>
+  <si>
+    <t>R67</t>
+  </si>
+  <si>
+    <t>R68</t>
+  </si>
+  <si>
+    <t>R69</t>
+  </si>
+  <si>
+    <t>R70</t>
+  </si>
+  <si>
+    <t>R71</t>
+  </si>
+  <si>
+    <t>R72</t>
+  </si>
+  <si>
+    <t>R73</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/AC0201FR-071KL?qs=NgbZBzc1CyFptxFyv5rTAw%3D%3D</t>
+  </si>
+  <si>
+    <t>AC0201FR-071KL Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>Resistance of High pass RC filter to append to each spectrum filter</t>
+  </si>
+  <si>
+    <t>C43</t>
+  </si>
+  <si>
+    <t>C44</t>
+  </si>
+  <si>
+    <t>C45</t>
+  </si>
+  <si>
+    <t>C46</t>
+  </si>
+  <si>
+    <t>C47</t>
+  </si>
+  <si>
+    <t>C48</t>
+  </si>
+  <si>
+    <t>C49</t>
+  </si>
+  <si>
+    <t>C50</t>
+  </si>
+  <si>
+    <t>Value (kOhms)/(nF)</t>
+  </si>
+  <si>
+    <t>10u</t>
+  </si>
+  <si>
+    <t>100u</t>
+  </si>
+  <si>
+    <t>1u</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Samsung-Electro-Mechanics/CL31A107MQHNNWE?qs=sGAEpiMZZMsh%252B1woXyUXj9e2R%2FOkAO5onETgw2lqCWQ%3D</t>
+  </si>
+  <si>
+    <t>3216</t>
+  </si>
+  <si>
+    <t>CL31A107MQHNNWE Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>Capacitance of High pass RC filter to append to each spectrum filter</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Samsung-Electro-Mechanics/CL21A106KOQNNNF?qs=sGAEpiMZZMsh%252B1woXyUXj%252BV5GOLijFH8pxknU5I2OYE%3D</t>
+  </si>
+  <si>
+    <t>CL21A106KOQNNNF Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>R66</t>
+  </si>
+  <si>
+    <t>Smoothing Caps for Power Circuitry</t>
+  </si>
+  <si>
+    <t>C51</t>
+  </si>
+  <si>
+    <t>C52</t>
+  </si>
+  <si>
+    <t>C53</t>
+  </si>
+  <si>
+    <t>C54</t>
+  </si>
+  <si>
+    <t>C55</t>
+  </si>
+  <si>
+    <t>C56</t>
+  </si>
+  <si>
+    <t>R74</t>
+  </si>
+  <si>
+    <t>Feedback Resistors for LT1054</t>
   </si>
 </sst>
 </file>
@@ -1200,7 +1332,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1235,12 +1367,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="mediumDashed">
+        <color auto="1"/>
+      </top>
+      <bottom style="mediumDashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1280,6 +1423,26 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2088,7 +2251,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>23</v>
@@ -2105,62 +2268,62 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B2" t="s">
         <v>242</v>
-      </c>
-      <c r="B2" t="s">
-        <v>243</v>
       </c>
       <c r="C2">
         <v>2.1800000000000002</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="E2" t="s">
         <v>244</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="3" t="s">
         <v>245</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C3">
         <v>0.60699999999999998</v>
       </c>
       <c r="D3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E3" t="s">
+        <v>248</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>249</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>250</v>
+      </c>
+      <c r="B4" t="s">
         <v>251</v>
-      </c>
-      <c r="B4" t="s">
-        <v>252</v>
       </c>
       <c r="C4">
         <v>0.71799999999999997</v>
       </c>
       <c r="D4" t="s">
+        <v>253</v>
+      </c>
+      <c r="E4" t="s">
+        <v>248</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>254</v>
-      </c>
-      <c r="E4" t="s">
-        <v>249</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -2168,19 +2331,19 @@
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C5">
         <v>0.13800000000000001</v>
       </c>
       <c r="D5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E5">
         <v>1608</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -2188,19 +2351,19 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C6">
         <v>0.13800000000000001</v>
       </c>
       <c r="D6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E6">
         <v>2012</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -2208,19 +2371,19 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C7">
         <v>0.13800000000000001</v>
       </c>
       <c r="D7" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E7">
         <v>1608</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -2228,159 +2391,159 @@
         <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C8">
         <v>0.13800000000000001</v>
       </c>
       <c r="D8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E8">
         <v>2012</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C9">
         <v>0.52400000000000002</v>
       </c>
       <c r="D9" t="s">
+        <v>263</v>
+      </c>
+      <c r="E9" t="s">
+        <v>248</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>264</v>
-      </c>
-      <c r="E9" t="s">
-        <v>249</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B10" t="s">
+        <v>267</v>
+      </c>
+      <c r="C10">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D10" t="s">
         <v>268</v>
-      </c>
-      <c r="C10">
-        <v>0.13800000000000001</v>
-      </c>
-      <c r="D10" t="s">
-        <v>269</v>
       </c>
       <c r="E10">
         <v>1005</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B11" t="s">
+        <v>270</v>
+      </c>
+      <c r="C11">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D11" t="s">
         <v>271</v>
-      </c>
-      <c r="C11">
-        <v>0.13800000000000001</v>
-      </c>
-      <c r="D11" t="s">
-        <v>272</v>
       </c>
       <c r="E11">
         <v>1005</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B12" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C12">
         <v>0.28999999999999998</v>
       </c>
       <c r="D12" t="s">
+        <v>274</v>
+      </c>
+      <c r="E12" t="s">
         <v>275</v>
       </c>
-      <c r="E12" t="s">
-        <v>276</v>
-      </c>
       <c r="F12" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B13" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C13">
         <v>0.28999999999999998</v>
       </c>
       <c r="D13" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B14" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C14">
         <v>0.28999999999999998</v>
       </c>
       <c r="D14" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E14" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B15" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C15">
         <v>0.28999999999999998</v>
       </c>
       <c r="D15" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E15" t="s">
+        <v>278</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>279</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -2388,19 +2551,19 @@
         <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C16">
         <v>0.20699999999999999</v>
       </c>
       <c r="D16" t="s">
+        <v>285</v>
+      </c>
+      <c r="E16" t="s">
         <v>286</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" s="3" t="s">
         <v>287</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -2408,19 +2571,19 @@
         <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C17">
         <v>0.20699999999999999</v>
       </c>
       <c r="D17" t="s">
+        <v>285</v>
+      </c>
+      <c r="E17" t="s">
         <v>286</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" s="3" t="s">
         <v>287</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -2428,19 +2591,19 @@
         <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C18">
         <v>0.20699999999999999</v>
       </c>
       <c r="D18" t="s">
+        <v>285</v>
+      </c>
+      <c r="E18" t="s">
         <v>286</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" s="3" t="s">
         <v>287</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -2448,24 +2611,24 @@
         <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C19">
         <v>0.20699999999999999</v>
       </c>
       <c r="D19" t="s">
+        <v>285</v>
+      </c>
+      <c r="E19" t="s">
         <v>286</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" s="3" t="s">
         <v>287</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C20">
         <f>SUM(C9:C19)</f>
@@ -2474,7 +2637,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C21">
         <f>SUM(C9:C19)+C4+C5+C6</f>
@@ -2509,8 +2672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C595792-1ED3-4550-B2C6-F49A784AB9C0}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2524,7 +2687,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>23</v>
@@ -2541,62 +2704,62 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B2" t="s">
         <v>242</v>
-      </c>
-      <c r="B2" t="s">
-        <v>243</v>
       </c>
       <c r="C2">
         <v>2.1800000000000002</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="E2" t="s">
         <v>244</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="3" t="s">
         <v>245</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C3">
         <v>0.69</v>
       </c>
       <c r="D3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B4" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C4">
         <v>3.81</v>
       </c>
       <c r="D4" t="s">
+        <v>357</v>
+      </c>
+      <c r="E4" t="s">
+        <v>349</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>358</v>
-      </c>
-      <c r="E4" t="s">
-        <v>350</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -2604,19 +2767,19 @@
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C5">
         <v>0.13800000000000001</v>
       </c>
       <c r="D5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E5">
         <v>1608</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -2624,19 +2787,19 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C6">
         <v>0.13800000000000001</v>
       </c>
       <c r="D6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E6">
         <v>2012</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -2644,19 +2807,19 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C7">
         <v>0.11</v>
       </c>
       <c r="D7" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E7">
         <v>1005</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -2664,19 +2827,19 @@
         <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C8">
         <v>0.11</v>
       </c>
       <c r="D8" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E8">
         <v>1005</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -2684,19 +2847,19 @@
         <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C9">
         <v>0.13800000000000001</v>
       </c>
       <c r="D9" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E9">
         <v>2012</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -2704,39 +2867,39 @@
         <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C10">
         <v>0.152</v>
       </c>
       <c r="D10" t="s">
+        <v>348</v>
+      </c>
+      <c r="E10" t="s">
         <v>349</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" s="3" t="s">
         <v>350</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B11" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C11">
         <v>0.13800000000000001</v>
       </c>
       <c r="D11" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E11">
         <v>1005</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -2744,19 +2907,19 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C12">
         <v>0.13800000000000001</v>
       </c>
       <c r="D12" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E12">
         <v>1608</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -2764,19 +2927,19 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C13">
         <v>0.13800000000000001</v>
       </c>
       <c r="D13" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E13">
         <v>1608</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -2840,7 +3003,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>23</v>
@@ -2857,70 +3020,70 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>288</v>
+      </c>
+      <c r="B2" t="s">
         <v>289</v>
-      </c>
-      <c r="B2" t="s">
-        <v>290</v>
       </c>
       <c r="C2">
         <v>2.98</v>
       </c>
       <c r="D2" t="s">
+        <v>290</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>291</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C3">
         <v>1.02</v>
       </c>
       <c r="D3" t="s">
+        <v>293</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>294</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>296</v>
+      </c>
+      <c r="B4" t="s">
         <v>297</v>
-      </c>
-      <c r="B4" t="s">
-        <v>298</v>
       </c>
       <c r="C4">
         <v>0.53800000000000003</v>
       </c>
       <c r="D4" t="s">
+        <v>298</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>299</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>300</v>
+      </c>
+      <c r="B5" t="s">
         <v>301</v>
-      </c>
-      <c r="B5" t="s">
-        <v>302</v>
       </c>
       <c r="C5">
         <v>0.92500000000000004</v>
       </c>
       <c r="D5" t="s">
+        <v>302</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>303</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>304</v>
       </c>
     </row>
   </sheetData>
@@ -2954,7 +3117,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>23</v>
@@ -2971,70 +3134,70 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>288</v>
+      </c>
+      <c r="B2" t="s">
         <v>289</v>
-      </c>
-      <c r="B2" t="s">
-        <v>290</v>
       </c>
       <c r="C2">
         <v>2.98</v>
       </c>
       <c r="D2" t="s">
+        <v>290</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>291</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C3">
         <v>1.19</v>
       </c>
       <c r="D3" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>296</v>
+      </c>
+      <c r="B4" t="s">
         <v>297</v>
-      </c>
-      <c r="B4" t="s">
-        <v>298</v>
       </c>
       <c r="C4">
         <v>0.53800000000000003</v>
       </c>
       <c r="D4" t="s">
+        <v>298</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>299</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>300</v>
+      </c>
+      <c r="B5" t="s">
         <v>301</v>
-      </c>
-      <c r="B5" t="s">
-        <v>302</v>
       </c>
       <c r="C5">
         <v>0.92500000000000004</v>
       </c>
       <c r="D5" t="s">
+        <v>302</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>303</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>304</v>
       </c>
     </row>
   </sheetData>
@@ -3067,7 +3230,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>23</v>
@@ -3084,36 +3247,36 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>304</v>
+      </c>
+      <c r="B2" t="s">
         <v>305</v>
-      </c>
-      <c r="B2" t="s">
-        <v>306</v>
       </c>
       <c r="C2">
         <v>16.59</v>
       </c>
       <c r="D2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>307</v>
+      </c>
+      <c r="B3" t="s">
         <v>308</v>
-      </c>
-      <c r="B3" t="s">
-        <v>309</v>
       </c>
       <c r="C3">
         <v>22.67</v>
       </c>
       <c r="D3" t="s">
+        <v>309</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>310</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -3121,19 +3284,19 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C4">
         <v>0.20699999999999999</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="E4" t="s">
         <v>286</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" s="3" t="s">
         <v>287</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -3141,19 +3304,19 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
+        <v>313</v>
+      </c>
+      <c r="C5">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D5" t="s">
         <v>314</v>
-      </c>
-      <c r="C5">
-        <v>0.13800000000000001</v>
-      </c>
-      <c r="D5" t="s">
-        <v>315</v>
       </c>
       <c r="E5">
         <v>1608</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -3161,19 +3324,19 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
+        <v>313</v>
+      </c>
+      <c r="C6">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D6" t="s">
         <v>314</v>
-      </c>
-      <c r="C6">
-        <v>0.13800000000000001</v>
-      </c>
-      <c r="D6" t="s">
-        <v>315</v>
       </c>
       <c r="E6">
         <v>1608</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -3181,19 +3344,19 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
+        <v>313</v>
+      </c>
+      <c r="C7">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D7" t="s">
         <v>314</v>
-      </c>
-      <c r="C7">
-        <v>0.13800000000000001</v>
-      </c>
-      <c r="D7" t="s">
-        <v>315</v>
       </c>
       <c r="E7">
         <v>1608</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -3201,19 +3364,19 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
+        <v>313</v>
+      </c>
+      <c r="C8">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D8" t="s">
         <v>314</v>
-      </c>
-      <c r="C8">
-        <v>0.13800000000000001</v>
-      </c>
-      <c r="D8" t="s">
-        <v>315</v>
       </c>
       <c r="E8">
         <v>1608</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -3221,19 +3384,19 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
+        <v>313</v>
+      </c>
+      <c r="C9">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D9" t="s">
         <v>314</v>
-      </c>
-      <c r="C9">
-        <v>0.13800000000000001</v>
-      </c>
-      <c r="D9" t="s">
-        <v>315</v>
       </c>
       <c r="E9">
         <v>1608</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -3241,19 +3404,19 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
+        <v>313</v>
+      </c>
+      <c r="C10">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D10" t="s">
         <v>314</v>
-      </c>
-      <c r="C10">
-        <v>0.13800000000000001</v>
-      </c>
-      <c r="D10" t="s">
-        <v>315</v>
       </c>
       <c r="E10">
         <v>1608</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -3261,93 +3424,93 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
+        <v>313</v>
+      </c>
+      <c r="C11">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D11" t="s">
         <v>314</v>
-      </c>
-      <c r="C11">
-        <v>0.13800000000000001</v>
-      </c>
-      <c r="D11" t="s">
-        <v>315</v>
       </c>
       <c r="E11">
         <v>1608</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>328</v>
+      </c>
+      <c r="B12" t="s">
         <v>329</v>
-      </c>
-      <c r="B12" t="s">
-        <v>330</v>
       </c>
       <c r="C12">
         <v>1.38</v>
       </c>
       <c r="D12" t="s">
+        <v>316</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>317</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>318</v>
+      </c>
+      <c r="B13" t="s">
         <v>319</v>
-      </c>
-      <c r="B13" t="s">
-        <v>320</v>
       </c>
       <c r="C13">
         <v>0.99399999999999999</v>
       </c>
       <c r="D13" t="s">
+        <v>320</v>
+      </c>
+      <c r="E13" t="s">
+        <v>322</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>321</v>
-      </c>
-      <c r="E13" t="s">
-        <v>323</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>323</v>
+      </c>
+      <c r="B14" t="s">
         <v>324</v>
-      </c>
-      <c r="B14" t="s">
-        <v>325</v>
       </c>
       <c r="C14">
         <v>0.71799999999999997</v>
       </c>
       <c r="D14" t="s">
+        <v>325</v>
+      </c>
+      <c r="E14" t="s">
         <v>326</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" s="3" t="s">
         <v>327</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B15" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C15">
         <v>1.38</v>
       </c>
       <c r="D15" t="s">
+        <v>316</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>317</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>318</v>
       </c>
     </row>
   </sheetData>
@@ -4197,7 +4360,7 @@
         <v>4.7</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F14" t="s">
         <v>80</v>
@@ -6326,19 +6489,19 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5E7DEB4-5FFB-4F8D-963A-C08EFBE9A2C1}">
-  <dimension ref="A1:G108"/>
+  <dimension ref="A1:G131"/>
   <sheetViews>
-    <sheetView topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="D77" sqref="D77"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="F135" sqref="F135:F136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="76.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -6346,7 +6509,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>148</v>
+        <v>392</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>23</v>
@@ -6360,8 +6523,8 @@
       <c r="F1" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>363</v>
+      <c r="G1" s="4" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -6383,8 +6546,8 @@
       <c r="F2" t="s">
         <v>88</v>
       </c>
-      <c r="G2">
-        <v>201</v>
+      <c r="G2" s="29" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -6406,9 +6569,7 @@
       <c r="F3" t="s">
         <v>88</v>
       </c>
-      <c r="G3">
-        <v>201</v>
-      </c>
+      <c r="G3" s="29"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -6429,9 +6590,7 @@
       <c r="F4" t="s">
         <v>88</v>
       </c>
-      <c r="G4">
-        <v>201</v>
-      </c>
+      <c r="G4" s="29"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -6452,9 +6611,7 @@
       <c r="F5" t="s">
         <v>90</v>
       </c>
-      <c r="G5">
-        <v>201</v>
-      </c>
+      <c r="G5" s="29"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -6475,9 +6632,7 @@
       <c r="F6" t="s">
         <v>88</v>
       </c>
-      <c r="G6">
-        <v>201</v>
-      </c>
+      <c r="G6" s="29"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -6498,9 +6653,7 @@
       <c r="F7" t="s">
         <v>88</v>
       </c>
-      <c r="G7">
-        <v>201</v>
-      </c>
+      <c r="G7" s="29"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -6521,9 +6674,7 @@
       <c r="F8" t="s">
         <v>91</v>
       </c>
-      <c r="G8">
-        <v>201</v>
-      </c>
+      <c r="G8" s="29"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -6544,9 +6695,7 @@
       <c r="F9" t="s">
         <v>91</v>
       </c>
-      <c r="G9">
-        <v>201</v>
-      </c>
+      <c r="G9" s="29"/>
     </row>
     <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
@@ -6567,11 +6716,9 @@
       <c r="F10" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="G10">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G10" s="29"/>
+    </row>
+    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -6590,10 +6737,13 @@
       <c r="F11" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G11" s="30" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B12">
         <v>90.9</v>
@@ -6610,10 +6760,11 @@
       <c r="F12" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G12" s="30"/>
+    </row>
+    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B13">
         <v>162</v>
@@ -6630,10 +6781,11 @@
       <c r="F13" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G13" s="30"/>
+    </row>
+    <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B14">
         <v>118</v>
@@ -6650,10 +6802,11 @@
       <c r="F14" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G14" s="30"/>
+    </row>
+    <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B15">
         <v>63.4</v>
@@ -6670,10 +6823,11 @@
       <c r="F15" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G15" s="30"/>
+    </row>
+    <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B16">
         <v>62</v>
@@ -6690,10 +6844,11 @@
       <c r="F16" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G16" s="30"/>
+    </row>
+    <row r="17" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B17">
         <v>309</v>
@@ -6710,10 +6865,11 @@
       <c r="F17" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G17" s="30"/>
+    </row>
+    <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B18">
         <v>68</v>
@@ -6730,10 +6886,11 @@
       <c r="F18" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G18" s="30"/>
+    </row>
+    <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B19">
         <v>66.5</v>
@@ -6750,10 +6907,11 @@
       <c r="F19" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G19" s="30"/>
+    </row>
+    <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B20" s="9">
         <v>332</v>
@@ -6770,10 +6928,11 @@
       <c r="F20" s="9" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G20" s="30"/>
+    </row>
+    <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B21">
         <v>137</v>
@@ -6790,10 +6949,13 @@
       <c r="F21" s="3" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G21" s="30" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B22">
         <v>45.3</v>
@@ -6810,10 +6972,11 @@
       <c r="F22" s="3" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G22" s="30"/>
+    </row>
+    <row r="23" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B23">
         <v>270</v>
@@ -6830,10 +6993,11 @@
       <c r="F23" s="3" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G23" s="30"/>
+    </row>
+    <row r="24" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B24">
         <v>143</v>
@@ -6850,10 +7014,11 @@
       <c r="F24" s="3" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G24" s="30"/>
+    </row>
+    <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B25">
         <v>19.100000000000001</v>
@@ -6870,10 +7035,11 @@
       <c r="F25" s="3" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G25" s="30"/>
+    </row>
+    <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B26">
         <v>590</v>
@@ -6890,10 +7056,11 @@
       <c r="F26" s="3" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G26" s="30"/>
+    </row>
+    <row r="27" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B27">
         <v>140</v>
@@ -6910,10 +7077,11 @@
       <c r="F27" s="3" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G27" s="30"/>
+    </row>
+    <row r="28" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B28">
         <v>19.100000000000001</v>
@@ -6930,10 +7098,11 @@
       <c r="F28" s="3" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G28" s="30"/>
+    </row>
+    <row r="29" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B29" s="9">
         <v>576</v>
@@ -6950,10 +7119,11 @@
       <c r="F29" s="12" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G29" s="30"/>
+    </row>
+    <row r="30" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B30">
         <v>100</v>
@@ -6970,10 +7140,13 @@
       <c r="F30" s="3" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G30" s="30" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B31">
         <v>100</v>
@@ -6990,10 +7163,11 @@
       <c r="F31" s="3" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G31" s="30"/>
+    </row>
+    <row r="32" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B32">
         <v>66.5</v>
@@ -7010,10 +7184,11 @@
       <c r="F32" s="3" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G32" s="30"/>
+    </row>
+    <row r="33" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B33">
         <v>33.200000000000003</v>
@@ -7030,10 +7205,11 @@
       <c r="F33" s="3" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G33" s="30"/>
+    </row>
+    <row r="34" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B34">
         <v>56</v>
@@ -7050,10 +7226,11 @@
       <c r="F34" s="3" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G34" s="30"/>
+    </row>
+    <row r="35" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B35">
         <v>48.7</v>
@@ -7070,10 +7247,11 @@
       <c r="F35" s="3" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G35" s="30"/>
+    </row>
+    <row r="36" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B36">
         <v>270</v>
@@ -7090,10 +7268,11 @@
       <c r="F36" s="3" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G36" s="30"/>
+    </row>
+    <row r="37" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B37">
         <v>66.5</v>
@@ -7110,10 +7289,11 @@
       <c r="F37" s="3" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G37" s="30"/>
+    </row>
+    <row r="38" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B38">
         <v>57.6</v>
@@ -7130,10 +7310,11 @@
       <c r="F38" s="3" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G38" s="30"/>
+    </row>
+    <row r="39" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B39" s="9">
         <v>324</v>
@@ -7150,10 +7331,11 @@
       <c r="F39" s="12" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G39" s="30"/>
+    </row>
+    <row r="40" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B40">
         <v>78.7</v>
@@ -7170,10 +7352,13 @@
       <c r="F40" s="3" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G40" s="30" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B41">
         <v>26.7</v>
@@ -7190,10 +7375,11 @@
       <c r="F41" s="3" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G41" s="30"/>
+    </row>
+    <row r="42" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B42">
         <v>160</v>
@@ -7210,10 +7396,11 @@
       <c r="F42" s="3" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G42" s="30"/>
+    </row>
+    <row r="43" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B43">
         <v>59</v>
@@ -7230,10 +7417,11 @@
       <c r="F43" s="3" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G43" s="30"/>
+    </row>
+    <row r="44" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B44">
         <v>7.87</v>
@@ -7250,10 +7438,11 @@
       <c r="F44" s="3" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G44" s="30"/>
+    </row>
+    <row r="45" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B45">
         <v>243</v>
@@ -7270,10 +7459,11 @@
       <c r="F45" s="3" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G45" s="30"/>
+    </row>
+    <row r="46" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B46">
         <v>107</v>
@@ -7290,10 +7480,11 @@
       <c r="F46" s="3" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G46" s="30"/>
+    </row>
+    <row r="47" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B47">
         <v>14.7</v>
@@ -7310,10 +7501,11 @@
       <c r="F47" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G47" s="30"/>
+    </row>
+    <row r="48" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B48" s="9">
         <v>453</v>
@@ -7330,10 +7522,11 @@
       <c r="F48" s="12" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G48" s="30"/>
+    </row>
+    <row r="49" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B49">
         <v>78.7</v>
@@ -7350,10 +7543,13 @@
       <c r="F49" s="3" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G49" s="30" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B50">
         <v>7.32</v>
@@ -7370,10 +7566,11 @@
       <c r="F50" s="3" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G50" s="30"/>
+    </row>
+    <row r="51" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B51">
         <v>160</v>
@@ -7390,10 +7587,11 @@
       <c r="F51" s="3" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G51" s="30"/>
+    </row>
+    <row r="52" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B52">
         <v>66.5</v>
@@ -7410,10 +7608,11 @@
       <c r="F52" s="3" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G52" s="30"/>
+    </row>
+    <row r="53" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B53">
         <v>2.87</v>
@@ -7430,10 +7629,11 @@
       <c r="F53" s="3" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G53" s="30"/>
+    </row>
+    <row r="54" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B54">
         <v>270</v>
@@ -7450,10 +7650,11 @@
       <c r="F54" s="3" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G54" s="30"/>
+    </row>
+    <row r="55" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B55">
         <v>95.3</v>
@@ -7470,10 +7671,11 @@
       <c r="F55" s="3" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G55" s="30"/>
+    </row>
+    <row r="56" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B56">
         <v>4.0199999999999996</v>
@@ -7490,10 +7692,11 @@
       <c r="F56" s="3" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G56" s="30"/>
+    </row>
+    <row r="57" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B57" s="9">
         <v>383</v>
@@ -7510,10 +7713,11 @@
       <c r="F57" s="12" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G57" s="30"/>
+    </row>
+    <row r="58" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B58">
         <v>11.5</v>
@@ -7530,10 +7734,13 @@
       <c r="F58" s="7" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G58" s="30" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B59">
         <v>48.7</v>
@@ -7550,10 +7757,11 @@
       <c r="F59" s="3" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G59" s="30"/>
+    </row>
+    <row r="60" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B60">
         <v>22.6</v>
@@ -7570,10 +7778,11 @@
       <c r="F60" s="3" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G60" s="30"/>
+    </row>
+    <row r="61" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B61">
         <v>8.06</v>
@@ -7590,10 +7799,11 @@
       <c r="F61" s="3" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G61" s="30"/>
+    </row>
+    <row r="62" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B62">
         <v>4.32</v>
@@ -7610,10 +7820,11 @@
       <c r="F62" s="3" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G62" s="30"/>
+    </row>
+    <row r="63" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B63">
         <v>37.4</v>
@@ -7630,10 +7841,11 @@
       <c r="F63" s="3" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G63" s="30"/>
+    </row>
+    <row r="64" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B64">
         <v>19.600000000000001</v>
@@ -7650,10 +7862,11 @@
       <c r="F64" s="3" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G64" s="30"/>
+    </row>
+    <row r="65" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B65">
         <v>10.7</v>
@@ -7670,10 +7883,11 @@
       <c r="F65" s="3" t="s">
         <v>146</v>
       </c>
+      <c r="G65" s="30"/>
     </row>
     <row r="66" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B66" s="9">
         <v>90.9</v>
@@ -7690,8 +7904,9 @@
       <c r="F66" s="12" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G66" s="30"/>
+    </row>
+    <row r="67" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>17</v>
       </c>
@@ -7710,8 +7925,11 @@
       <c r="F67" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G67" s="30" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>18</v>
       </c>
@@ -7730,8 +7948,9 @@
       <c r="F68" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G68" s="30"/>
+    </row>
+    <row r="69" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>19</v>
       </c>
@@ -7750,8 +7969,9 @@
       <c r="F69" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G69" s="30"/>
+    </row>
+    <row r="70" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>20</v>
       </c>
@@ -7770,8 +7990,9 @@
       <c r="F70" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G70" s="30"/>
+    </row>
+    <row r="71" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>21</v>
       </c>
@@ -7790,6 +8011,7 @@
       <c r="F71" t="s">
         <v>95</v>
       </c>
+      <c r="G71" s="30"/>
     </row>
     <row r="72" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="9" t="s">
@@ -7810,10 +8032,11 @@
       <c r="F72" s="9" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G72" s="30"/>
+    </row>
+    <row r="73" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A73" s="14" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B73">
         <v>13</v>
@@ -7830,13 +8053,13 @@
       <c r="F73" t="s">
         <v>97</v>
       </c>
-      <c r="G73">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G73" s="30" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A74" s="14" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B74">
         <v>13</v>
@@ -7853,13 +8076,11 @@
       <c r="F74" t="s">
         <v>97</v>
       </c>
-      <c r="G74">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G74" s="30"/>
+    </row>
+    <row r="75" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="14" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B75">
         <v>6.8</v>
@@ -7876,13 +8097,11 @@
       <c r="F75" t="s">
         <v>98</v>
       </c>
-      <c r="G75">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G75" s="30"/>
+    </row>
+    <row r="76" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A76" s="14" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B76">
         <v>6.8</v>
@@ -7899,13 +8118,11 @@
       <c r="F76" t="s">
         <v>98</v>
       </c>
-      <c r="G76">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G76" s="30"/>
+    </row>
+    <row r="77" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A77" s="14" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B77">
         <v>24</v>
@@ -7922,13 +8139,11 @@
       <c r="F77" t="s">
         <v>100</v>
       </c>
-      <c r="G77">
-        <v>805</v>
-      </c>
+      <c r="G77" s="30"/>
     </row>
     <row r="78" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="15" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B78" s="9">
         <v>24</v>
@@ -7945,13 +8160,11 @@
       <c r="F78" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="G78">
-        <v>805</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G78" s="30"/>
+    </row>
+    <row r="79" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A79" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B79">
         <v>4.7</v>
@@ -7968,10 +8181,13 @@
       <c r="F79" s="3" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G79" s="30" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A80" s="14" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B80">
         <v>4.7</v>
@@ -7988,10 +8204,11 @@
       <c r="F80" s="3" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G80" s="30"/>
+    </row>
+    <row r="81" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A81" s="14" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B81">
         <v>3.3</v>
@@ -8008,10 +8225,11 @@
       <c r="F81" s="3" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G81" s="30"/>
+    </row>
+    <row r="82" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A82" s="14" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B82">
         <v>3.3</v>
@@ -8028,10 +8246,11 @@
       <c r="F82" s="3" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G82" s="30"/>
+    </row>
+    <row r="83" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A83" s="14" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B83">
         <v>6.2</v>
@@ -8048,10 +8267,11 @@
       <c r="F83" s="3" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G83" s="30"/>
+    </row>
+    <row r="84" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A84" s="15" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B84" s="9">
         <v>6.2</v>
@@ -8068,10 +8288,11 @@
       <c r="F84" s="12" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G84" s="30"/>
+    </row>
+    <row r="85" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A85" s="14" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B85">
         <v>1.6</v>
@@ -8088,10 +8309,13 @@
       <c r="F85" s="3" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G85" s="30" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A86" s="14" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B86">
         <v>1.6</v>
@@ -8108,10 +8332,11 @@
       <c r="F86" s="3" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G86" s="30"/>
+    </row>
+    <row r="87" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A87" s="14" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B87">
         <v>1</v>
@@ -8128,10 +8353,11 @@
       <c r="F87" s="3" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G87" s="30"/>
+    </row>
+    <row r="88" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A88" s="14" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B88">
         <v>1</v>
@@ -8148,10 +8374,11 @@
       <c r="F88" s="3" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G88" s="30"/>
+    </row>
+    <row r="89" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A89" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B89">
         <v>3</v>
@@ -8168,10 +8395,11 @@
       <c r="F89" s="3" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G89" s="30"/>
+    </row>
+    <row r="90" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A90" s="15" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B90" s="9">
         <v>3</v>
@@ -8188,10 +8416,11 @@
       <c r="F90" s="12" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G90" s="30"/>
+    </row>
+    <row r="91" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A91" s="14" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B91">
         <v>1</v>
@@ -8208,10 +8437,13 @@
       <c r="F91" s="3" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G91" s="30" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A92" s="14" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B92">
         <v>1</v>
@@ -8228,10 +8460,11 @@
       <c r="F92" s="3" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G92" s="30"/>
+    </row>
+    <row r="93" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A93" s="14" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B93">
         <v>1</v>
@@ -8248,10 +8481,11 @@
       <c r="F93" s="3" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G93" s="30"/>
+    </row>
+    <row r="94" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A94" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B94">
         <v>1</v>
@@ -8268,10 +8502,11 @@
       <c r="F94" s="3" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G94" s="30"/>
+    </row>
+    <row r="95" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A95" s="14" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B95">
         <v>1</v>
@@ -8288,10 +8523,11 @@
       <c r="F95" s="3" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G95" s="30"/>
+    </row>
+    <row r="96" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A96" s="15" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B96" s="9">
         <v>1</v>
@@ -8308,10 +8544,11 @@
       <c r="F96" s="12" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G96" s="30"/>
+    </row>
+    <row r="97" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A97" s="20" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B97" s="21">
         <v>1</v>
@@ -8328,10 +8565,13 @@
       <c r="F97" s="24" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G97" s="30" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A98" s="14" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B98" s="16">
         <v>1</v>
@@ -8348,10 +8588,11 @@
       <c r="F98" s="19" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G98" s="30"/>
+    </row>
+    <row r="99" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A99" s="14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B99" s="16">
         <v>1</v>
@@ -8368,10 +8609,11 @@
       <c r="F99" s="19" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G99" s="30"/>
+    </row>
+    <row r="100" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A100" s="14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B100" s="16">
         <v>1</v>
@@ -8388,10 +8630,11 @@
       <c r="F100" s="19" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G100" s="30"/>
+    </row>
+    <row r="101" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A101" s="14" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B101" s="16">
         <v>1</v>
@@ -8408,10 +8651,11 @@
       <c r="F101" s="19" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="102" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G101" s="30"/>
+    </row>
+    <row r="102" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A102" s="15" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B102" s="9">
         <v>1</v>
@@ -8428,10 +8672,11 @@
       <c r="F102" s="12" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G102" s="30"/>
+    </row>
+    <row r="103" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A103" s="14" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B103">
         <v>1</v>
@@ -8448,10 +8693,13 @@
       <c r="F103" s="3" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G103" s="30" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A104" s="14" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B104">
         <v>1</v>
@@ -8468,10 +8716,11 @@
       <c r="F104" s="3" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G104" s="30"/>
+    </row>
+    <row r="105" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A105" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B105">
         <v>1</v>
@@ -8488,10 +8737,11 @@
       <c r="F105" s="3" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G105" s="30"/>
+    </row>
+    <row r="106" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A106" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B106">
         <v>1</v>
@@ -8508,10 +8758,11 @@
       <c r="F106" s="3" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G106" s="30"/>
+    </row>
+    <row r="107" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A107" s="14" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B107">
         <v>1</v>
@@ -8528,10 +8779,11 @@
       <c r="F107" s="3" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="108" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G107" s="30"/>
+    </row>
+    <row r="108" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A108" s="15" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B108" s="9">
         <v>1</v>
@@ -8548,8 +8800,520 @@
       <c r="F108" s="12" t="s">
         <v>123</v>
       </c>
+      <c r="G108" s="30"/>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A109" s="14" t="s">
+        <v>402</v>
+      </c>
+      <c r="B109" s="14">
+        <v>1</v>
+      </c>
+      <c r="C109" s="25">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D109" t="s">
+        <v>381</v>
+      </c>
+      <c r="E109" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F109" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="G109" s="28" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A110" s="14" t="s">
+        <v>374</v>
+      </c>
+      <c r="B110" s="14">
+        <v>1</v>
+      </c>
+      <c r="C110" s="25">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D110" t="s">
+        <v>381</v>
+      </c>
+      <c r="E110" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F110" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="G110" s="27"/>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A111" s="14" t="s">
+        <v>375</v>
+      </c>
+      <c r="B111" s="14">
+        <v>1</v>
+      </c>
+      <c r="C111" s="25">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D111" t="s">
+        <v>381</v>
+      </c>
+      <c r="E111" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F111" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="G111" s="27"/>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A112" s="14" t="s">
+        <v>376</v>
+      </c>
+      <c r="B112" s="14">
+        <v>1</v>
+      </c>
+      <c r="C112" s="25">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D112" t="s">
+        <v>381</v>
+      </c>
+      <c r="E112" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F112" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="G112" s="27"/>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A113" s="14" t="s">
+        <v>377</v>
+      </c>
+      <c r="B113" s="14">
+        <v>1</v>
+      </c>
+      <c r="C113" s="25">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D113" t="s">
+        <v>381</v>
+      </c>
+      <c r="E113" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F113" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="G113" s="27"/>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A114" s="14" t="s">
+        <v>378</v>
+      </c>
+      <c r="B114" s="14">
+        <v>1</v>
+      </c>
+      <c r="C114" s="25">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D114" t="s">
+        <v>381</v>
+      </c>
+      <c r="E114" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F114" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="G114" s="27"/>
+    </row>
+    <row r="115" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A115" s="15" t="s">
+        <v>379</v>
+      </c>
+      <c r="B115" s="15">
+        <v>1</v>
+      </c>
+      <c r="C115" s="26">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D115" s="9" t="s">
+        <v>381</v>
+      </c>
+      <c r="E115" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="F115" s="12" t="s">
+        <v>382</v>
+      </c>
+      <c r="G115" s="27"/>
+    </row>
+    <row r="116" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A116" s="14" t="s">
+        <v>384</v>
+      </c>
+      <c r="B116" s="14" t="s">
+        <v>394</v>
+      </c>
+      <c r="C116" s="25">
+        <v>0.60699999999999998</v>
+      </c>
+      <c r="D116" t="s">
+        <v>396</v>
+      </c>
+      <c r="E116" s="5" t="s">
+        <v>397</v>
+      </c>
+      <c r="F116" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="G116" s="31" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A117" s="14" t="s">
+        <v>385</v>
+      </c>
+      <c r="B117" s="14" t="s">
+        <v>394</v>
+      </c>
+      <c r="C117" s="25">
+        <v>0.60699999999999998</v>
+      </c>
+      <c r="D117" t="s">
+        <v>396</v>
+      </c>
+      <c r="E117" s="5" t="s">
+        <v>397</v>
+      </c>
+      <c r="F117" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="G117" s="31"/>
+    </row>
+    <row r="118" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A118" s="14" t="s">
+        <v>386</v>
+      </c>
+      <c r="B118" t="s">
+        <v>393</v>
+      </c>
+      <c r="C118" s="25">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D118" t="s">
+        <v>400</v>
+      </c>
+      <c r="E118" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="F118" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="G118" s="31"/>
+    </row>
+    <row r="119" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A119" s="14" t="s">
+        <v>387</v>
+      </c>
+      <c r="B119" t="s">
+        <v>393</v>
+      </c>
+      <c r="C119" s="25">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D119" t="s">
+        <v>400</v>
+      </c>
+      <c r="E119" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="F119" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="G119" s="31"/>
+    </row>
+    <row r="120" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A120" s="14" t="s">
+        <v>388</v>
+      </c>
+      <c r="B120" t="s">
+        <v>395</v>
+      </c>
+      <c r="C120" s="25">
+        <v>0.11</v>
+      </c>
+      <c r="D120" t="s">
+        <v>344</v>
+      </c>
+      <c r="E120" s="6">
+        <v>1005</v>
+      </c>
+      <c r="F120" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="G120" s="31"/>
+    </row>
+    <row r="121" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A121" s="14" t="s">
+        <v>389</v>
+      </c>
+      <c r="B121" t="s">
+        <v>395</v>
+      </c>
+      <c r="C121" s="25">
+        <v>0.11</v>
+      </c>
+      <c r="D121" t="s">
+        <v>344</v>
+      </c>
+      <c r="E121" s="6">
+        <v>1005</v>
+      </c>
+      <c r="F121" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="G121" s="31"/>
+    </row>
+    <row r="122" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A122" s="15" t="s">
+        <v>390</v>
+      </c>
+      <c r="B122" s="9" t="s">
+        <v>395</v>
+      </c>
+      <c r="C122" s="26">
+        <v>0.11</v>
+      </c>
+      <c r="D122" s="9" t="s">
+        <v>344</v>
+      </c>
+      <c r="E122" s="13">
+        <v>1005</v>
+      </c>
+      <c r="F122" s="12" t="s">
+        <v>345</v>
+      </c>
+      <c r="G122" s="31"/>
+    </row>
+    <row r="123" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A123" s="14" t="s">
+        <v>391</v>
+      </c>
+      <c r="B123" t="s">
+        <v>255</v>
+      </c>
+      <c r="C123" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D123" t="s">
+        <v>257</v>
+      </c>
+      <c r="E123" s="6">
+        <v>1608</v>
+      </c>
+      <c r="F123" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="G123" s="31" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A124" s="14" t="s">
+        <v>404</v>
+      </c>
+      <c r="B124" t="s">
+        <v>256</v>
+      </c>
+      <c r="C124" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D124" t="s">
+        <v>259</v>
+      </c>
+      <c r="E124" s="6">
+        <v>2012</v>
+      </c>
+      <c r="F124" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="G124" s="31"/>
+    </row>
+    <row r="125" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A125" s="14" t="s">
+        <v>405</v>
+      </c>
+      <c r="B125" t="s">
+        <v>343</v>
+      </c>
+      <c r="C125" s="2">
+        <v>0.11</v>
+      </c>
+      <c r="D125" t="s">
+        <v>344</v>
+      </c>
+      <c r="E125" s="6">
+        <v>1005</v>
+      </c>
+      <c r="F125" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="G125" s="31"/>
+    </row>
+    <row r="126" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A126" s="14" t="s">
+        <v>406</v>
+      </c>
+      <c r="B126" t="s">
+        <v>343</v>
+      </c>
+      <c r="C126" s="2">
+        <v>0.11</v>
+      </c>
+      <c r="D126" t="s">
+        <v>344</v>
+      </c>
+      <c r="E126" s="6">
+        <v>1005</v>
+      </c>
+      <c r="F126" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="G126" s="31"/>
+    </row>
+    <row r="127" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A127" s="14" t="s">
+        <v>407</v>
+      </c>
+      <c r="B127" t="s">
+        <v>338</v>
+      </c>
+      <c r="C127" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D127" t="s">
+        <v>346</v>
+      </c>
+      <c r="E127" s="6">
+        <v>2012</v>
+      </c>
+      <c r="F127" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="G127" s="31"/>
+    </row>
+    <row r="128" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A128" s="14" t="s">
+        <v>408</v>
+      </c>
+      <c r="B128" t="s">
+        <v>339</v>
+      </c>
+      <c r="C128" s="2">
+        <v>0.152</v>
+      </c>
+      <c r="D128" t="s">
+        <v>348</v>
+      </c>
+      <c r="E128" s="6" t="s">
+        <v>349</v>
+      </c>
+      <c r="F128" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="G128" s="31"/>
+    </row>
+    <row r="129" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A129" s="15" t="s">
+        <v>409</v>
+      </c>
+      <c r="B129" s="9" t="s">
+        <v>340</v>
+      </c>
+      <c r="C129" s="10">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D129" s="9" t="s">
+        <v>351</v>
+      </c>
+      <c r="E129" s="13">
+        <v>1005</v>
+      </c>
+      <c r="F129" s="12" t="s">
+        <v>352</v>
+      </c>
+      <c r="G129" s="31"/>
+    </row>
+    <row r="130" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A130" s="14" t="s">
+        <v>380</v>
+      </c>
+      <c r="B130" t="s">
+        <v>341</v>
+      </c>
+      <c r="C130" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D130" t="s">
+        <v>353</v>
+      </c>
+      <c r="E130" s="6">
+        <v>1608</v>
+      </c>
+      <c r="F130" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="G130" s="32" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A131" s="15" t="s">
+        <v>410</v>
+      </c>
+      <c r="B131" s="9" t="s">
+        <v>342</v>
+      </c>
+      <c r="C131" s="10">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D131" s="9" t="s">
+        <v>355</v>
+      </c>
+      <c r="E131" s="13">
+        <v>1608</v>
+      </c>
+      <c r="F131" s="12" t="s">
+        <v>356</v>
+      </c>
+      <c r="G131" s="32"/>
     </row>
   </sheetData>
+  <mergeCells count="18">
+    <mergeCell ref="G109:G115"/>
+    <mergeCell ref="G116:G122"/>
+    <mergeCell ref="G123:G129"/>
+    <mergeCell ref="G130:G131"/>
+    <mergeCell ref="G97:G102"/>
+    <mergeCell ref="G103:G108"/>
+    <mergeCell ref="G58:G66"/>
+    <mergeCell ref="G67:G72"/>
+    <mergeCell ref="G73:G78"/>
+    <mergeCell ref="G79:G84"/>
+    <mergeCell ref="G85:G90"/>
+    <mergeCell ref="G91:G96"/>
+    <mergeCell ref="G2:G10"/>
+    <mergeCell ref="G11:G20"/>
+    <mergeCell ref="G21:G29"/>
+    <mergeCell ref="G30:G39"/>
+    <mergeCell ref="G40:G48"/>
+    <mergeCell ref="G49:G57"/>
+  </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="F21" r:id="rId1" display="https://www.mouser.ca/datasheet/2/447/PYu_RC_Group_51_RoHS_L_10-1664068.pdf" xr:uid="{FD9529E3-40C1-4269-9308-A90EB6F99C44}"/>
@@ -8629,9 +9393,30 @@
     <hyperlink ref="F106" r:id="rId75" display="https://www.mouser.ca/datasheet/2/281/1/GRM0335C1E102JA01_01A-1980306.pdf" xr:uid="{71183E3C-1321-4C74-9C36-AF467F1E7694}"/>
     <hyperlink ref="F107" r:id="rId76" display="https://www.mouser.ca/datasheet/2/281/1/GRM0335C1E102JA01_01A-1980306.pdf" xr:uid="{6107289D-2BCB-46B1-914E-5EA5AB170858}"/>
     <hyperlink ref="F108" r:id="rId77" display="https://www.mouser.ca/datasheet/2/281/1/GRM0335C1E102JA01_01A-1980306.pdf" xr:uid="{E5DD7520-2C5E-4FF1-8071-DF8F821AA0D7}"/>
+    <hyperlink ref="F109" r:id="rId78" display="https://www.mouser.ca/datasheet/2/447/Yageo_PYu_AC_51_RoHS_L_7_1714230-1874691.pdf" xr:uid="{B0BDD487-534D-4157-9AF7-A3F931673830}"/>
+    <hyperlink ref="F110" r:id="rId79" display="https://www.mouser.ca/datasheet/2/447/Yageo_PYu_AC_51_RoHS_L_7_1714230-1874691.pdf" xr:uid="{C3270AFC-4A20-4E79-8608-D0A2CFF69F45}"/>
+    <hyperlink ref="F111" r:id="rId80" display="https://www.mouser.ca/datasheet/2/447/Yageo_PYu_AC_51_RoHS_L_7_1714230-1874691.pdf" xr:uid="{BFE38213-311D-41C8-B72A-65076ABBCC38}"/>
+    <hyperlink ref="F113" r:id="rId81" display="https://www.mouser.ca/datasheet/2/447/Yageo_PYu_AC_51_RoHS_L_7_1714230-1874691.pdf" xr:uid="{561862D7-7705-4E84-9F6D-8DA013279938}"/>
+    <hyperlink ref="F115" r:id="rId82" display="https://www.mouser.ca/datasheet/2/447/Yageo_PYu_AC_51_RoHS_L_7_1714230-1874691.pdf" xr:uid="{B4D8312C-A448-4277-81EB-7F58DDDF0FE2}"/>
+    <hyperlink ref="F112" r:id="rId83" display="https://www.mouser.ca/datasheet/2/447/Yageo_PYu_AC_51_RoHS_L_7_1714230-1874691.pdf" xr:uid="{AE210F25-69EB-4DA2-A7F5-7B73966DF30C}"/>
+    <hyperlink ref="F114" r:id="rId84" display="https://www.mouser.ca/datasheet/2/447/Yageo_PYu_AC_51_RoHS_L_7_1714230-1874691.pdf" xr:uid="{DFAB973F-DCCE-4FA8-8A24-00D34ABEF2A2}"/>
+    <hyperlink ref="F116" r:id="rId85" display="https://www.mouser.ca/datasheet/2/585/MLCC-1837944.pdf" xr:uid="{3B6F062A-90D9-47BB-A841-52D8756E7212}"/>
+    <hyperlink ref="F117" r:id="rId86" display="https://www.mouser.ca/datasheet/2/585/MLCC-1837944.pdf" xr:uid="{783BDC3E-A0DE-4562-9407-4DE5BD7BC975}"/>
+    <hyperlink ref="F118" r:id="rId87" display="https://www.mouser.ca/datasheet/2/585/MLCC-1837944.pdf" xr:uid="{7EFF3B80-113D-45CE-8741-3D65476E76D0}"/>
+    <hyperlink ref="F119" r:id="rId88" display="https://www.mouser.ca/datasheet/2/585/MLCC-1837944.pdf" xr:uid="{FA90DB72-6BA3-4A01-A8C6-09E8BE59A66C}"/>
+    <hyperlink ref="F120" r:id="rId89" display="https://www.mouser.ca/datasheet/2/212/KEM_C1023_X7R_AUTO_SMD-1093309.pdf" xr:uid="{7E9D5081-77C7-41DB-94A7-CDDCDCD88544}"/>
+    <hyperlink ref="F121" r:id="rId90" display="https://www.mouser.ca/datasheet/2/212/KEM_C1023_X7R_AUTO_SMD-1093309.pdf" xr:uid="{FC110397-D8B4-47A2-AB43-C43106B96A4D}"/>
+    <hyperlink ref="F122" r:id="rId91" display="https://www.mouser.ca/datasheet/2/212/KEM_C1023_X7R_AUTO_SMD-1093309.pdf" xr:uid="{5A4F4F38-0775-4B61-89C9-4303519A9E37}"/>
+    <hyperlink ref="F123" r:id="rId92" display="https://www.mouser.ca/datasheet/2/445/885012206074-1727575.pdf" xr:uid="{042EA7AE-8347-47DB-80F5-4255A5F88750}"/>
+    <hyperlink ref="F124" r:id="rId93" display="https://www.mouser.ca/datasheet/2/585/MLCC-1837944.pdf" xr:uid="{5B4B4222-9375-4598-903C-A429AE3C6E83}"/>
+    <hyperlink ref="F125" r:id="rId94" display="https://www.mouser.ca/datasheet/2/212/1/C0603X102K4RACAUTO-2933386.pdf" xr:uid="{2C59D38E-E45A-404E-A16C-59F1115750E8}"/>
+    <hyperlink ref="F126" r:id="rId95" display="https://www.mouser.ca/datasheet/2/212/1/C0603X102K4RACAUTO-2933386.pdf" xr:uid="{3518936D-A980-4CE2-99A2-FB67A208614B}"/>
+    <hyperlink ref="F127" r:id="rId96" display="https://www.mouser.ca/datasheet/2/585/MLCC-1837944.pdf" xr:uid="{F5506774-2647-4180-A630-3F869F90200C}"/>
+    <hyperlink ref="F128" r:id="rId97" display="https://www.mouser.ca/datasheet/2/445/860010372006-1725314.pdf" xr:uid="{76B8DFED-7E19-40D0-883F-323E54884DB7}"/>
+    <hyperlink ref="F129" r:id="rId98" display="https://www.mouser.ca/datasheet/2/447/yago_s_a0003557223_1-2286436.pdf" xr:uid="{E9C3E476-E5B1-42E2-96A4-99E21333D366}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId78"/>
+  <pageSetup orientation="portrait" r:id="rId99"/>
 </worksheet>
 </file>
 
@@ -8655,7 +9440,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>23</v>
@@ -8672,122 +9457,122 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
+        <v>331</v>
+      </c>
+      <c r="B2" t="s">
         <v>332</v>
-      </c>
-      <c r="B2" t="s">
-        <v>333</v>
       </c>
       <c r="C2">
         <v>0.75900000000000001</v>
       </c>
       <c r="D2" t="s">
+        <v>333</v>
+      </c>
+      <c r="E2" t="s">
         <v>334</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="3" t="s">
         <v>335</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
+        <v>331</v>
+      </c>
+      <c r="B3" t="s">
         <v>332</v>
-      </c>
-      <c r="B3" t="s">
-        <v>333</v>
       </c>
       <c r="C3">
         <v>0.75900000000000001</v>
       </c>
       <c r="D3" t="s">
+        <v>333</v>
+      </c>
+      <c r="E3" t="s">
         <v>334</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" s="3" t="s">
         <v>335</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
+        <v>331</v>
+      </c>
+      <c r="B4" t="s">
         <v>332</v>
-      </c>
-      <c r="B4" t="s">
-        <v>333</v>
       </c>
       <c r="C4">
         <v>0.75900000000000001</v>
       </c>
       <c r="D4" t="s">
+        <v>333</v>
+      </c>
+      <c r="E4" t="s">
         <v>334</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" s="3" t="s">
         <v>335</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
+        <v>331</v>
+      </c>
+      <c r="B5" t="s">
         <v>332</v>
-      </c>
-      <c r="B5" t="s">
-        <v>333</v>
       </c>
       <c r="C5">
         <v>0.75900000000000001</v>
       </c>
       <c r="D5" t="s">
+        <v>333</v>
+      </c>
+      <c r="E5" t="s">
         <v>334</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" s="3" t="s">
         <v>335</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
+        <v>331</v>
+      </c>
+      <c r="B6" t="s">
         <v>332</v>
-      </c>
-      <c r="B6" t="s">
-        <v>333</v>
       </c>
       <c r="C6">
         <v>0.75900000000000001</v>
       </c>
       <c r="D6" t="s">
+        <v>333</v>
+      </c>
+      <c r="E6" t="s">
         <v>334</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" s="3" t="s">
         <v>335</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
+        <v>331</v>
+      </c>
+      <c r="B7" t="s">
         <v>332</v>
-      </c>
-      <c r="B7" t="s">
-        <v>333</v>
       </c>
       <c r="C7">
         <v>0.75900000000000001</v>
       </c>
       <c r="D7" t="s">
+        <v>333</v>
+      </c>
+      <c r="E7" t="s">
         <v>334</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" s="3" t="s">
         <v>335</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>336</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished LED Driver Sub-Circuit and updated BOM
</commit_message>
<xml_diff>
--- a/Documents/BOM.xlsx
+++ b/Documents/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ECE_Projects\Music_Visualizer\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D92922C-D975-4A4F-B4FC-A34910A45881}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{298A03DC-F2F9-4473-91A9-564C85B06A1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="824" activeTab="7" xr2:uid="{1F4A7036-4694-4970-BB5D-7CBECC831452}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="824" activeTab="13" xr2:uid="{1F4A7036-4694-4970-BB5D-7CBECC831452}"/>
   </bookViews>
   <sheets>
     <sheet name="Sub-Bass" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1395" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1449" uniqueCount="427">
   <si>
     <t>Component</t>
   </si>
@@ -1284,6 +1284,51 @@
   </si>
   <si>
     <t>Feedback Resistors for LT1054</t>
+  </si>
+  <si>
+    <t>R75</t>
+  </si>
+  <si>
+    <t>R76</t>
+  </si>
+  <si>
+    <t>R77</t>
+  </si>
+  <si>
+    <t>R78</t>
+  </si>
+  <si>
+    <t>R79</t>
+  </si>
+  <si>
+    <t>R80</t>
+  </si>
+  <si>
+    <t>R81</t>
+  </si>
+  <si>
+    <t>680 ohm</t>
+  </si>
+  <si>
+    <t>C57</t>
+  </si>
+  <si>
+    <t>C58</t>
+  </si>
+  <si>
+    <t>C59</t>
+  </si>
+  <si>
+    <t>M20-9990246</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Harwin/M20-9990246?qs=Jph8NoUxIfWjw4WmyRvzag%3D%3D</t>
+  </si>
+  <si>
+    <t>2.54 mm header for jumper</t>
+  </si>
+  <si>
+    <t>M20-9990246 Datasheet (PDF)</t>
   </si>
 </sst>
 </file>
@@ -1425,23 +1470,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3213,16 +3258,16 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{422FDBAB-416A-4921-A7D0-3405100F2A2C}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3301,47 +3346,47 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>313</v>
-      </c>
-      <c r="C5">
-        <v>0.13800000000000001</v>
+        <v>395</v>
+      </c>
+      <c r="C5" s="25">
+        <v>0.11</v>
       </c>
       <c r="D5" t="s">
-        <v>314</v>
-      </c>
-      <c r="E5">
-        <v>1608</v>
+        <v>344</v>
+      </c>
+      <c r="E5" s="6">
+        <v>1005</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>315</v>
+        <v>345</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>313</v>
-      </c>
-      <c r="C6">
-        <v>0.13800000000000001</v>
+        <v>395</v>
+      </c>
+      <c r="C6" s="25">
+        <v>0.11</v>
       </c>
       <c r="D6" t="s">
-        <v>314</v>
-      </c>
-      <c r="E6">
-        <v>1608</v>
+        <v>344</v>
+      </c>
+      <c r="E6" s="6">
+        <v>1005</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>315</v>
+        <v>345</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B7" t="s">
         <v>313</v>
@@ -3361,7 +3406,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B8" t="s">
         <v>313</v>
@@ -3381,7 +3426,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s">
         <v>313</v>
@@ -3401,7 +3446,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B10" t="s">
         <v>313</v>
@@ -3421,7 +3466,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B11" t="s">
         <v>313</v>
@@ -3441,76 +3486,136 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>328</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>329</v>
+        <v>313</v>
       </c>
       <c r="C12">
-        <v>1.38</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="D12" t="s">
-        <v>316</v>
+        <v>314</v>
+      </c>
+      <c r="E12">
+        <v>1608</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>318</v>
+        <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="C13">
-        <v>0.99399999999999999</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="D13" t="s">
-        <v>320</v>
-      </c>
-      <c r="E13" t="s">
-        <v>322</v>
+        <v>314</v>
+      </c>
+      <c r="E13">
+        <v>1608</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
       <c r="B14" t="s">
-        <v>324</v>
+        <v>329</v>
       </c>
       <c r="C14">
-        <v>0.71799999999999997</v>
+        <v>1.38</v>
       </c>
       <c r="D14" t="s">
-        <v>325</v>
-      </c>
-      <c r="E14" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>327</v>
+        <v>317</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>318</v>
+      </c>
+      <c r="B15" t="s">
+        <v>319</v>
+      </c>
+      <c r="C15">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="D15" t="s">
+        <v>320</v>
+      </c>
+      <c r="E15" t="s">
+        <v>322</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>323</v>
+      </c>
+      <c r="B16" t="s">
+        <v>324</v>
+      </c>
+      <c r="C16">
+        <v>0.71799999999999997</v>
+      </c>
+      <c r="D16" t="s">
+        <v>325</v>
+      </c>
+      <c r="E16" t="s">
+        <v>326</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>328</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B17" t="s">
         <v>330</v>
       </c>
-      <c r="C15">
+      <c r="C17">
         <v>1.38</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D17" t="s">
         <v>316</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F17" s="3" t="s">
         <v>317</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>423</v>
+      </c>
+      <c r="B18" t="s">
+        <v>425</v>
+      </c>
+      <c r="C18">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="D18" t="s">
+        <v>424</v>
+      </c>
+      <c r="E18" t="s">
+        <v>349</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>426</v>
       </c>
     </row>
   </sheetData>
@@ -3519,13 +3624,16 @@
     <hyperlink ref="F3" r:id="rId1" xr:uid="{4086144A-D13C-4CF7-B0A2-04DC9FD2E687}"/>
     <hyperlink ref="F4" r:id="rId2" display="https://www.mouser.ca/datasheet/2/445/860020273009-1725581.pdf" xr:uid="{DF0F49A7-30B6-415A-AA6E-5F9F70F3E664}"/>
     <hyperlink ref="D4" r:id="rId3" xr:uid="{502E7D33-C429-41BF-8FAA-6D1BB65BAFC1}"/>
-    <hyperlink ref="F12" r:id="rId4" display="https://www.mouser.ca/datasheet/2/54/ptv09-777818.pdf" xr:uid="{BBF2E0E5-0197-4455-B910-736161147ECB}"/>
-    <hyperlink ref="F13" r:id="rId5" display="https://www.mouser.ca/datasheet/2/308/1/NCS333_D-2317376.pdf" xr:uid="{7C0CF1F9-6D8B-4838-AF4F-5E3806F151A2}"/>
-    <hyperlink ref="F14" r:id="rId6" display="https://www.mouser.ca/datasheet/2/308/1/NCP161_D-2316989.pdf" xr:uid="{7A98D1F1-404F-44D8-89D1-D9D1436D893F}"/>
-    <hyperlink ref="F15" r:id="rId7" display="https://www.mouser.ca/datasheet/2/54/ptv09-777818.pdf" xr:uid="{8236BBA3-E1C5-477D-B2F7-BBC0C6E41223}"/>
+    <hyperlink ref="F14" r:id="rId4" display="https://www.mouser.ca/datasheet/2/54/ptv09-777818.pdf" xr:uid="{BBF2E0E5-0197-4455-B910-736161147ECB}"/>
+    <hyperlink ref="F15" r:id="rId5" display="https://www.mouser.ca/datasheet/2/308/1/NCS333_D-2317376.pdf" xr:uid="{7C0CF1F9-6D8B-4838-AF4F-5E3806F151A2}"/>
+    <hyperlink ref="F16" r:id="rId6" display="https://www.mouser.ca/datasheet/2/308/1/NCP161_D-2316989.pdf" xr:uid="{7A98D1F1-404F-44D8-89D1-D9D1436D893F}"/>
+    <hyperlink ref="F17" r:id="rId7" display="https://www.mouser.ca/datasheet/2/54/ptv09-777818.pdf" xr:uid="{8236BBA3-E1C5-477D-B2F7-BBC0C6E41223}"/>
+    <hyperlink ref="F5" r:id="rId8" display="https://www.mouser.ca/datasheet/2/212/KEM_C1023_X7R_AUTO_SMD-1093309.pdf" xr:uid="{4124399B-DA79-4405-AB72-D8B1FDAF4819}"/>
+    <hyperlink ref="F6" r:id="rId9" display="https://www.mouser.ca/datasheet/2/212/KEM_C1023_X7R_AUTO_SMD-1093309.pdf" xr:uid="{F2E5697D-C749-490A-9831-2DFDF15AF7E1}"/>
+    <hyperlink ref="F18" r:id="rId10" display="https://www.mouser.ca/datasheet/2/181/M20-999-1218971.pdf" xr:uid="{01275A75-EDA2-4738-A48D-85BCFEA831AF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
 
@@ -6489,10 +6597,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5E7DEB4-5FFB-4F8D-963A-C08EFBE9A2C1}">
-  <dimension ref="A1:G131"/>
+  <dimension ref="A1:G141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="F135" sqref="F135:F136"/>
+    <sheetView topLeftCell="A114" workbookViewId="0">
+      <selection activeCell="B140" sqref="B140:F141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6546,7 +6654,7 @@
       <c r="F2" t="s">
         <v>88</v>
       </c>
-      <c r="G2" s="29" t="s">
+      <c r="G2" s="32" t="s">
         <v>367</v>
       </c>
     </row>
@@ -6569,7 +6677,7 @@
       <c r="F3" t="s">
         <v>88</v>
       </c>
-      <c r="G3" s="29"/>
+      <c r="G3" s="32"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -6590,7 +6698,7 @@
       <c r="F4" t="s">
         <v>88</v>
       </c>
-      <c r="G4" s="29"/>
+      <c r="G4" s="32"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -6611,7 +6719,7 @@
       <c r="F5" t="s">
         <v>90</v>
       </c>
-      <c r="G5" s="29"/>
+      <c r="G5" s="32"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -6632,7 +6740,7 @@
       <c r="F6" t="s">
         <v>88</v>
       </c>
-      <c r="G6" s="29"/>
+      <c r="G6" s="32"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -6653,7 +6761,7 @@
       <c r="F7" t="s">
         <v>88</v>
       </c>
-      <c r="G7" s="29"/>
+      <c r="G7" s="32"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -6674,7 +6782,7 @@
       <c r="F8" t="s">
         <v>91</v>
       </c>
-      <c r="G8" s="29"/>
+      <c r="G8" s="32"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -6695,7 +6803,7 @@
       <c r="F9" t="s">
         <v>91</v>
       </c>
-      <c r="G9" s="29"/>
+      <c r="G9" s="32"/>
     </row>
     <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
@@ -6716,7 +6824,7 @@
       <c r="F10" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="G10" s="29"/>
+      <c r="G10" s="32"/>
     </row>
     <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
@@ -6737,7 +6845,7 @@
       <c r="F11" t="s">
         <v>88</v>
       </c>
-      <c r="G11" s="30" t="s">
+      <c r="G11" s="31" t="s">
         <v>368</v>
       </c>
     </row>
@@ -6760,7 +6868,7 @@
       <c r="F12" t="s">
         <v>90</v>
       </c>
-      <c r="G12" s="30"/>
+      <c r="G12" s="31"/>
     </row>
     <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -6781,7 +6889,7 @@
       <c r="F13" t="s">
         <v>88</v>
       </c>
-      <c r="G13" s="30"/>
+      <c r="G13" s="31"/>
     </row>
     <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
@@ -6802,7 +6910,7 @@
       <c r="F14" t="s">
         <v>88</v>
       </c>
-      <c r="G14" s="30"/>
+      <c r="G14" s="31"/>
     </row>
     <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
@@ -6823,7 +6931,7 @@
       <c r="F15" t="s">
         <v>88</v>
       </c>
-      <c r="G15" s="30"/>
+      <c r="G15" s="31"/>
     </row>
     <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
@@ -6844,7 +6952,7 @@
       <c r="F16" t="s">
         <v>88</v>
       </c>
-      <c r="G16" s="30"/>
+      <c r="G16" s="31"/>
     </row>
     <row r="17" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
@@ -6865,7 +6973,7 @@
       <c r="F17" t="s">
         <v>88</v>
       </c>
-      <c r="G17" s="30"/>
+      <c r="G17" s="31"/>
     </row>
     <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
@@ -6886,7 +6994,7 @@
       <c r="F18" t="s">
         <v>96</v>
       </c>
-      <c r="G18" s="30"/>
+      <c r="G18" s="31"/>
     </row>
     <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
@@ -6907,7 +7015,7 @@
       <c r="F19" t="s">
         <v>88</v>
       </c>
-      <c r="G19" s="30"/>
+      <c r="G19" s="31"/>
     </row>
     <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
@@ -6928,7 +7036,7 @@
       <c r="F20" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="G20" s="30"/>
+      <c r="G20" s="31"/>
     </row>
     <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
@@ -6949,7 +7057,7 @@
       <c r="F21" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="G21" s="30" t="s">
+      <c r="G21" s="31" t="s">
         <v>369</v>
       </c>
     </row>
@@ -6972,7 +7080,7 @@
       <c r="F22" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G22" s="30"/>
+      <c r="G22" s="31"/>
     </row>
     <row r="23" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
@@ -6993,7 +7101,7 @@
       <c r="F23" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="G23" s="30"/>
+      <c r="G23" s="31"/>
     </row>
     <row r="24" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
@@ -7014,7 +7122,7 @@
       <c r="F24" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="G24" s="30"/>
+      <c r="G24" s="31"/>
     </row>
     <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
@@ -7035,7 +7143,7 @@
       <c r="F25" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="G25" s="30"/>
+      <c r="G25" s="31"/>
     </row>
     <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
@@ -7056,7 +7164,7 @@
       <c r="F26" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="G26" s="30"/>
+      <c r="G26" s="31"/>
     </row>
     <row r="27" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
@@ -7077,7 +7185,7 @@
       <c r="F27" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="G27" s="30"/>
+      <c r="G27" s="31"/>
     </row>
     <row r="28" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
@@ -7098,7 +7206,7 @@
       <c r="F28" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="G28" s="30"/>
+      <c r="G28" s="31"/>
     </row>
     <row r="29" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="9" t="s">
@@ -7119,7 +7227,7 @@
       <c r="F29" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="G29" s="30"/>
+      <c r="G29" s="31"/>
     </row>
     <row r="30" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
@@ -7140,7 +7248,7 @@
       <c r="F30" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="G30" s="30" t="s">
+      <c r="G30" s="31" t="s">
         <v>370</v>
       </c>
     </row>
@@ -7163,7 +7271,7 @@
       <c r="F31" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="G31" s="30"/>
+      <c r="G31" s="31"/>
     </row>
     <row r="32" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
@@ -7184,7 +7292,7 @@
       <c r="F32" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="G32" s="30"/>
+      <c r="G32" s="31"/>
     </row>
     <row r="33" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
@@ -7205,7 +7313,7 @@
       <c r="F33" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="G33" s="30"/>
+      <c r="G33" s="31"/>
     </row>
     <row r="34" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
@@ -7226,7 +7334,7 @@
       <c r="F34" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="G34" s="30"/>
+      <c r="G34" s="31"/>
     </row>
     <row r="35" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
@@ -7247,7 +7355,7 @@
       <c r="F35" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="G35" s="30"/>
+      <c r="G35" s="31"/>
     </row>
     <row r="36" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
@@ -7268,7 +7376,7 @@
       <c r="F36" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="G36" s="30"/>
+      <c r="G36" s="31"/>
     </row>
     <row r="37" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
@@ -7289,7 +7397,7 @@
       <c r="F37" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="G37" s="30"/>
+      <c r="G37" s="31"/>
     </row>
     <row r="38" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
@@ -7310,7 +7418,7 @@
       <c r="F38" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="G38" s="30"/>
+      <c r="G38" s="31"/>
     </row>
     <row r="39" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="9" t="s">
@@ -7331,7 +7439,7 @@
       <c r="F39" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="G39" s="30"/>
+      <c r="G39" s="31"/>
     </row>
     <row r="40" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
@@ -7352,7 +7460,7 @@
       <c r="F40" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="G40" s="30" t="s">
+      <c r="G40" s="31" t="s">
         <v>371</v>
       </c>
     </row>
@@ -7375,7 +7483,7 @@
       <c r="F41" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="G41" s="30"/>
+      <c r="G41" s="31"/>
     </row>
     <row r="42" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
@@ -7396,7 +7504,7 @@
       <c r="F42" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="G42" s="30"/>
+      <c r="G42" s="31"/>
     </row>
     <row r="43" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
@@ -7417,7 +7525,7 @@
       <c r="F43" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="G43" s="30"/>
+      <c r="G43" s="31"/>
     </row>
     <row r="44" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
@@ -7438,7 +7546,7 @@
       <c r="F44" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="G44" s="30"/>
+      <c r="G44" s="31"/>
     </row>
     <row r="45" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
@@ -7459,7 +7567,7 @@
       <c r="F45" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="G45" s="30"/>
+      <c r="G45" s="31"/>
     </row>
     <row r="46" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
@@ -7480,7 +7588,7 @@
       <c r="F46" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="G46" s="30"/>
+      <c r="G46" s="31"/>
     </row>
     <row r="47" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
@@ -7501,7 +7609,7 @@
       <c r="F47" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="G47" s="30"/>
+      <c r="G47" s="31"/>
     </row>
     <row r="48" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="9" t="s">
@@ -7522,7 +7630,7 @@
       <c r="F48" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="G48" s="30"/>
+      <c r="G48" s="31"/>
     </row>
     <row r="49" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
@@ -7543,7 +7651,7 @@
       <c r="F49" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="G49" s="30" t="s">
+      <c r="G49" s="31" t="s">
         <v>372</v>
       </c>
     </row>
@@ -7566,7 +7674,7 @@
       <c r="F50" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="G50" s="30"/>
+      <c r="G50" s="31"/>
     </row>
     <row r="51" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
@@ -7587,7 +7695,7 @@
       <c r="F51" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="G51" s="30"/>
+      <c r="G51" s="31"/>
     </row>
     <row r="52" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
@@ -7608,7 +7716,7 @@
       <c r="F52" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="G52" s="30"/>
+      <c r="G52" s="31"/>
     </row>
     <row r="53" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
@@ -7629,7 +7737,7 @@
       <c r="F53" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="G53" s="30"/>
+      <c r="G53" s="31"/>
     </row>
     <row r="54" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
@@ -7650,7 +7758,7 @@
       <c r="F54" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="G54" s="30"/>
+      <c r="G54" s="31"/>
     </row>
     <row r="55" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
@@ -7671,7 +7779,7 @@
       <c r="F55" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="G55" s="30"/>
+      <c r="G55" s="31"/>
     </row>
     <row r="56" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
@@ -7692,7 +7800,7 @@
       <c r="F56" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="G56" s="30"/>
+      <c r="G56" s="31"/>
     </row>
     <row r="57" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="9" t="s">
@@ -7713,7 +7821,7 @@
       <c r="F57" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="G57" s="30"/>
+      <c r="G57" s="31"/>
     </row>
     <row r="58" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
@@ -7734,7 +7842,7 @@
       <c r="F58" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="G58" s="30" t="s">
+      <c r="G58" s="31" t="s">
         <v>373</v>
       </c>
     </row>
@@ -7757,7 +7865,7 @@
       <c r="F59" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="G59" s="30"/>
+      <c r="G59" s="31"/>
     </row>
     <row r="60" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
@@ -7778,7 +7886,7 @@
       <c r="F60" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="G60" s="30"/>
+      <c r="G60" s="31"/>
     </row>
     <row r="61" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
@@ -7799,7 +7907,7 @@
       <c r="F61" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="G61" s="30"/>
+      <c r="G61" s="31"/>
     </row>
     <row r="62" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
@@ -7820,7 +7928,7 @@
       <c r="F62" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="G62" s="30"/>
+      <c r="G62" s="31"/>
     </row>
     <row r="63" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
@@ -7841,7 +7949,7 @@
       <c r="F63" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="G63" s="30"/>
+      <c r="G63" s="31"/>
     </row>
     <row r="64" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
@@ -7862,7 +7970,7 @@
       <c r="F64" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="G64" s="30"/>
+      <c r="G64" s="31"/>
     </row>
     <row r="65" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
@@ -7883,7 +7991,7 @@
       <c r="F65" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="G65" s="30"/>
+      <c r="G65" s="31"/>
     </row>
     <row r="66" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="9" t="s">
@@ -7904,7 +8012,7 @@
       <c r="F66" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="G66" s="30"/>
+      <c r="G66" s="31"/>
     </row>
     <row r="67" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
@@ -7925,7 +8033,7 @@
       <c r="F67" t="s">
         <v>93</v>
       </c>
-      <c r="G67" s="30" t="s">
+      <c r="G67" s="31" t="s">
         <v>367</v>
       </c>
     </row>
@@ -7948,7 +8056,7 @@
       <c r="F68" t="s">
         <v>93</v>
       </c>
-      <c r="G68" s="30"/>
+      <c r="G68" s="31"/>
     </row>
     <row r="69" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
@@ -7969,7 +8077,7 @@
       <c r="F69" t="s">
         <v>94</v>
       </c>
-      <c r="G69" s="30"/>
+      <c r="G69" s="31"/>
     </row>
     <row r="70" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
@@ -7990,7 +8098,7 @@
       <c r="F70" t="s">
         <v>94</v>
       </c>
-      <c r="G70" s="30"/>
+      <c r="G70" s="31"/>
     </row>
     <row r="71" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
@@ -8011,7 +8119,7 @@
       <c r="F71" t="s">
         <v>95</v>
       </c>
-      <c r="G71" s="30"/>
+      <c r="G71" s="31"/>
     </row>
     <row r="72" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="9" t="s">
@@ -8032,7 +8140,7 @@
       <c r="F72" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="G72" s="30"/>
+      <c r="G72" s="31"/>
     </row>
     <row r="73" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A73" s="14" t="s">
@@ -8053,7 +8161,7 @@
       <c r="F73" t="s">
         <v>97</v>
       </c>
-      <c r="G73" s="30" t="s">
+      <c r="G73" s="31" t="s">
         <v>368</v>
       </c>
     </row>
@@ -8076,7 +8184,7 @@
       <c r="F74" t="s">
         <v>97</v>
       </c>
-      <c r="G74" s="30"/>
+      <c r="G74" s="31"/>
     </row>
     <row r="75" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="14" t="s">
@@ -8097,7 +8205,7 @@
       <c r="F75" t="s">
         <v>98</v>
       </c>
-      <c r="G75" s="30"/>
+      <c r="G75" s="31"/>
     </row>
     <row r="76" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A76" s="14" t="s">
@@ -8118,7 +8226,7 @@
       <c r="F76" t="s">
         <v>98</v>
       </c>
-      <c r="G76" s="30"/>
+      <c r="G76" s="31"/>
     </row>
     <row r="77" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A77" s="14" t="s">
@@ -8139,7 +8247,7 @@
       <c r="F77" t="s">
         <v>100</v>
       </c>
-      <c r="G77" s="30"/>
+      <c r="G77" s="31"/>
     </row>
     <row r="78" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="15" t="s">
@@ -8160,7 +8268,7 @@
       <c r="F78" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="G78" s="30"/>
+      <c r="G78" s="31"/>
     </row>
     <row r="79" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A79" s="14" t="s">
@@ -8181,7 +8289,7 @@
       <c r="F79" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="G79" s="30" t="s">
+      <c r="G79" s="31" t="s">
         <v>369</v>
       </c>
     </row>
@@ -8204,7 +8312,7 @@
       <c r="F80" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="G80" s="30"/>
+      <c r="G80" s="31"/>
     </row>
     <row r="81" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A81" s="14" t="s">
@@ -8225,7 +8333,7 @@
       <c r="F81" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="G81" s="30"/>
+      <c r="G81" s="31"/>
     </row>
     <row r="82" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A82" s="14" t="s">
@@ -8246,7 +8354,7 @@
       <c r="F82" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="G82" s="30"/>
+      <c r="G82" s="31"/>
     </row>
     <row r="83" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A83" s="14" t="s">
@@ -8267,7 +8375,7 @@
       <c r="F83" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="G83" s="30"/>
+      <c r="G83" s="31"/>
     </row>
     <row r="84" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A84" s="15" t="s">
@@ -8288,7 +8396,7 @@
       <c r="F84" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="G84" s="30"/>
+      <c r="G84" s="31"/>
     </row>
     <row r="85" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A85" s="14" t="s">
@@ -8309,7 +8417,7 @@
       <c r="F85" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="G85" s="30" t="s">
+      <c r="G85" s="31" t="s">
         <v>370</v>
       </c>
     </row>
@@ -8332,7 +8440,7 @@
       <c r="F86" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="G86" s="30"/>
+      <c r="G86" s="31"/>
     </row>
     <row r="87" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A87" s="14" t="s">
@@ -8353,7 +8461,7 @@
       <c r="F87" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G87" s="30"/>
+      <c r="G87" s="31"/>
     </row>
     <row r="88" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A88" s="14" t="s">
@@ -8374,7 +8482,7 @@
       <c r="F88" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G88" s="30"/>
+      <c r="G88" s="31"/>
     </row>
     <row r="89" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A89" s="14" t="s">
@@ -8395,7 +8503,7 @@
       <c r="F89" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="G89" s="30"/>
+      <c r="G89" s="31"/>
     </row>
     <row r="90" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A90" s="15" t="s">
@@ -8416,7 +8524,7 @@
       <c r="F90" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="G90" s="30"/>
+      <c r="G90" s="31"/>
     </row>
     <row r="91" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A91" s="14" t="s">
@@ -8437,7 +8545,7 @@
       <c r="F91" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G91" s="30" t="s">
+      <c r="G91" s="31" t="s">
         <v>371</v>
       </c>
     </row>
@@ -8460,7 +8568,7 @@
       <c r="F92" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G92" s="30"/>
+      <c r="G92" s="31"/>
     </row>
     <row r="93" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A93" s="14" t="s">
@@ -8481,7 +8589,7 @@
       <c r="F93" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G93" s="30"/>
+      <c r="G93" s="31"/>
     </row>
     <row r="94" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A94" s="14" t="s">
@@ -8502,7 +8610,7 @@
       <c r="F94" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G94" s="30"/>
+      <c r="G94" s="31"/>
     </row>
     <row r="95" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A95" s="14" t="s">
@@ -8523,7 +8631,7 @@
       <c r="F95" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G95" s="30"/>
+      <c r="G95" s="31"/>
     </row>
     <row r="96" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A96" s="15" t="s">
@@ -8544,7 +8652,7 @@
       <c r="F96" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="G96" s="30"/>
+      <c r="G96" s="31"/>
     </row>
     <row r="97" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A97" s="20" t="s">
@@ -8565,7 +8673,7 @@
       <c r="F97" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="G97" s="30" t="s">
+      <c r="G97" s="31" t="s">
         <v>372</v>
       </c>
     </row>
@@ -8588,7 +8696,7 @@
       <c r="F98" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="G98" s="30"/>
+      <c r="G98" s="31"/>
     </row>
     <row r="99" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A99" s="14" t="s">
@@ -8609,7 +8717,7 @@
       <c r="F99" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="G99" s="30"/>
+      <c r="G99" s="31"/>
     </row>
     <row r="100" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A100" s="14" t="s">
@@ -8630,7 +8738,7 @@
       <c r="F100" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="G100" s="30"/>
+      <c r="G100" s="31"/>
     </row>
     <row r="101" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A101" s="14" t="s">
@@ -8651,7 +8759,7 @@
       <c r="F101" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="G101" s="30"/>
+      <c r="G101" s="31"/>
     </row>
     <row r="102" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A102" s="15" t="s">
@@ -8672,7 +8780,7 @@
       <c r="F102" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="G102" s="30"/>
+      <c r="G102" s="31"/>
     </row>
     <row r="103" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A103" s="14" t="s">
@@ -8693,7 +8801,7 @@
       <c r="F103" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G103" s="30" t="s">
+      <c r="G103" s="31" t="s">
         <v>373</v>
       </c>
     </row>
@@ -8716,7 +8824,7 @@
       <c r="F104" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G104" s="30"/>
+      <c r="G104" s="31"/>
     </row>
     <row r="105" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A105" s="14" t="s">
@@ -8737,7 +8845,7 @@
       <c r="F105" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G105" s="30"/>
+      <c r="G105" s="31"/>
     </row>
     <row r="106" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A106" s="14" t="s">
@@ -8758,7 +8866,7 @@
       <c r="F106" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G106" s="30"/>
+      <c r="G106" s="31"/>
     </row>
     <row r="107" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A107" s="14" t="s">
@@ -8779,7 +8887,7 @@
       <c r="F107" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G107" s="30"/>
+      <c r="G107" s="31"/>
     </row>
     <row r="108" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A108" s="15" t="s">
@@ -8800,7 +8908,7 @@
       <c r="F108" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="G108" s="30"/>
+      <c r="G108" s="31"/>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109" s="14" t="s">
@@ -8821,7 +8929,7 @@
       <c r="F109" s="3" t="s">
         <v>382</v>
       </c>
-      <c r="G109" s="28" t="s">
+      <c r="G109" s="27" t="s">
         <v>383</v>
       </c>
     </row>
@@ -8844,7 +8952,7 @@
       <c r="F110" s="3" t="s">
         <v>382</v>
       </c>
-      <c r="G110" s="27"/>
+      <c r="G110" s="28"/>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111" s="14" t="s">
@@ -8865,7 +8973,7 @@
       <c r="F111" s="3" t="s">
         <v>382</v>
       </c>
-      <c r="G111" s="27"/>
+      <c r="G111" s="28"/>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112" s="14" t="s">
@@ -8886,7 +8994,7 @@
       <c r="F112" s="3" t="s">
         <v>382</v>
       </c>
-      <c r="G112" s="27"/>
+      <c r="G112" s="28"/>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113" s="14" t="s">
@@ -8907,7 +9015,7 @@
       <c r="F113" s="3" t="s">
         <v>382</v>
       </c>
-      <c r="G113" s="27"/>
+      <c r="G113" s="28"/>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114" s="14" t="s">
@@ -8928,7 +9036,7 @@
       <c r="F114" s="3" t="s">
         <v>382</v>
       </c>
-      <c r="G114" s="27"/>
+      <c r="G114" s="28"/>
     </row>
     <row r="115" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A115" s="15" t="s">
@@ -8949,7 +9057,7 @@
       <c r="F115" s="12" t="s">
         <v>382</v>
       </c>
-      <c r="G115" s="27"/>
+      <c r="G115" s="28"/>
     </row>
     <row r="116" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A116" s="14" t="s">
@@ -8970,7 +9078,7 @@
       <c r="F116" s="3" t="s">
         <v>398</v>
       </c>
-      <c r="G116" s="31" t="s">
+      <c r="G116" s="29" t="s">
         <v>399</v>
       </c>
     </row>
@@ -8993,7 +9101,7 @@
       <c r="F117" s="3" t="s">
         <v>398</v>
       </c>
-      <c r="G117" s="31"/>
+      <c r="G117" s="29"/>
     </row>
     <row r="118" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A118" s="14" t="s">
@@ -9014,7 +9122,7 @@
       <c r="F118" s="3" t="s">
         <v>401</v>
       </c>
-      <c r="G118" s="31"/>
+      <c r="G118" s="29"/>
     </row>
     <row r="119" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A119" s="14" t="s">
@@ -9035,7 +9143,7 @@
       <c r="F119" s="3" t="s">
         <v>401</v>
       </c>
-      <c r="G119" s="31"/>
+      <c r="G119" s="29"/>
     </row>
     <row r="120" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A120" s="14" t="s">
@@ -9056,7 +9164,7 @@
       <c r="F120" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="G120" s="31"/>
+      <c r="G120" s="29"/>
     </row>
     <row r="121" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A121" s="14" t="s">
@@ -9077,7 +9185,7 @@
       <c r="F121" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="G121" s="31"/>
+      <c r="G121" s="29"/>
     </row>
     <row r="122" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A122" s="15" t="s">
@@ -9098,7 +9206,7 @@
       <c r="F122" s="12" t="s">
         <v>345</v>
       </c>
-      <c r="G122" s="31"/>
+      <c r="G122" s="29"/>
     </row>
     <row r="123" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A123" s="14" t="s">
@@ -9119,7 +9227,7 @@
       <c r="F123" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="G123" s="31" t="s">
+      <c r="G123" s="29" t="s">
         <v>403</v>
       </c>
     </row>
@@ -9142,7 +9250,7 @@
       <c r="F124" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="G124" s="31"/>
+      <c r="G124" s="29"/>
     </row>
     <row r="125" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A125" s="14" t="s">
@@ -9163,7 +9271,7 @@
       <c r="F125" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="G125" s="31"/>
+      <c r="G125" s="29"/>
     </row>
     <row r="126" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A126" s="14" t="s">
@@ -9184,7 +9292,7 @@
       <c r="F126" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="G126" s="31"/>
+      <c r="G126" s="29"/>
     </row>
     <row r="127" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A127" s="14" t="s">
@@ -9205,7 +9313,7 @@
       <c r="F127" s="3" t="s">
         <v>347</v>
       </c>
-      <c r="G127" s="31"/>
+      <c r="G127" s="29"/>
     </row>
     <row r="128" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A128" s="14" t="s">
@@ -9226,7 +9334,7 @@
       <c r="F128" s="3" t="s">
         <v>350</v>
       </c>
-      <c r="G128" s="31"/>
+      <c r="G128" s="29"/>
     </row>
     <row r="129" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A129" s="15" t="s">
@@ -9247,7 +9355,7 @@
       <c r="F129" s="12" t="s">
         <v>352</v>
       </c>
-      <c r="G129" s="31"/>
+      <c r="G129" s="29"/>
     </row>
     <row r="130" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A130" s="14" t="s">
@@ -9268,7 +9376,7 @@
       <c r="F130" s="3" t="s">
         <v>354</v>
       </c>
-      <c r="G130" s="32" t="s">
+      <c r="G130" s="30" t="s">
         <v>411</v>
       </c>
     </row>
@@ -9291,21 +9399,210 @@
       <c r="F131" s="12" t="s">
         <v>356</v>
       </c>
-      <c r="G131" s="32"/>
+      <c r="G131" s="30"/>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A132" s="14" t="s">
+        <v>412</v>
+      </c>
+      <c r="B132" t="s">
+        <v>419</v>
+      </c>
+      <c r="C132" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D132" t="s">
+        <v>314</v>
+      </c>
+      <c r="E132" s="6">
+        <v>1608</v>
+      </c>
+      <c r="F132" s="3" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A133" s="14" t="s">
+        <v>413</v>
+      </c>
+      <c r="B133" t="s">
+        <v>419</v>
+      </c>
+      <c r="C133" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D133" t="s">
+        <v>314</v>
+      </c>
+      <c r="E133" s="6">
+        <v>1608</v>
+      </c>
+      <c r="F133" s="3" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A134" s="14" t="s">
+        <v>414</v>
+      </c>
+      <c r="B134" t="s">
+        <v>419</v>
+      </c>
+      <c r="C134" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D134" t="s">
+        <v>314</v>
+      </c>
+      <c r="E134" s="6">
+        <v>1608</v>
+      </c>
+      <c r="F134" s="3" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A135" s="14" t="s">
+        <v>415</v>
+      </c>
+      <c r="B135" t="s">
+        <v>419</v>
+      </c>
+      <c r="C135" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D135" t="s">
+        <v>314</v>
+      </c>
+      <c r="E135" s="6">
+        <v>1608</v>
+      </c>
+      <c r="F135" s="3" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A136" s="14" t="s">
+        <v>416</v>
+      </c>
+      <c r="B136" t="s">
+        <v>419</v>
+      </c>
+      <c r="C136" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D136" t="s">
+        <v>314</v>
+      </c>
+      <c r="E136" s="6">
+        <v>1608</v>
+      </c>
+      <c r="F136" s="3" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A137" s="14" t="s">
+        <v>417</v>
+      </c>
+      <c r="B137" t="s">
+        <v>419</v>
+      </c>
+      <c r="C137" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D137" t="s">
+        <v>314</v>
+      </c>
+      <c r="E137" s="6">
+        <v>1608</v>
+      </c>
+      <c r="F137" s="3" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A138" s="14" t="s">
+        <v>418</v>
+      </c>
+      <c r="B138" t="s">
+        <v>419</v>
+      </c>
+      <c r="C138" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D138" t="s">
+        <v>314</v>
+      </c>
+      <c r="E138" s="6">
+        <v>1608</v>
+      </c>
+      <c r="F138" s="3" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A139" s="14" t="s">
+        <v>420</v>
+      </c>
+      <c r="B139" t="s">
+        <v>312</v>
+      </c>
+      <c r="C139" s="2">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="D139" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="E139" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="F139" s="3" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A140" s="14" t="s">
+        <v>421</v>
+      </c>
+      <c r="B140" t="s">
+        <v>395</v>
+      </c>
+      <c r="C140" s="25">
+        <v>0.11</v>
+      </c>
+      <c r="D140" t="s">
+        <v>344</v>
+      </c>
+      <c r="E140" s="6">
+        <v>1005</v>
+      </c>
+      <c r="F140" s="3" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A141" s="14" t="s">
+        <v>422</v>
+      </c>
+      <c r="B141" t="s">
+        <v>395</v>
+      </c>
+      <c r="C141" s="25">
+        <v>0.11</v>
+      </c>
+      <c r="D141" t="s">
+        <v>344</v>
+      </c>
+      <c r="E141" s="6">
+        <v>1005</v>
+      </c>
+      <c r="F141" s="3" t="s">
+        <v>345</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="G109:G115"/>
-    <mergeCell ref="G116:G122"/>
-    <mergeCell ref="G123:G129"/>
-    <mergeCell ref="G130:G131"/>
-    <mergeCell ref="G97:G102"/>
-    <mergeCell ref="G103:G108"/>
-    <mergeCell ref="G58:G66"/>
-    <mergeCell ref="G67:G72"/>
-    <mergeCell ref="G73:G78"/>
-    <mergeCell ref="G79:G84"/>
-    <mergeCell ref="G85:G90"/>
     <mergeCell ref="G91:G96"/>
     <mergeCell ref="G2:G10"/>
     <mergeCell ref="G11:G20"/>
@@ -9313,6 +9610,17 @@
     <mergeCell ref="G30:G39"/>
     <mergeCell ref="G40:G48"/>
     <mergeCell ref="G49:G57"/>
+    <mergeCell ref="G58:G66"/>
+    <mergeCell ref="G67:G72"/>
+    <mergeCell ref="G73:G78"/>
+    <mergeCell ref="G79:G84"/>
+    <mergeCell ref="G85:G90"/>
+    <mergeCell ref="G109:G115"/>
+    <mergeCell ref="G116:G122"/>
+    <mergeCell ref="G123:G129"/>
+    <mergeCell ref="G130:G131"/>
+    <mergeCell ref="G97:G102"/>
+    <mergeCell ref="G103:G108"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -9414,9 +9722,13 @@
     <hyperlink ref="F127" r:id="rId96" display="https://www.mouser.ca/datasheet/2/585/MLCC-1837944.pdf" xr:uid="{F5506774-2647-4180-A630-3F869F90200C}"/>
     <hyperlink ref="F128" r:id="rId97" display="https://www.mouser.ca/datasheet/2/445/860010372006-1725314.pdf" xr:uid="{76B8DFED-7E19-40D0-883F-323E54884DB7}"/>
     <hyperlink ref="F129" r:id="rId98" display="https://www.mouser.ca/datasheet/2/447/yago_s_a0003557223_1-2286436.pdf" xr:uid="{E9C3E476-E5B1-42E2-96A4-99E21333D366}"/>
+    <hyperlink ref="F139" r:id="rId99" display="https://www.mouser.ca/datasheet/2/445/860020273009-1725581.pdf" xr:uid="{FCE204EF-6DC7-4555-94B1-FBA8CF609B24}"/>
+    <hyperlink ref="D139" r:id="rId100" xr:uid="{2B4A96D9-73B2-4284-9F00-05D1DF0F219B}"/>
+    <hyperlink ref="F140" r:id="rId101" display="https://www.mouser.ca/datasheet/2/212/KEM_C1023_X7R_AUTO_SMD-1093309.pdf" xr:uid="{EF096566-3DC3-4D51-A03D-30B625A0CE18}"/>
+    <hyperlink ref="F141" r:id="rId102" display="https://www.mouser.ca/datasheet/2/212/KEM_C1023_X7R_AUTO_SMD-1093309.pdf" xr:uid="{CCB90840-C615-48E9-A50C-D72AE500BCAC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId99"/>
+  <pageSetup orientation="portrait" r:id="rId103"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Organized all subcircuits in PCB editor
</commit_message>
<xml_diff>
--- a/Documents/BOM.xlsx
+++ b/Documents/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ECE_Projects\Music_Visualizer\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72560098-43A2-4CB1-8B36-C4A593EF1971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4488E054-3C9A-4984-9B33-9E1DF80FDF92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="824" activeTab="7" xr2:uid="{1F4A7036-4694-4970-BB5D-7CBECC831452}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="824" activeTab="7" xr2:uid="{1F4A7036-4694-4970-BB5D-7CBECC831452}"/>
   </bookViews>
   <sheets>
     <sheet name="Sub-Bass" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,13 @@
     <sheet name="Presence" sheetId="6" r:id="rId6"/>
     <sheet name="Brilliance" sheetId="7" r:id="rId7"/>
     <sheet name="AllPassives" sheetId="8" r:id="rId8"/>
-    <sheet name="FilterAmps" sheetId="12" r:id="rId9"/>
-    <sheet name="PowerV1" sheetId="9" r:id="rId10"/>
-    <sheet name="PowerV2" sheetId="13" r:id="rId11"/>
-    <sheet name="Audio Input" sheetId="10" r:id="rId12"/>
-    <sheet name="Audio Input  V2" sheetId="14" r:id="rId13"/>
-    <sheet name="LED" sheetId="11" r:id="rId14"/>
+    <sheet name="Sheet1" sheetId="15" r:id="rId9"/>
+    <sheet name="FilterAmps" sheetId="12" r:id="rId10"/>
+    <sheet name="PowerV1" sheetId="9" r:id="rId11"/>
+    <sheet name="PowerV2" sheetId="13" r:id="rId12"/>
+    <sheet name="Audio Input" sheetId="10" r:id="rId13"/>
+    <sheet name="Audio Input  V2" sheetId="14" r:id="rId14"/>
+    <sheet name="LED" sheetId="11" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1449" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1450" uniqueCount="428">
   <si>
     <t>Component</t>
   </si>
@@ -1329,6 +1330,9 @@
   </si>
   <si>
     <t>M20-9990246 Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
   </si>
 </sst>
 </file>
@@ -1470,12 +1474,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1487,6 +1485,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2278,11 +2282,177 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F0F8697-67F6-479D-8A67-86E9F1D85B02}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
+        <v>331</v>
+      </c>
+      <c r="B2" t="s">
+        <v>332</v>
+      </c>
+      <c r="C2">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="D2" t="s">
+        <v>333</v>
+      </c>
+      <c r="E2" t="s">
+        <v>334</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
+        <v>331</v>
+      </c>
+      <c r="B3" t="s">
+        <v>332</v>
+      </c>
+      <c r="C3">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="D3" t="s">
+        <v>333</v>
+      </c>
+      <c r="E3" t="s">
+        <v>334</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="14" t="s">
+        <v>331</v>
+      </c>
+      <c r="B4" t="s">
+        <v>332</v>
+      </c>
+      <c r="C4">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="D4" t="s">
+        <v>333</v>
+      </c>
+      <c r="E4" t="s">
+        <v>334</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="14" t="s">
+        <v>331</v>
+      </c>
+      <c r="B5" t="s">
+        <v>332</v>
+      </c>
+      <c r="C5">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="D5" t="s">
+        <v>333</v>
+      </c>
+      <c r="E5" t="s">
+        <v>334</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="14" t="s">
+        <v>331</v>
+      </c>
+      <c r="B6" t="s">
+        <v>332</v>
+      </c>
+      <c r="C6">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="D6" t="s">
+        <v>333</v>
+      </c>
+      <c r="E6" t="s">
+        <v>334</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="14" t="s">
+        <v>331</v>
+      </c>
+      <c r="B7" t="s">
+        <v>332</v>
+      </c>
+      <c r="C7">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="D7" t="s">
+        <v>333</v>
+      </c>
+      <c r="E7" t="s">
+        <v>334</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>335</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" display="https://www.mouser.ca/datasheet/2/308/1/LM324_D-2314880.pdf" xr:uid="{5738DCC6-A9AF-4BAB-9BBE-7D8F57A9641C}"/>
+    <hyperlink ref="F3:F7" r:id="rId2" display="https://www.mouser.ca/datasheet/2/308/1/LM324_D-2314880.pdf" xr:uid="{B27EA078-2732-42F6-BF1D-C143F533A3FB}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D76251E-3DCF-437B-AB0F-DECE015281CC}">
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F19"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2713,7 +2883,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C595792-1ED3-4550-B2C6-F49A784AB9C0}">
   <dimension ref="A1:F19"/>
   <sheetViews>
@@ -3029,7 +3199,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DDCAF3D-5C32-4D35-8B8A-81DDBAD115B7}">
   <dimension ref="A1:F5"/>
   <sheetViews>
@@ -3143,7 +3313,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBB0EED6-7AEC-4823-91A2-5A66F8F096F2}">
   <dimension ref="A1:F5"/>
   <sheetViews>
@@ -3256,7 +3426,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{422FDBAB-416A-4921-A7D0-3405100F2A2C}">
   <dimension ref="A1:F18"/>
   <sheetViews>
@@ -6597,10 +6767,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5E7DEB4-5FFB-4F8D-963A-C08EFBE9A2C1}">
-  <dimension ref="A1:G141"/>
+  <dimension ref="A1:G147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="B140" sqref="B140:F141"/>
+    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
+      <selection activeCell="C142" sqref="C142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6654,7 +6824,7 @@
       <c r="F2" t="s">
         <v>88</v>
       </c>
-      <c r="G2" s="28" t="s">
+      <c r="G2" s="32" t="s">
         <v>367</v>
       </c>
     </row>
@@ -6677,7 +6847,7 @@
       <c r="F3" t="s">
         <v>88</v>
       </c>
-      <c r="G3" s="28"/>
+      <c r="G3" s="32"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -6698,7 +6868,7 @@
       <c r="F4" t="s">
         <v>88</v>
       </c>
-      <c r="G4" s="28"/>
+      <c r="G4" s="32"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -6719,7 +6889,7 @@
       <c r="F5" t="s">
         <v>90</v>
       </c>
-      <c r="G5" s="28"/>
+      <c r="G5" s="32"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -6740,7 +6910,7 @@
       <c r="F6" t="s">
         <v>88</v>
       </c>
-      <c r="G6" s="28"/>
+      <c r="G6" s="32"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -6761,7 +6931,7 @@
       <c r="F7" t="s">
         <v>88</v>
       </c>
-      <c r="G7" s="28"/>
+      <c r="G7" s="32"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -6782,7 +6952,7 @@
       <c r="F8" t="s">
         <v>91</v>
       </c>
-      <c r="G8" s="28"/>
+      <c r="G8" s="32"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -6803,7 +6973,7 @@
       <c r="F9" t="s">
         <v>91</v>
       </c>
-      <c r="G9" s="28"/>
+      <c r="G9" s="32"/>
     </row>
     <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
@@ -6824,7 +6994,7 @@
       <c r="F10" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="G10" s="28"/>
+      <c r="G10" s="32"/>
     </row>
     <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
@@ -6845,7 +7015,7 @@
       <c r="F11" t="s">
         <v>88</v>
       </c>
-      <c r="G11" s="27" t="s">
+      <c r="G11" s="31" t="s">
         <v>368</v>
       </c>
     </row>
@@ -6868,7 +7038,7 @@
       <c r="F12" t="s">
         <v>90</v>
       </c>
-      <c r="G12" s="27"/>
+      <c r="G12" s="31"/>
     </row>
     <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -6889,7 +7059,7 @@
       <c r="F13" t="s">
         <v>88</v>
       </c>
-      <c r="G13" s="27"/>
+      <c r="G13" s="31"/>
     </row>
     <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
@@ -6910,7 +7080,7 @@
       <c r="F14" t="s">
         <v>88</v>
       </c>
-      <c r="G14" s="27"/>
+      <c r="G14" s="31"/>
     </row>
     <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
@@ -6931,7 +7101,7 @@
       <c r="F15" t="s">
         <v>88</v>
       </c>
-      <c r="G15" s="27"/>
+      <c r="G15" s="31"/>
     </row>
     <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
@@ -6952,7 +7122,7 @@
       <c r="F16" t="s">
         <v>88</v>
       </c>
-      <c r="G16" s="27"/>
+      <c r="G16" s="31"/>
     </row>
     <row r="17" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
@@ -6973,7 +7143,7 @@
       <c r="F17" t="s">
         <v>88</v>
       </c>
-      <c r="G17" s="27"/>
+      <c r="G17" s="31"/>
     </row>
     <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
@@ -6994,7 +7164,7 @@
       <c r="F18" t="s">
         <v>96</v>
       </c>
-      <c r="G18" s="27"/>
+      <c r="G18" s="31"/>
     </row>
     <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
@@ -7015,7 +7185,7 @@
       <c r="F19" t="s">
         <v>88</v>
       </c>
-      <c r="G19" s="27"/>
+      <c r="G19" s="31"/>
     </row>
     <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
@@ -7036,7 +7206,7 @@
       <c r="F20" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="G20" s="27"/>
+      <c r="G20" s="31"/>
     </row>
     <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
@@ -7057,7 +7227,7 @@
       <c r="F21" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="G21" s="27" t="s">
+      <c r="G21" s="31" t="s">
         <v>369</v>
       </c>
     </row>
@@ -7080,7 +7250,7 @@
       <c r="F22" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G22" s="27"/>
+      <c r="G22" s="31"/>
     </row>
     <row r="23" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
@@ -7101,7 +7271,7 @@
       <c r="F23" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="G23" s="27"/>
+      <c r="G23" s="31"/>
     </row>
     <row r="24" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
@@ -7122,7 +7292,7 @@
       <c r="F24" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="G24" s="27"/>
+      <c r="G24" s="31"/>
     </row>
     <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
@@ -7143,7 +7313,7 @@
       <c r="F25" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="G25" s="27"/>
+      <c r="G25" s="31"/>
     </row>
     <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
@@ -7164,7 +7334,7 @@
       <c r="F26" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="G26" s="27"/>
+      <c r="G26" s="31"/>
     </row>
     <row r="27" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
@@ -7185,7 +7355,7 @@
       <c r="F27" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="G27" s="27"/>
+      <c r="G27" s="31"/>
     </row>
     <row r="28" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
@@ -7206,7 +7376,7 @@
       <c r="F28" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="G28" s="27"/>
+      <c r="G28" s="31"/>
     </row>
     <row r="29" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="9" t="s">
@@ -7227,7 +7397,7 @@
       <c r="F29" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="G29" s="27"/>
+      <c r="G29" s="31"/>
     </row>
     <row r="30" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
@@ -7248,7 +7418,7 @@
       <c r="F30" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="G30" s="27" t="s">
+      <c r="G30" s="31" t="s">
         <v>370</v>
       </c>
     </row>
@@ -7271,7 +7441,7 @@
       <c r="F31" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="G31" s="27"/>
+      <c r="G31" s="31"/>
     </row>
     <row r="32" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
@@ -7292,7 +7462,7 @@
       <c r="F32" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="G32" s="27"/>
+      <c r="G32" s="31"/>
     </row>
     <row r="33" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
@@ -7313,7 +7483,7 @@
       <c r="F33" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="G33" s="27"/>
+      <c r="G33" s="31"/>
     </row>
     <row r="34" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
@@ -7334,7 +7504,7 @@
       <c r="F34" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="G34" s="27"/>
+      <c r="G34" s="31"/>
     </row>
     <row r="35" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
@@ -7355,7 +7525,7 @@
       <c r="F35" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="G35" s="27"/>
+      <c r="G35" s="31"/>
     </row>
     <row r="36" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
@@ -7376,7 +7546,7 @@
       <c r="F36" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="G36" s="27"/>
+      <c r="G36" s="31"/>
     </row>
     <row r="37" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
@@ -7397,7 +7567,7 @@
       <c r="F37" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="G37" s="27"/>
+      <c r="G37" s="31"/>
     </row>
     <row r="38" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
@@ -7418,7 +7588,7 @@
       <c r="F38" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="G38" s="27"/>
+      <c r="G38" s="31"/>
     </row>
     <row r="39" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="9" t="s">
@@ -7439,7 +7609,7 @@
       <c r="F39" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="G39" s="27"/>
+      <c r="G39" s="31"/>
     </row>
     <row r="40" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
@@ -7460,7 +7630,7 @@
       <c r="F40" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="G40" s="27" t="s">
+      <c r="G40" s="31" t="s">
         <v>371</v>
       </c>
     </row>
@@ -7483,7 +7653,7 @@
       <c r="F41" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="G41" s="27"/>
+      <c r="G41" s="31"/>
     </row>
     <row r="42" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
@@ -7504,7 +7674,7 @@
       <c r="F42" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="G42" s="27"/>
+      <c r="G42" s="31"/>
     </row>
     <row r="43" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
@@ -7525,7 +7695,7 @@
       <c r="F43" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="G43" s="27"/>
+      <c r="G43" s="31"/>
     </row>
     <row r="44" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
@@ -7546,7 +7716,7 @@
       <c r="F44" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="G44" s="27"/>
+      <c r="G44" s="31"/>
     </row>
     <row r="45" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
@@ -7567,7 +7737,7 @@
       <c r="F45" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="G45" s="27"/>
+      <c r="G45" s="31"/>
     </row>
     <row r="46" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
@@ -7588,7 +7758,7 @@
       <c r="F46" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="G46" s="27"/>
+      <c r="G46" s="31"/>
     </row>
     <row r="47" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
@@ -7609,7 +7779,7 @@
       <c r="F47" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="G47" s="27"/>
+      <c r="G47" s="31"/>
     </row>
     <row r="48" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="9" t="s">
@@ -7630,7 +7800,7 @@
       <c r="F48" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="G48" s="27"/>
+      <c r="G48" s="31"/>
     </row>
     <row r="49" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
@@ -7651,7 +7821,7 @@
       <c r="F49" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="G49" s="27" t="s">
+      <c r="G49" s="31" t="s">
         <v>372</v>
       </c>
     </row>
@@ -7674,7 +7844,7 @@
       <c r="F50" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="G50" s="27"/>
+      <c r="G50" s="31"/>
     </row>
     <row r="51" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
@@ -7695,7 +7865,7 @@
       <c r="F51" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="G51" s="27"/>
+      <c r="G51" s="31"/>
     </row>
     <row r="52" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
@@ -7716,7 +7886,7 @@
       <c r="F52" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="G52" s="27"/>
+      <c r="G52" s="31"/>
     </row>
     <row r="53" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
@@ -7737,7 +7907,7 @@
       <c r="F53" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="G53" s="27"/>
+      <c r="G53" s="31"/>
     </row>
     <row r="54" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
@@ -7758,7 +7928,7 @@
       <c r="F54" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="G54" s="27"/>
+      <c r="G54" s="31"/>
     </row>
     <row r="55" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
@@ -7779,7 +7949,7 @@
       <c r="F55" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="G55" s="27"/>
+      <c r="G55" s="31"/>
     </row>
     <row r="56" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
@@ -7800,7 +7970,7 @@
       <c r="F56" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="G56" s="27"/>
+      <c r="G56" s="31"/>
     </row>
     <row r="57" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="9" t="s">
@@ -7821,7 +7991,7 @@
       <c r="F57" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="G57" s="27"/>
+      <c r="G57" s="31"/>
     </row>
     <row r="58" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
@@ -7842,7 +8012,7 @@
       <c r="F58" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="G58" s="27" t="s">
+      <c r="G58" s="31" t="s">
         <v>373</v>
       </c>
     </row>
@@ -7865,7 +8035,7 @@
       <c r="F59" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="G59" s="27"/>
+      <c r="G59" s="31"/>
     </row>
     <row r="60" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
@@ -7886,7 +8056,7 @@
       <c r="F60" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="G60" s="27"/>
+      <c r="G60" s="31"/>
     </row>
     <row r="61" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
@@ -7907,7 +8077,7 @@
       <c r="F61" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="G61" s="27"/>
+      <c r="G61" s="31"/>
     </row>
     <row r="62" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
@@ -7928,7 +8098,7 @@
       <c r="F62" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="G62" s="27"/>
+      <c r="G62" s="31"/>
     </row>
     <row r="63" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
@@ -7949,7 +8119,7 @@
       <c r="F63" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="G63" s="27"/>
+      <c r="G63" s="31"/>
     </row>
     <row r="64" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
@@ -7970,7 +8140,7 @@
       <c r="F64" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="G64" s="27"/>
+      <c r="G64" s="31"/>
     </row>
     <row r="65" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
@@ -7991,7 +8161,7 @@
       <c r="F65" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="G65" s="27"/>
+      <c r="G65" s="31"/>
     </row>
     <row r="66" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="9" t="s">
@@ -8012,7 +8182,7 @@
       <c r="F66" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="G66" s="27"/>
+      <c r="G66" s="31"/>
     </row>
     <row r="67" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
@@ -8033,7 +8203,7 @@
       <c r="F67" t="s">
         <v>93</v>
       </c>
-      <c r="G67" s="27" t="s">
+      <c r="G67" s="31" t="s">
         <v>367</v>
       </c>
     </row>
@@ -8056,7 +8226,7 @@
       <c r="F68" t="s">
         <v>93</v>
       </c>
-      <c r="G68" s="27"/>
+      <c r="G68" s="31"/>
     </row>
     <row r="69" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
@@ -8077,7 +8247,7 @@
       <c r="F69" t="s">
         <v>94</v>
       </c>
-      <c r="G69" s="27"/>
+      <c r="G69" s="31"/>
     </row>
     <row r="70" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
@@ -8098,7 +8268,7 @@
       <c r="F70" t="s">
         <v>94</v>
       </c>
-      <c r="G70" s="27"/>
+      <c r="G70" s="31"/>
     </row>
     <row r="71" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
@@ -8119,7 +8289,7 @@
       <c r="F71" t="s">
         <v>95</v>
       </c>
-      <c r="G71" s="27"/>
+      <c r="G71" s="31"/>
     </row>
     <row r="72" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="9" t="s">
@@ -8140,7 +8310,7 @@
       <c r="F72" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="G72" s="27"/>
+      <c r="G72" s="31"/>
     </row>
     <row r="73" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A73" s="14" t="s">
@@ -8161,7 +8331,7 @@
       <c r="F73" t="s">
         <v>97</v>
       </c>
-      <c r="G73" s="27" t="s">
+      <c r="G73" s="31" t="s">
         <v>368</v>
       </c>
     </row>
@@ -8184,7 +8354,7 @@
       <c r="F74" t="s">
         <v>97</v>
       </c>
-      <c r="G74" s="27"/>
+      <c r="G74" s="31"/>
     </row>
     <row r="75" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="14" t="s">
@@ -8205,7 +8375,7 @@
       <c r="F75" t="s">
         <v>98</v>
       </c>
-      <c r="G75" s="27"/>
+      <c r="G75" s="31"/>
     </row>
     <row r="76" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A76" s="14" t="s">
@@ -8226,7 +8396,7 @@
       <c r="F76" t="s">
         <v>98</v>
       </c>
-      <c r="G76" s="27"/>
+      <c r="G76" s="31"/>
     </row>
     <row r="77" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A77" s="14" t="s">
@@ -8247,7 +8417,7 @@
       <c r="F77" t="s">
         <v>100</v>
       </c>
-      <c r="G77" s="27"/>
+      <c r="G77" s="31"/>
     </row>
     <row r="78" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="15" t="s">
@@ -8268,7 +8438,7 @@
       <c r="F78" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="G78" s="27"/>
+      <c r="G78" s="31"/>
     </row>
     <row r="79" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A79" s="14" t="s">
@@ -8289,7 +8459,7 @@
       <c r="F79" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="G79" s="27" t="s">
+      <c r="G79" s="31" t="s">
         <v>369</v>
       </c>
     </row>
@@ -8312,7 +8482,7 @@
       <c r="F80" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="G80" s="27"/>
+      <c r="G80" s="31"/>
     </row>
     <row r="81" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A81" s="14" t="s">
@@ -8333,7 +8503,7 @@
       <c r="F81" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="G81" s="27"/>
+      <c r="G81" s="31"/>
     </row>
     <row r="82" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A82" s="14" t="s">
@@ -8354,7 +8524,7 @@
       <c r="F82" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="G82" s="27"/>
+      <c r="G82" s="31"/>
     </row>
     <row r="83" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A83" s="14" t="s">
@@ -8375,7 +8545,7 @@
       <c r="F83" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="G83" s="27"/>
+      <c r="G83" s="31"/>
     </row>
     <row r="84" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A84" s="15" t="s">
@@ -8396,7 +8566,7 @@
       <c r="F84" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="G84" s="27"/>
+      <c r="G84" s="31"/>
     </row>
     <row r="85" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A85" s="14" t="s">
@@ -8417,7 +8587,7 @@
       <c r="F85" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="G85" s="27" t="s">
+      <c r="G85" s="31" t="s">
         <v>370</v>
       </c>
     </row>
@@ -8440,7 +8610,7 @@
       <c r="F86" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="G86" s="27"/>
+      <c r="G86" s="31"/>
     </row>
     <row r="87" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A87" s="14" t="s">
@@ -8461,7 +8631,7 @@
       <c r="F87" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G87" s="27"/>
+      <c r="G87" s="31"/>
     </row>
     <row r="88" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A88" s="14" t="s">
@@ -8482,7 +8652,7 @@
       <c r="F88" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G88" s="27"/>
+      <c r="G88" s="31"/>
     </row>
     <row r="89" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A89" s="14" t="s">
@@ -8503,7 +8673,7 @@
       <c r="F89" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="G89" s="27"/>
+      <c r="G89" s="31"/>
     </row>
     <row r="90" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A90" s="15" t="s">
@@ -8524,7 +8694,7 @@
       <c r="F90" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="G90" s="27"/>
+      <c r="G90" s="31"/>
     </row>
     <row r="91" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A91" s="14" t="s">
@@ -8545,7 +8715,7 @@
       <c r="F91" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G91" s="27" t="s">
+      <c r="G91" s="31" t="s">
         <v>371</v>
       </c>
     </row>
@@ -8568,7 +8738,7 @@
       <c r="F92" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G92" s="27"/>
+      <c r="G92" s="31"/>
     </row>
     <row r="93" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A93" s="14" t="s">
@@ -8589,7 +8759,7 @@
       <c r="F93" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G93" s="27"/>
+      <c r="G93" s="31"/>
     </row>
     <row r="94" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A94" s="14" t="s">
@@ -8610,7 +8780,7 @@
       <c r="F94" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G94" s="27"/>
+      <c r="G94" s="31"/>
     </row>
     <row r="95" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A95" s="14" t="s">
@@ -8631,7 +8801,7 @@
       <c r="F95" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G95" s="27"/>
+      <c r="G95" s="31"/>
     </row>
     <row r="96" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A96" s="15" t="s">
@@ -8652,7 +8822,7 @@
       <c r="F96" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="G96" s="27"/>
+      <c r="G96" s="31"/>
     </row>
     <row r="97" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A97" s="20" t="s">
@@ -8673,7 +8843,7 @@
       <c r="F97" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="G97" s="27" t="s">
+      <c r="G97" s="31" t="s">
         <v>372</v>
       </c>
     </row>
@@ -8696,7 +8866,7 @@
       <c r="F98" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="G98" s="27"/>
+      <c r="G98" s="31"/>
     </row>
     <row r="99" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A99" s="14" t="s">
@@ -8717,7 +8887,7 @@
       <c r="F99" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="G99" s="27"/>
+      <c r="G99" s="31"/>
     </row>
     <row r="100" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A100" s="14" t="s">
@@ -8738,7 +8908,7 @@
       <c r="F100" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="G100" s="27"/>
+      <c r="G100" s="31"/>
     </row>
     <row r="101" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A101" s="14" t="s">
@@ -8759,7 +8929,7 @@
       <c r="F101" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="G101" s="27"/>
+      <c r="G101" s="31"/>
     </row>
     <row r="102" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A102" s="15" t="s">
@@ -8780,7 +8950,7 @@
       <c r="F102" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="G102" s="27"/>
+      <c r="G102" s="31"/>
     </row>
     <row r="103" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A103" s="14" t="s">
@@ -8801,7 +8971,7 @@
       <c r="F103" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G103" s="27" t="s">
+      <c r="G103" s="31" t="s">
         <v>373</v>
       </c>
     </row>
@@ -8824,7 +8994,7 @@
       <c r="F104" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G104" s="27"/>
+      <c r="G104" s="31"/>
     </row>
     <row r="105" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A105" s="14" t="s">
@@ -8845,7 +9015,7 @@
       <c r="F105" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G105" s="27"/>
+      <c r="G105" s="31"/>
     </row>
     <row r="106" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A106" s="14" t="s">
@@ -8866,7 +9036,7 @@
       <c r="F106" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G106" s="27"/>
+      <c r="G106" s="31"/>
     </row>
     <row r="107" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A107" s="14" t="s">
@@ -8887,7 +9057,7 @@
       <c r="F107" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G107" s="27"/>
+      <c r="G107" s="31"/>
     </row>
     <row r="108" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A108" s="15" t="s">
@@ -8908,7 +9078,7 @@
       <c r="F108" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="G108" s="27"/>
+      <c r="G108" s="31"/>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109" s="14" t="s">
@@ -8929,7 +9099,7 @@
       <c r="F109" s="3" t="s">
         <v>382</v>
       </c>
-      <c r="G109" s="29" t="s">
+      <c r="G109" s="27" t="s">
         <v>383</v>
       </c>
     </row>
@@ -8952,7 +9122,7 @@
       <c r="F110" s="3" t="s">
         <v>382</v>
       </c>
-      <c r="G110" s="30"/>
+      <c r="G110" s="28"/>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111" s="14" t="s">
@@ -8973,7 +9143,7 @@
       <c r="F111" s="3" t="s">
         <v>382</v>
       </c>
-      <c r="G111" s="30"/>
+      <c r="G111" s="28"/>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112" s="14" t="s">
@@ -8994,7 +9164,7 @@
       <c r="F112" s="3" t="s">
         <v>382</v>
       </c>
-      <c r="G112" s="30"/>
+      <c r="G112" s="28"/>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113" s="14" t="s">
@@ -9015,7 +9185,7 @@
       <c r="F113" s="3" t="s">
         <v>382</v>
       </c>
-      <c r="G113" s="30"/>
+      <c r="G113" s="28"/>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114" s="14" t="s">
@@ -9036,7 +9206,7 @@
       <c r="F114" s="3" t="s">
         <v>382</v>
       </c>
-      <c r="G114" s="30"/>
+      <c r="G114" s="28"/>
     </row>
     <row r="115" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A115" s="15" t="s">
@@ -9057,7 +9227,7 @@
       <c r="F115" s="12" t="s">
         <v>382</v>
       </c>
-      <c r="G115" s="30"/>
+      <c r="G115" s="28"/>
     </row>
     <row r="116" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A116" s="14" t="s">
@@ -9078,7 +9248,7 @@
       <c r="F116" s="3" t="s">
         <v>398</v>
       </c>
-      <c r="G116" s="31" t="s">
+      <c r="G116" s="29" t="s">
         <v>399</v>
       </c>
     </row>
@@ -9101,7 +9271,7 @@
       <c r="F117" s="3" t="s">
         <v>398</v>
       </c>
-      <c r="G117" s="31"/>
+      <c r="G117" s="29"/>
     </row>
     <row r="118" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A118" s="14" t="s">
@@ -9122,7 +9292,7 @@
       <c r="F118" s="3" t="s">
         <v>401</v>
       </c>
-      <c r="G118" s="31"/>
+      <c r="G118" s="29"/>
     </row>
     <row r="119" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A119" s="14" t="s">
@@ -9143,7 +9313,7 @@
       <c r="F119" s="3" t="s">
         <v>401</v>
       </c>
-      <c r="G119" s="31"/>
+      <c r="G119" s="29"/>
     </row>
     <row r="120" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A120" s="14" t="s">
@@ -9164,7 +9334,7 @@
       <c r="F120" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="G120" s="31"/>
+      <c r="G120" s="29"/>
     </row>
     <row r="121" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A121" s="14" t="s">
@@ -9185,7 +9355,7 @@
       <c r="F121" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="G121" s="31"/>
+      <c r="G121" s="29"/>
     </row>
     <row r="122" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A122" s="15" t="s">
@@ -9206,7 +9376,7 @@
       <c r="F122" s="12" t="s">
         <v>345</v>
       </c>
-      <c r="G122" s="31"/>
+      <c r="G122" s="29"/>
     </row>
     <row r="123" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A123" s="14" t="s">
@@ -9227,7 +9397,7 @@
       <c r="F123" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="G123" s="31" t="s">
+      <c r="G123" s="29" t="s">
         <v>403</v>
       </c>
     </row>
@@ -9250,7 +9420,7 @@
       <c r="F124" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="G124" s="31"/>
+      <c r="G124" s="29"/>
     </row>
     <row r="125" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A125" s="14" t="s">
@@ -9271,7 +9441,7 @@
       <c r="F125" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="G125" s="31"/>
+      <c r="G125" s="29"/>
     </row>
     <row r="126" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A126" s="14" t="s">
@@ -9292,7 +9462,7 @@
       <c r="F126" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="G126" s="31"/>
+      <c r="G126" s="29"/>
     </row>
     <row r="127" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A127" s="14" t="s">
@@ -9313,7 +9483,7 @@
       <c r="F127" s="3" t="s">
         <v>347</v>
       </c>
-      <c r="G127" s="31"/>
+      <c r="G127" s="29"/>
     </row>
     <row r="128" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A128" s="14" t="s">
@@ -9334,7 +9504,7 @@
       <c r="F128" s="3" t="s">
         <v>350</v>
       </c>
-      <c r="G128" s="31"/>
+      <c r="G128" s="29"/>
     </row>
     <row r="129" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A129" s="15" t="s">
@@ -9355,7 +9525,7 @@
       <c r="F129" s="12" t="s">
         <v>352</v>
       </c>
-      <c r="G129" s="31"/>
+      <c r="G129" s="29"/>
     </row>
     <row r="130" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A130" s="14" t="s">
@@ -9376,7 +9546,7 @@
       <c r="F130" s="3" t="s">
         <v>354</v>
       </c>
-      <c r="G130" s="32" t="s">
+      <c r="G130" s="30" t="s">
         <v>411</v>
       </c>
     </row>
@@ -9399,7 +9569,7 @@
       <c r="F131" s="12" t="s">
         <v>356</v>
       </c>
-      <c r="G131" s="32"/>
+      <c r="G131" s="30"/>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132" s="14" t="s">
@@ -9601,14 +9771,16 @@
         <v>345</v>
       </c>
     </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C142" s="2"/>
+    </row>
+    <row r="147" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E147" t="s">
+        <v>427</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="G109:G115"/>
-    <mergeCell ref="G116:G122"/>
-    <mergeCell ref="G123:G129"/>
-    <mergeCell ref="G130:G131"/>
-    <mergeCell ref="G97:G102"/>
-    <mergeCell ref="G103:G108"/>
     <mergeCell ref="G91:G96"/>
     <mergeCell ref="G2:G10"/>
     <mergeCell ref="G11:G20"/>
@@ -9621,6 +9793,12 @@
     <mergeCell ref="G73:G78"/>
     <mergeCell ref="G79:G84"/>
     <mergeCell ref="G85:G90"/>
+    <mergeCell ref="G109:G115"/>
+    <mergeCell ref="G116:G122"/>
+    <mergeCell ref="G123:G129"/>
+    <mergeCell ref="G130:G131"/>
+    <mergeCell ref="G97:G102"/>
+    <mergeCell ref="G103:G108"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -9733,167 +9911,13 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F0F8697-67F6-479D-8A67-86E9F1D85B02}">
-  <dimension ref="A1:F7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BBEB1EC-89A0-4D7F-A4AC-4752C6AE04A2}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.88671875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
-        <v>331</v>
-      </c>
-      <c r="B2" t="s">
-        <v>332</v>
-      </c>
-      <c r="C2">
-        <v>0.75900000000000001</v>
-      </c>
-      <c r="D2" t="s">
-        <v>333</v>
-      </c>
-      <c r="E2" t="s">
-        <v>334</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="s">
-        <v>331</v>
-      </c>
-      <c r="B3" t="s">
-        <v>332</v>
-      </c>
-      <c r="C3">
-        <v>0.75900000000000001</v>
-      </c>
-      <c r="D3" t="s">
-        <v>333</v>
-      </c>
-      <c r="E3" t="s">
-        <v>334</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
-        <v>331</v>
-      </c>
-      <c r="B4" t="s">
-        <v>332</v>
-      </c>
-      <c r="C4">
-        <v>0.75900000000000001</v>
-      </c>
-      <c r="D4" t="s">
-        <v>333</v>
-      </c>
-      <c r="E4" t="s">
-        <v>334</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
-        <v>331</v>
-      </c>
-      <c r="B5" t="s">
-        <v>332</v>
-      </c>
-      <c r="C5">
-        <v>0.75900000000000001</v>
-      </c>
-      <c r="D5" t="s">
-        <v>333</v>
-      </c>
-      <c r="E5" t="s">
-        <v>334</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="14" t="s">
-        <v>331</v>
-      </c>
-      <c r="B6" t="s">
-        <v>332</v>
-      </c>
-      <c r="C6">
-        <v>0.75900000000000001</v>
-      </c>
-      <c r="D6" t="s">
-        <v>333</v>
-      </c>
-      <c r="E6" t="s">
-        <v>334</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="14" t="s">
-        <v>331</v>
-      </c>
-      <c r="B7" t="s">
-        <v>332</v>
-      </c>
-      <c r="C7">
-        <v>0.75900000000000001</v>
-      </c>
-      <c r="D7" t="s">
-        <v>333</v>
-      </c>
-      <c r="E7" t="s">
-        <v>334</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>335</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="https://www.mouser.ca/datasheet/2/308/1/LM324_D-2314880.pdf" xr:uid="{5738DCC6-A9AF-4BAB-9BBE-7D8F57A9641C}"/>
-    <hyperlink ref="F3:F7" r:id="rId2" display="https://www.mouser.ca/datasheet/2/308/1/LM324_D-2314880.pdf" xr:uid="{B27EA078-2732-42F6-BF1D-C143F533A3FB}"/>
-  </hyperlinks>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Sourced on_off switch and added on_off switch/indicator circuit
</commit_message>
<xml_diff>
--- a/Documents/BOM.xlsx
+++ b/Documents/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ECE_Projects\Music_Visualizer\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4488E054-3C9A-4984-9B33-9E1DF80FDF92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F350AF6-C531-42E8-A127-2A7DFC1D8C3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="824" activeTab="7" xr2:uid="{1F4A7036-4694-4970-BB5D-7CBECC831452}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="824" activeTab="11" xr2:uid="{1F4A7036-4694-4970-BB5D-7CBECC831452}"/>
   </bookViews>
   <sheets>
     <sheet name="Sub-Bass" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1450" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1467" uniqueCount="440">
   <si>
     <t>Component</t>
   </si>
@@ -1333,6 +1333,42 @@
   </si>
   <si>
     <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>Rv1</t>
+  </si>
+  <si>
+    <t>Rv2</t>
+  </si>
+  <si>
+    <t>5k pot</t>
+  </si>
+  <si>
+    <t>330 ohm</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/ROHM-Semiconductor/SDR03EZPD3300?qs=sGAEpiMZZMtlubZbdhIBIK8AeiPKd8jICi7j%252BlRYMkQ%3D</t>
+  </si>
+  <si>
+    <t>SDR03EZPD3300 Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>R82</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9V Indicator R </t>
+  </si>
+  <si>
+    <t>RR511D1121</t>
+  </si>
+  <si>
+    <t>On/Off E-switch</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/E-Switch/RR511D1121?qs=vOb5o%2F429vO6kE%2F8XITwgA%3D%3D</t>
+  </si>
+  <si>
+    <t>RR511D1121 Datasheet (PDF)</t>
   </si>
 </sst>
 </file>
@@ -1474,6 +1510,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1485,12 +1527,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2887,8 +2923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C595792-1ED3-4550-B2C6-F49A784AB9C0}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12:F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3158,14 +3194,41 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C14">
-        <f>SUM(C2:C13)</f>
-        <v>7.88</v>
-      </c>
-      <c r="F14" s="3"/>
+      <c r="A14" s="14" t="s">
+        <v>434</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>431</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="D14" t="s">
+        <v>432</v>
+      </c>
+      <c r="E14" s="6">
+        <v>1608</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>433</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F15" s="3"/>
+      <c r="A15" t="s">
+        <v>436</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>437</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1.55</v>
+      </c>
+      <c r="D15" t="s">
+        <v>438</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>439</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F16" s="3"/>
@@ -3193,9 +3256,10 @@
     <hyperlink ref="F10" r:id="rId9" display="https://www.mouser.ca/datasheet/2/445/860010372006-1725314.pdf" xr:uid="{DBA0956B-B8D9-4F30-93A7-E5D8C434E760}"/>
     <hyperlink ref="F11" r:id="rId10" display="https://www.mouser.ca/datasheet/2/447/yago_s_a0003557223_1-2286436.pdf" xr:uid="{2BF698B5-2BBF-4440-9932-2433F49FF139}"/>
     <hyperlink ref="F4" r:id="rId11" display="https://www.ti.com/general/docs/suppproductinfo.tsp?distId=26&amp;gotoUrl=https://www.ti.com/lit/gpn/lt1054" xr:uid="{3B0922DB-30FA-4D77-8674-D69A0BABD8CF}"/>
+    <hyperlink ref="F14" r:id="rId12" display="https://fscdn.rohm.com/en/products/databook/datasheet/passive/resistor/chip_resistor/sdr-e.pdf" xr:uid="{BE7E562E-F50A-47EA-B9F3-8D919D5C6B81}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
 
@@ -6769,8 +6833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5E7DEB4-5FFB-4F8D-963A-C08EFBE9A2C1}">
   <dimension ref="A1:G147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
-      <selection activeCell="C142" sqref="C142"/>
+    <sheetView topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="A144" sqref="A144:G144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6824,7 +6888,7 @@
       <c r="F2" t="s">
         <v>88</v>
       </c>
-      <c r="G2" s="32" t="s">
+      <c r="G2" s="28" t="s">
         <v>367</v>
       </c>
     </row>
@@ -6847,7 +6911,7 @@
       <c r="F3" t="s">
         <v>88</v>
       </c>
-      <c r="G3" s="32"/>
+      <c r="G3" s="28"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -6868,7 +6932,7 @@
       <c r="F4" t="s">
         <v>88</v>
       </c>
-      <c r="G4" s="32"/>
+      <c r="G4" s="28"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -6889,7 +6953,7 @@
       <c r="F5" t="s">
         <v>90</v>
       </c>
-      <c r="G5" s="32"/>
+      <c r="G5" s="28"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -6910,7 +6974,7 @@
       <c r="F6" t="s">
         <v>88</v>
       </c>
-      <c r="G6" s="32"/>
+      <c r="G6" s="28"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -6931,7 +6995,7 @@
       <c r="F7" t="s">
         <v>88</v>
       </c>
-      <c r="G7" s="32"/>
+      <c r="G7" s="28"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -6952,7 +7016,7 @@
       <c r="F8" t="s">
         <v>91</v>
       </c>
-      <c r="G8" s="32"/>
+      <c r="G8" s="28"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -6973,7 +7037,7 @@
       <c r="F9" t="s">
         <v>91</v>
       </c>
-      <c r="G9" s="32"/>
+      <c r="G9" s="28"/>
     </row>
     <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
@@ -6994,7 +7058,7 @@
       <c r="F10" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="G10" s="32"/>
+      <c r="G10" s="28"/>
     </row>
     <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
@@ -7015,7 +7079,7 @@
       <c r="F11" t="s">
         <v>88</v>
       </c>
-      <c r="G11" s="31" t="s">
+      <c r="G11" s="27" t="s">
         <v>368</v>
       </c>
     </row>
@@ -7038,7 +7102,7 @@
       <c r="F12" t="s">
         <v>90</v>
       </c>
-      <c r="G12" s="31"/>
+      <c r="G12" s="27"/>
     </row>
     <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -7059,7 +7123,7 @@
       <c r="F13" t="s">
         <v>88</v>
       </c>
-      <c r="G13" s="31"/>
+      <c r="G13" s="27"/>
     </row>
     <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
@@ -7080,7 +7144,7 @@
       <c r="F14" t="s">
         <v>88</v>
       </c>
-      <c r="G14" s="31"/>
+      <c r="G14" s="27"/>
     </row>
     <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
@@ -7101,7 +7165,7 @@
       <c r="F15" t="s">
         <v>88</v>
       </c>
-      <c r="G15" s="31"/>
+      <c r="G15" s="27"/>
     </row>
     <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
@@ -7122,7 +7186,7 @@
       <c r="F16" t="s">
         <v>88</v>
       </c>
-      <c r="G16" s="31"/>
+      <c r="G16" s="27"/>
     </row>
     <row r="17" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
@@ -7143,7 +7207,7 @@
       <c r="F17" t="s">
         <v>88</v>
       </c>
-      <c r="G17" s="31"/>
+      <c r="G17" s="27"/>
     </row>
     <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
@@ -7164,7 +7228,7 @@
       <c r="F18" t="s">
         <v>96</v>
       </c>
-      <c r="G18" s="31"/>
+      <c r="G18" s="27"/>
     </row>
     <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
@@ -7185,7 +7249,7 @@
       <c r="F19" t="s">
         <v>88</v>
       </c>
-      <c r="G19" s="31"/>
+      <c r="G19" s="27"/>
     </row>
     <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
@@ -7206,7 +7270,7 @@
       <c r="F20" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="G20" s="31"/>
+      <c r="G20" s="27"/>
     </row>
     <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
@@ -7227,7 +7291,7 @@
       <c r="F21" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="G21" s="31" t="s">
+      <c r="G21" s="27" t="s">
         <v>369</v>
       </c>
     </row>
@@ -7250,7 +7314,7 @@
       <c r="F22" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G22" s="31"/>
+      <c r="G22" s="27"/>
     </row>
     <row r="23" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
@@ -7271,7 +7335,7 @@
       <c r="F23" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="G23" s="31"/>
+      <c r="G23" s="27"/>
     </row>
     <row r="24" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
@@ -7292,7 +7356,7 @@
       <c r="F24" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="G24" s="31"/>
+      <c r="G24" s="27"/>
     </row>
     <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
@@ -7313,7 +7377,7 @@
       <c r="F25" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="G25" s="31"/>
+      <c r="G25" s="27"/>
     </row>
     <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
@@ -7334,7 +7398,7 @@
       <c r="F26" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="G26" s="31"/>
+      <c r="G26" s="27"/>
     </row>
     <row r="27" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
@@ -7355,7 +7419,7 @@
       <c r="F27" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="G27" s="31"/>
+      <c r="G27" s="27"/>
     </row>
     <row r="28" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
@@ -7376,7 +7440,7 @@
       <c r="F28" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="G28" s="31"/>
+      <c r="G28" s="27"/>
     </row>
     <row r="29" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="9" t="s">
@@ -7397,7 +7461,7 @@
       <c r="F29" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="G29" s="31"/>
+      <c r="G29" s="27"/>
     </row>
     <row r="30" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
@@ -7418,7 +7482,7 @@
       <c r="F30" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="G30" s="31" t="s">
+      <c r="G30" s="27" t="s">
         <v>370</v>
       </c>
     </row>
@@ -7441,7 +7505,7 @@
       <c r="F31" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="G31" s="31"/>
+      <c r="G31" s="27"/>
     </row>
     <row r="32" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
@@ -7462,7 +7526,7 @@
       <c r="F32" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="G32" s="31"/>
+      <c r="G32" s="27"/>
     </row>
     <row r="33" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
@@ -7483,7 +7547,7 @@
       <c r="F33" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="G33" s="31"/>
+      <c r="G33" s="27"/>
     </row>
     <row r="34" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
@@ -7504,7 +7568,7 @@
       <c r="F34" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="G34" s="31"/>
+      <c r="G34" s="27"/>
     </row>
     <row r="35" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
@@ -7525,7 +7589,7 @@
       <c r="F35" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="G35" s="31"/>
+      <c r="G35" s="27"/>
     </row>
     <row r="36" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
@@ -7546,7 +7610,7 @@
       <c r="F36" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="G36" s="31"/>
+      <c r="G36" s="27"/>
     </row>
     <row r="37" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
@@ -7567,7 +7631,7 @@
       <c r="F37" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="G37" s="31"/>
+      <c r="G37" s="27"/>
     </row>
     <row r="38" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
@@ -7588,7 +7652,7 @@
       <c r="F38" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="G38" s="31"/>
+      <c r="G38" s="27"/>
     </row>
     <row r="39" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="9" t="s">
@@ -7609,7 +7673,7 @@
       <c r="F39" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="G39" s="31"/>
+      <c r="G39" s="27"/>
     </row>
     <row r="40" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
@@ -7630,7 +7694,7 @@
       <c r="F40" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="G40" s="31" t="s">
+      <c r="G40" s="27" t="s">
         <v>371</v>
       </c>
     </row>
@@ -7653,7 +7717,7 @@
       <c r="F41" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="G41" s="31"/>
+      <c r="G41" s="27"/>
     </row>
     <row r="42" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
@@ -7674,7 +7738,7 @@
       <c r="F42" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="G42" s="31"/>
+      <c r="G42" s="27"/>
     </row>
     <row r="43" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
@@ -7695,7 +7759,7 @@
       <c r="F43" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="G43" s="31"/>
+      <c r="G43" s="27"/>
     </row>
     <row r="44" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
@@ -7716,7 +7780,7 @@
       <c r="F44" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="G44" s="31"/>
+      <c r="G44" s="27"/>
     </row>
     <row r="45" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
@@ -7737,7 +7801,7 @@
       <c r="F45" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="G45" s="31"/>
+      <c r="G45" s="27"/>
     </row>
     <row r="46" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
@@ -7758,7 +7822,7 @@
       <c r="F46" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="G46" s="31"/>
+      <c r="G46" s="27"/>
     </row>
     <row r="47" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
@@ -7779,7 +7843,7 @@
       <c r="F47" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="G47" s="31"/>
+      <c r="G47" s="27"/>
     </row>
     <row r="48" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="9" t="s">
@@ -7800,7 +7864,7 @@
       <c r="F48" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="G48" s="31"/>
+      <c r="G48" s="27"/>
     </row>
     <row r="49" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
@@ -7821,7 +7885,7 @@
       <c r="F49" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="G49" s="31" t="s">
+      <c r="G49" s="27" t="s">
         <v>372</v>
       </c>
     </row>
@@ -7844,7 +7908,7 @@
       <c r="F50" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="G50" s="31"/>
+      <c r="G50" s="27"/>
     </row>
     <row r="51" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
@@ -7865,7 +7929,7 @@
       <c r="F51" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="G51" s="31"/>
+      <c r="G51" s="27"/>
     </row>
     <row r="52" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
@@ -7886,7 +7950,7 @@
       <c r="F52" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="G52" s="31"/>
+      <c r="G52" s="27"/>
     </row>
     <row r="53" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
@@ -7907,7 +7971,7 @@
       <c r="F53" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="G53" s="31"/>
+      <c r="G53" s="27"/>
     </row>
     <row r="54" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
@@ -7928,7 +7992,7 @@
       <c r="F54" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="G54" s="31"/>
+      <c r="G54" s="27"/>
     </row>
     <row r="55" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
@@ -7949,7 +8013,7 @@
       <c r="F55" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="G55" s="31"/>
+      <c r="G55" s="27"/>
     </row>
     <row r="56" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
@@ -7970,7 +8034,7 @@
       <c r="F56" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="G56" s="31"/>
+      <c r="G56" s="27"/>
     </row>
     <row r="57" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="9" t="s">
@@ -7991,7 +8055,7 @@
       <c r="F57" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="G57" s="31"/>
+      <c r="G57" s="27"/>
     </row>
     <row r="58" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
@@ -8012,7 +8076,7 @@
       <c r="F58" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="G58" s="31" t="s">
+      <c r="G58" s="27" t="s">
         <v>373</v>
       </c>
     </row>
@@ -8035,7 +8099,7 @@
       <c r="F59" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="G59" s="31"/>
+      <c r="G59" s="27"/>
     </row>
     <row r="60" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
@@ -8056,7 +8120,7 @@
       <c r="F60" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="G60" s="31"/>
+      <c r="G60" s="27"/>
     </row>
     <row r="61" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
@@ -8077,7 +8141,7 @@
       <c r="F61" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="G61" s="31"/>
+      <c r="G61" s="27"/>
     </row>
     <row r="62" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
@@ -8098,7 +8162,7 @@
       <c r="F62" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="G62" s="31"/>
+      <c r="G62" s="27"/>
     </row>
     <row r="63" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
@@ -8119,7 +8183,7 @@
       <c r="F63" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="G63" s="31"/>
+      <c r="G63" s="27"/>
     </row>
     <row r="64" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
@@ -8140,7 +8204,7 @@
       <c r="F64" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="G64" s="31"/>
+      <c r="G64" s="27"/>
     </row>
     <row r="65" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
@@ -8161,7 +8225,7 @@
       <c r="F65" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="G65" s="31"/>
+      <c r="G65" s="27"/>
     </row>
     <row r="66" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="9" t="s">
@@ -8182,7 +8246,7 @@
       <c r="F66" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="G66" s="31"/>
+      <c r="G66" s="27"/>
     </row>
     <row r="67" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
@@ -8203,7 +8267,7 @@
       <c r="F67" t="s">
         <v>93</v>
       </c>
-      <c r="G67" s="31" t="s">
+      <c r="G67" s="27" t="s">
         <v>367</v>
       </c>
     </row>
@@ -8226,7 +8290,7 @@
       <c r="F68" t="s">
         <v>93</v>
       </c>
-      <c r="G68" s="31"/>
+      <c r="G68" s="27"/>
     </row>
     <row r="69" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
@@ -8247,7 +8311,7 @@
       <c r="F69" t="s">
         <v>94</v>
       </c>
-      <c r="G69" s="31"/>
+      <c r="G69" s="27"/>
     </row>
     <row r="70" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
@@ -8268,7 +8332,7 @@
       <c r="F70" t="s">
         <v>94</v>
       </c>
-      <c r="G70" s="31"/>
+      <c r="G70" s="27"/>
     </row>
     <row r="71" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
@@ -8289,7 +8353,7 @@
       <c r="F71" t="s">
         <v>95</v>
       </c>
-      <c r="G71" s="31"/>
+      <c r="G71" s="27"/>
     </row>
     <row r="72" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="9" t="s">
@@ -8310,7 +8374,7 @@
       <c r="F72" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="G72" s="31"/>
+      <c r="G72" s="27"/>
     </row>
     <row r="73" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A73" s="14" t="s">
@@ -8331,7 +8395,7 @@
       <c r="F73" t="s">
         <v>97</v>
       </c>
-      <c r="G73" s="31" t="s">
+      <c r="G73" s="27" t="s">
         <v>368</v>
       </c>
     </row>
@@ -8354,7 +8418,7 @@
       <c r="F74" t="s">
         <v>97</v>
       </c>
-      <c r="G74" s="31"/>
+      <c r="G74" s="27"/>
     </row>
     <row r="75" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="14" t="s">
@@ -8375,7 +8439,7 @@
       <c r="F75" t="s">
         <v>98</v>
       </c>
-      <c r="G75" s="31"/>
+      <c r="G75" s="27"/>
     </row>
     <row r="76" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A76" s="14" t="s">
@@ -8396,7 +8460,7 @@
       <c r="F76" t="s">
         <v>98</v>
       </c>
-      <c r="G76" s="31"/>
+      <c r="G76" s="27"/>
     </row>
     <row r="77" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A77" s="14" t="s">
@@ -8417,7 +8481,7 @@
       <c r="F77" t="s">
         <v>100</v>
       </c>
-      <c r="G77" s="31"/>
+      <c r="G77" s="27"/>
     </row>
     <row r="78" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="15" t="s">
@@ -8438,7 +8502,7 @@
       <c r="F78" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="G78" s="31"/>
+      <c r="G78" s="27"/>
     </row>
     <row r="79" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A79" s="14" t="s">
@@ -8459,7 +8523,7 @@
       <c r="F79" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="G79" s="31" t="s">
+      <c r="G79" s="27" t="s">
         <v>369</v>
       </c>
     </row>
@@ -8482,7 +8546,7 @@
       <c r="F80" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="G80" s="31"/>
+      <c r="G80" s="27"/>
     </row>
     <row r="81" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A81" s="14" t="s">
@@ -8503,7 +8567,7 @@
       <c r="F81" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="G81" s="31"/>
+      <c r="G81" s="27"/>
     </row>
     <row r="82" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A82" s="14" t="s">
@@ -8524,7 +8588,7 @@
       <c r="F82" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="G82" s="31"/>
+      <c r="G82" s="27"/>
     </row>
     <row r="83" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A83" s="14" t="s">
@@ -8545,7 +8609,7 @@
       <c r="F83" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="G83" s="31"/>
+      <c r="G83" s="27"/>
     </row>
     <row r="84" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A84" s="15" t="s">
@@ -8566,7 +8630,7 @@
       <c r="F84" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="G84" s="31"/>
+      <c r="G84" s="27"/>
     </row>
     <row r="85" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A85" s="14" t="s">
@@ -8587,7 +8651,7 @@
       <c r="F85" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="G85" s="31" t="s">
+      <c r="G85" s="27" t="s">
         <v>370</v>
       </c>
     </row>
@@ -8610,7 +8674,7 @@
       <c r="F86" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="G86" s="31"/>
+      <c r="G86" s="27"/>
     </row>
     <row r="87" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A87" s="14" t="s">
@@ -8631,7 +8695,7 @@
       <c r="F87" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G87" s="31"/>
+      <c r="G87" s="27"/>
     </row>
     <row r="88" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A88" s="14" t="s">
@@ -8652,7 +8716,7 @@
       <c r="F88" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G88" s="31"/>
+      <c r="G88" s="27"/>
     </row>
     <row r="89" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A89" s="14" t="s">
@@ -8673,7 +8737,7 @@
       <c r="F89" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="G89" s="31"/>
+      <c r="G89" s="27"/>
     </row>
     <row r="90" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A90" s="15" t="s">
@@ -8694,7 +8758,7 @@
       <c r="F90" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="G90" s="31"/>
+      <c r="G90" s="27"/>
     </row>
     <row r="91" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A91" s="14" t="s">
@@ -8715,7 +8779,7 @@
       <c r="F91" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G91" s="31" t="s">
+      <c r="G91" s="27" t="s">
         <v>371</v>
       </c>
     </row>
@@ -8738,7 +8802,7 @@
       <c r="F92" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G92" s="31"/>
+      <c r="G92" s="27"/>
     </row>
     <row r="93" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A93" s="14" t="s">
@@ -8759,7 +8823,7 @@
       <c r="F93" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G93" s="31"/>
+      <c r="G93" s="27"/>
     </row>
     <row r="94" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A94" s="14" t="s">
@@ -8780,7 +8844,7 @@
       <c r="F94" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G94" s="31"/>
+      <c r="G94" s="27"/>
     </row>
     <row r="95" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A95" s="14" t="s">
@@ -8801,7 +8865,7 @@
       <c r="F95" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G95" s="31"/>
+      <c r="G95" s="27"/>
     </row>
     <row r="96" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A96" s="15" t="s">
@@ -8822,7 +8886,7 @@
       <c r="F96" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="G96" s="31"/>
+      <c r="G96" s="27"/>
     </row>
     <row r="97" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A97" s="20" t="s">
@@ -8843,7 +8907,7 @@
       <c r="F97" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="G97" s="31" t="s">
+      <c r="G97" s="27" t="s">
         <v>372</v>
       </c>
     </row>
@@ -8866,7 +8930,7 @@
       <c r="F98" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="G98" s="31"/>
+      <c r="G98" s="27"/>
     </row>
     <row r="99" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A99" s="14" t="s">
@@ -8887,7 +8951,7 @@
       <c r="F99" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="G99" s="31"/>
+      <c r="G99" s="27"/>
     </row>
     <row r="100" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A100" s="14" t="s">
@@ -8908,7 +8972,7 @@
       <c r="F100" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="G100" s="31"/>
+      <c r="G100" s="27"/>
     </row>
     <row r="101" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A101" s="14" t="s">
@@ -8929,7 +8993,7 @@
       <c r="F101" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="G101" s="31"/>
+      <c r="G101" s="27"/>
     </row>
     <row r="102" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A102" s="15" t="s">
@@ -8950,7 +9014,7 @@
       <c r="F102" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="G102" s="31"/>
+      <c r="G102" s="27"/>
     </row>
     <row r="103" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A103" s="14" t="s">
@@ -8971,7 +9035,7 @@
       <c r="F103" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G103" s="31" t="s">
+      <c r="G103" s="27" t="s">
         <v>373</v>
       </c>
     </row>
@@ -8994,7 +9058,7 @@
       <c r="F104" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G104" s="31"/>
+      <c r="G104" s="27"/>
     </row>
     <row r="105" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A105" s="14" t="s">
@@ -9015,7 +9079,7 @@
       <c r="F105" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G105" s="31"/>
+      <c r="G105" s="27"/>
     </row>
     <row r="106" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A106" s="14" t="s">
@@ -9036,7 +9100,7 @@
       <c r="F106" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G106" s="31"/>
+      <c r="G106" s="27"/>
     </row>
     <row r="107" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A107" s="14" t="s">
@@ -9057,7 +9121,7 @@
       <c r="F107" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G107" s="31"/>
+      <c r="G107" s="27"/>
     </row>
     <row r="108" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A108" s="15" t="s">
@@ -9078,7 +9142,7 @@
       <c r="F108" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="G108" s="31"/>
+      <c r="G108" s="27"/>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109" s="14" t="s">
@@ -9099,7 +9163,7 @@
       <c r="F109" s="3" t="s">
         <v>382</v>
       </c>
-      <c r="G109" s="27" t="s">
+      <c r="G109" s="29" t="s">
         <v>383</v>
       </c>
     </row>
@@ -9122,7 +9186,7 @@
       <c r="F110" s="3" t="s">
         <v>382</v>
       </c>
-      <c r="G110" s="28"/>
+      <c r="G110" s="30"/>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111" s="14" t="s">
@@ -9143,7 +9207,7 @@
       <c r="F111" s="3" t="s">
         <v>382</v>
       </c>
-      <c r="G111" s="28"/>
+      <c r="G111" s="30"/>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112" s="14" t="s">
@@ -9164,7 +9228,7 @@
       <c r="F112" s="3" t="s">
         <v>382</v>
       </c>
-      <c r="G112" s="28"/>
+      <c r="G112" s="30"/>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113" s="14" t="s">
@@ -9185,7 +9249,7 @@
       <c r="F113" s="3" t="s">
         <v>382</v>
       </c>
-      <c r="G113" s="28"/>
+      <c r="G113" s="30"/>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114" s="14" t="s">
@@ -9206,7 +9270,7 @@
       <c r="F114" s="3" t="s">
         <v>382</v>
       </c>
-      <c r="G114" s="28"/>
+      <c r="G114" s="30"/>
     </row>
     <row r="115" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A115" s="15" t="s">
@@ -9227,7 +9291,7 @@
       <c r="F115" s="12" t="s">
         <v>382</v>
       </c>
-      <c r="G115" s="28"/>
+      <c r="G115" s="30"/>
     </row>
     <row r="116" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A116" s="14" t="s">
@@ -9248,7 +9312,7 @@
       <c r="F116" s="3" t="s">
         <v>398</v>
       </c>
-      <c r="G116" s="29" t="s">
+      <c r="G116" s="31" t="s">
         <v>399</v>
       </c>
     </row>
@@ -9271,7 +9335,7 @@
       <c r="F117" s="3" t="s">
         <v>398</v>
       </c>
-      <c r="G117" s="29"/>
+      <c r="G117" s="31"/>
     </row>
     <row r="118" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A118" s="14" t="s">
@@ -9292,7 +9356,7 @@
       <c r="F118" s="3" t="s">
         <v>401</v>
       </c>
-      <c r="G118" s="29"/>
+      <c r="G118" s="31"/>
     </row>
     <row r="119" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A119" s="14" t="s">
@@ -9313,7 +9377,7 @@
       <c r="F119" s="3" t="s">
         <v>401</v>
       </c>
-      <c r="G119" s="29"/>
+      <c r="G119" s="31"/>
     </row>
     <row r="120" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A120" s="14" t="s">
@@ -9334,7 +9398,7 @@
       <c r="F120" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="G120" s="29"/>
+      <c r="G120" s="31"/>
     </row>
     <row r="121" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A121" s="14" t="s">
@@ -9355,7 +9419,7 @@
       <c r="F121" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="G121" s="29"/>
+      <c r="G121" s="31"/>
     </row>
     <row r="122" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A122" s="15" t="s">
@@ -9376,7 +9440,7 @@
       <c r="F122" s="12" t="s">
         <v>345</v>
       </c>
-      <c r="G122" s="29"/>
+      <c r="G122" s="31"/>
     </row>
     <row r="123" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A123" s="14" t="s">
@@ -9397,7 +9461,7 @@
       <c r="F123" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="G123" s="29" t="s">
+      <c r="G123" s="31" t="s">
         <v>403</v>
       </c>
     </row>
@@ -9420,7 +9484,7 @@
       <c r="F124" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="G124" s="29"/>
+      <c r="G124" s="31"/>
     </row>
     <row r="125" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A125" s="14" t="s">
@@ -9441,7 +9505,7 @@
       <c r="F125" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="G125" s="29"/>
+      <c r="G125" s="31"/>
     </row>
     <row r="126" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A126" s="14" t="s">
@@ -9462,7 +9526,7 @@
       <c r="F126" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="G126" s="29"/>
+      <c r="G126" s="31"/>
     </row>
     <row r="127" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A127" s="14" t="s">
@@ -9483,7 +9547,7 @@
       <c r="F127" s="3" t="s">
         <v>347</v>
       </c>
-      <c r="G127" s="29"/>
+      <c r="G127" s="31"/>
     </row>
     <row r="128" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A128" s="14" t="s">
@@ -9504,7 +9568,7 @@
       <c r="F128" s="3" t="s">
         <v>350</v>
       </c>
-      <c r="G128" s="29"/>
+      <c r="G128" s="31"/>
     </row>
     <row r="129" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A129" s="15" t="s">
@@ -9525,7 +9589,7 @@
       <c r="F129" s="12" t="s">
         <v>352</v>
       </c>
-      <c r="G129" s="29"/>
+      <c r="G129" s="31"/>
     </row>
     <row r="130" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A130" s="14" t="s">
@@ -9546,7 +9610,7 @@
       <c r="F130" s="3" t="s">
         <v>354</v>
       </c>
-      <c r="G130" s="30" t="s">
+      <c r="G130" s="32" t="s">
         <v>411</v>
       </c>
     </row>
@@ -9569,7 +9633,7 @@
       <c r="F131" s="12" t="s">
         <v>356</v>
       </c>
-      <c r="G131" s="30"/>
+      <c r="G131" s="32"/>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132" s="14" t="s">
@@ -9772,7 +9836,49 @@
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A142" s="14" t="s">
+        <v>428</v>
+      </c>
+      <c r="B142" t="s">
+        <v>430</v>
+      </c>
       <c r="C142" s="2"/>
+    </row>
+    <row r="143" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A143" s="15" t="s">
+        <v>429</v>
+      </c>
+      <c r="B143" s="9" t="s">
+        <v>430</v>
+      </c>
+      <c r="C143" s="9"/>
+      <c r="D143" s="9"/>
+      <c r="E143" s="9"/>
+      <c r="F143" s="9"/>
+      <c r="G143" s="9"/>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A144" s="14" t="s">
+        <v>434</v>
+      </c>
+      <c r="B144" s="14" t="s">
+        <v>431</v>
+      </c>
+      <c r="C144" s="2">
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="D144" t="s">
+        <v>432</v>
+      </c>
+      <c r="E144" s="6">
+        <v>1608</v>
+      </c>
+      <c r="F144" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="G144" t="s">
+        <v>435</v>
+      </c>
     </row>
     <row r="147" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E147" t="s">
@@ -9781,6 +9887,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="G109:G115"/>
+    <mergeCell ref="G116:G122"/>
+    <mergeCell ref="G123:G129"/>
+    <mergeCell ref="G130:G131"/>
+    <mergeCell ref="G97:G102"/>
+    <mergeCell ref="G103:G108"/>
     <mergeCell ref="G91:G96"/>
     <mergeCell ref="G2:G10"/>
     <mergeCell ref="G11:G20"/>
@@ -9793,12 +9905,6 @@
     <mergeCell ref="G73:G78"/>
     <mergeCell ref="G79:G84"/>
     <mergeCell ref="G85:G90"/>
-    <mergeCell ref="G109:G115"/>
-    <mergeCell ref="G116:G122"/>
-    <mergeCell ref="G123:G129"/>
-    <mergeCell ref="G130:G131"/>
-    <mergeCell ref="G97:G102"/>
-    <mergeCell ref="G103:G108"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -9904,9 +10010,10 @@
     <hyperlink ref="D139" r:id="rId100" xr:uid="{2B4A96D9-73B2-4284-9F00-05D1DF0F219B}"/>
     <hyperlink ref="F140" r:id="rId101" display="https://www.mouser.ca/datasheet/2/212/KEM_C1023_X7R_AUTO_SMD-1093309.pdf" xr:uid="{EF096566-3DC3-4D51-A03D-30B625A0CE18}"/>
     <hyperlink ref="F141" r:id="rId102" display="https://www.mouser.ca/datasheet/2/212/KEM_C1023_X7R_AUTO_SMD-1093309.pdf" xr:uid="{CCB90840-C615-48E9-A50C-D72AE500BCAC}"/>
+    <hyperlink ref="F144" r:id="rId103" display="https://fscdn.rohm.com/en/products/databook/datasheet/passive/resistor/chip_resistor/sdr-e.pdf" xr:uid="{33C7962E-E358-4301-8B9C-6188F4CE89A3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId103"/>
+  <pageSetup orientation="portrait" r:id="rId104"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Both parts ar PVT09A 5K ohms, corrected footprint terminal labels
</commit_message>
<xml_diff>
--- a/Documents/BOM.xlsx
+++ b/Documents/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ECE_Projects\Music_Visualizer\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F350AF6-C531-42E8-A127-2A7DFC1D8C3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7AB034D-9BF0-4FEB-BCC6-80173250007A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="824" activeTab="11" xr2:uid="{1F4A7036-4694-4970-BB5D-7CBECC831452}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="824" activeTab="14" xr2:uid="{1F4A7036-4694-4970-BB5D-7CBECC831452}"/>
   </bookViews>
   <sheets>
     <sheet name="Sub-Bass" sheetId="1" r:id="rId1"/>
@@ -1510,12 +1510,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1527,6 +1521,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2923,8 +2923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C595792-1ED3-4550-B2C6-F49A784AB9C0}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R7" sqref="R7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3268,7 +3268,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3494,8 +3494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{422FDBAB-416A-4921-A7D0-3405100F2A2C}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6888,7 +6888,7 @@
       <c r="F2" t="s">
         <v>88</v>
       </c>
-      <c r="G2" s="28" t="s">
+      <c r="G2" s="32" t="s">
         <v>367</v>
       </c>
     </row>
@@ -6911,7 +6911,7 @@
       <c r="F3" t="s">
         <v>88</v>
       </c>
-      <c r="G3" s="28"/>
+      <c r="G3" s="32"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -6932,7 +6932,7 @@
       <c r="F4" t="s">
         <v>88</v>
       </c>
-      <c r="G4" s="28"/>
+      <c r="G4" s="32"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -6953,7 +6953,7 @@
       <c r="F5" t="s">
         <v>90</v>
       </c>
-      <c r="G5" s="28"/>
+      <c r="G5" s="32"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -6974,7 +6974,7 @@
       <c r="F6" t="s">
         <v>88</v>
       </c>
-      <c r="G6" s="28"/>
+      <c r="G6" s="32"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -6995,7 +6995,7 @@
       <c r="F7" t="s">
         <v>88</v>
       </c>
-      <c r="G7" s="28"/>
+      <c r="G7" s="32"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -7016,7 +7016,7 @@
       <c r="F8" t="s">
         <v>91</v>
       </c>
-      <c r="G8" s="28"/>
+      <c r="G8" s="32"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -7037,7 +7037,7 @@
       <c r="F9" t="s">
         <v>91</v>
       </c>
-      <c r="G9" s="28"/>
+      <c r="G9" s="32"/>
     </row>
     <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
@@ -7058,7 +7058,7 @@
       <c r="F10" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="G10" s="28"/>
+      <c r="G10" s="32"/>
     </row>
     <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
@@ -7079,7 +7079,7 @@
       <c r="F11" t="s">
         <v>88</v>
       </c>
-      <c r="G11" s="27" t="s">
+      <c r="G11" s="31" t="s">
         <v>368</v>
       </c>
     </row>
@@ -7102,7 +7102,7 @@
       <c r="F12" t="s">
         <v>90</v>
       </c>
-      <c r="G12" s="27"/>
+      <c r="G12" s="31"/>
     </row>
     <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -7123,7 +7123,7 @@
       <c r="F13" t="s">
         <v>88</v>
       </c>
-      <c r="G13" s="27"/>
+      <c r="G13" s="31"/>
     </row>
     <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
@@ -7144,7 +7144,7 @@
       <c r="F14" t="s">
         <v>88</v>
       </c>
-      <c r="G14" s="27"/>
+      <c r="G14" s="31"/>
     </row>
     <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
@@ -7165,7 +7165,7 @@
       <c r="F15" t="s">
         <v>88</v>
       </c>
-      <c r="G15" s="27"/>
+      <c r="G15" s="31"/>
     </row>
     <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
@@ -7186,7 +7186,7 @@
       <c r="F16" t="s">
         <v>88</v>
       </c>
-      <c r="G16" s="27"/>
+      <c r="G16" s="31"/>
     </row>
     <row r="17" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
@@ -7207,7 +7207,7 @@
       <c r="F17" t="s">
         <v>88</v>
       </c>
-      <c r="G17" s="27"/>
+      <c r="G17" s="31"/>
     </row>
     <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
@@ -7228,7 +7228,7 @@
       <c r="F18" t="s">
         <v>96</v>
       </c>
-      <c r="G18" s="27"/>
+      <c r="G18" s="31"/>
     </row>
     <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
@@ -7249,7 +7249,7 @@
       <c r="F19" t="s">
         <v>88</v>
       </c>
-      <c r="G19" s="27"/>
+      <c r="G19" s="31"/>
     </row>
     <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
@@ -7270,7 +7270,7 @@
       <c r="F20" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="G20" s="27"/>
+      <c r="G20" s="31"/>
     </row>
     <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
@@ -7291,7 +7291,7 @@
       <c r="F21" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="G21" s="27" t="s">
+      <c r="G21" s="31" t="s">
         <v>369</v>
       </c>
     </row>
@@ -7314,7 +7314,7 @@
       <c r="F22" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G22" s="27"/>
+      <c r="G22" s="31"/>
     </row>
     <row r="23" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
@@ -7335,7 +7335,7 @@
       <c r="F23" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="G23" s="27"/>
+      <c r="G23" s="31"/>
     </row>
     <row r="24" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
@@ -7356,7 +7356,7 @@
       <c r="F24" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="G24" s="27"/>
+      <c r="G24" s="31"/>
     </row>
     <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
@@ -7377,7 +7377,7 @@
       <c r="F25" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="G25" s="27"/>
+      <c r="G25" s="31"/>
     </row>
     <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
@@ -7398,7 +7398,7 @@
       <c r="F26" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="G26" s="27"/>
+      <c r="G26" s="31"/>
     </row>
     <row r="27" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
@@ -7419,7 +7419,7 @@
       <c r="F27" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="G27" s="27"/>
+      <c r="G27" s="31"/>
     </row>
     <row r="28" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
@@ -7440,7 +7440,7 @@
       <c r="F28" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="G28" s="27"/>
+      <c r="G28" s="31"/>
     </row>
     <row r="29" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="9" t="s">
@@ -7461,7 +7461,7 @@
       <c r="F29" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="G29" s="27"/>
+      <c r="G29" s="31"/>
     </row>
     <row r="30" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
@@ -7482,7 +7482,7 @@
       <c r="F30" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="G30" s="27" t="s">
+      <c r="G30" s="31" t="s">
         <v>370</v>
       </c>
     </row>
@@ -7505,7 +7505,7 @@
       <c r="F31" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="G31" s="27"/>
+      <c r="G31" s="31"/>
     </row>
     <row r="32" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
@@ -7526,7 +7526,7 @@
       <c r="F32" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="G32" s="27"/>
+      <c r="G32" s="31"/>
     </row>
     <row r="33" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
@@ -7547,7 +7547,7 @@
       <c r="F33" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="G33" s="27"/>
+      <c r="G33" s="31"/>
     </row>
     <row r="34" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
@@ -7568,7 +7568,7 @@
       <c r="F34" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="G34" s="27"/>
+      <c r="G34" s="31"/>
     </row>
     <row r="35" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
@@ -7589,7 +7589,7 @@
       <c r="F35" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="G35" s="27"/>
+      <c r="G35" s="31"/>
     </row>
     <row r="36" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
@@ -7610,7 +7610,7 @@
       <c r="F36" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="G36" s="27"/>
+      <c r="G36" s="31"/>
     </row>
     <row r="37" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
@@ -7631,7 +7631,7 @@
       <c r="F37" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="G37" s="27"/>
+      <c r="G37" s="31"/>
     </row>
     <row r="38" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
@@ -7652,7 +7652,7 @@
       <c r="F38" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="G38" s="27"/>
+      <c r="G38" s="31"/>
     </row>
     <row r="39" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="9" t="s">
@@ -7673,7 +7673,7 @@
       <c r="F39" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="G39" s="27"/>
+      <c r="G39" s="31"/>
     </row>
     <row r="40" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
@@ -7694,7 +7694,7 @@
       <c r="F40" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="G40" s="27" t="s">
+      <c r="G40" s="31" t="s">
         <v>371</v>
       </c>
     </row>
@@ -7717,7 +7717,7 @@
       <c r="F41" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="G41" s="27"/>
+      <c r="G41" s="31"/>
     </row>
     <row r="42" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
@@ -7738,7 +7738,7 @@
       <c r="F42" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="G42" s="27"/>
+      <c r="G42" s="31"/>
     </row>
     <row r="43" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
@@ -7759,7 +7759,7 @@
       <c r="F43" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="G43" s="27"/>
+      <c r="G43" s="31"/>
     </row>
     <row r="44" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
@@ -7780,7 +7780,7 @@
       <c r="F44" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="G44" s="27"/>
+      <c r="G44" s="31"/>
     </row>
     <row r="45" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
@@ -7801,7 +7801,7 @@
       <c r="F45" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="G45" s="27"/>
+      <c r="G45" s="31"/>
     </row>
     <row r="46" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
@@ -7822,7 +7822,7 @@
       <c r="F46" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="G46" s="27"/>
+      <c r="G46" s="31"/>
     </row>
     <row r="47" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
@@ -7843,7 +7843,7 @@
       <c r="F47" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="G47" s="27"/>
+      <c r="G47" s="31"/>
     </row>
     <row r="48" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="9" t="s">
@@ -7864,7 +7864,7 @@
       <c r="F48" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="G48" s="27"/>
+      <c r="G48" s="31"/>
     </row>
     <row r="49" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
@@ -7885,7 +7885,7 @@
       <c r="F49" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="G49" s="27" t="s">
+      <c r="G49" s="31" t="s">
         <v>372</v>
       </c>
     </row>
@@ -7908,7 +7908,7 @@
       <c r="F50" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="G50" s="27"/>
+      <c r="G50" s="31"/>
     </row>
     <row r="51" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
@@ -7929,7 +7929,7 @@
       <c r="F51" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="G51" s="27"/>
+      <c r="G51" s="31"/>
     </row>
     <row r="52" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
@@ -7950,7 +7950,7 @@
       <c r="F52" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="G52" s="27"/>
+      <c r="G52" s="31"/>
     </row>
     <row r="53" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
@@ -7971,7 +7971,7 @@
       <c r="F53" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="G53" s="27"/>
+      <c r="G53" s="31"/>
     </row>
     <row r="54" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
@@ -7992,7 +7992,7 @@
       <c r="F54" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="G54" s="27"/>
+      <c r="G54" s="31"/>
     </row>
     <row r="55" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
@@ -8013,7 +8013,7 @@
       <c r="F55" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="G55" s="27"/>
+      <c r="G55" s="31"/>
     </row>
     <row r="56" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
@@ -8034,7 +8034,7 @@
       <c r="F56" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="G56" s="27"/>
+      <c r="G56" s="31"/>
     </row>
     <row r="57" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="9" t="s">
@@ -8055,7 +8055,7 @@
       <c r="F57" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="G57" s="27"/>
+      <c r="G57" s="31"/>
     </row>
     <row r="58" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
@@ -8076,7 +8076,7 @@
       <c r="F58" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="G58" s="27" t="s">
+      <c r="G58" s="31" t="s">
         <v>373</v>
       </c>
     </row>
@@ -8099,7 +8099,7 @@
       <c r="F59" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="G59" s="27"/>
+      <c r="G59" s="31"/>
     </row>
     <row r="60" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
@@ -8120,7 +8120,7 @@
       <c r="F60" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="G60" s="27"/>
+      <c r="G60" s="31"/>
     </row>
     <row r="61" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
@@ -8141,7 +8141,7 @@
       <c r="F61" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="G61" s="27"/>
+      <c r="G61" s="31"/>
     </row>
     <row r="62" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
@@ -8162,7 +8162,7 @@
       <c r="F62" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="G62" s="27"/>
+      <c r="G62" s="31"/>
     </row>
     <row r="63" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
@@ -8183,7 +8183,7 @@
       <c r="F63" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="G63" s="27"/>
+      <c r="G63" s="31"/>
     </row>
     <row r="64" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
@@ -8204,7 +8204,7 @@
       <c r="F64" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="G64" s="27"/>
+      <c r="G64" s="31"/>
     </row>
     <row r="65" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
@@ -8225,7 +8225,7 @@
       <c r="F65" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="G65" s="27"/>
+      <c r="G65" s="31"/>
     </row>
     <row r="66" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="9" t="s">
@@ -8246,7 +8246,7 @@
       <c r="F66" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="G66" s="27"/>
+      <c r="G66" s="31"/>
     </row>
     <row r="67" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
@@ -8267,7 +8267,7 @@
       <c r="F67" t="s">
         <v>93</v>
       </c>
-      <c r="G67" s="27" t="s">
+      <c r="G67" s="31" t="s">
         <v>367</v>
       </c>
     </row>
@@ -8290,7 +8290,7 @@
       <c r="F68" t="s">
         <v>93</v>
       </c>
-      <c r="G68" s="27"/>
+      <c r="G68" s="31"/>
     </row>
     <row r="69" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
@@ -8311,7 +8311,7 @@
       <c r="F69" t="s">
         <v>94</v>
       </c>
-      <c r="G69" s="27"/>
+      <c r="G69" s="31"/>
     </row>
     <row r="70" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
@@ -8332,7 +8332,7 @@
       <c r="F70" t="s">
         <v>94</v>
       </c>
-      <c r="G70" s="27"/>
+      <c r="G70" s="31"/>
     </row>
     <row r="71" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
@@ -8353,7 +8353,7 @@
       <c r="F71" t="s">
         <v>95</v>
       </c>
-      <c r="G71" s="27"/>
+      <c r="G71" s="31"/>
     </row>
     <row r="72" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="9" t="s">
@@ -8374,7 +8374,7 @@
       <c r="F72" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="G72" s="27"/>
+      <c r="G72" s="31"/>
     </row>
     <row r="73" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A73" s="14" t="s">
@@ -8395,7 +8395,7 @@
       <c r="F73" t="s">
         <v>97</v>
       </c>
-      <c r="G73" s="27" t="s">
+      <c r="G73" s="31" t="s">
         <v>368</v>
       </c>
     </row>
@@ -8418,7 +8418,7 @@
       <c r="F74" t="s">
         <v>97</v>
       </c>
-      <c r="G74" s="27"/>
+      <c r="G74" s="31"/>
     </row>
     <row r="75" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="14" t="s">
@@ -8439,7 +8439,7 @@
       <c r="F75" t="s">
         <v>98</v>
       </c>
-      <c r="G75" s="27"/>
+      <c r="G75" s="31"/>
     </row>
     <row r="76" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A76" s="14" t="s">
@@ -8460,7 +8460,7 @@
       <c r="F76" t="s">
         <v>98</v>
       </c>
-      <c r="G76" s="27"/>
+      <c r="G76" s="31"/>
     </row>
     <row r="77" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A77" s="14" t="s">
@@ -8481,7 +8481,7 @@
       <c r="F77" t="s">
         <v>100</v>
       </c>
-      <c r="G77" s="27"/>
+      <c r="G77" s="31"/>
     </row>
     <row r="78" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="15" t="s">
@@ -8502,7 +8502,7 @@
       <c r="F78" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="G78" s="27"/>
+      <c r="G78" s="31"/>
     </row>
     <row r="79" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A79" s="14" t="s">
@@ -8523,7 +8523,7 @@
       <c r="F79" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="G79" s="27" t="s">
+      <c r="G79" s="31" t="s">
         <v>369</v>
       </c>
     </row>
@@ -8546,7 +8546,7 @@
       <c r="F80" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="G80" s="27"/>
+      <c r="G80" s="31"/>
     </row>
     <row r="81" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A81" s="14" t="s">
@@ -8567,7 +8567,7 @@
       <c r="F81" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="G81" s="27"/>
+      <c r="G81" s="31"/>
     </row>
     <row r="82" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A82" s="14" t="s">
@@ -8588,7 +8588,7 @@
       <c r="F82" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="G82" s="27"/>
+      <c r="G82" s="31"/>
     </row>
     <row r="83" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A83" s="14" t="s">
@@ -8609,7 +8609,7 @@
       <c r="F83" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="G83" s="27"/>
+      <c r="G83" s="31"/>
     </row>
     <row r="84" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A84" s="15" t="s">
@@ -8630,7 +8630,7 @@
       <c r="F84" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="G84" s="27"/>
+      <c r="G84" s="31"/>
     </row>
     <row r="85" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A85" s="14" t="s">
@@ -8651,7 +8651,7 @@
       <c r="F85" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="G85" s="27" t="s">
+      <c r="G85" s="31" t="s">
         <v>370</v>
       </c>
     </row>
@@ -8674,7 +8674,7 @@
       <c r="F86" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="G86" s="27"/>
+      <c r="G86" s="31"/>
     </row>
     <row r="87" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A87" s="14" t="s">
@@ -8695,7 +8695,7 @@
       <c r="F87" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G87" s="27"/>
+      <c r="G87" s="31"/>
     </row>
     <row r="88" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A88" s="14" t="s">
@@ -8716,7 +8716,7 @@
       <c r="F88" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G88" s="27"/>
+      <c r="G88" s="31"/>
     </row>
     <row r="89" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A89" s="14" t="s">
@@ -8737,7 +8737,7 @@
       <c r="F89" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="G89" s="27"/>
+      <c r="G89" s="31"/>
     </row>
     <row r="90" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A90" s="15" t="s">
@@ -8758,7 +8758,7 @@
       <c r="F90" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="G90" s="27"/>
+      <c r="G90" s="31"/>
     </row>
     <row r="91" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A91" s="14" t="s">
@@ -8779,7 +8779,7 @@
       <c r="F91" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G91" s="27" t="s">
+      <c r="G91" s="31" t="s">
         <v>371</v>
       </c>
     </row>
@@ -8802,7 +8802,7 @@
       <c r="F92" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G92" s="27"/>
+      <c r="G92" s="31"/>
     </row>
     <row r="93" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A93" s="14" t="s">
@@ -8823,7 +8823,7 @@
       <c r="F93" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G93" s="27"/>
+      <c r="G93" s="31"/>
     </row>
     <row r="94" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A94" s="14" t="s">
@@ -8844,7 +8844,7 @@
       <c r="F94" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G94" s="27"/>
+      <c r="G94" s="31"/>
     </row>
     <row r="95" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A95" s="14" t="s">
@@ -8865,7 +8865,7 @@
       <c r="F95" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G95" s="27"/>
+      <c r="G95" s="31"/>
     </row>
     <row r="96" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A96" s="15" t="s">
@@ -8886,7 +8886,7 @@
       <c r="F96" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="G96" s="27"/>
+      <c r="G96" s="31"/>
     </row>
     <row r="97" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A97" s="20" t="s">
@@ -8907,7 +8907,7 @@
       <c r="F97" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="G97" s="27" t="s">
+      <c r="G97" s="31" t="s">
         <v>372</v>
       </c>
     </row>
@@ -8930,7 +8930,7 @@
       <c r="F98" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="G98" s="27"/>
+      <c r="G98" s="31"/>
     </row>
     <row r="99" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A99" s="14" t="s">
@@ -8951,7 +8951,7 @@
       <c r="F99" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="G99" s="27"/>
+      <c r="G99" s="31"/>
     </row>
     <row r="100" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A100" s="14" t="s">
@@ -8972,7 +8972,7 @@
       <c r="F100" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="G100" s="27"/>
+      <c r="G100" s="31"/>
     </row>
     <row r="101" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A101" s="14" t="s">
@@ -8993,7 +8993,7 @@
       <c r="F101" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="G101" s="27"/>
+      <c r="G101" s="31"/>
     </row>
     <row r="102" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A102" s="15" t="s">
@@ -9014,7 +9014,7 @@
       <c r="F102" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="G102" s="27"/>
+      <c r="G102" s="31"/>
     </row>
     <row r="103" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A103" s="14" t="s">
@@ -9035,7 +9035,7 @@
       <c r="F103" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G103" s="27" t="s">
+      <c r="G103" s="31" t="s">
         <v>373</v>
       </c>
     </row>
@@ -9058,7 +9058,7 @@
       <c r="F104" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G104" s="27"/>
+      <c r="G104" s="31"/>
     </row>
     <row r="105" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A105" s="14" t="s">
@@ -9079,7 +9079,7 @@
       <c r="F105" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G105" s="27"/>
+      <c r="G105" s="31"/>
     </row>
     <row r="106" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A106" s="14" t="s">
@@ -9100,7 +9100,7 @@
       <c r="F106" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G106" s="27"/>
+      <c r="G106" s="31"/>
     </row>
     <row r="107" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A107" s="14" t="s">
@@ -9121,7 +9121,7 @@
       <c r="F107" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G107" s="27"/>
+      <c r="G107" s="31"/>
     </row>
     <row r="108" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A108" s="15" t="s">
@@ -9142,7 +9142,7 @@
       <c r="F108" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="G108" s="27"/>
+      <c r="G108" s="31"/>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109" s="14" t="s">
@@ -9163,7 +9163,7 @@
       <c r="F109" s="3" t="s">
         <v>382</v>
       </c>
-      <c r="G109" s="29" t="s">
+      <c r="G109" s="27" t="s">
         <v>383</v>
       </c>
     </row>
@@ -9186,7 +9186,7 @@
       <c r="F110" s="3" t="s">
         <v>382</v>
       </c>
-      <c r="G110" s="30"/>
+      <c r="G110" s="28"/>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111" s="14" t="s">
@@ -9207,7 +9207,7 @@
       <c r="F111" s="3" t="s">
         <v>382</v>
       </c>
-      <c r="G111" s="30"/>
+      <c r="G111" s="28"/>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112" s="14" t="s">
@@ -9228,7 +9228,7 @@
       <c r="F112" s="3" t="s">
         <v>382</v>
       </c>
-      <c r="G112" s="30"/>
+      <c r="G112" s="28"/>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113" s="14" t="s">
@@ -9249,7 +9249,7 @@
       <c r="F113" s="3" t="s">
         <v>382</v>
       </c>
-      <c r="G113" s="30"/>
+      <c r="G113" s="28"/>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114" s="14" t="s">
@@ -9270,7 +9270,7 @@
       <c r="F114" s="3" t="s">
         <v>382</v>
       </c>
-      <c r="G114" s="30"/>
+      <c r="G114" s="28"/>
     </row>
     <row r="115" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A115" s="15" t="s">
@@ -9291,7 +9291,7 @@
       <c r="F115" s="12" t="s">
         <v>382</v>
       </c>
-      <c r="G115" s="30"/>
+      <c r="G115" s="28"/>
     </row>
     <row r="116" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A116" s="14" t="s">
@@ -9312,7 +9312,7 @@
       <c r="F116" s="3" t="s">
         <v>398</v>
       </c>
-      <c r="G116" s="31" t="s">
+      <c r="G116" s="29" t="s">
         <v>399</v>
       </c>
     </row>
@@ -9335,7 +9335,7 @@
       <c r="F117" s="3" t="s">
         <v>398</v>
       </c>
-      <c r="G117" s="31"/>
+      <c r="G117" s="29"/>
     </row>
     <row r="118" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A118" s="14" t="s">
@@ -9356,7 +9356,7 @@
       <c r="F118" s="3" t="s">
         <v>401</v>
       </c>
-      <c r="G118" s="31"/>
+      <c r="G118" s="29"/>
     </row>
     <row r="119" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A119" s="14" t="s">
@@ -9377,7 +9377,7 @@
       <c r="F119" s="3" t="s">
         <v>401</v>
       </c>
-      <c r="G119" s="31"/>
+      <c r="G119" s="29"/>
     </row>
     <row r="120" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A120" s="14" t="s">
@@ -9398,7 +9398,7 @@
       <c r="F120" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="G120" s="31"/>
+      <c r="G120" s="29"/>
     </row>
     <row r="121" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A121" s="14" t="s">
@@ -9419,7 +9419,7 @@
       <c r="F121" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="G121" s="31"/>
+      <c r="G121" s="29"/>
     </row>
     <row r="122" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A122" s="15" t="s">
@@ -9440,7 +9440,7 @@
       <c r="F122" s="12" t="s">
         <v>345</v>
       </c>
-      <c r="G122" s="31"/>
+      <c r="G122" s="29"/>
     </row>
     <row r="123" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A123" s="14" t="s">
@@ -9461,7 +9461,7 @@
       <c r="F123" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="G123" s="31" t="s">
+      <c r="G123" s="29" t="s">
         <v>403</v>
       </c>
     </row>
@@ -9484,7 +9484,7 @@
       <c r="F124" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="G124" s="31"/>
+      <c r="G124" s="29"/>
     </row>
     <row r="125" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A125" s="14" t="s">
@@ -9505,7 +9505,7 @@
       <c r="F125" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="G125" s="31"/>
+      <c r="G125" s="29"/>
     </row>
     <row r="126" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A126" s="14" t="s">
@@ -9526,7 +9526,7 @@
       <c r="F126" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="G126" s="31"/>
+      <c r="G126" s="29"/>
     </row>
     <row r="127" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A127" s="14" t="s">
@@ -9547,7 +9547,7 @@
       <c r="F127" s="3" t="s">
         <v>347</v>
       </c>
-      <c r="G127" s="31"/>
+      <c r="G127" s="29"/>
     </row>
     <row r="128" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A128" s="14" t="s">
@@ -9568,7 +9568,7 @@
       <c r="F128" s="3" t="s">
         <v>350</v>
       </c>
-      <c r="G128" s="31"/>
+      <c r="G128" s="29"/>
     </row>
     <row r="129" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A129" s="15" t="s">
@@ -9589,7 +9589,7 @@
       <c r="F129" s="12" t="s">
         <v>352</v>
       </c>
-      <c r="G129" s="31"/>
+      <c r="G129" s="29"/>
     </row>
     <row r="130" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A130" s="14" t="s">
@@ -9610,7 +9610,7 @@
       <c r="F130" s="3" t="s">
         <v>354</v>
       </c>
-      <c r="G130" s="32" t="s">
+      <c r="G130" s="30" t="s">
         <v>411</v>
       </c>
     </row>
@@ -9633,7 +9633,7 @@
       <c r="F131" s="12" t="s">
         <v>356</v>
       </c>
-      <c r="G131" s="32"/>
+      <c r="G131" s="30"/>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132" s="14" t="s">
@@ -9887,12 +9887,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="G109:G115"/>
-    <mergeCell ref="G116:G122"/>
-    <mergeCell ref="G123:G129"/>
-    <mergeCell ref="G130:G131"/>
-    <mergeCell ref="G97:G102"/>
-    <mergeCell ref="G103:G108"/>
     <mergeCell ref="G91:G96"/>
     <mergeCell ref="G2:G10"/>
     <mergeCell ref="G11:G20"/>
@@ -9905,6 +9899,12 @@
     <mergeCell ref="G73:G78"/>
     <mergeCell ref="G79:G84"/>
     <mergeCell ref="G85:G90"/>
+    <mergeCell ref="G109:G115"/>
+    <mergeCell ref="G116:G122"/>
+    <mergeCell ref="G123:G129"/>
+    <mergeCell ref="G130:G131"/>
+    <mergeCell ref="G97:G102"/>
+    <mergeCell ref="G103:G108"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Added 10 uF polarized smoothing capacitors to LED driver ciruit
</commit_message>
<xml_diff>
--- a/Documents/BOM.xlsx
+++ b/Documents/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ECE_Projects\Music_Visualizer\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7AB034D-9BF0-4FEB-BCC6-80173250007A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC2D811-B549-41CA-8E25-5FF0C551CD3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="824" activeTab="14" xr2:uid="{1F4A7036-4694-4970-BB5D-7CBECC831452}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="824" activeTab="7" xr2:uid="{1F4A7036-4694-4970-BB5D-7CBECC831452}"/>
   </bookViews>
   <sheets>
     <sheet name="Sub-Bass" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1467" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1533" uniqueCount="447">
   <si>
     <t>Component</t>
   </si>
@@ -987,9 +987,6 @@
     <t>https://cdn-shop.adafruit.com/datasheets/WP7113SRD-D.pdf</t>
   </si>
   <si>
-    <t>220u</t>
-  </si>
-  <si>
     <t>680ohm</t>
   </si>
   <si>
@@ -1332,9 +1329,6 @@
     <t>M20-9990246 Datasheet (PDF)</t>
   </si>
   <si>
-    <t xml:space="preserve">  </t>
-  </si>
-  <si>
     <t>Rv1</t>
   </si>
   <si>
@@ -1369,6 +1363,33 @@
   </si>
   <si>
     <t>RR511D1121 Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Wurth-Elektronik/860010372001?qs=sGAEpiMZZMvwFf0viD3Y3aZipiehufnXEJE5VXphUV5UaXXfxNlTNw%3D%3D</t>
+  </si>
+  <si>
+    <t> 860010372001 Datasheet (PDF)</t>
+  </si>
+  <si>
+    <t>C60</t>
+  </si>
+  <si>
+    <t>C61</t>
+  </si>
+  <si>
+    <t>C62</t>
+  </si>
+  <si>
+    <t>C63</t>
+  </si>
+  <si>
+    <t>C64</t>
+  </si>
+  <si>
+    <t>C65</t>
+  </si>
+  <si>
+    <t>Passives For LED Driver Circuit</t>
   </si>
 </sst>
 </file>
@@ -1468,7 +1489,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1510,6 +1531,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1522,11 +1549,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2354,122 +2378,122 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="B2" t="s">
         <v>331</v>
-      </c>
-      <c r="B2" t="s">
-        <v>332</v>
       </c>
       <c r="C2">
         <v>0.75900000000000001</v>
       </c>
       <c r="D2" t="s">
+        <v>332</v>
+      </c>
+      <c r="E2" t="s">
         <v>333</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="3" t="s">
         <v>334</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="B3" t="s">
         <v>331</v>
-      </c>
-      <c r="B3" t="s">
-        <v>332</v>
       </c>
       <c r="C3">
         <v>0.75900000000000001</v>
       </c>
       <c r="D3" t="s">
+        <v>332</v>
+      </c>
+      <c r="E3" t="s">
         <v>333</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" s="3" t="s">
         <v>334</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="B4" t="s">
         <v>331</v>
-      </c>
-      <c r="B4" t="s">
-        <v>332</v>
       </c>
       <c r="C4">
         <v>0.75900000000000001</v>
       </c>
       <c r="D4" t="s">
+        <v>332</v>
+      </c>
+      <c r="E4" t="s">
         <v>333</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" s="3" t="s">
         <v>334</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="B5" t="s">
         <v>331</v>
-      </c>
-      <c r="B5" t="s">
-        <v>332</v>
       </c>
       <c r="C5">
         <v>0.75900000000000001</v>
       </c>
       <c r="D5" t="s">
+        <v>332</v>
+      </c>
+      <c r="E5" t="s">
         <v>333</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" s="3" t="s">
         <v>334</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="B6" t="s">
         <v>331</v>
-      </c>
-      <c r="B6" t="s">
-        <v>332</v>
       </c>
       <c r="C6">
         <v>0.75900000000000001</v>
       </c>
       <c r="D6" t="s">
+        <v>332</v>
+      </c>
+      <c r="E6" t="s">
         <v>333</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" s="3" t="s">
         <v>334</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="B7" t="s">
         <v>331</v>
-      </c>
-      <c r="B7" t="s">
-        <v>332</v>
       </c>
       <c r="C7">
         <v>0.75900000000000001</v>
       </c>
       <c r="D7" t="s">
+        <v>332</v>
+      </c>
+      <c r="E7" t="s">
         <v>333</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" s="3" t="s">
         <v>334</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>335</v>
       </c>
     </row>
   </sheetData>
@@ -2879,7 +2903,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C20">
         <f>SUM(C9:C19)</f>
@@ -2888,7 +2912,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C21">
         <f>SUM(C9:C19)+C4+C5+C6</f>
@@ -2975,10 +2999,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B3" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C3">
         <v>0.69</v>
@@ -2987,7 +3011,7 @@
         <v>246</v>
       </c>
       <c r="E3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>249</v>
@@ -2995,22 +3019,22 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C4">
         <v>3.81</v>
       </c>
       <c r="D4" t="s">
+        <v>356</v>
+      </c>
+      <c r="E4" t="s">
+        <v>348</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>357</v>
-      </c>
-      <c r="E4" t="s">
-        <v>349</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -3058,19 +3082,19 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C7">
         <v>0.11</v>
       </c>
       <c r="D7" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E7">
         <v>1005</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -3078,19 +3102,19 @@
         <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C8">
         <v>0.11</v>
       </c>
       <c r="D8" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E8">
         <v>1005</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -3098,19 +3122,19 @@
         <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C9">
         <v>0.13800000000000001</v>
       </c>
       <c r="D9" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E9">
         <v>2012</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -3118,19 +3142,19 @@
         <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C10">
         <v>0.152</v>
       </c>
       <c r="D10" t="s">
+        <v>347</v>
+      </c>
+      <c r="E10" t="s">
         <v>348</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" s="3" t="s">
         <v>349</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -3138,19 +3162,19 @@
         <v>203</v>
       </c>
       <c r="B11" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C11">
         <v>0.13800000000000001</v>
       </c>
       <c r="D11" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E11">
         <v>1005</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -3158,19 +3182,19 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C12">
         <v>0.13800000000000001</v>
       </c>
       <c r="D12" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E12">
         <v>1608</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -3178,56 +3202,56 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C13">
         <v>0.13800000000000001</v>
       </c>
       <c r="D13" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E13">
         <v>1608</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C14" s="2">
         <v>0.30399999999999999</v>
       </c>
       <c r="D14" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="E14" s="6">
         <v>1608</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C15" s="2">
         <v>1.55</v>
       </c>
       <c r="D15" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -3430,7 +3454,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B3" t="s">
         <v>295</v>
@@ -3439,10 +3463,10 @@
         <v>1.19</v>
       </c>
       <c r="D3" t="s">
+        <v>362</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>363</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -3492,10 +3516,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{422FDBAB-416A-4921-A7D0-3405100F2A2C}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20:F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3563,19 +3587,19 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>312</v>
-      </c>
-      <c r="C4">
-        <v>0.20699999999999999</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>285</v>
-      </c>
-      <c r="E4" t="s">
-        <v>286</v>
+        <v>394</v>
+      </c>
+      <c r="C4" s="25">
+        <v>0.11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>343</v>
+      </c>
+      <c r="E4" s="6">
+        <v>1005</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>287</v>
+        <v>344</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -3583,288 +3607,408 @@
         <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C5" s="25">
         <v>0.11</v>
       </c>
       <c r="D5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E5" s="6">
         <v>1005</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>395</v>
-      </c>
-      <c r="C6" s="25">
-        <v>0.11</v>
+        <v>337</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.13800000000000001</v>
       </c>
       <c r="D6" t="s">
-        <v>344</v>
-      </c>
-      <c r="E6" s="6">
-        <v>1005</v>
+        <v>438</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>348</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>345</v>
+        <v>439</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>313</v>
-      </c>
-      <c r="C7">
+        <v>337</v>
+      </c>
+      <c r="C7" s="2">
         <v>0.13800000000000001</v>
       </c>
       <c r="D7" t="s">
-        <v>314</v>
-      </c>
-      <c r="E7">
-        <v>1608</v>
+        <v>438</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>348</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>315</v>
+        <v>439</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>2</v>
+      <c r="A8" s="14" t="s">
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>313</v>
-      </c>
-      <c r="C8">
+        <v>337</v>
+      </c>
+      <c r="C8" s="2">
         <v>0.13800000000000001</v>
       </c>
       <c r="D8" t="s">
-        <v>314</v>
-      </c>
-      <c r="E8">
-        <v>1608</v>
+        <v>438</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>348</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>315</v>
+        <v>439</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>313</v>
-      </c>
-      <c r="C9">
+        <v>337</v>
+      </c>
+      <c r="C9" s="2">
         <v>0.13800000000000001</v>
       </c>
       <c r="D9" t="s">
-        <v>314</v>
-      </c>
-      <c r="E9">
-        <v>1608</v>
+        <v>438</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>348</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>315</v>
+        <v>439</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>4</v>
+      <c r="A10" s="14" t="s">
+        <v>203</v>
       </c>
       <c r="B10" t="s">
-        <v>313</v>
-      </c>
-      <c r="C10">
+        <v>337</v>
+      </c>
+      <c r="C10" s="2">
         <v>0.13800000000000001</v>
       </c>
       <c r="D10" t="s">
-        <v>314</v>
-      </c>
-      <c r="E10">
-        <v>1608</v>
+        <v>438</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>348</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>315</v>
+        <v>439</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>204</v>
       </c>
       <c r="B11" t="s">
-        <v>313</v>
-      </c>
-      <c r="C11">
+        <v>337</v>
+      </c>
+      <c r="C11" s="2">
         <v>0.13800000000000001</v>
       </c>
       <c r="D11" t="s">
-        <v>314</v>
-      </c>
-      <c r="E11">
-        <v>1608</v>
+        <v>438</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>348</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>315</v>
+        <v>439</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>6</v>
+      <c r="A12" s="14" t="s">
+        <v>205</v>
       </c>
       <c r="B12" t="s">
-        <v>313</v>
-      </c>
-      <c r="C12">
+        <v>337</v>
+      </c>
+      <c r="C12" s="2">
         <v>0.13800000000000001</v>
       </c>
       <c r="D12" t="s">
-        <v>314</v>
-      </c>
-      <c r="E12">
-        <v>1608</v>
+        <v>438</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>348</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>315</v>
+        <v>439</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B13" t="s">
+        <v>312</v>
+      </c>
+      <c r="C13">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D13" t="s">
         <v>313</v>
-      </c>
-      <c r="C13">
-        <v>0.13800000000000001</v>
-      </c>
-      <c r="D13" t="s">
-        <v>314</v>
       </c>
       <c r="E13">
         <v>1608</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>328</v>
+        <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>329</v>
+        <v>312</v>
       </c>
       <c r="C14">
-        <v>1.38</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="D14" t="s">
-        <v>316</v>
+        <v>313</v>
+      </c>
+      <c r="E14">
+        <v>1608</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>318</v>
+        <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="C15">
-        <v>0.99399999999999999</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="D15" t="s">
-        <v>320</v>
-      </c>
-      <c r="E15" t="s">
-        <v>322</v>
+        <v>313</v>
+      </c>
+      <c r="E15">
+        <v>1608</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>323</v>
+        <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>324</v>
+        <v>312</v>
       </c>
       <c r="C16">
-        <v>0.71799999999999997</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="D16" t="s">
-        <v>325</v>
-      </c>
-      <c r="E16" t="s">
-        <v>326</v>
+        <v>313</v>
+      </c>
+      <c r="E16">
+        <v>1608</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>327</v>
+        <v>314</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>328</v>
+        <v>5</v>
       </c>
       <c r="B17" t="s">
-        <v>330</v>
+        <v>312</v>
       </c>
       <c r="C17">
-        <v>1.38</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="D17" t="s">
-        <v>316</v>
+        <v>313</v>
+      </c>
+      <c r="E17">
+        <v>1608</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" t="s">
+        <v>312</v>
+      </c>
+      <c r="C18">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D18" t="s">
+        <v>313</v>
+      </c>
+      <c r="E18">
+        <v>1608</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" t="s">
+        <v>312</v>
+      </c>
+      <c r="C19">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D19" t="s">
+        <v>313</v>
+      </c>
+      <c r="E19">
+        <v>1608</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>327</v>
+      </c>
+      <c r="B20" t="s">
+        <v>328</v>
+      </c>
+      <c r="C20">
+        <v>1.38</v>
+      </c>
+      <c r="D20" t="s">
+        <v>315</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>317</v>
+      </c>
+      <c r="B21" t="s">
+        <v>318</v>
+      </c>
+      <c r="C21">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="D21" t="s">
+        <v>319</v>
+      </c>
+      <c r="E21" t="s">
+        <v>321</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>322</v>
+      </c>
+      <c r="B22" t="s">
+        <v>323</v>
+      </c>
+      <c r="C22">
+        <v>0.71799999999999997</v>
+      </c>
+      <c r="D22" t="s">
+        <v>324</v>
+      </c>
+      <c r="E22" t="s">
+        <v>325</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>327</v>
+      </c>
+      <c r="B23" t="s">
+        <v>329</v>
+      </c>
+      <c r="C23">
+        <v>1.38</v>
+      </c>
+      <c r="D23" t="s">
+        <v>315</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>422</v>
+      </c>
+      <c r="B24" t="s">
+        <v>424</v>
+      </c>
+      <c r="C24">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="D24" t="s">
         <v>423</v>
       </c>
-      <c r="B18" t="s">
+      <c r="E24" t="s">
+        <v>348</v>
+      </c>
+      <c r="F24" s="3" t="s">
         <v>425</v>
-      </c>
-      <c r="C18">
-        <v>0.23499999999999999</v>
-      </c>
-      <c r="D18" t="s">
-        <v>424</v>
-      </c>
-      <c r="E18" t="s">
-        <v>349</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>426</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="F3" r:id="rId1" xr:uid="{4086144A-D13C-4CF7-B0A2-04DC9FD2E687}"/>
-    <hyperlink ref="F4" r:id="rId2" display="https://www.mouser.ca/datasheet/2/445/860020273009-1725581.pdf" xr:uid="{DF0F49A7-30B6-415A-AA6E-5F9F70F3E664}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{502E7D33-C429-41BF-8FAA-6D1BB65BAFC1}"/>
-    <hyperlink ref="F14" r:id="rId4" display="https://www.mouser.ca/datasheet/2/54/ptv09-777818.pdf" xr:uid="{BBF2E0E5-0197-4455-B910-736161147ECB}"/>
-    <hyperlink ref="F15" r:id="rId5" display="https://www.mouser.ca/datasheet/2/308/1/NCS333_D-2317376.pdf" xr:uid="{7C0CF1F9-6D8B-4838-AF4F-5E3806F151A2}"/>
-    <hyperlink ref="F16" r:id="rId6" display="https://www.mouser.ca/datasheet/2/308/1/NCP161_D-2316989.pdf" xr:uid="{7A98D1F1-404F-44D8-89D1-D9D1436D893F}"/>
-    <hyperlink ref="F17" r:id="rId7" display="https://www.mouser.ca/datasheet/2/54/ptv09-777818.pdf" xr:uid="{8236BBA3-E1C5-477D-B2F7-BBC0C6E41223}"/>
-    <hyperlink ref="F5" r:id="rId8" display="https://www.mouser.ca/datasheet/2/212/KEM_C1023_X7R_AUTO_SMD-1093309.pdf" xr:uid="{4124399B-DA79-4405-AB72-D8B1FDAF4819}"/>
-    <hyperlink ref="F6" r:id="rId9" display="https://www.mouser.ca/datasheet/2/212/KEM_C1023_X7R_AUTO_SMD-1093309.pdf" xr:uid="{F2E5697D-C749-490A-9831-2DFDF15AF7E1}"/>
-    <hyperlink ref="F18" r:id="rId10" display="https://www.mouser.ca/datasheet/2/181/M20-999-1218971.pdf" xr:uid="{01275A75-EDA2-4738-A48D-85BCFEA831AF}"/>
+    <hyperlink ref="F20" r:id="rId2" display="https://www.mouser.ca/datasheet/2/54/ptv09-777818.pdf" xr:uid="{BBF2E0E5-0197-4455-B910-736161147ECB}"/>
+    <hyperlink ref="F21" r:id="rId3" display="https://www.mouser.ca/datasheet/2/308/1/NCS333_D-2317376.pdf" xr:uid="{7C0CF1F9-6D8B-4838-AF4F-5E3806F151A2}"/>
+    <hyperlink ref="F22" r:id="rId4" display="https://www.mouser.ca/datasheet/2/308/1/NCP161_D-2316989.pdf" xr:uid="{7A98D1F1-404F-44D8-89D1-D9D1436D893F}"/>
+    <hyperlink ref="F23" r:id="rId5" display="https://www.mouser.ca/datasheet/2/54/ptv09-777818.pdf" xr:uid="{8236BBA3-E1C5-477D-B2F7-BBC0C6E41223}"/>
+    <hyperlink ref="F4" r:id="rId6" display="https://www.mouser.ca/datasheet/2/212/KEM_C1023_X7R_AUTO_SMD-1093309.pdf" xr:uid="{4124399B-DA79-4405-AB72-D8B1FDAF4819}"/>
+    <hyperlink ref="F5" r:id="rId7" display="https://www.mouser.ca/datasheet/2/212/KEM_C1023_X7R_AUTO_SMD-1093309.pdf" xr:uid="{F2E5697D-C749-490A-9831-2DFDF15AF7E1}"/>
+    <hyperlink ref="F24" r:id="rId8" display="https://www.mouser.ca/datasheet/2/181/M20-999-1218971.pdf" xr:uid="{01275A75-EDA2-4738-A48D-85BCFEA831AF}"/>
+    <hyperlink ref="F6" r:id="rId9" display="https://www.mouser.ca/datasheet/2/445/860010372001-1725373.pdf" xr:uid="{2412561B-63A9-475A-93AF-8D7B6EEB26BD}"/>
+    <hyperlink ref="F7:F12" r:id="rId10" display="https://www.mouser.ca/datasheet/2/445/860010372001-1725373.pdf" xr:uid="{3B738D25-CA68-4983-9BE7-96AB1D15E30A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId11"/>
@@ -6831,10 +6975,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5E7DEB4-5FFB-4F8D-963A-C08EFBE9A2C1}">
-  <dimension ref="A1:G147"/>
+  <dimension ref="A1:G150"/>
   <sheetViews>
-    <sheetView topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="A144" sqref="A144:G144"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="B154" sqref="B154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6851,7 +6995,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>23</v>
@@ -6866,7 +7010,7 @@
         <v>87</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -6888,8 +7032,8 @@
       <c r="F2" t="s">
         <v>88</v>
       </c>
-      <c r="G2" s="32" t="s">
-        <v>367</v>
+      <c r="G2" s="28" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -6911,7 +7055,7 @@
       <c r="F3" t="s">
         <v>88</v>
       </c>
-      <c r="G3" s="32"/>
+      <c r="G3" s="28"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -6932,7 +7076,7 @@
       <c r="F4" t="s">
         <v>88</v>
       </c>
-      <c r="G4" s="32"/>
+      <c r="G4" s="28"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -6953,7 +7097,7 @@
       <c r="F5" t="s">
         <v>90</v>
       </c>
-      <c r="G5" s="32"/>
+      <c r="G5" s="28"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -6974,7 +7118,7 @@
       <c r="F6" t="s">
         <v>88</v>
       </c>
-      <c r="G6" s="32"/>
+      <c r="G6" s="28"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -6995,7 +7139,7 @@
       <c r="F7" t="s">
         <v>88</v>
       </c>
-      <c r="G7" s="32"/>
+      <c r="G7" s="28"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -7016,7 +7160,7 @@
       <c r="F8" t="s">
         <v>91</v>
       </c>
-      <c r="G8" s="32"/>
+      <c r="G8" s="28"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -7037,7 +7181,7 @@
       <c r="F9" t="s">
         <v>91</v>
       </c>
-      <c r="G9" s="32"/>
+      <c r="G9" s="28"/>
     </row>
     <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
@@ -7058,7 +7202,7 @@
       <c r="F10" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="G10" s="32"/>
+      <c r="G10" s="28"/>
     </row>
     <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
@@ -7079,8 +7223,8 @@
       <c r="F11" t="s">
         <v>88</v>
       </c>
-      <c r="G11" s="31" t="s">
-        <v>368</v>
+      <c r="G11" s="27" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -7102,7 +7246,7 @@
       <c r="F12" t="s">
         <v>90</v>
       </c>
-      <c r="G12" s="31"/>
+      <c r="G12" s="27"/>
     </row>
     <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -7123,7 +7267,7 @@
       <c r="F13" t="s">
         <v>88</v>
       </c>
-      <c r="G13" s="31"/>
+      <c r="G13" s="27"/>
     </row>
     <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
@@ -7144,7 +7288,7 @@
       <c r="F14" t="s">
         <v>88</v>
       </c>
-      <c r="G14" s="31"/>
+      <c r="G14" s="27"/>
     </row>
     <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
@@ -7165,7 +7309,7 @@
       <c r="F15" t="s">
         <v>88</v>
       </c>
-      <c r="G15" s="31"/>
+      <c r="G15" s="27"/>
     </row>
     <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
@@ -7186,7 +7330,7 @@
       <c r="F16" t="s">
         <v>88</v>
       </c>
-      <c r="G16" s="31"/>
+      <c r="G16" s="27"/>
     </row>
     <row r="17" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
@@ -7207,7 +7351,7 @@
       <c r="F17" t="s">
         <v>88</v>
       </c>
-      <c r="G17" s="31"/>
+      <c r="G17" s="27"/>
     </row>
     <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
@@ -7228,7 +7372,7 @@
       <c r="F18" t="s">
         <v>96</v>
       </c>
-      <c r="G18" s="31"/>
+      <c r="G18" s="27"/>
     </row>
     <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
@@ -7249,7 +7393,7 @@
       <c r="F19" t="s">
         <v>88</v>
       </c>
-      <c r="G19" s="31"/>
+      <c r="G19" s="27"/>
     </row>
     <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
@@ -7270,7 +7414,7 @@
       <c r="F20" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="G20" s="31"/>
+      <c r="G20" s="27"/>
     </row>
     <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
@@ -7291,8 +7435,8 @@
       <c r="F21" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="G21" s="31" t="s">
-        <v>369</v>
+      <c r="G21" s="27" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -7314,7 +7458,7 @@
       <c r="F22" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G22" s="31"/>
+      <c r="G22" s="27"/>
     </row>
     <row r="23" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
@@ -7335,7 +7479,7 @@
       <c r="F23" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="G23" s="31"/>
+      <c r="G23" s="27"/>
     </row>
     <row r="24" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
@@ -7356,7 +7500,7 @@
       <c r="F24" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="G24" s="31"/>
+      <c r="G24" s="27"/>
     </row>
     <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
@@ -7377,7 +7521,7 @@
       <c r="F25" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="G25" s="31"/>
+      <c r="G25" s="27"/>
     </row>
     <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
@@ -7398,7 +7542,7 @@
       <c r="F26" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="G26" s="31"/>
+      <c r="G26" s="27"/>
     </row>
     <row r="27" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
@@ -7419,7 +7563,7 @@
       <c r="F27" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="G27" s="31"/>
+      <c r="G27" s="27"/>
     </row>
     <row r="28" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
@@ -7440,7 +7584,7 @@
       <c r="F28" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="G28" s="31"/>
+      <c r="G28" s="27"/>
     </row>
     <row r="29" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="9" t="s">
@@ -7461,7 +7605,7 @@
       <c r="F29" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="G29" s="31"/>
+      <c r="G29" s="27"/>
     </row>
     <row r="30" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
@@ -7482,8 +7626,8 @@
       <c r="F30" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="G30" s="31" t="s">
-        <v>370</v>
+      <c r="G30" s="27" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -7505,7 +7649,7 @@
       <c r="F31" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="G31" s="31"/>
+      <c r="G31" s="27"/>
     </row>
     <row r="32" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
@@ -7526,7 +7670,7 @@
       <c r="F32" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="G32" s="31"/>
+      <c r="G32" s="27"/>
     </row>
     <row r="33" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
@@ -7547,7 +7691,7 @@
       <c r="F33" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="G33" s="31"/>
+      <c r="G33" s="27"/>
     </row>
     <row r="34" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
@@ -7568,7 +7712,7 @@
       <c r="F34" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="G34" s="31"/>
+      <c r="G34" s="27"/>
     </row>
     <row r="35" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
@@ -7589,7 +7733,7 @@
       <c r="F35" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="G35" s="31"/>
+      <c r="G35" s="27"/>
     </row>
     <row r="36" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
@@ -7610,7 +7754,7 @@
       <c r="F36" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="G36" s="31"/>
+      <c r="G36" s="27"/>
     </row>
     <row r="37" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
@@ -7631,7 +7775,7 @@
       <c r="F37" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="G37" s="31"/>
+      <c r="G37" s="27"/>
     </row>
     <row r="38" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
@@ -7652,7 +7796,7 @@
       <c r="F38" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="G38" s="31"/>
+      <c r="G38" s="27"/>
     </row>
     <row r="39" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="9" t="s">
@@ -7673,7 +7817,7 @@
       <c r="F39" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="G39" s="31"/>
+      <c r="G39" s="27"/>
     </row>
     <row r="40" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
@@ -7694,8 +7838,8 @@
       <c r="F40" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="G40" s="31" t="s">
-        <v>371</v>
+      <c r="G40" s="27" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -7717,7 +7861,7 @@
       <c r="F41" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="G41" s="31"/>
+      <c r="G41" s="27"/>
     </row>
     <row r="42" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
@@ -7738,7 +7882,7 @@
       <c r="F42" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="G42" s="31"/>
+      <c r="G42" s="27"/>
     </row>
     <row r="43" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
@@ -7759,7 +7903,7 @@
       <c r="F43" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="G43" s="31"/>
+      <c r="G43" s="27"/>
     </row>
     <row r="44" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
@@ -7780,7 +7924,7 @@
       <c r="F44" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="G44" s="31"/>
+      <c r="G44" s="27"/>
     </row>
     <row r="45" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
@@ -7801,7 +7945,7 @@
       <c r="F45" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="G45" s="31"/>
+      <c r="G45" s="27"/>
     </row>
     <row r="46" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
@@ -7822,7 +7966,7 @@
       <c r="F46" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="G46" s="31"/>
+      <c r="G46" s="27"/>
     </row>
     <row r="47" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
@@ -7843,7 +7987,7 @@
       <c r="F47" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="G47" s="31"/>
+      <c r="G47" s="27"/>
     </row>
     <row r="48" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="9" t="s">
@@ -7864,7 +8008,7 @@
       <c r="F48" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="G48" s="31"/>
+      <c r="G48" s="27"/>
     </row>
     <row r="49" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
@@ -7885,8 +8029,8 @@
       <c r="F49" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="G49" s="31" t="s">
-        <v>372</v>
+      <c r="G49" s="27" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -7908,7 +8052,7 @@
       <c r="F50" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="G50" s="31"/>
+      <c r="G50" s="27"/>
     </row>
     <row r="51" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
@@ -7929,7 +8073,7 @@
       <c r="F51" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="G51" s="31"/>
+      <c r="G51" s="27"/>
     </row>
     <row r="52" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
@@ -7950,7 +8094,7 @@
       <c r="F52" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="G52" s="31"/>
+      <c r="G52" s="27"/>
     </row>
     <row r="53" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
@@ -7971,7 +8115,7 @@
       <c r="F53" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="G53" s="31"/>
+      <c r="G53" s="27"/>
     </row>
     <row r="54" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
@@ -7992,7 +8136,7 @@
       <c r="F54" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="G54" s="31"/>
+      <c r="G54" s="27"/>
     </row>
     <row r="55" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
@@ -8013,7 +8157,7 @@
       <c r="F55" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="G55" s="31"/>
+      <c r="G55" s="27"/>
     </row>
     <row r="56" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
@@ -8034,7 +8178,7 @@
       <c r="F56" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="G56" s="31"/>
+      <c r="G56" s="27"/>
     </row>
     <row r="57" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="9" t="s">
@@ -8055,7 +8199,7 @@
       <c r="F57" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="G57" s="31"/>
+      <c r="G57" s="27"/>
     </row>
     <row r="58" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
@@ -8076,8 +8220,8 @@
       <c r="F58" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="G58" s="31" t="s">
-        <v>373</v>
+      <c r="G58" s="27" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -8099,7 +8243,7 @@
       <c r="F59" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="G59" s="31"/>
+      <c r="G59" s="27"/>
     </row>
     <row r="60" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
@@ -8120,7 +8264,7 @@
       <c r="F60" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="G60" s="31"/>
+      <c r="G60" s="27"/>
     </row>
     <row r="61" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
@@ -8141,7 +8285,7 @@
       <c r="F61" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="G61" s="31"/>
+      <c r="G61" s="27"/>
     </row>
     <row r="62" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
@@ -8162,7 +8306,7 @@
       <c r="F62" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="G62" s="31"/>
+      <c r="G62" s="27"/>
     </row>
     <row r="63" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
@@ -8183,7 +8327,7 @@
       <c r="F63" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="G63" s="31"/>
+      <c r="G63" s="27"/>
     </row>
     <row r="64" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
@@ -8204,7 +8348,7 @@
       <c r="F64" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="G64" s="31"/>
+      <c r="G64" s="27"/>
     </row>
     <row r="65" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
@@ -8225,7 +8369,7 @@
       <c r="F65" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="G65" s="31"/>
+      <c r="G65" s="27"/>
     </row>
     <row r="66" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="9" t="s">
@@ -8246,7 +8390,7 @@
       <c r="F66" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="G66" s="31"/>
+      <c r="G66" s="27"/>
     </row>
     <row r="67" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
@@ -8267,8 +8411,8 @@
       <c r="F67" t="s">
         <v>93</v>
       </c>
-      <c r="G67" s="31" t="s">
-        <v>367</v>
+      <c r="G67" s="27" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -8290,7 +8434,7 @@
       <c r="F68" t="s">
         <v>93</v>
       </c>
-      <c r="G68" s="31"/>
+      <c r="G68" s="27"/>
     </row>
     <row r="69" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
@@ -8311,7 +8455,7 @@
       <c r="F69" t="s">
         <v>94</v>
       </c>
-      <c r="G69" s="31"/>
+      <c r="G69" s="27"/>
     </row>
     <row r="70" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
@@ -8332,7 +8476,7 @@
       <c r="F70" t="s">
         <v>94</v>
       </c>
-      <c r="G70" s="31"/>
+      <c r="G70" s="27"/>
     </row>
     <row r="71" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
@@ -8353,7 +8497,7 @@
       <c r="F71" t="s">
         <v>95</v>
       </c>
-      <c r="G71" s="31"/>
+      <c r="G71" s="27"/>
     </row>
     <row r="72" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="9" t="s">
@@ -8374,7 +8518,7 @@
       <c r="F72" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="G72" s="31"/>
+      <c r="G72" s="27"/>
     </row>
     <row r="73" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A73" s="14" t="s">
@@ -8395,8 +8539,8 @@
       <c r="F73" t="s">
         <v>97</v>
       </c>
-      <c r="G73" s="31" t="s">
-        <v>368</v>
+      <c r="G73" s="27" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -8418,7 +8562,7 @@
       <c r="F74" t="s">
         <v>97</v>
       </c>
-      <c r="G74" s="31"/>
+      <c r="G74" s="27"/>
     </row>
     <row r="75" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="14" t="s">
@@ -8439,7 +8583,7 @@
       <c r="F75" t="s">
         <v>98</v>
       </c>
-      <c r="G75" s="31"/>
+      <c r="G75" s="27"/>
     </row>
     <row r="76" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A76" s="14" t="s">
@@ -8460,7 +8604,7 @@
       <c r="F76" t="s">
         <v>98</v>
       </c>
-      <c r="G76" s="31"/>
+      <c r="G76" s="27"/>
     </row>
     <row r="77" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A77" s="14" t="s">
@@ -8481,7 +8625,7 @@
       <c r="F77" t="s">
         <v>100</v>
       </c>
-      <c r="G77" s="31"/>
+      <c r="G77" s="27"/>
     </row>
     <row r="78" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="15" t="s">
@@ -8502,7 +8646,7 @@
       <c r="F78" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="G78" s="31"/>
+      <c r="G78" s="27"/>
     </row>
     <row r="79" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A79" s="14" t="s">
@@ -8523,8 +8667,8 @@
       <c r="F79" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="G79" s="31" t="s">
-        <v>369</v>
+      <c r="G79" s="27" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -8546,7 +8690,7 @@
       <c r="F80" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="G80" s="31"/>
+      <c r="G80" s="27"/>
     </row>
     <row r="81" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A81" s="14" t="s">
@@ -8567,7 +8711,7 @@
       <c r="F81" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="G81" s="31"/>
+      <c r="G81" s="27"/>
     </row>
     <row r="82" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A82" s="14" t="s">
@@ -8588,7 +8732,7 @@
       <c r="F82" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="G82" s="31"/>
+      <c r="G82" s="27"/>
     </row>
     <row r="83" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A83" s="14" t="s">
@@ -8609,7 +8753,7 @@
       <c r="F83" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="G83" s="31"/>
+      <c r="G83" s="27"/>
     </row>
     <row r="84" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A84" s="15" t="s">
@@ -8630,7 +8774,7 @@
       <c r="F84" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="G84" s="31"/>
+      <c r="G84" s="27"/>
     </row>
     <row r="85" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A85" s="14" t="s">
@@ -8651,8 +8795,8 @@
       <c r="F85" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="G85" s="31" t="s">
-        <v>370</v>
+      <c r="G85" s="27" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -8674,7 +8818,7 @@
       <c r="F86" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="G86" s="31"/>
+      <c r="G86" s="27"/>
     </row>
     <row r="87" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A87" s="14" t="s">
@@ -8695,7 +8839,7 @@
       <c r="F87" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G87" s="31"/>
+      <c r="G87" s="27"/>
     </row>
     <row r="88" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A88" s="14" t="s">
@@ -8716,7 +8860,7 @@
       <c r="F88" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G88" s="31"/>
+      <c r="G88" s="27"/>
     </row>
     <row r="89" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A89" s="14" t="s">
@@ -8737,7 +8881,7 @@
       <c r="F89" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="G89" s="31"/>
+      <c r="G89" s="27"/>
     </row>
     <row r="90" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A90" s="15" t="s">
@@ -8758,7 +8902,7 @@
       <c r="F90" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="G90" s="31"/>
+      <c r="G90" s="27"/>
     </row>
     <row r="91" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A91" s="14" t="s">
@@ -8779,8 +8923,8 @@
       <c r="F91" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G91" s="31" t="s">
-        <v>371</v>
+      <c r="G91" s="27" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="92" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -8802,7 +8946,7 @@
       <c r="F92" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G92" s="31"/>
+      <c r="G92" s="27"/>
     </row>
     <row r="93" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A93" s="14" t="s">
@@ -8823,7 +8967,7 @@
       <c r="F93" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G93" s="31"/>
+      <c r="G93" s="27"/>
     </row>
     <row r="94" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A94" s="14" t="s">
@@ -8844,7 +8988,7 @@
       <c r="F94" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G94" s="31"/>
+      <c r="G94" s="27"/>
     </row>
     <row r="95" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A95" s="14" t="s">
@@ -8865,7 +9009,7 @@
       <c r="F95" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G95" s="31"/>
+      <c r="G95" s="27"/>
     </row>
     <row r="96" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A96" s="15" t="s">
@@ -8886,7 +9030,7 @@
       <c r="F96" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="G96" s="31"/>
+      <c r="G96" s="27"/>
     </row>
     <row r="97" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A97" s="20" t="s">
@@ -8907,8 +9051,8 @@
       <c r="F97" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="G97" s="31" t="s">
-        <v>372</v>
+      <c r="G97" s="27" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="98" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -8930,7 +9074,7 @@
       <c r="F98" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="G98" s="31"/>
+      <c r="G98" s="27"/>
     </row>
     <row r="99" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A99" s="14" t="s">
@@ -8951,7 +9095,7 @@
       <c r="F99" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="G99" s="31"/>
+      <c r="G99" s="27"/>
     </row>
     <row r="100" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A100" s="14" t="s">
@@ -8972,7 +9116,7 @@
       <c r="F100" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="G100" s="31"/>
+      <c r="G100" s="27"/>
     </row>
     <row r="101" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A101" s="14" t="s">
@@ -8993,7 +9137,7 @@
       <c r="F101" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="G101" s="31"/>
+      <c r="G101" s="27"/>
     </row>
     <row r="102" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A102" s="15" t="s">
@@ -9014,7 +9158,7 @@
       <c r="F102" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="G102" s="31"/>
+      <c r="G102" s="27"/>
     </row>
     <row r="103" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A103" s="14" t="s">
@@ -9035,8 +9179,8 @@
       <c r="F103" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G103" s="31" t="s">
-        <v>373</v>
+      <c r="G103" s="27" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="104" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -9058,7 +9202,7 @@
       <c r="F104" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G104" s="31"/>
+      <c r="G104" s="27"/>
     </row>
     <row r="105" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A105" s="14" t="s">
@@ -9079,7 +9223,7 @@
       <c r="F105" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G105" s="31"/>
+      <c r="G105" s="27"/>
     </row>
     <row r="106" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A106" s="14" t="s">
@@ -9100,7 +9244,7 @@
       <c r="F106" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G106" s="31"/>
+      <c r="G106" s="27"/>
     </row>
     <row r="107" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A107" s="14" t="s">
@@ -9121,7 +9265,7 @@
       <c r="F107" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G107" s="31"/>
+      <c r="G107" s="27"/>
     </row>
     <row r="108" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A108" s="15" t="s">
@@ -9142,11 +9286,11 @@
       <c r="F108" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="G108" s="31"/>
+      <c r="G108" s="27"/>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109" s="14" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B109" s="14">
         <v>1</v>
@@ -9155,21 +9299,21 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="D109" t="s">
+        <v>380</v>
+      </c>
+      <c r="E109" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F109" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="E109" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F109" s="3" t="s">
+      <c r="G109" s="29" t="s">
         <v>382</v>
-      </c>
-      <c r="G109" s="27" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110" s="14" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B110" s="14">
         <v>1</v>
@@ -9178,19 +9322,19 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="D110" t="s">
+        <v>380</v>
+      </c>
+      <c r="E110" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F110" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="E110" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F110" s="3" t="s">
-        <v>382</v>
-      </c>
-      <c r="G110" s="28"/>
+      <c r="G110" s="30"/>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111" s="14" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B111" s="14">
         <v>1</v>
@@ -9199,19 +9343,19 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="D111" t="s">
+        <v>380</v>
+      </c>
+      <c r="E111" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F111" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="E111" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F111" s="3" t="s">
-        <v>382</v>
-      </c>
-      <c r="G111" s="28"/>
+      <c r="G111" s="30"/>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112" s="14" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B112" s="14">
         <v>1</v>
@@ -9220,19 +9364,19 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="D112" t="s">
+        <v>380</v>
+      </c>
+      <c r="E112" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F112" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="E112" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F112" s="3" t="s">
-        <v>382</v>
-      </c>
-      <c r="G112" s="28"/>
+      <c r="G112" s="30"/>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113" s="14" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B113" s="14">
         <v>1</v>
@@ -9241,19 +9385,19 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="D113" t="s">
+        <v>380</v>
+      </c>
+      <c r="E113" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F113" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="E113" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F113" s="3" t="s">
-        <v>382</v>
-      </c>
-      <c r="G113" s="28"/>
+      <c r="G113" s="30"/>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114" s="14" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B114" s="14">
         <v>1</v>
@@ -9262,19 +9406,19 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="D114" t="s">
+        <v>380</v>
+      </c>
+      <c r="E114" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F114" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="E114" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F114" s="3" t="s">
-        <v>382</v>
-      </c>
-      <c r="G114" s="28"/>
+      <c r="G114" s="30"/>
     </row>
     <row r="115" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A115" s="15" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B115" s="15">
         <v>1</v>
@@ -9283,168 +9427,168 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="D115" s="9" t="s">
+        <v>380</v>
+      </c>
+      <c r="E115" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="F115" s="12" t="s">
         <v>381</v>
       </c>
-      <c r="E115" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="F115" s="12" t="s">
-        <v>382</v>
-      </c>
-      <c r="G115" s="28"/>
+      <c r="G115" s="30"/>
     </row>
     <row r="116" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A116" s="14" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B116" s="14" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C116" s="25">
         <v>0.60699999999999998</v>
       </c>
       <c r="D116" t="s">
+        <v>395</v>
+      </c>
+      <c r="E116" s="5" t="s">
         <v>396</v>
       </c>
-      <c r="E116" s="5" t="s">
+      <c r="F116" s="3" t="s">
         <v>397</v>
       </c>
-      <c r="F116" s="3" t="s">
+      <c r="G116" s="31" t="s">
         <v>398</v>
-      </c>
-      <c r="G116" s="29" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="117" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A117" s="14" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B117" s="14" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C117" s="25">
         <v>0.60699999999999998</v>
       </c>
       <c r="D117" t="s">
+        <v>395</v>
+      </c>
+      <c r="E117" s="5" t="s">
         <v>396</v>
       </c>
-      <c r="E117" s="5" t="s">
+      <c r="F117" s="3" t="s">
         <v>397</v>
       </c>
-      <c r="F117" s="3" t="s">
-        <v>398</v>
-      </c>
-      <c r="G117" s="29"/>
+      <c r="G117" s="31"/>
     </row>
     <row r="118" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A118" s="14" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B118" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C118" s="25">
         <v>0.13800000000000001</v>
       </c>
       <c r="D118" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E118" s="5" t="s">
         <v>99</v>
       </c>
       <c r="F118" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="G118" s="29"/>
+        <v>400</v>
+      </c>
+      <c r="G118" s="31"/>
     </row>
     <row r="119" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A119" s="14" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B119" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C119" s="25">
         <v>0.13800000000000001</v>
       </c>
       <c r="D119" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E119" s="5" t="s">
         <v>99</v>
       </c>
       <c r="F119" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="G119" s="29"/>
+        <v>400</v>
+      </c>
+      <c r="G119" s="31"/>
     </row>
     <row r="120" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A120" s="14" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B120" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C120" s="25">
         <v>0.11</v>
       </c>
       <c r="D120" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E120" s="6">
         <v>1005</v>
       </c>
       <c r="F120" s="3" t="s">
-        <v>345</v>
-      </c>
-      <c r="G120" s="29"/>
+        <v>344</v>
+      </c>
+      <c r="G120" s="31"/>
     </row>
     <row r="121" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A121" s="14" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B121" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C121" s="25">
         <v>0.11</v>
       </c>
       <c r="D121" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E121" s="6">
         <v>1005</v>
       </c>
       <c r="F121" s="3" t="s">
-        <v>345</v>
-      </c>
-      <c r="G121" s="29"/>
+        <v>344</v>
+      </c>
+      <c r="G121" s="31"/>
     </row>
     <row r="122" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A122" s="15" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B122" s="9" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C122" s="26">
         <v>0.11</v>
       </c>
       <c r="D122" s="9" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E122" s="13">
         <v>1005</v>
       </c>
       <c r="F122" s="12" t="s">
-        <v>345</v>
-      </c>
-      <c r="G122" s="29"/>
+        <v>344</v>
+      </c>
+      <c r="G122" s="31"/>
     </row>
     <row r="123" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A123" s="14" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B123" t="s">
         <v>255</v>
@@ -9461,13 +9605,13 @@
       <c r="F123" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="G123" s="29" t="s">
-        <v>403</v>
+      <c r="G123" s="31" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="124" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A124" s="14" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B124" t="s">
         <v>256</v>
@@ -9484,409 +9628,569 @@
       <c r="F124" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="G124" s="29"/>
+      <c r="G124" s="31"/>
     </row>
     <row r="125" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A125" s="14" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B125" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C125" s="2">
         <v>0.11</v>
       </c>
       <c r="D125" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E125" s="6">
         <v>1005</v>
       </c>
       <c r="F125" s="3" t="s">
-        <v>345</v>
-      </c>
-      <c r="G125" s="29"/>
+        <v>344</v>
+      </c>
+      <c r="G125" s="31"/>
     </row>
     <row r="126" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A126" s="14" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B126" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C126" s="2">
         <v>0.11</v>
       </c>
       <c r="D126" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E126" s="6">
         <v>1005</v>
       </c>
       <c r="F126" s="3" t="s">
-        <v>345</v>
-      </c>
-      <c r="G126" s="29"/>
+        <v>344</v>
+      </c>
+      <c r="G126" s="31"/>
     </row>
     <row r="127" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A127" s="14" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B127" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C127" s="2">
         <v>0.13800000000000001</v>
       </c>
       <c r="D127" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E127" s="6">
         <v>2012</v>
       </c>
       <c r="F127" s="3" t="s">
-        <v>347</v>
-      </c>
-      <c r="G127" s="29"/>
+        <v>346</v>
+      </c>
+      <c r="G127" s="31"/>
     </row>
     <row r="128" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A128" s="14" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B128" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C128" s="2">
         <v>0.152</v>
       </c>
       <c r="D128" t="s">
+        <v>347</v>
+      </c>
+      <c r="E128" s="6" t="s">
         <v>348</v>
       </c>
-      <c r="E128" s="6" t="s">
+      <c r="F128" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="F128" s="3" t="s">
-        <v>350</v>
-      </c>
-      <c r="G128" s="29"/>
+      <c r="G128" s="31"/>
     </row>
     <row r="129" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A129" s="15" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B129" s="9" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C129" s="10">
         <v>0.13800000000000001</v>
       </c>
       <c r="D129" s="9" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E129" s="13">
         <v>1005</v>
       </c>
       <c r="F129" s="12" t="s">
-        <v>352</v>
-      </c>
-      <c r="G129" s="29"/>
+        <v>351</v>
+      </c>
+      <c r="G129" s="31"/>
     </row>
     <row r="130" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A130" s="14" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B130" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C130" s="2">
         <v>0.13800000000000001</v>
       </c>
       <c r="D130" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E130" s="6">
         <v>1608</v>
       </c>
       <c r="F130" s="3" t="s">
-        <v>354</v>
-      </c>
-      <c r="G130" s="30" t="s">
-        <v>411</v>
+        <v>353</v>
+      </c>
+      <c r="G130" s="32" t="s">
+        <v>410</v>
       </c>
     </row>
     <row r="131" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A131" s="15" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B131" s="9" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C131" s="10">
         <v>0.13800000000000001</v>
       </c>
       <c r="D131" s="9" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E131" s="13">
         <v>1608</v>
       </c>
       <c r="F131" s="12" t="s">
-        <v>356</v>
-      </c>
-      <c r="G131" s="30"/>
+        <v>355</v>
+      </c>
+      <c r="G131" s="32"/>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132" s="14" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B132" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C132" s="2">
         <v>0.13800000000000001</v>
       </c>
       <c r="D132" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E132" s="6">
         <v>1608</v>
       </c>
       <c r="F132" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
+      </c>
+      <c r="G132" s="29" t="s">
+        <v>446</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A133" s="14" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B133" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C133" s="2">
         <v>0.13800000000000001</v>
       </c>
       <c r="D133" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E133" s="6">
         <v>1608</v>
       </c>
       <c r="F133" s="3" t="s">
-        <v>315</v>
-      </c>
+        <v>314</v>
+      </c>
+      <c r="G133" s="30"/>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A134" s="14" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B134" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C134" s="2">
         <v>0.13800000000000001</v>
       </c>
       <c r="D134" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E134" s="6">
         <v>1608</v>
       </c>
       <c r="F134" s="3" t="s">
-        <v>315</v>
-      </c>
+        <v>314</v>
+      </c>
+      <c r="G134" s="30"/>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A135" s="14" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B135" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C135" s="2">
         <v>0.13800000000000001</v>
       </c>
       <c r="D135" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E135" s="6">
         <v>1608</v>
       </c>
       <c r="F135" s="3" t="s">
-        <v>315</v>
-      </c>
+        <v>314</v>
+      </c>
+      <c r="G135" s="30"/>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A136" s="14" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B136" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C136" s="2">
         <v>0.13800000000000001</v>
       </c>
       <c r="D136" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E136" s="6">
         <v>1608</v>
       </c>
       <c r="F136" s="3" t="s">
-        <v>315</v>
-      </c>
+        <v>314</v>
+      </c>
+      <c r="G136" s="30"/>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A137" s="14" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B137" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C137" s="2">
         <v>0.13800000000000001</v>
       </c>
       <c r="D137" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E137" s="6">
         <v>1608</v>
       </c>
       <c r="F137" s="3" t="s">
-        <v>315</v>
-      </c>
+        <v>314</v>
+      </c>
+      <c r="G137" s="30"/>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A138" s="14" t="s">
+        <v>417</v>
+      </c>
+      <c r="B138" t="s">
         <v>418</v>
       </c>
-      <c r="B138" t="s">
-        <v>419</v>
-      </c>
       <c r="C138" s="2">
         <v>0.13800000000000001</v>
       </c>
       <c r="D138" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E138" s="6">
         <v>1608</v>
       </c>
       <c r="F138" s="3" t="s">
-        <v>315</v>
-      </c>
+        <v>314</v>
+      </c>
+      <c r="G138" s="30"/>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A139" s="14" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B139" t="s">
-        <v>312</v>
-      </c>
-      <c r="C139" s="2">
-        <v>0.20699999999999999</v>
-      </c>
-      <c r="D139" s="3" t="s">
-        <v>285</v>
-      </c>
-      <c r="E139" s="6" t="s">
-        <v>286</v>
+        <v>394</v>
+      </c>
+      <c r="C139" s="25">
+        <v>0.11</v>
+      </c>
+      <c r="D139" t="s">
+        <v>343</v>
+      </c>
+      <c r="E139" s="6">
+        <v>1005</v>
       </c>
       <c r="F139" s="3" t="s">
-        <v>287</v>
-      </c>
+        <v>344</v>
+      </c>
+      <c r="G139" s="30"/>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A140" s="14" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B140" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C140" s="25">
         <v>0.11</v>
       </c>
       <c r="D140" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E140" s="6">
         <v>1005</v>
       </c>
       <c r="F140" s="3" t="s">
-        <v>345</v>
-      </c>
+        <v>344</v>
+      </c>
+      <c r="G140" s="30"/>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A141" s="14" t="s">
-        <v>422</v>
+        <v>426</v>
       </c>
       <c r="B141" t="s">
-        <v>395</v>
-      </c>
-      <c r="C141" s="25">
-        <v>0.11</v>
+        <v>428</v>
+      </c>
+      <c r="C141" s="2">
+        <v>1.38</v>
       </c>
       <c r="D141" t="s">
-        <v>344</v>
-      </c>
-      <c r="E141" s="6">
-        <v>1005</v>
+        <v>315</v>
+      </c>
+      <c r="E141" s="6" t="s">
+        <v>348</v>
       </c>
       <c r="F141" s="3" t="s">
-        <v>345</v>
-      </c>
+        <v>316</v>
+      </c>
+      <c r="G141" s="30"/>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A142" s="14" t="s">
+        <v>427</v>
+      </c>
+      <c r="B142" s="16" t="s">
         <v>428</v>
       </c>
-      <c r="B142" t="s">
-        <v>430</v>
-      </c>
-      <c r="C142" s="2"/>
-    </row>
-    <row r="143" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A143" s="15" t="s">
-        <v>429</v>
-      </c>
-      <c r="B143" s="9" t="s">
-        <v>430</v>
-      </c>
-      <c r="C143" s="9"/>
-      <c r="D143" s="9"/>
-      <c r="E143" s="9"/>
-      <c r="F143" s="9"/>
-      <c r="G143" s="9"/>
+      <c r="C142" s="2">
+        <v>1.38</v>
+      </c>
+      <c r="D142" t="s">
+        <v>315</v>
+      </c>
+      <c r="E142" s="6" t="s">
+        <v>348</v>
+      </c>
+      <c r="F142" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="G142" s="30"/>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A143" s="14" t="s">
+        <v>421</v>
+      </c>
+      <c r="B143" t="s">
+        <v>337</v>
+      </c>
+      <c r="C143" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D143" t="s">
+        <v>438</v>
+      </c>
+      <c r="E143" s="6" t="s">
+        <v>348</v>
+      </c>
+      <c r="F143" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="G143" s="30"/>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A144" s="14" t="s">
-        <v>434</v>
-      </c>
-      <c r="B144" s="14" t="s">
+        <v>440</v>
+      </c>
+      <c r="B144" t="s">
+        <v>337</v>
+      </c>
+      <c r="C144" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D144" t="s">
+        <v>438</v>
+      </c>
+      <c r="E144" s="6" t="s">
+        <v>348</v>
+      </c>
+      <c r="F144" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="G144" s="30"/>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A145" s="14" t="s">
+        <v>441</v>
+      </c>
+      <c r="B145" t="s">
+        <v>337</v>
+      </c>
+      <c r="C145" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D145" t="s">
+        <v>438</v>
+      </c>
+      <c r="E145" s="6" t="s">
+        <v>348</v>
+      </c>
+      <c r="F145" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="G145" s="30"/>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A146" s="14" t="s">
+        <v>442</v>
+      </c>
+      <c r="B146" t="s">
+        <v>337</v>
+      </c>
+      <c r="C146" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D146" t="s">
+        <v>438</v>
+      </c>
+      <c r="E146" s="6" t="s">
+        <v>348</v>
+      </c>
+      <c r="F146" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="G146" s="30"/>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A147" s="14" t="s">
+        <v>443</v>
+      </c>
+      <c r="B147" t="s">
+        <v>337</v>
+      </c>
+      <c r="C147" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D147" t="s">
+        <v>438</v>
+      </c>
+      <c r="E147" s="6" t="s">
+        <v>348</v>
+      </c>
+      <c r="F147" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="G147" s="30"/>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A148" s="14" t="s">
+        <v>444</v>
+      </c>
+      <c r="B148" t="s">
+        <v>337</v>
+      </c>
+      <c r="C148" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D148" t="s">
+        <v>438</v>
+      </c>
+      <c r="E148" s="6" t="s">
+        <v>348</v>
+      </c>
+      <c r="F148" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="G148" s="30"/>
+    </row>
+    <row r="149" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A149" s="15" t="s">
+        <v>445</v>
+      </c>
+      <c r="B149" s="9" t="s">
+        <v>337</v>
+      </c>
+      <c r="C149" s="10">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D149" s="9" t="s">
+        <v>438</v>
+      </c>
+      <c r="E149" s="13" t="s">
+        <v>348</v>
+      </c>
+      <c r="F149" s="12" t="s">
+        <v>439</v>
+      </c>
+      <c r="G149" s="33"/>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A150" s="14" t="s">
+        <v>432</v>
+      </c>
+      <c r="B150" s="14" t="s">
+        <v>429</v>
+      </c>
+      <c r="C150" s="2">
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="D150" t="s">
+        <v>430</v>
+      </c>
+      <c r="E150" s="6">
+        <v>1608</v>
+      </c>
+      <c r="F150" s="3" t="s">
         <v>431</v>
       </c>
-      <c r="C144" s="2">
-        <v>0.30399999999999999</v>
-      </c>
-      <c r="D144" t="s">
-        <v>432</v>
-      </c>
-      <c r="E144" s="6">
-        <v>1608</v>
-      </c>
-      <c r="F144" s="3" t="s">
+      <c r="G150" t="s">
         <v>433</v>
       </c>
-      <c r="G144" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="147" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E147" t="s">
-        <v>427</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="19">
+    <mergeCell ref="G132:G149"/>
+    <mergeCell ref="G109:G115"/>
+    <mergeCell ref="G116:G122"/>
+    <mergeCell ref="G123:G129"/>
+    <mergeCell ref="G130:G131"/>
+    <mergeCell ref="G97:G102"/>
+    <mergeCell ref="G103:G108"/>
     <mergeCell ref="G91:G96"/>
     <mergeCell ref="G2:G10"/>
     <mergeCell ref="G11:G20"/>
@@ -9899,12 +10203,6 @@
     <mergeCell ref="G73:G78"/>
     <mergeCell ref="G79:G84"/>
     <mergeCell ref="G85:G90"/>
-    <mergeCell ref="G109:G115"/>
-    <mergeCell ref="G116:G122"/>
-    <mergeCell ref="G123:G129"/>
-    <mergeCell ref="G130:G131"/>
-    <mergeCell ref="G97:G102"/>
-    <mergeCell ref="G103:G108"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -10006,14 +10304,16 @@
     <hyperlink ref="F127" r:id="rId96" display="https://www.mouser.ca/datasheet/2/585/MLCC-1837944.pdf" xr:uid="{F5506774-2647-4180-A630-3F869F90200C}"/>
     <hyperlink ref="F128" r:id="rId97" display="https://www.mouser.ca/datasheet/2/445/860010372006-1725314.pdf" xr:uid="{76B8DFED-7E19-40D0-883F-323E54884DB7}"/>
     <hyperlink ref="F129" r:id="rId98" display="https://www.mouser.ca/datasheet/2/447/yago_s_a0003557223_1-2286436.pdf" xr:uid="{E9C3E476-E5B1-42E2-96A4-99E21333D366}"/>
-    <hyperlink ref="F139" r:id="rId99" display="https://www.mouser.ca/datasheet/2/445/860020273009-1725581.pdf" xr:uid="{FCE204EF-6DC7-4555-94B1-FBA8CF609B24}"/>
-    <hyperlink ref="D139" r:id="rId100" xr:uid="{2B4A96D9-73B2-4284-9F00-05D1DF0F219B}"/>
-    <hyperlink ref="F140" r:id="rId101" display="https://www.mouser.ca/datasheet/2/212/KEM_C1023_X7R_AUTO_SMD-1093309.pdf" xr:uid="{EF096566-3DC3-4D51-A03D-30B625A0CE18}"/>
-    <hyperlink ref="F141" r:id="rId102" display="https://www.mouser.ca/datasheet/2/212/KEM_C1023_X7R_AUTO_SMD-1093309.pdf" xr:uid="{CCB90840-C615-48E9-A50C-D72AE500BCAC}"/>
-    <hyperlink ref="F144" r:id="rId103" display="https://fscdn.rohm.com/en/products/databook/datasheet/passive/resistor/chip_resistor/sdr-e.pdf" xr:uid="{33C7962E-E358-4301-8B9C-6188F4CE89A3}"/>
+    <hyperlink ref="F139" r:id="rId99" display="https://www.mouser.ca/datasheet/2/212/KEM_C1023_X7R_AUTO_SMD-1093309.pdf" xr:uid="{EF096566-3DC3-4D51-A03D-30B625A0CE18}"/>
+    <hyperlink ref="F140" r:id="rId100" display="https://www.mouser.ca/datasheet/2/212/KEM_C1023_X7R_AUTO_SMD-1093309.pdf" xr:uid="{CCB90840-C615-48E9-A50C-D72AE500BCAC}"/>
+    <hyperlink ref="F150" r:id="rId101" display="https://fscdn.rohm.com/en/products/databook/datasheet/passive/resistor/chip_resistor/sdr-e.pdf" xr:uid="{33C7962E-E358-4301-8B9C-6188F4CE89A3}"/>
+    <hyperlink ref="F143" r:id="rId102" display="https://www.mouser.ca/datasheet/2/445/860010372001-1725373.pdf" xr:uid="{F0BB76DD-F0A4-4505-B6A6-52B14B35D37E}"/>
+    <hyperlink ref="F144:F149" r:id="rId103" display="https://www.mouser.ca/datasheet/2/445/860010372001-1725373.pdf" xr:uid="{9F6621BE-C8A7-43F8-AD68-780426F80C79}"/>
+    <hyperlink ref="F141" r:id="rId104" display="https://www.mouser.ca/datasheet/2/54/ptv09-777818.pdf" xr:uid="{97382D42-0D14-4D18-8CB2-2E008C09F270}"/>
+    <hyperlink ref="F142" r:id="rId105" display="https://www.mouser.ca/datasheet/2/54/ptv09-777818.pdf" xr:uid="{6A3EA8F4-9E8D-4EFA-A6DB-F7499686F8F7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId104"/>
+  <pageSetup orientation="portrait" r:id="rId106"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added screw port terminal block to connect male audio jack, traceed audio input and header, all nets have now been traced
</commit_message>
<xml_diff>
--- a/Documents/BOM.xlsx
+++ b/Documents/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ECE_Projects\Music_Visualizer\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC2D811-B549-41CA-8E25-5FF0C551CD3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47826A37-FEAF-49FC-AEBE-B5D5F29F8103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="824" activeTab="7" xr2:uid="{1F4A7036-4694-4970-BB5D-7CBECC831452}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="824" activeTab="13" xr2:uid="{1F4A7036-4694-4970-BB5D-7CBECC831452}"/>
   </bookViews>
   <sheets>
     <sheet name="Sub-Bass" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1533" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1537" uniqueCount="451">
   <si>
     <t>Component</t>
   </si>
@@ -1390,6 +1390,18 @@
   </si>
   <si>
     <t>Passives For LED Driver Circuit</t>
+  </si>
+  <si>
+    <t>Phoenix Contact 1725656</t>
+  </si>
+  <si>
+    <t>Male Jack Terminal</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Phoenix-Contact/1725656?qs=Ul7CXFMnlWWQeccayYbRmw%3D%3D&amp;mgh=1&amp;gclid=Cj0KCQjwj7CZBhDHARIsAPPWv3eH9Gr5ezg0IfqzBDGvfizmMMzmce4ZnoD8_Tk4EqWgZ3Z6qSYQwwgaApKeEALw_wcB</t>
+  </si>
+  <si>
+    <t> 1725656 Datasheet</t>
   </si>
 </sst>
 </file>
@@ -1531,16 +1543,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1549,8 +1558,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3403,15 +3415,15 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBB0EED6-7AEC-4823-91A2-5A66F8F096F2}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3503,14 +3515,33 @@
         <v>303</v>
       </c>
     </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>447</v>
+      </c>
+      <c r="B6" t="s">
+        <v>448</v>
+      </c>
+      <c r="C6">
+        <v>2.66</v>
+      </c>
+      <c r="D6" t="s">
+        <v>449</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>450</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" display="https://www.mouser.ca/datasheet/2/670/sp_3533_02-1779105.pdf" xr:uid="{64024244-CF4B-4410-93D1-8014F099D798}"/>
     <hyperlink ref="F4" r:id="rId2" display="https://www.mouser.ca/datasheet/2/60/os-1841429.pdf" xr:uid="{358D795B-5584-405C-9659-E433776CC60B}"/>
     <hyperlink ref="F5" r:id="rId3" display="https://www.mouser.ca/datasheet/2/140/ESCH_S_A0005379088_1-2548267.pdf" xr:uid="{72A05A94-118D-4533-B3B9-93B88199E5DB}"/>
     <hyperlink ref="F3" r:id="rId4" display="https://www.mouser.ca/datasheet/2/670/sj_352x_smt-1779397.pdf" xr:uid="{D42553CD-8A54-404C-A56C-02200684FF6B}"/>
+    <hyperlink ref="F6" r:id="rId5" display="https://www.phoenixcontact.com/us/products/1725656/pdf" xr:uid="{7DB870D4-B99A-4529-922C-F29194F2A783}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -6977,7 +7008,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5E7DEB4-5FFB-4F8D-963A-C08EFBE9A2C1}">
   <dimension ref="A1:G150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+    <sheetView topLeftCell="A118" workbookViewId="0">
       <selection activeCell="B154" sqref="B154"/>
     </sheetView>
   </sheetViews>
@@ -7032,7 +7063,7 @@
       <c r="F2" t="s">
         <v>88</v>
       </c>
-      <c r="G2" s="28" t="s">
+      <c r="G2" s="33" t="s">
         <v>366</v>
       </c>
     </row>
@@ -7055,7 +7086,7 @@
       <c r="F3" t="s">
         <v>88</v>
       </c>
-      <c r="G3" s="28"/>
+      <c r="G3" s="33"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -7076,7 +7107,7 @@
       <c r="F4" t="s">
         <v>88</v>
       </c>
-      <c r="G4" s="28"/>
+      <c r="G4" s="33"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -7097,7 +7128,7 @@
       <c r="F5" t="s">
         <v>90</v>
       </c>
-      <c r="G5" s="28"/>
+      <c r="G5" s="33"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -7118,7 +7149,7 @@
       <c r="F6" t="s">
         <v>88</v>
       </c>
-      <c r="G6" s="28"/>
+      <c r="G6" s="33"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -7139,7 +7170,7 @@
       <c r="F7" t="s">
         <v>88</v>
       </c>
-      <c r="G7" s="28"/>
+      <c r="G7" s="33"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -7160,7 +7191,7 @@
       <c r="F8" t="s">
         <v>91</v>
       </c>
-      <c r="G8" s="28"/>
+      <c r="G8" s="33"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -7181,7 +7212,7 @@
       <c r="F9" t="s">
         <v>91</v>
       </c>
-      <c r="G9" s="28"/>
+      <c r="G9" s="33"/>
     </row>
     <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
@@ -7202,7 +7233,7 @@
       <c r="F10" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="G10" s="28"/>
+      <c r="G10" s="33"/>
     </row>
     <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
@@ -7223,7 +7254,7 @@
       <c r="F11" t="s">
         <v>88</v>
       </c>
-      <c r="G11" s="27" t="s">
+      <c r="G11" s="32" t="s">
         <v>367</v>
       </c>
     </row>
@@ -7246,7 +7277,7 @@
       <c r="F12" t="s">
         <v>90</v>
       </c>
-      <c r="G12" s="27"/>
+      <c r="G12" s="32"/>
     </row>
     <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -7267,7 +7298,7 @@
       <c r="F13" t="s">
         <v>88</v>
       </c>
-      <c r="G13" s="27"/>
+      <c r="G13" s="32"/>
     </row>
     <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
@@ -7288,7 +7319,7 @@
       <c r="F14" t="s">
         <v>88</v>
       </c>
-      <c r="G14" s="27"/>
+      <c r="G14" s="32"/>
     </row>
     <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
@@ -7309,7 +7340,7 @@
       <c r="F15" t="s">
         <v>88</v>
       </c>
-      <c r="G15" s="27"/>
+      <c r="G15" s="32"/>
     </row>
     <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
@@ -7330,7 +7361,7 @@
       <c r="F16" t="s">
         <v>88</v>
       </c>
-      <c r="G16" s="27"/>
+      <c r="G16" s="32"/>
     </row>
     <row r="17" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
@@ -7351,7 +7382,7 @@
       <c r="F17" t="s">
         <v>88</v>
       </c>
-      <c r="G17" s="27"/>
+      <c r="G17" s="32"/>
     </row>
     <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
@@ -7372,7 +7403,7 @@
       <c r="F18" t="s">
         <v>96</v>
       </c>
-      <c r="G18" s="27"/>
+      <c r="G18" s="32"/>
     </row>
     <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
@@ -7393,7 +7424,7 @@
       <c r="F19" t="s">
         <v>88</v>
       </c>
-      <c r="G19" s="27"/>
+      <c r="G19" s="32"/>
     </row>
     <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
@@ -7414,7 +7445,7 @@
       <c r="F20" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="G20" s="27"/>
+      <c r="G20" s="32"/>
     </row>
     <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
@@ -7435,7 +7466,7 @@
       <c r="F21" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="G21" s="27" t="s">
+      <c r="G21" s="32" t="s">
         <v>368</v>
       </c>
     </row>
@@ -7458,7 +7489,7 @@
       <c r="F22" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G22" s="27"/>
+      <c r="G22" s="32"/>
     </row>
     <row r="23" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
@@ -7479,7 +7510,7 @@
       <c r="F23" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="G23" s="27"/>
+      <c r="G23" s="32"/>
     </row>
     <row r="24" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
@@ -7500,7 +7531,7 @@
       <c r="F24" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="G24" s="27"/>
+      <c r="G24" s="32"/>
     </row>
     <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
@@ -7521,7 +7552,7 @@
       <c r="F25" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="G25" s="27"/>
+      <c r="G25" s="32"/>
     </row>
     <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
@@ -7542,7 +7573,7 @@
       <c r="F26" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="G26" s="27"/>
+      <c r="G26" s="32"/>
     </row>
     <row r="27" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
@@ -7563,7 +7594,7 @@
       <c r="F27" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="G27" s="27"/>
+      <c r="G27" s="32"/>
     </row>
     <row r="28" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
@@ -7584,7 +7615,7 @@
       <c r="F28" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="G28" s="27"/>
+      <c r="G28" s="32"/>
     </row>
     <row r="29" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="9" t="s">
@@ -7605,7 +7636,7 @@
       <c r="F29" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="G29" s="27"/>
+      <c r="G29" s="32"/>
     </row>
     <row r="30" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
@@ -7626,7 +7657,7 @@
       <c r="F30" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="G30" s="27" t="s">
+      <c r="G30" s="32" t="s">
         <v>369</v>
       </c>
     </row>
@@ -7649,7 +7680,7 @@
       <c r="F31" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="G31" s="27"/>
+      <c r="G31" s="32"/>
     </row>
     <row r="32" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
@@ -7670,7 +7701,7 @@
       <c r="F32" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="G32" s="27"/>
+      <c r="G32" s="32"/>
     </row>
     <row r="33" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
@@ -7691,7 +7722,7 @@
       <c r="F33" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="G33" s="27"/>
+      <c r="G33" s="32"/>
     </row>
     <row r="34" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
@@ -7712,7 +7743,7 @@
       <c r="F34" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="G34" s="27"/>
+      <c r="G34" s="32"/>
     </row>
     <row r="35" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
@@ -7733,7 +7764,7 @@
       <c r="F35" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="G35" s="27"/>
+      <c r="G35" s="32"/>
     </row>
     <row r="36" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
@@ -7754,7 +7785,7 @@
       <c r="F36" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="G36" s="27"/>
+      <c r="G36" s="32"/>
     </row>
     <row r="37" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
@@ -7775,7 +7806,7 @@
       <c r="F37" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="G37" s="27"/>
+      <c r="G37" s="32"/>
     </row>
     <row r="38" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
@@ -7796,7 +7827,7 @@
       <c r="F38" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="G38" s="27"/>
+      <c r="G38" s="32"/>
     </row>
     <row r="39" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="9" t="s">
@@ -7817,7 +7848,7 @@
       <c r="F39" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="G39" s="27"/>
+      <c r="G39" s="32"/>
     </row>
     <row r="40" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
@@ -7838,7 +7869,7 @@
       <c r="F40" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="G40" s="27" t="s">
+      <c r="G40" s="32" t="s">
         <v>370</v>
       </c>
     </row>
@@ -7861,7 +7892,7 @@
       <c r="F41" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="G41" s="27"/>
+      <c r="G41" s="32"/>
     </row>
     <row r="42" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
@@ -7882,7 +7913,7 @@
       <c r="F42" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="G42" s="27"/>
+      <c r="G42" s="32"/>
     </row>
     <row r="43" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
@@ -7903,7 +7934,7 @@
       <c r="F43" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="G43" s="27"/>
+      <c r="G43" s="32"/>
     </row>
     <row r="44" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
@@ -7924,7 +7955,7 @@
       <c r="F44" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="G44" s="27"/>
+      <c r="G44" s="32"/>
     </row>
     <row r="45" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
@@ -7945,7 +7976,7 @@
       <c r="F45" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="G45" s="27"/>
+      <c r="G45" s="32"/>
     </row>
     <row r="46" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
@@ -7966,7 +7997,7 @@
       <c r="F46" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="G46" s="27"/>
+      <c r="G46" s="32"/>
     </row>
     <row r="47" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
@@ -7987,7 +8018,7 @@
       <c r="F47" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="G47" s="27"/>
+      <c r="G47" s="32"/>
     </row>
     <row r="48" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="9" t="s">
@@ -8008,7 +8039,7 @@
       <c r="F48" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="G48" s="27"/>
+      <c r="G48" s="32"/>
     </row>
     <row r="49" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
@@ -8029,7 +8060,7 @@
       <c r="F49" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="G49" s="27" t="s">
+      <c r="G49" s="32" t="s">
         <v>371</v>
       </c>
     </row>
@@ -8052,7 +8083,7 @@
       <c r="F50" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="G50" s="27"/>
+      <c r="G50" s="32"/>
     </row>
     <row r="51" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
@@ -8073,7 +8104,7 @@
       <c r="F51" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="G51" s="27"/>
+      <c r="G51" s="32"/>
     </row>
     <row r="52" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
@@ -8094,7 +8125,7 @@
       <c r="F52" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="G52" s="27"/>
+      <c r="G52" s="32"/>
     </row>
     <row r="53" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
@@ -8115,7 +8146,7 @@
       <c r="F53" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="G53" s="27"/>
+      <c r="G53" s="32"/>
     </row>
     <row r="54" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
@@ -8136,7 +8167,7 @@
       <c r="F54" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="G54" s="27"/>
+      <c r="G54" s="32"/>
     </row>
     <row r="55" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
@@ -8157,7 +8188,7 @@
       <c r="F55" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="G55" s="27"/>
+      <c r="G55" s="32"/>
     </row>
     <row r="56" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
@@ -8178,7 +8209,7 @@
       <c r="F56" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="G56" s="27"/>
+      <c r="G56" s="32"/>
     </row>
     <row r="57" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="9" t="s">
@@ -8199,7 +8230,7 @@
       <c r="F57" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="G57" s="27"/>
+      <c r="G57" s="32"/>
     </row>
     <row r="58" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
@@ -8220,7 +8251,7 @@
       <c r="F58" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="G58" s="27" t="s">
+      <c r="G58" s="32" t="s">
         <v>372</v>
       </c>
     </row>
@@ -8243,7 +8274,7 @@
       <c r="F59" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="G59" s="27"/>
+      <c r="G59" s="32"/>
     </row>
     <row r="60" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
@@ -8264,7 +8295,7 @@
       <c r="F60" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="G60" s="27"/>
+      <c r="G60" s="32"/>
     </row>
     <row r="61" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
@@ -8285,7 +8316,7 @@
       <c r="F61" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="G61" s="27"/>
+      <c r="G61" s="32"/>
     </row>
     <row r="62" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
@@ -8306,7 +8337,7 @@
       <c r="F62" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="G62" s="27"/>
+      <c r="G62" s="32"/>
     </row>
     <row r="63" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
@@ -8327,7 +8358,7 @@
       <c r="F63" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="G63" s="27"/>
+      <c r="G63" s="32"/>
     </row>
     <row r="64" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
@@ -8348,7 +8379,7 @@
       <c r="F64" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="G64" s="27"/>
+      <c r="G64" s="32"/>
     </row>
     <row r="65" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
@@ -8369,7 +8400,7 @@
       <c r="F65" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="G65" s="27"/>
+      <c r="G65" s="32"/>
     </row>
     <row r="66" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="9" t="s">
@@ -8390,7 +8421,7 @@
       <c r="F66" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="G66" s="27"/>
+      <c r="G66" s="32"/>
     </row>
     <row r="67" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
@@ -8411,7 +8442,7 @@
       <c r="F67" t="s">
         <v>93</v>
       </c>
-      <c r="G67" s="27" t="s">
+      <c r="G67" s="32" t="s">
         <v>366</v>
       </c>
     </row>
@@ -8434,7 +8465,7 @@
       <c r="F68" t="s">
         <v>93</v>
       </c>
-      <c r="G68" s="27"/>
+      <c r="G68" s="32"/>
     </row>
     <row r="69" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
@@ -8455,7 +8486,7 @@
       <c r="F69" t="s">
         <v>94</v>
       </c>
-      <c r="G69" s="27"/>
+      <c r="G69" s="32"/>
     </row>
     <row r="70" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
@@ -8476,7 +8507,7 @@
       <c r="F70" t="s">
         <v>94</v>
       </c>
-      <c r="G70" s="27"/>
+      <c r="G70" s="32"/>
     </row>
     <row r="71" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
@@ -8497,7 +8528,7 @@
       <c r="F71" t="s">
         <v>95</v>
       </c>
-      <c r="G71" s="27"/>
+      <c r="G71" s="32"/>
     </row>
     <row r="72" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="9" t="s">
@@ -8518,7 +8549,7 @@
       <c r="F72" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="G72" s="27"/>
+      <c r="G72" s="32"/>
     </row>
     <row r="73" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A73" s="14" t="s">
@@ -8539,7 +8570,7 @@
       <c r="F73" t="s">
         <v>97</v>
       </c>
-      <c r="G73" s="27" t="s">
+      <c r="G73" s="32" t="s">
         <v>367</v>
       </c>
     </row>
@@ -8562,7 +8593,7 @@
       <c r="F74" t="s">
         <v>97</v>
       </c>
-      <c r="G74" s="27"/>
+      <c r="G74" s="32"/>
     </row>
     <row r="75" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="14" t="s">
@@ -8583,7 +8614,7 @@
       <c r="F75" t="s">
         <v>98</v>
       </c>
-      <c r="G75" s="27"/>
+      <c r="G75" s="32"/>
     </row>
     <row r="76" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A76" s="14" t="s">
@@ -8604,7 +8635,7 @@
       <c r="F76" t="s">
         <v>98</v>
       </c>
-      <c r="G76" s="27"/>
+      <c r="G76" s="32"/>
     </row>
     <row r="77" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A77" s="14" t="s">
@@ -8625,7 +8656,7 @@
       <c r="F77" t="s">
         <v>100</v>
       </c>
-      <c r="G77" s="27"/>
+      <c r="G77" s="32"/>
     </row>
     <row r="78" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="15" t="s">
@@ -8646,7 +8677,7 @@
       <c r="F78" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="G78" s="27"/>
+      <c r="G78" s="32"/>
     </row>
     <row r="79" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A79" s="14" t="s">
@@ -8667,7 +8698,7 @@
       <c r="F79" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="G79" s="27" t="s">
+      <c r="G79" s="32" t="s">
         <v>368</v>
       </c>
     </row>
@@ -8690,7 +8721,7 @@
       <c r="F80" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="G80" s="27"/>
+      <c r="G80" s="32"/>
     </row>
     <row r="81" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A81" s="14" t="s">
@@ -8711,7 +8742,7 @@
       <c r="F81" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="G81" s="27"/>
+      <c r="G81" s="32"/>
     </row>
     <row r="82" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A82" s="14" t="s">
@@ -8732,7 +8763,7 @@
       <c r="F82" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="G82" s="27"/>
+      <c r="G82" s="32"/>
     </row>
     <row r="83" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A83" s="14" t="s">
@@ -8753,7 +8784,7 @@
       <c r="F83" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="G83" s="27"/>
+      <c r="G83" s="32"/>
     </row>
     <row r="84" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A84" s="15" t="s">
@@ -8774,7 +8805,7 @@
       <c r="F84" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="G84" s="27"/>
+      <c r="G84" s="32"/>
     </row>
     <row r="85" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A85" s="14" t="s">
@@ -8795,7 +8826,7 @@
       <c r="F85" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="G85" s="27" t="s">
+      <c r="G85" s="32" t="s">
         <v>369</v>
       </c>
     </row>
@@ -8818,7 +8849,7 @@
       <c r="F86" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="G86" s="27"/>
+      <c r="G86" s="32"/>
     </row>
     <row r="87" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A87" s="14" t="s">
@@ -8839,7 +8870,7 @@
       <c r="F87" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G87" s="27"/>
+      <c r="G87" s="32"/>
     </row>
     <row r="88" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A88" s="14" t="s">
@@ -8860,7 +8891,7 @@
       <c r="F88" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G88" s="27"/>
+      <c r="G88" s="32"/>
     </row>
     <row r="89" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A89" s="14" t="s">
@@ -8881,7 +8912,7 @@
       <c r="F89" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="G89" s="27"/>
+      <c r="G89" s="32"/>
     </row>
     <row r="90" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A90" s="15" t="s">
@@ -8902,7 +8933,7 @@
       <c r="F90" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="G90" s="27"/>
+      <c r="G90" s="32"/>
     </row>
     <row r="91" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A91" s="14" t="s">
@@ -8923,7 +8954,7 @@
       <c r="F91" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G91" s="27" t="s">
+      <c r="G91" s="32" t="s">
         <v>370</v>
       </c>
     </row>
@@ -8946,7 +8977,7 @@
       <c r="F92" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G92" s="27"/>
+      <c r="G92" s="32"/>
     </row>
     <row r="93" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A93" s="14" t="s">
@@ -8967,7 +8998,7 @@
       <c r="F93" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G93" s="27"/>
+      <c r="G93" s="32"/>
     </row>
     <row r="94" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A94" s="14" t="s">
@@ -8988,7 +9019,7 @@
       <c r="F94" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G94" s="27"/>
+      <c r="G94" s="32"/>
     </row>
     <row r="95" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A95" s="14" t="s">
@@ -9009,7 +9040,7 @@
       <c r="F95" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G95" s="27"/>
+      <c r="G95" s="32"/>
     </row>
     <row r="96" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A96" s="15" t="s">
@@ -9030,7 +9061,7 @@
       <c r="F96" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="G96" s="27"/>
+      <c r="G96" s="32"/>
     </row>
     <row r="97" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A97" s="20" t="s">
@@ -9051,7 +9082,7 @@
       <c r="F97" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="G97" s="27" t="s">
+      <c r="G97" s="32" t="s">
         <v>371</v>
       </c>
     </row>
@@ -9074,7 +9105,7 @@
       <c r="F98" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="G98" s="27"/>
+      <c r="G98" s="32"/>
     </row>
     <row r="99" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A99" s="14" t="s">
@@ -9095,7 +9126,7 @@
       <c r="F99" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="G99" s="27"/>
+      <c r="G99" s="32"/>
     </row>
     <row r="100" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A100" s="14" t="s">
@@ -9116,7 +9147,7 @@
       <c r="F100" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="G100" s="27"/>
+      <c r="G100" s="32"/>
     </row>
     <row r="101" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A101" s="14" t="s">
@@ -9137,7 +9168,7 @@
       <c r="F101" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="G101" s="27"/>
+      <c r="G101" s="32"/>
     </row>
     <row r="102" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A102" s="15" t="s">
@@ -9158,7 +9189,7 @@
       <c r="F102" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="G102" s="27"/>
+      <c r="G102" s="32"/>
     </row>
     <row r="103" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A103" s="14" t="s">
@@ -9179,7 +9210,7 @@
       <c r="F103" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G103" s="27" t="s">
+      <c r="G103" s="32" t="s">
         <v>372</v>
       </c>
     </row>
@@ -9202,7 +9233,7 @@
       <c r="F104" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G104" s="27"/>
+      <c r="G104" s="32"/>
     </row>
     <row r="105" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A105" s="14" t="s">
@@ -9223,7 +9254,7 @@
       <c r="F105" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G105" s="27"/>
+      <c r="G105" s="32"/>
     </row>
     <row r="106" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A106" s="14" t="s">
@@ -9244,7 +9275,7 @@
       <c r="F106" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G106" s="27"/>
+      <c r="G106" s="32"/>
     </row>
     <row r="107" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A107" s="14" t="s">
@@ -9265,7 +9296,7 @@
       <c r="F107" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G107" s="27"/>
+      <c r="G107" s="32"/>
     </row>
     <row r="108" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A108" s="15" t="s">
@@ -9286,7 +9317,7 @@
       <c r="F108" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="G108" s="27"/>
+      <c r="G108" s="32"/>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109" s="14" t="s">
@@ -9307,7 +9338,7 @@
       <c r="F109" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="G109" s="29" t="s">
+      <c r="G109" s="27" t="s">
         <v>382</v>
       </c>
     </row>
@@ -9330,7 +9361,7 @@
       <c r="F110" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="G110" s="30"/>
+      <c r="G110" s="28"/>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111" s="14" t="s">
@@ -9351,7 +9382,7 @@
       <c r="F111" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="G111" s="30"/>
+      <c r="G111" s="28"/>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112" s="14" t="s">
@@ -9372,7 +9403,7 @@
       <c r="F112" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="G112" s="30"/>
+      <c r="G112" s="28"/>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113" s="14" t="s">
@@ -9393,7 +9424,7 @@
       <c r="F113" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="G113" s="30"/>
+      <c r="G113" s="28"/>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114" s="14" t="s">
@@ -9414,7 +9445,7 @@
       <c r="F114" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="G114" s="30"/>
+      <c r="G114" s="28"/>
     </row>
     <row r="115" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A115" s="15" t="s">
@@ -9435,7 +9466,7 @@
       <c r="F115" s="12" t="s">
         <v>381</v>
       </c>
-      <c r="G115" s="30"/>
+      <c r="G115" s="28"/>
     </row>
     <row r="116" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A116" s="14" t="s">
@@ -9456,7 +9487,7 @@
       <c r="F116" s="3" t="s">
         <v>397</v>
       </c>
-      <c r="G116" s="31" t="s">
+      <c r="G116" s="30" t="s">
         <v>398</v>
       </c>
     </row>
@@ -9479,7 +9510,7 @@
       <c r="F117" s="3" t="s">
         <v>397</v>
       </c>
-      <c r="G117" s="31"/>
+      <c r="G117" s="30"/>
     </row>
     <row r="118" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A118" s="14" t="s">
@@ -9500,7 +9531,7 @@
       <c r="F118" s="3" t="s">
         <v>400</v>
       </c>
-      <c r="G118" s="31"/>
+      <c r="G118" s="30"/>
     </row>
     <row r="119" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A119" s="14" t="s">
@@ -9521,7 +9552,7 @@
       <c r="F119" s="3" t="s">
         <v>400</v>
       </c>
-      <c r="G119" s="31"/>
+      <c r="G119" s="30"/>
     </row>
     <row r="120" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A120" s="14" t="s">
@@ -9542,7 +9573,7 @@
       <c r="F120" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="G120" s="31"/>
+      <c r="G120" s="30"/>
     </row>
     <row r="121" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A121" s="14" t="s">
@@ -9563,7 +9594,7 @@
       <c r="F121" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="G121" s="31"/>
+      <c r="G121" s="30"/>
     </row>
     <row r="122" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A122" s="15" t="s">
@@ -9584,7 +9615,7 @@
       <c r="F122" s="12" t="s">
         <v>344</v>
       </c>
-      <c r="G122" s="31"/>
+      <c r="G122" s="30"/>
     </row>
     <row r="123" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A123" s="14" t="s">
@@ -9605,7 +9636,7 @@
       <c r="F123" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="G123" s="31" t="s">
+      <c r="G123" s="30" t="s">
         <v>402</v>
       </c>
     </row>
@@ -9628,7 +9659,7 @@
       <c r="F124" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="G124" s="31"/>
+      <c r="G124" s="30"/>
     </row>
     <row r="125" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A125" s="14" t="s">
@@ -9649,7 +9680,7 @@
       <c r="F125" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="G125" s="31"/>
+      <c r="G125" s="30"/>
     </row>
     <row r="126" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A126" s="14" t="s">
@@ -9670,7 +9701,7 @@
       <c r="F126" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="G126" s="31"/>
+      <c r="G126" s="30"/>
     </row>
     <row r="127" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A127" s="14" t="s">
@@ -9691,7 +9722,7 @@
       <c r="F127" s="3" t="s">
         <v>346</v>
       </c>
-      <c r="G127" s="31"/>
+      <c r="G127" s="30"/>
     </row>
     <row r="128" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A128" s="14" t="s">
@@ -9712,7 +9743,7 @@
       <c r="F128" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="G128" s="31"/>
+      <c r="G128" s="30"/>
     </row>
     <row r="129" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A129" s="15" t="s">
@@ -9733,7 +9764,7 @@
       <c r="F129" s="12" t="s">
         <v>351</v>
       </c>
-      <c r="G129" s="31"/>
+      <c r="G129" s="30"/>
     </row>
     <row r="130" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A130" s="14" t="s">
@@ -9754,7 +9785,7 @@
       <c r="F130" s="3" t="s">
         <v>353</v>
       </c>
-      <c r="G130" s="32" t="s">
+      <c r="G130" s="31" t="s">
         <v>410</v>
       </c>
     </row>
@@ -9777,7 +9808,7 @@
       <c r="F131" s="12" t="s">
         <v>355</v>
       </c>
-      <c r="G131" s="32"/>
+      <c r="G131" s="31"/>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132" s="14" t="s">
@@ -9798,7 +9829,7 @@
       <c r="F132" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="G132" s="29" t="s">
+      <c r="G132" s="27" t="s">
         <v>446</v>
       </c>
     </row>
@@ -9821,7 +9852,7 @@
       <c r="F133" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="G133" s="30"/>
+      <c r="G133" s="28"/>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A134" s="14" t="s">
@@ -9842,7 +9873,7 @@
       <c r="F134" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="G134" s="30"/>
+      <c r="G134" s="28"/>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A135" s="14" t="s">
@@ -9863,7 +9894,7 @@
       <c r="F135" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="G135" s="30"/>
+      <c r="G135" s="28"/>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A136" s="14" t="s">
@@ -9884,7 +9915,7 @@
       <c r="F136" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="G136" s="30"/>
+      <c r="G136" s="28"/>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A137" s="14" t="s">
@@ -9905,7 +9936,7 @@
       <c r="F137" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="G137" s="30"/>
+      <c r="G137" s="28"/>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A138" s="14" t="s">
@@ -9926,7 +9957,7 @@
       <c r="F138" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="G138" s="30"/>
+      <c r="G138" s="28"/>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A139" s="14" t="s">
@@ -9947,7 +9978,7 @@
       <c r="F139" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="G139" s="30"/>
+      <c r="G139" s="28"/>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A140" s="14" t="s">
@@ -9968,7 +9999,7 @@
       <c r="F140" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="G140" s="30"/>
+      <c r="G140" s="28"/>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A141" s="14" t="s">
@@ -9989,7 +10020,7 @@
       <c r="F141" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="G141" s="30"/>
+      <c r="G141" s="28"/>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A142" s="14" t="s">
@@ -10010,7 +10041,7 @@
       <c r="F142" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="G142" s="30"/>
+      <c r="G142" s="28"/>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A143" s="14" t="s">
@@ -10031,7 +10062,7 @@
       <c r="F143" s="3" t="s">
         <v>439</v>
       </c>
-      <c r="G143" s="30"/>
+      <c r="G143" s="28"/>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A144" s="14" t="s">
@@ -10052,7 +10083,7 @@
       <c r="F144" s="3" t="s">
         <v>439</v>
       </c>
-      <c r="G144" s="30"/>
+      <c r="G144" s="28"/>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A145" s="14" t="s">
@@ -10073,7 +10104,7 @@
       <c r="F145" s="3" t="s">
         <v>439</v>
       </c>
-      <c r="G145" s="30"/>
+      <c r="G145" s="28"/>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A146" s="14" t="s">
@@ -10094,7 +10125,7 @@
       <c r="F146" s="3" t="s">
         <v>439</v>
       </c>
-      <c r="G146" s="30"/>
+      <c r="G146" s="28"/>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A147" s="14" t="s">
@@ -10115,7 +10146,7 @@
       <c r="F147" s="3" t="s">
         <v>439</v>
       </c>
-      <c r="G147" s="30"/>
+      <c r="G147" s="28"/>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A148" s="14" t="s">
@@ -10136,7 +10167,7 @@
       <c r="F148" s="3" t="s">
         <v>439</v>
       </c>
-      <c r="G148" s="30"/>
+      <c r="G148" s="28"/>
     </row>
     <row r="149" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A149" s="15" t="s">
@@ -10157,7 +10188,7 @@
       <c r="F149" s="12" t="s">
         <v>439</v>
       </c>
-      <c r="G149" s="33"/>
+      <c r="G149" s="29"/>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A150" s="14" t="s">
@@ -10184,11 +10215,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="G132:G149"/>
-    <mergeCell ref="G109:G115"/>
-    <mergeCell ref="G116:G122"/>
-    <mergeCell ref="G123:G129"/>
-    <mergeCell ref="G130:G131"/>
     <mergeCell ref="G97:G102"/>
     <mergeCell ref="G103:G108"/>
     <mergeCell ref="G91:G96"/>
@@ -10203,6 +10229,11 @@
     <mergeCell ref="G73:G78"/>
     <mergeCell ref="G79:G84"/>
     <mergeCell ref="G85:G90"/>
+    <mergeCell ref="G132:G149"/>
+    <mergeCell ref="G109:G115"/>
+    <mergeCell ref="G116:G122"/>
+    <mergeCell ref="G123:G129"/>
+    <mergeCell ref="G130:G131"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Updated BOM, experimented with some circuit parameters
</commit_message>
<xml_diff>
--- a/Documents/BOM.xlsx
+++ b/Documents/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ECE_Projects\Music_Visualizer\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47826A37-FEAF-49FC-AEBE-B5D5F29F8103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50C3F1FD-1E4C-4162-820A-6F786C83F422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="824" activeTab="13" xr2:uid="{1F4A7036-4694-4970-BB5D-7CBECC831452}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="824" firstSheet="1" activeTab="14" xr2:uid="{1F4A7036-4694-4970-BB5D-7CBECC831452}"/>
   </bookViews>
   <sheets>
     <sheet name="Sub-Bass" sheetId="1" r:id="rId1"/>
@@ -1543,6 +1543,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1557,12 +1563,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2355,10 +2355,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F0F8697-67F6-479D-8A67-86E9F1D85B02}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2506,6 +2506,12 @@
       </c>
       <c r="F7" s="3" t="s">
         <v>334</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C8">
+        <f>SUM(C2:C7)</f>
+        <v>4.5540000000000003</v>
       </c>
     </row>
   </sheetData>
@@ -2960,7 +2966,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3267,6 +3273,10 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C16" s="2">
+        <f>C2+C3+C4+C15</f>
+        <v>8.23</v>
+      </c>
       <c r="F16" s="3"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.3">
@@ -3304,7 +3314,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3415,10 +3425,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBB0EED6-7AEC-4823-91A2-5A66F8F096F2}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3530,6 +3540,12 @@
       </c>
       <c r="F6" s="3" t="s">
         <v>450</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <f>SUM(C2:C6)</f>
+        <v>8.2929999999999993</v>
       </c>
     </row>
   </sheetData>
@@ -3547,10 +3563,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{422FDBAB-416A-4921-A7D0-3405100F2A2C}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20:F20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4025,6 +4041,12 @@
       </c>
       <c r="F24" s="3" t="s">
         <v>425</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C25">
+        <f>SUM(C2,C3,C20,C21,C22,C23,C24)</f>
+        <v>43.967000000000006</v>
       </c>
     </row>
   </sheetData>
@@ -7006,10 +7028,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5E7DEB4-5FFB-4F8D-963A-C08EFBE9A2C1}">
-  <dimension ref="A1:G150"/>
+  <dimension ref="A1:G151"/>
   <sheetViews>
-    <sheetView topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="B154" sqref="B154"/>
+    <sheetView topLeftCell="A125" workbookViewId="0">
+      <selection activeCell="C152" sqref="C152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7063,7 +7085,7 @@
       <c r="F2" t="s">
         <v>88</v>
       </c>
-      <c r="G2" s="33" t="s">
+      <c r="G2" s="28" t="s">
         <v>366</v>
       </c>
     </row>
@@ -7086,7 +7108,7 @@
       <c r="F3" t="s">
         <v>88</v>
       </c>
-      <c r="G3" s="33"/>
+      <c r="G3" s="28"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -7107,7 +7129,7 @@
       <c r="F4" t="s">
         <v>88</v>
       </c>
-      <c r="G4" s="33"/>
+      <c r="G4" s="28"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -7128,7 +7150,7 @@
       <c r="F5" t="s">
         <v>90</v>
       </c>
-      <c r="G5" s="33"/>
+      <c r="G5" s="28"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -7149,7 +7171,7 @@
       <c r="F6" t="s">
         <v>88</v>
       </c>
-      <c r="G6" s="33"/>
+      <c r="G6" s="28"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -7170,7 +7192,7 @@
       <c r="F7" t="s">
         <v>88</v>
       </c>
-      <c r="G7" s="33"/>
+      <c r="G7" s="28"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -7191,7 +7213,7 @@
       <c r="F8" t="s">
         <v>91</v>
       </c>
-      <c r="G8" s="33"/>
+      <c r="G8" s="28"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -7212,7 +7234,7 @@
       <c r="F9" t="s">
         <v>91</v>
       </c>
-      <c r="G9" s="33"/>
+      <c r="G9" s="28"/>
     </row>
     <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
@@ -7233,7 +7255,7 @@
       <c r="F10" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="G10" s="33"/>
+      <c r="G10" s="28"/>
     </row>
     <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
@@ -7254,7 +7276,7 @@
       <c r="F11" t="s">
         <v>88</v>
       </c>
-      <c r="G11" s="32" t="s">
+      <c r="G11" s="27" t="s">
         <v>367</v>
       </c>
     </row>
@@ -7277,7 +7299,7 @@
       <c r="F12" t="s">
         <v>90</v>
       </c>
-      <c r="G12" s="32"/>
+      <c r="G12" s="27"/>
     </row>
     <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -7298,7 +7320,7 @@
       <c r="F13" t="s">
         <v>88</v>
       </c>
-      <c r="G13" s="32"/>
+      <c r="G13" s="27"/>
     </row>
     <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
@@ -7319,7 +7341,7 @@
       <c r="F14" t="s">
         <v>88</v>
       </c>
-      <c r="G14" s="32"/>
+      <c r="G14" s="27"/>
     </row>
     <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
@@ -7340,7 +7362,7 @@
       <c r="F15" t="s">
         <v>88</v>
       </c>
-      <c r="G15" s="32"/>
+      <c r="G15" s="27"/>
     </row>
     <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
@@ -7361,7 +7383,7 @@
       <c r="F16" t="s">
         <v>88</v>
       </c>
-      <c r="G16" s="32"/>
+      <c r="G16" s="27"/>
     </row>
     <row r="17" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
@@ -7382,7 +7404,7 @@
       <c r="F17" t="s">
         <v>88</v>
       </c>
-      <c r="G17" s="32"/>
+      <c r="G17" s="27"/>
     </row>
     <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
@@ -7403,7 +7425,7 @@
       <c r="F18" t="s">
         <v>96</v>
       </c>
-      <c r="G18" s="32"/>
+      <c r="G18" s="27"/>
     </row>
     <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
@@ -7424,7 +7446,7 @@
       <c r="F19" t="s">
         <v>88</v>
       </c>
-      <c r="G19" s="32"/>
+      <c r="G19" s="27"/>
     </row>
     <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
@@ -7445,7 +7467,7 @@
       <c r="F20" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="G20" s="32"/>
+      <c r="G20" s="27"/>
     </row>
     <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
@@ -7466,7 +7488,7 @@
       <c r="F21" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="G21" s="32" t="s">
+      <c r="G21" s="27" t="s">
         <v>368</v>
       </c>
     </row>
@@ -7489,7 +7511,7 @@
       <c r="F22" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G22" s="32"/>
+      <c r="G22" s="27"/>
     </row>
     <row r="23" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
@@ -7510,7 +7532,7 @@
       <c r="F23" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="G23" s="32"/>
+      <c r="G23" s="27"/>
     </row>
     <row r="24" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
@@ -7531,7 +7553,7 @@
       <c r="F24" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="G24" s="32"/>
+      <c r="G24" s="27"/>
     </row>
     <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
@@ -7552,7 +7574,7 @@
       <c r="F25" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="G25" s="32"/>
+      <c r="G25" s="27"/>
     </row>
     <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
@@ -7573,7 +7595,7 @@
       <c r="F26" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="G26" s="32"/>
+      <c r="G26" s="27"/>
     </row>
     <row r="27" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
@@ -7594,7 +7616,7 @@
       <c r="F27" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="G27" s="32"/>
+      <c r="G27" s="27"/>
     </row>
     <row r="28" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
@@ -7615,7 +7637,7 @@
       <c r="F28" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="G28" s="32"/>
+      <c r="G28" s="27"/>
     </row>
     <row r="29" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="9" t="s">
@@ -7636,7 +7658,7 @@
       <c r="F29" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="G29" s="32"/>
+      <c r="G29" s="27"/>
     </row>
     <row r="30" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
@@ -7657,7 +7679,7 @@
       <c r="F30" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="G30" s="32" t="s">
+      <c r="G30" s="27" t="s">
         <v>369</v>
       </c>
     </row>
@@ -7680,7 +7702,7 @@
       <c r="F31" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="G31" s="32"/>
+      <c r="G31" s="27"/>
     </row>
     <row r="32" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
@@ -7701,7 +7723,7 @@
       <c r="F32" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="G32" s="32"/>
+      <c r="G32" s="27"/>
     </row>
     <row r="33" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
@@ -7722,7 +7744,7 @@
       <c r="F33" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="G33" s="32"/>
+      <c r="G33" s="27"/>
     </row>
     <row r="34" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
@@ -7743,7 +7765,7 @@
       <c r="F34" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="G34" s="32"/>
+      <c r="G34" s="27"/>
     </row>
     <row r="35" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
@@ -7764,7 +7786,7 @@
       <c r="F35" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="G35" s="32"/>
+      <c r="G35" s="27"/>
     </row>
     <row r="36" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
@@ -7785,7 +7807,7 @@
       <c r="F36" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="G36" s="32"/>
+      <c r="G36" s="27"/>
     </row>
     <row r="37" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
@@ -7806,7 +7828,7 @@
       <c r="F37" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="G37" s="32"/>
+      <c r="G37" s="27"/>
     </row>
     <row r="38" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
@@ -7827,7 +7849,7 @@
       <c r="F38" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="G38" s="32"/>
+      <c r="G38" s="27"/>
     </row>
     <row r="39" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="9" t="s">
@@ -7848,7 +7870,7 @@
       <c r="F39" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="G39" s="32"/>
+      <c r="G39" s="27"/>
     </row>
     <row r="40" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
@@ -7869,7 +7891,7 @@
       <c r="F40" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="G40" s="32" t="s">
+      <c r="G40" s="27" t="s">
         <v>370</v>
       </c>
     </row>
@@ -7892,7 +7914,7 @@
       <c r="F41" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="G41" s="32"/>
+      <c r="G41" s="27"/>
     </row>
     <row r="42" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
@@ -7913,7 +7935,7 @@
       <c r="F42" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="G42" s="32"/>
+      <c r="G42" s="27"/>
     </row>
     <row r="43" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
@@ -7934,7 +7956,7 @@
       <c r="F43" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="G43" s="32"/>
+      <c r="G43" s="27"/>
     </row>
     <row r="44" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
@@ -7955,7 +7977,7 @@
       <c r="F44" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="G44" s="32"/>
+      <c r="G44" s="27"/>
     </row>
     <row r="45" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
@@ -7976,7 +7998,7 @@
       <c r="F45" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="G45" s="32"/>
+      <c r="G45" s="27"/>
     </row>
     <row r="46" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
@@ -7997,7 +8019,7 @@
       <c r="F46" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="G46" s="32"/>
+      <c r="G46" s="27"/>
     </row>
     <row r="47" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
@@ -8018,7 +8040,7 @@
       <c r="F47" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="G47" s="32"/>
+      <c r="G47" s="27"/>
     </row>
     <row r="48" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="9" t="s">
@@ -8039,7 +8061,7 @@
       <c r="F48" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="G48" s="32"/>
+      <c r="G48" s="27"/>
     </row>
     <row r="49" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
@@ -8060,7 +8082,7 @@
       <c r="F49" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="G49" s="32" t="s">
+      <c r="G49" s="27" t="s">
         <v>371</v>
       </c>
     </row>
@@ -8083,7 +8105,7 @@
       <c r="F50" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="G50" s="32"/>
+      <c r="G50" s="27"/>
     </row>
     <row r="51" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
@@ -8104,7 +8126,7 @@
       <c r="F51" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="G51" s="32"/>
+      <c r="G51" s="27"/>
     </row>
     <row r="52" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
@@ -8125,7 +8147,7 @@
       <c r="F52" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="G52" s="32"/>
+      <c r="G52" s="27"/>
     </row>
     <row r="53" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
@@ -8146,7 +8168,7 @@
       <c r="F53" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="G53" s="32"/>
+      <c r="G53" s="27"/>
     </row>
     <row r="54" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
@@ -8167,7 +8189,7 @@
       <c r="F54" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="G54" s="32"/>
+      <c r="G54" s="27"/>
     </row>
     <row r="55" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
@@ -8188,7 +8210,7 @@
       <c r="F55" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="G55" s="32"/>
+      <c r="G55" s="27"/>
     </row>
     <row r="56" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
@@ -8209,7 +8231,7 @@
       <c r="F56" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="G56" s="32"/>
+      <c r="G56" s="27"/>
     </row>
     <row r="57" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="9" t="s">
@@ -8230,7 +8252,7 @@
       <c r="F57" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="G57" s="32"/>
+      <c r="G57" s="27"/>
     </row>
     <row r="58" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
@@ -8251,7 +8273,7 @@
       <c r="F58" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="G58" s="32" t="s">
+      <c r="G58" s="27" t="s">
         <v>372</v>
       </c>
     </row>
@@ -8274,7 +8296,7 @@
       <c r="F59" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="G59" s="32"/>
+      <c r="G59" s="27"/>
     </row>
     <row r="60" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
@@ -8295,7 +8317,7 @@
       <c r="F60" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="G60" s="32"/>
+      <c r="G60" s="27"/>
     </row>
     <row r="61" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
@@ -8316,7 +8338,7 @@
       <c r="F61" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="G61" s="32"/>
+      <c r="G61" s="27"/>
     </row>
     <row r="62" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
@@ -8337,7 +8359,7 @@
       <c r="F62" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="G62" s="32"/>
+      <c r="G62" s="27"/>
     </row>
     <row r="63" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
@@ -8358,7 +8380,7 @@
       <c r="F63" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="G63" s="32"/>
+      <c r="G63" s="27"/>
     </row>
     <row r="64" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
@@ -8379,7 +8401,7 @@
       <c r="F64" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="G64" s="32"/>
+      <c r="G64" s="27"/>
     </row>
     <row r="65" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
@@ -8400,7 +8422,7 @@
       <c r="F65" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="G65" s="32"/>
+      <c r="G65" s="27"/>
     </row>
     <row r="66" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="9" t="s">
@@ -8421,7 +8443,7 @@
       <c r="F66" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="G66" s="32"/>
+      <c r="G66" s="27"/>
     </row>
     <row r="67" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
@@ -8442,7 +8464,7 @@
       <c r="F67" t="s">
         <v>93</v>
       </c>
-      <c r="G67" s="32" t="s">
+      <c r="G67" s="27" t="s">
         <v>366</v>
       </c>
     </row>
@@ -8465,7 +8487,7 @@
       <c r="F68" t="s">
         <v>93</v>
       </c>
-      <c r="G68" s="32"/>
+      <c r="G68" s="27"/>
     </row>
     <row r="69" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
@@ -8486,7 +8508,7 @@
       <c r="F69" t="s">
         <v>94</v>
       </c>
-      <c r="G69" s="32"/>
+      <c r="G69" s="27"/>
     </row>
     <row r="70" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
@@ -8507,7 +8529,7 @@
       <c r="F70" t="s">
         <v>94</v>
       </c>
-      <c r="G70" s="32"/>
+      <c r="G70" s="27"/>
     </row>
     <row r="71" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
@@ -8528,7 +8550,7 @@
       <c r="F71" t="s">
         <v>95</v>
       </c>
-      <c r="G71" s="32"/>
+      <c r="G71" s="27"/>
     </row>
     <row r="72" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="9" t="s">
@@ -8549,7 +8571,7 @@
       <c r="F72" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="G72" s="32"/>
+      <c r="G72" s="27"/>
     </row>
     <row r="73" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A73" s="14" t="s">
@@ -8570,7 +8592,7 @@
       <c r="F73" t="s">
         <v>97</v>
       </c>
-      <c r="G73" s="32" t="s">
+      <c r="G73" s="27" t="s">
         <v>367</v>
       </c>
     </row>
@@ -8593,7 +8615,7 @@
       <c r="F74" t="s">
         <v>97</v>
       </c>
-      <c r="G74" s="32"/>
+      <c r="G74" s="27"/>
     </row>
     <row r="75" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="14" t="s">
@@ -8614,7 +8636,7 @@
       <c r="F75" t="s">
         <v>98</v>
       </c>
-      <c r="G75" s="32"/>
+      <c r="G75" s="27"/>
     </row>
     <row r="76" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A76" s="14" t="s">
@@ -8635,7 +8657,7 @@
       <c r="F76" t="s">
         <v>98</v>
       </c>
-      <c r="G76" s="32"/>
+      <c r="G76" s="27"/>
     </row>
     <row r="77" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A77" s="14" t="s">
@@ -8656,7 +8678,7 @@
       <c r="F77" t="s">
         <v>100</v>
       </c>
-      <c r="G77" s="32"/>
+      <c r="G77" s="27"/>
     </row>
     <row r="78" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="15" t="s">
@@ -8677,7 +8699,7 @@
       <c r="F78" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="G78" s="32"/>
+      <c r="G78" s="27"/>
     </row>
     <row r="79" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A79" s="14" t="s">
@@ -8698,7 +8720,7 @@
       <c r="F79" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="G79" s="32" t="s">
+      <c r="G79" s="27" t="s">
         <v>368</v>
       </c>
     </row>
@@ -8721,7 +8743,7 @@
       <c r="F80" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="G80" s="32"/>
+      <c r="G80" s="27"/>
     </row>
     <row r="81" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A81" s="14" t="s">
@@ -8742,7 +8764,7 @@
       <c r="F81" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="G81" s="32"/>
+      <c r="G81" s="27"/>
     </row>
     <row r="82" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A82" s="14" t="s">
@@ -8763,7 +8785,7 @@
       <c r="F82" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="G82" s="32"/>
+      <c r="G82" s="27"/>
     </row>
     <row r="83" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A83" s="14" t="s">
@@ -8784,7 +8806,7 @@
       <c r="F83" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="G83" s="32"/>
+      <c r="G83" s="27"/>
     </row>
     <row r="84" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A84" s="15" t="s">
@@ -8805,7 +8827,7 @@
       <c r="F84" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="G84" s="32"/>
+      <c r="G84" s="27"/>
     </row>
     <row r="85" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A85" s="14" t="s">
@@ -8826,7 +8848,7 @@
       <c r="F85" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="G85" s="32" t="s">
+      <c r="G85" s="27" t="s">
         <v>369</v>
       </c>
     </row>
@@ -8849,7 +8871,7 @@
       <c r="F86" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="G86" s="32"/>
+      <c r="G86" s="27"/>
     </row>
     <row r="87" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A87" s="14" t="s">
@@ -8870,7 +8892,7 @@
       <c r="F87" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G87" s="32"/>
+      <c r="G87" s="27"/>
     </row>
     <row r="88" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A88" s="14" t="s">
@@ -8891,7 +8913,7 @@
       <c r="F88" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G88" s="32"/>
+      <c r="G88" s="27"/>
     </row>
     <row r="89" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A89" s="14" t="s">
@@ -8912,7 +8934,7 @@
       <c r="F89" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="G89" s="32"/>
+      <c r="G89" s="27"/>
     </row>
     <row r="90" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A90" s="15" t="s">
@@ -8933,7 +8955,7 @@
       <c r="F90" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="G90" s="32"/>
+      <c r="G90" s="27"/>
     </row>
     <row r="91" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A91" s="14" t="s">
@@ -8954,7 +8976,7 @@
       <c r="F91" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G91" s="32" t="s">
+      <c r="G91" s="27" t="s">
         <v>370</v>
       </c>
     </row>
@@ -8977,7 +8999,7 @@
       <c r="F92" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G92" s="32"/>
+      <c r="G92" s="27"/>
     </row>
     <row r="93" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A93" s="14" t="s">
@@ -8998,7 +9020,7 @@
       <c r="F93" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G93" s="32"/>
+      <c r="G93" s="27"/>
     </row>
     <row r="94" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A94" s="14" t="s">
@@ -9019,7 +9041,7 @@
       <c r="F94" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G94" s="32"/>
+      <c r="G94" s="27"/>
     </row>
     <row r="95" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A95" s="14" t="s">
@@ -9040,7 +9062,7 @@
       <c r="F95" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G95" s="32"/>
+      <c r="G95" s="27"/>
     </row>
     <row r="96" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A96" s="15" t="s">
@@ -9061,7 +9083,7 @@
       <c r="F96" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="G96" s="32"/>
+      <c r="G96" s="27"/>
     </row>
     <row r="97" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A97" s="20" t="s">
@@ -9082,7 +9104,7 @@
       <c r="F97" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="G97" s="32" t="s">
+      <c r="G97" s="27" t="s">
         <v>371</v>
       </c>
     </row>
@@ -9105,7 +9127,7 @@
       <c r="F98" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="G98" s="32"/>
+      <c r="G98" s="27"/>
     </row>
     <row r="99" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A99" s="14" t="s">
@@ -9126,7 +9148,7 @@
       <c r="F99" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="G99" s="32"/>
+      <c r="G99" s="27"/>
     </row>
     <row r="100" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A100" s="14" t="s">
@@ -9147,7 +9169,7 @@
       <c r="F100" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="G100" s="32"/>
+      <c r="G100" s="27"/>
     </row>
     <row r="101" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A101" s="14" t="s">
@@ -9168,7 +9190,7 @@
       <c r="F101" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="G101" s="32"/>
+      <c r="G101" s="27"/>
     </row>
     <row r="102" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A102" s="15" t="s">
@@ -9189,7 +9211,7 @@
       <c r="F102" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="G102" s="32"/>
+      <c r="G102" s="27"/>
     </row>
     <row r="103" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A103" s="14" t="s">
@@ -9210,7 +9232,7 @@
       <c r="F103" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G103" s="32" t="s">
+      <c r="G103" s="27" t="s">
         <v>372</v>
       </c>
     </row>
@@ -9233,7 +9255,7 @@
       <c r="F104" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G104" s="32"/>
+      <c r="G104" s="27"/>
     </row>
     <row r="105" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A105" s="14" t="s">
@@ -9254,7 +9276,7 @@
       <c r="F105" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G105" s="32"/>
+      <c r="G105" s="27"/>
     </row>
     <row r="106" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A106" s="14" t="s">
@@ -9275,7 +9297,7 @@
       <c r="F106" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G106" s="32"/>
+      <c r="G106" s="27"/>
     </row>
     <row r="107" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A107" s="14" t="s">
@@ -9296,7 +9318,7 @@
       <c r="F107" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G107" s="32"/>
+      <c r="G107" s="27"/>
     </row>
     <row r="108" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A108" s="15" t="s">
@@ -9317,7 +9339,7 @@
       <c r="F108" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="G108" s="32"/>
+      <c r="G108" s="27"/>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109" s="14" t="s">
@@ -9338,7 +9360,7 @@
       <c r="F109" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="G109" s="27" t="s">
+      <c r="G109" s="29" t="s">
         <v>382</v>
       </c>
     </row>
@@ -9361,7 +9383,7 @@
       <c r="F110" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="G110" s="28"/>
+      <c r="G110" s="30"/>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111" s="14" t="s">
@@ -9382,7 +9404,7 @@
       <c r="F111" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="G111" s="28"/>
+      <c r="G111" s="30"/>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112" s="14" t="s">
@@ -9403,7 +9425,7 @@
       <c r="F112" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="G112" s="28"/>
+      <c r="G112" s="30"/>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113" s="14" t="s">
@@ -9424,7 +9446,7 @@
       <c r="F113" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="G113" s="28"/>
+      <c r="G113" s="30"/>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114" s="14" t="s">
@@ -9445,7 +9467,7 @@
       <c r="F114" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="G114" s="28"/>
+      <c r="G114" s="30"/>
     </row>
     <row r="115" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A115" s="15" t="s">
@@ -9466,7 +9488,7 @@
       <c r="F115" s="12" t="s">
         <v>381</v>
       </c>
-      <c r="G115" s="28"/>
+      <c r="G115" s="30"/>
     </row>
     <row r="116" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A116" s="14" t="s">
@@ -9487,7 +9509,7 @@
       <c r="F116" s="3" t="s">
         <v>397</v>
       </c>
-      <c r="G116" s="30" t="s">
+      <c r="G116" s="32" t="s">
         <v>398</v>
       </c>
     </row>
@@ -9510,7 +9532,7 @@
       <c r="F117" s="3" t="s">
         <v>397</v>
       </c>
-      <c r="G117" s="30"/>
+      <c r="G117" s="32"/>
     </row>
     <row r="118" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A118" s="14" t="s">
@@ -9531,7 +9553,7 @@
       <c r="F118" s="3" t="s">
         <v>400</v>
       </c>
-      <c r="G118" s="30"/>
+      <c r="G118" s="32"/>
     </row>
     <row r="119" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A119" s="14" t="s">
@@ -9552,7 +9574,7 @@
       <c r="F119" s="3" t="s">
         <v>400</v>
       </c>
-      <c r="G119" s="30"/>
+      <c r="G119" s="32"/>
     </row>
     <row r="120" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A120" s="14" t="s">
@@ -9573,7 +9595,7 @@
       <c r="F120" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="G120" s="30"/>
+      <c r="G120" s="32"/>
     </row>
     <row r="121" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A121" s="14" t="s">
@@ -9594,7 +9616,7 @@
       <c r="F121" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="G121" s="30"/>
+      <c r="G121" s="32"/>
     </row>
     <row r="122" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A122" s="15" t="s">
@@ -9615,7 +9637,7 @@
       <c r="F122" s="12" t="s">
         <v>344</v>
       </c>
-      <c r="G122" s="30"/>
+      <c r="G122" s="32"/>
     </row>
     <row r="123" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A123" s="14" t="s">
@@ -9636,7 +9658,7 @@
       <c r="F123" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="G123" s="30" t="s">
+      <c r="G123" s="32" t="s">
         <v>402</v>
       </c>
     </row>
@@ -9659,7 +9681,7 @@
       <c r="F124" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="G124" s="30"/>
+      <c r="G124" s="32"/>
     </row>
     <row r="125" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A125" s="14" t="s">
@@ -9680,7 +9702,7 @@
       <c r="F125" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="G125" s="30"/>
+      <c r="G125" s="32"/>
     </row>
     <row r="126" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A126" s="14" t="s">
@@ -9701,7 +9723,7 @@
       <c r="F126" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="G126" s="30"/>
+      <c r="G126" s="32"/>
     </row>
     <row r="127" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A127" s="14" t="s">
@@ -9722,7 +9744,7 @@
       <c r="F127" s="3" t="s">
         <v>346</v>
       </c>
-      <c r="G127" s="30"/>
+      <c r="G127" s="32"/>
     </row>
     <row r="128" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A128" s="14" t="s">
@@ -9743,7 +9765,7 @@
       <c r="F128" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="G128" s="30"/>
+      <c r="G128" s="32"/>
     </row>
     <row r="129" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A129" s="15" t="s">
@@ -9764,7 +9786,7 @@
       <c r="F129" s="12" t="s">
         <v>351</v>
       </c>
-      <c r="G129" s="30"/>
+      <c r="G129" s="32"/>
     </row>
     <row r="130" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A130" s="14" t="s">
@@ -9785,7 +9807,7 @@
       <c r="F130" s="3" t="s">
         <v>353</v>
       </c>
-      <c r="G130" s="31" t="s">
+      <c r="G130" s="33" t="s">
         <v>410</v>
       </c>
     </row>
@@ -9808,7 +9830,7 @@
       <c r="F131" s="12" t="s">
         <v>355</v>
       </c>
-      <c r="G131" s="31"/>
+      <c r="G131" s="33"/>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132" s="14" t="s">
@@ -9829,7 +9851,7 @@
       <c r="F132" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="G132" s="27" t="s">
+      <c r="G132" s="29" t="s">
         <v>446</v>
       </c>
     </row>
@@ -9852,7 +9874,7 @@
       <c r="F133" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="G133" s="28"/>
+      <c r="G133" s="30"/>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A134" s="14" t="s">
@@ -9873,7 +9895,7 @@
       <c r="F134" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="G134" s="28"/>
+      <c r="G134" s="30"/>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A135" s="14" t="s">
@@ -9894,7 +9916,7 @@
       <c r="F135" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="G135" s="28"/>
+      <c r="G135" s="30"/>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A136" s="14" t="s">
@@ -9915,7 +9937,7 @@
       <c r="F136" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="G136" s="28"/>
+      <c r="G136" s="30"/>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A137" s="14" t="s">
@@ -9936,7 +9958,7 @@
       <c r="F137" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="G137" s="28"/>
+      <c r="G137" s="30"/>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A138" s="14" t="s">
@@ -9957,7 +9979,7 @@
       <c r="F138" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="G138" s="28"/>
+      <c r="G138" s="30"/>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A139" s="14" t="s">
@@ -9978,7 +10000,7 @@
       <c r="F139" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="G139" s="28"/>
+      <c r="G139" s="30"/>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A140" s="14" t="s">
@@ -9999,7 +10021,7 @@
       <c r="F140" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="G140" s="28"/>
+      <c r="G140" s="30"/>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A141" s="14" t="s">
@@ -10020,7 +10042,7 @@
       <c r="F141" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="G141" s="28"/>
+      <c r="G141" s="30"/>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A142" s="14" t="s">
@@ -10041,7 +10063,7 @@
       <c r="F142" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="G142" s="28"/>
+      <c r="G142" s="30"/>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A143" s="14" t="s">
@@ -10062,7 +10084,7 @@
       <c r="F143" s="3" t="s">
         <v>439</v>
       </c>
-      <c r="G143" s="28"/>
+      <c r="G143" s="30"/>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A144" s="14" t="s">
@@ -10083,7 +10105,7 @@
       <c r="F144" s="3" t="s">
         <v>439</v>
       </c>
-      <c r="G144" s="28"/>
+      <c r="G144" s="30"/>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A145" s="14" t="s">
@@ -10104,7 +10126,7 @@
       <c r="F145" s="3" t="s">
         <v>439</v>
       </c>
-      <c r="G145" s="28"/>
+      <c r="G145" s="30"/>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A146" s="14" t="s">
@@ -10125,7 +10147,7 @@
       <c r="F146" s="3" t="s">
         <v>439</v>
       </c>
-      <c r="G146" s="28"/>
+      <c r="G146" s="30"/>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A147" s="14" t="s">
@@ -10146,7 +10168,7 @@
       <c r="F147" s="3" t="s">
         <v>439</v>
       </c>
-      <c r="G147" s="28"/>
+      <c r="G147" s="30"/>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A148" s="14" t="s">
@@ -10167,7 +10189,7 @@
       <c r="F148" s="3" t="s">
         <v>439</v>
       </c>
-      <c r="G148" s="28"/>
+      <c r="G148" s="30"/>
     </row>
     <row r="149" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A149" s="15" t="s">
@@ -10188,7 +10210,7 @@
       <c r="F149" s="12" t="s">
         <v>439</v>
       </c>
-      <c r="G149" s="29"/>
+      <c r="G149" s="31"/>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A150" s="14" t="s">
@@ -10213,8 +10235,19 @@
         <v>433</v>
       </c>
     </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C151" s="2">
+        <f>SUM(C2:C150)</f>
+        <v>26.940000000000058</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="G132:G149"/>
+    <mergeCell ref="G109:G115"/>
+    <mergeCell ref="G116:G122"/>
+    <mergeCell ref="G123:G129"/>
+    <mergeCell ref="G130:G131"/>
     <mergeCell ref="G97:G102"/>
     <mergeCell ref="G103:G108"/>
     <mergeCell ref="G91:G96"/>
@@ -10229,11 +10262,6 @@
     <mergeCell ref="G73:G78"/>
     <mergeCell ref="G79:G84"/>
     <mergeCell ref="G85:G90"/>
-    <mergeCell ref="G132:G149"/>
-    <mergeCell ref="G109:G115"/>
-    <mergeCell ref="G116:G122"/>
-    <mergeCell ref="G123:G129"/>
-    <mergeCell ref="G130:G131"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Finished digi-key BOM and made appropriate changes to schematic and PCB
</commit_message>
<xml_diff>
--- a/Documents/BOM.xlsx
+++ b/Documents/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ECE_Projects\Music_Visualizer\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50C3F1FD-1E4C-4162-820A-6F786C83F422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50382A14-6E1C-44C4-8369-A101FCB78335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="824" firstSheet="1" activeTab="14" xr2:uid="{1F4A7036-4694-4970-BB5D-7CBECC831452}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="824" activeTab="13" xr2:uid="{1F4A7036-4694-4970-BB5D-7CBECC831452}"/>
   </bookViews>
   <sheets>
     <sheet name="Sub-Bass" sheetId="1" r:id="rId1"/>
@@ -1543,12 +1543,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1563,6 +1557,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2358,7 +2358,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2966,7 +2966,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3314,7 +3314,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3427,8 +3427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBB0EED6-7AEC-4823-91A2-5A66F8F096F2}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3565,8 +3565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{422FDBAB-416A-4921-A7D0-3405100F2A2C}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7030,8 +7030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5E7DEB4-5FFB-4F8D-963A-C08EFBE9A2C1}">
   <dimension ref="A1:G151"/>
   <sheetViews>
-    <sheetView topLeftCell="A125" workbookViewId="0">
-      <selection activeCell="C152" sqref="C152"/>
+    <sheetView topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="D142" sqref="D142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7085,7 +7085,7 @@
       <c r="F2" t="s">
         <v>88</v>
       </c>
-      <c r="G2" s="28" t="s">
+      <c r="G2" s="33" t="s">
         <v>366</v>
       </c>
     </row>
@@ -7108,7 +7108,7 @@
       <c r="F3" t="s">
         <v>88</v>
       </c>
-      <c r="G3" s="28"/>
+      <c r="G3" s="33"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -7129,7 +7129,7 @@
       <c r="F4" t="s">
         <v>88</v>
       </c>
-      <c r="G4" s="28"/>
+      <c r="G4" s="33"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -7150,7 +7150,7 @@
       <c r="F5" t="s">
         <v>90</v>
       </c>
-      <c r="G5" s="28"/>
+      <c r="G5" s="33"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -7171,7 +7171,7 @@
       <c r="F6" t="s">
         <v>88</v>
       </c>
-      <c r="G6" s="28"/>
+      <c r="G6" s="33"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -7192,7 +7192,7 @@
       <c r="F7" t="s">
         <v>88</v>
       </c>
-      <c r="G7" s="28"/>
+      <c r="G7" s="33"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -7213,7 +7213,7 @@
       <c r="F8" t="s">
         <v>91</v>
       </c>
-      <c r="G8" s="28"/>
+      <c r="G8" s="33"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -7234,7 +7234,7 @@
       <c r="F9" t="s">
         <v>91</v>
       </c>
-      <c r="G9" s="28"/>
+      <c r="G9" s="33"/>
     </row>
     <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
@@ -7255,7 +7255,7 @@
       <c r="F10" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="G10" s="28"/>
+      <c r="G10" s="33"/>
     </row>
     <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
@@ -7276,7 +7276,7 @@
       <c r="F11" t="s">
         <v>88</v>
       </c>
-      <c r="G11" s="27" t="s">
+      <c r="G11" s="32" t="s">
         <v>367</v>
       </c>
     </row>
@@ -7299,7 +7299,7 @@
       <c r="F12" t="s">
         <v>90</v>
       </c>
-      <c r="G12" s="27"/>
+      <c r="G12" s="32"/>
     </row>
     <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -7320,7 +7320,7 @@
       <c r="F13" t="s">
         <v>88</v>
       </c>
-      <c r="G13" s="27"/>
+      <c r="G13" s="32"/>
     </row>
     <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
@@ -7341,7 +7341,7 @@
       <c r="F14" t="s">
         <v>88</v>
       </c>
-      <c r="G14" s="27"/>
+      <c r="G14" s="32"/>
     </row>
     <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
@@ -7362,7 +7362,7 @@
       <c r="F15" t="s">
         <v>88</v>
       </c>
-      <c r="G15" s="27"/>
+      <c r="G15" s="32"/>
     </row>
     <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
@@ -7383,7 +7383,7 @@
       <c r="F16" t="s">
         <v>88</v>
       </c>
-      <c r="G16" s="27"/>
+      <c r="G16" s="32"/>
     </row>
     <row r="17" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
@@ -7404,7 +7404,7 @@
       <c r="F17" t="s">
         <v>88</v>
       </c>
-      <c r="G17" s="27"/>
+      <c r="G17" s="32"/>
     </row>
     <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
@@ -7425,7 +7425,7 @@
       <c r="F18" t="s">
         <v>96</v>
       </c>
-      <c r="G18" s="27"/>
+      <c r="G18" s="32"/>
     </row>
     <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
@@ -7446,7 +7446,7 @@
       <c r="F19" t="s">
         <v>88</v>
       </c>
-      <c r="G19" s="27"/>
+      <c r="G19" s="32"/>
     </row>
     <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
@@ -7467,7 +7467,7 @@
       <c r="F20" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="G20" s="27"/>
+      <c r="G20" s="32"/>
     </row>
     <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
@@ -7488,7 +7488,7 @@
       <c r="F21" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="G21" s="27" t="s">
+      <c r="G21" s="32" t="s">
         <v>368</v>
       </c>
     </row>
@@ -7511,7 +7511,7 @@
       <c r="F22" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G22" s="27"/>
+      <c r="G22" s="32"/>
     </row>
     <row r="23" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
@@ -7532,7 +7532,7 @@
       <c r="F23" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="G23" s="27"/>
+      <c r="G23" s="32"/>
     </row>
     <row r="24" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
@@ -7553,7 +7553,7 @@
       <c r="F24" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="G24" s="27"/>
+      <c r="G24" s="32"/>
     </row>
     <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
@@ -7574,7 +7574,7 @@
       <c r="F25" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="G25" s="27"/>
+      <c r="G25" s="32"/>
     </row>
     <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
@@ -7595,7 +7595,7 @@
       <c r="F26" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="G26" s="27"/>
+      <c r="G26" s="32"/>
     </row>
     <row r="27" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
@@ -7616,7 +7616,7 @@
       <c r="F27" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="G27" s="27"/>
+      <c r="G27" s="32"/>
     </row>
     <row r="28" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
@@ -7637,7 +7637,7 @@
       <c r="F28" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="G28" s="27"/>
+      <c r="G28" s="32"/>
     </row>
     <row r="29" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="9" t="s">
@@ -7658,7 +7658,7 @@
       <c r="F29" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="G29" s="27"/>
+      <c r="G29" s="32"/>
     </row>
     <row r="30" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
@@ -7679,7 +7679,7 @@
       <c r="F30" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="G30" s="27" t="s">
+      <c r="G30" s="32" t="s">
         <v>369</v>
       </c>
     </row>
@@ -7702,7 +7702,7 @@
       <c r="F31" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="G31" s="27"/>
+      <c r="G31" s="32"/>
     </row>
     <row r="32" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
@@ -7723,7 +7723,7 @@
       <c r="F32" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="G32" s="27"/>
+      <c r="G32" s="32"/>
     </row>
     <row r="33" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
@@ -7744,7 +7744,7 @@
       <c r="F33" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="G33" s="27"/>
+      <c r="G33" s="32"/>
     </row>
     <row r="34" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
@@ -7765,7 +7765,7 @@
       <c r="F34" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="G34" s="27"/>
+      <c r="G34" s="32"/>
     </row>
     <row r="35" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
@@ -7786,7 +7786,7 @@
       <c r="F35" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="G35" s="27"/>
+      <c r="G35" s="32"/>
     </row>
     <row r="36" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
@@ -7807,7 +7807,7 @@
       <c r="F36" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="G36" s="27"/>
+      <c r="G36" s="32"/>
     </row>
     <row r="37" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
@@ -7828,7 +7828,7 @@
       <c r="F37" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="G37" s="27"/>
+      <c r="G37" s="32"/>
     </row>
     <row r="38" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
@@ -7849,7 +7849,7 @@
       <c r="F38" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="G38" s="27"/>
+      <c r="G38" s="32"/>
     </row>
     <row r="39" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="9" t="s">
@@ -7870,7 +7870,7 @@
       <c r="F39" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="G39" s="27"/>
+      <c r="G39" s="32"/>
     </row>
     <row r="40" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
@@ -7891,7 +7891,7 @@
       <c r="F40" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="G40" s="27" t="s">
+      <c r="G40" s="32" t="s">
         <v>370</v>
       </c>
     </row>
@@ -7914,7 +7914,7 @@
       <c r="F41" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="G41" s="27"/>
+      <c r="G41" s="32"/>
     </row>
     <row r="42" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
@@ -7935,7 +7935,7 @@
       <c r="F42" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="G42" s="27"/>
+      <c r="G42" s="32"/>
     </row>
     <row r="43" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
@@ -7956,7 +7956,7 @@
       <c r="F43" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="G43" s="27"/>
+      <c r="G43" s="32"/>
     </row>
     <row r="44" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
@@ -7977,7 +7977,7 @@
       <c r="F44" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="G44" s="27"/>
+      <c r="G44" s="32"/>
     </row>
     <row r="45" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
@@ -7998,7 +7998,7 @@
       <c r="F45" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="G45" s="27"/>
+      <c r="G45" s="32"/>
     </row>
     <row r="46" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
@@ -8019,7 +8019,7 @@
       <c r="F46" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="G46" s="27"/>
+      <c r="G46" s="32"/>
     </row>
     <row r="47" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
@@ -8040,7 +8040,7 @@
       <c r="F47" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="G47" s="27"/>
+      <c r="G47" s="32"/>
     </row>
     <row r="48" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="9" t="s">
@@ -8061,7 +8061,7 @@
       <c r="F48" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="G48" s="27"/>
+      <c r="G48" s="32"/>
     </row>
     <row r="49" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
@@ -8082,7 +8082,7 @@
       <c r="F49" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="G49" s="27" t="s">
+      <c r="G49" s="32" t="s">
         <v>371</v>
       </c>
     </row>
@@ -8105,7 +8105,7 @@
       <c r="F50" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="G50" s="27"/>
+      <c r="G50" s="32"/>
     </row>
     <row r="51" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
@@ -8126,7 +8126,7 @@
       <c r="F51" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="G51" s="27"/>
+      <c r="G51" s="32"/>
     </row>
     <row r="52" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
@@ -8147,7 +8147,7 @@
       <c r="F52" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="G52" s="27"/>
+      <c r="G52" s="32"/>
     </row>
     <row r="53" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
@@ -8168,7 +8168,7 @@
       <c r="F53" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="G53" s="27"/>
+      <c r="G53" s="32"/>
     </row>
     <row r="54" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
@@ -8189,7 +8189,7 @@
       <c r="F54" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="G54" s="27"/>
+      <c r="G54" s="32"/>
     </row>
     <row r="55" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
@@ -8210,7 +8210,7 @@
       <c r="F55" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="G55" s="27"/>
+      <c r="G55" s="32"/>
     </row>
     <row r="56" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
@@ -8231,7 +8231,7 @@
       <c r="F56" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="G56" s="27"/>
+      <c r="G56" s="32"/>
     </row>
     <row r="57" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="9" t="s">
@@ -8252,7 +8252,7 @@
       <c r="F57" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="G57" s="27"/>
+      <c r="G57" s="32"/>
     </row>
     <row r="58" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
@@ -8273,7 +8273,7 @@
       <c r="F58" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="G58" s="27" t="s">
+      <c r="G58" s="32" t="s">
         <v>372</v>
       </c>
     </row>
@@ -8296,7 +8296,7 @@
       <c r="F59" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="G59" s="27"/>
+      <c r="G59" s="32"/>
     </row>
     <row r="60" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
@@ -8317,7 +8317,7 @@
       <c r="F60" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="G60" s="27"/>
+      <c r="G60" s="32"/>
     </row>
     <row r="61" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
@@ -8338,7 +8338,7 @@
       <c r="F61" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="G61" s="27"/>
+      <c r="G61" s="32"/>
     </row>
     <row r="62" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
@@ -8359,7 +8359,7 @@
       <c r="F62" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="G62" s="27"/>
+      <c r="G62" s="32"/>
     </row>
     <row r="63" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
@@ -8380,7 +8380,7 @@
       <c r="F63" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="G63" s="27"/>
+      <c r="G63" s="32"/>
     </row>
     <row r="64" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
@@ -8401,7 +8401,7 @@
       <c r="F64" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="G64" s="27"/>
+      <c r="G64" s="32"/>
     </row>
     <row r="65" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
@@ -8422,7 +8422,7 @@
       <c r="F65" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="G65" s="27"/>
+      <c r="G65" s="32"/>
     </row>
     <row r="66" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="9" t="s">
@@ -8443,7 +8443,7 @@
       <c r="F66" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="G66" s="27"/>
+      <c r="G66" s="32"/>
     </row>
     <row r="67" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
@@ -8464,7 +8464,7 @@
       <c r="F67" t="s">
         <v>93</v>
       </c>
-      <c r="G67" s="27" t="s">
+      <c r="G67" s="32" t="s">
         <v>366</v>
       </c>
     </row>
@@ -8487,7 +8487,7 @@
       <c r="F68" t="s">
         <v>93</v>
       </c>
-      <c r="G68" s="27"/>
+      <c r="G68" s="32"/>
     </row>
     <row r="69" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
@@ -8508,7 +8508,7 @@
       <c r="F69" t="s">
         <v>94</v>
       </c>
-      <c r="G69" s="27"/>
+      <c r="G69" s="32"/>
     </row>
     <row r="70" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
@@ -8529,7 +8529,7 @@
       <c r="F70" t="s">
         <v>94</v>
       </c>
-      <c r="G70" s="27"/>
+      <c r="G70" s="32"/>
     </row>
     <row r="71" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
@@ -8550,7 +8550,7 @@
       <c r="F71" t="s">
         <v>95</v>
       </c>
-      <c r="G71" s="27"/>
+      <c r="G71" s="32"/>
     </row>
     <row r="72" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="9" t="s">
@@ -8571,7 +8571,7 @@
       <c r="F72" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="G72" s="27"/>
+      <c r="G72" s="32"/>
     </row>
     <row r="73" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A73" s="14" t="s">
@@ -8592,7 +8592,7 @@
       <c r="F73" t="s">
         <v>97</v>
       </c>
-      <c r="G73" s="27" t="s">
+      <c r="G73" s="32" t="s">
         <v>367</v>
       </c>
     </row>
@@ -8615,7 +8615,7 @@
       <c r="F74" t="s">
         <v>97</v>
       </c>
-      <c r="G74" s="27"/>
+      <c r="G74" s="32"/>
     </row>
     <row r="75" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="14" t="s">
@@ -8636,7 +8636,7 @@
       <c r="F75" t="s">
         <v>98</v>
       </c>
-      <c r="G75" s="27"/>
+      <c r="G75" s="32"/>
     </row>
     <row r="76" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A76" s="14" t="s">
@@ -8657,7 +8657,7 @@
       <c r="F76" t="s">
         <v>98</v>
       </c>
-      <c r="G76" s="27"/>
+      <c r="G76" s="32"/>
     </row>
     <row r="77" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A77" s="14" t="s">
@@ -8678,7 +8678,7 @@
       <c r="F77" t="s">
         <v>100</v>
       </c>
-      <c r="G77" s="27"/>
+      <c r="G77" s="32"/>
     </row>
     <row r="78" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="15" t="s">
@@ -8699,7 +8699,7 @@
       <c r="F78" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="G78" s="27"/>
+      <c r="G78" s="32"/>
     </row>
     <row r="79" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A79" s="14" t="s">
@@ -8720,7 +8720,7 @@
       <c r="F79" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="G79" s="27" t="s">
+      <c r="G79" s="32" t="s">
         <v>368</v>
       </c>
     </row>
@@ -8743,7 +8743,7 @@
       <c r="F80" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="G80" s="27"/>
+      <c r="G80" s="32"/>
     </row>
     <row r="81" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A81" s="14" t="s">
@@ -8764,7 +8764,7 @@
       <c r="F81" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="G81" s="27"/>
+      <c r="G81" s="32"/>
     </row>
     <row r="82" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A82" s="14" t="s">
@@ -8785,7 +8785,7 @@
       <c r="F82" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="G82" s="27"/>
+      <c r="G82" s="32"/>
     </row>
     <row r="83" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A83" s="14" t="s">
@@ -8806,7 +8806,7 @@
       <c r="F83" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="G83" s="27"/>
+      <c r="G83" s="32"/>
     </row>
     <row r="84" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A84" s="15" t="s">
@@ -8827,7 +8827,7 @@
       <c r="F84" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="G84" s="27"/>
+      <c r="G84" s="32"/>
     </row>
     <row r="85" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A85" s="14" t="s">
@@ -8848,7 +8848,7 @@
       <c r="F85" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="G85" s="27" t="s">
+      <c r="G85" s="32" t="s">
         <v>369</v>
       </c>
     </row>
@@ -8871,7 +8871,7 @@
       <c r="F86" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="G86" s="27"/>
+      <c r="G86" s="32"/>
     </row>
     <row r="87" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A87" s="14" t="s">
@@ -8892,7 +8892,7 @@
       <c r="F87" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G87" s="27"/>
+      <c r="G87" s="32"/>
     </row>
     <row r="88" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A88" s="14" t="s">
@@ -8913,7 +8913,7 @@
       <c r="F88" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G88" s="27"/>
+      <c r="G88" s="32"/>
     </row>
     <row r="89" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A89" s="14" t="s">
@@ -8934,7 +8934,7 @@
       <c r="F89" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="G89" s="27"/>
+      <c r="G89" s="32"/>
     </row>
     <row r="90" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A90" s="15" t="s">
@@ -8955,7 +8955,7 @@
       <c r="F90" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="G90" s="27"/>
+      <c r="G90" s="32"/>
     </row>
     <row r="91" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A91" s="14" t="s">
@@ -8976,7 +8976,7 @@
       <c r="F91" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G91" s="27" t="s">
+      <c r="G91" s="32" t="s">
         <v>370</v>
       </c>
     </row>
@@ -8999,7 +8999,7 @@
       <c r="F92" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G92" s="27"/>
+      <c r="G92" s="32"/>
     </row>
     <row r="93" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A93" s="14" t="s">
@@ -9020,7 +9020,7 @@
       <c r="F93" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G93" s="27"/>
+      <c r="G93" s="32"/>
     </row>
     <row r="94" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A94" s="14" t="s">
@@ -9041,7 +9041,7 @@
       <c r="F94" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G94" s="27"/>
+      <c r="G94" s="32"/>
     </row>
     <row r="95" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A95" s="14" t="s">
@@ -9062,7 +9062,7 @@
       <c r="F95" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G95" s="27"/>
+      <c r="G95" s="32"/>
     </row>
     <row r="96" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A96" s="15" t="s">
@@ -9083,7 +9083,7 @@
       <c r="F96" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="G96" s="27"/>
+      <c r="G96" s="32"/>
     </row>
     <row r="97" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A97" s="20" t="s">
@@ -9104,7 +9104,7 @@
       <c r="F97" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="G97" s="27" t="s">
+      <c r="G97" s="32" t="s">
         <v>371</v>
       </c>
     </row>
@@ -9127,7 +9127,7 @@
       <c r="F98" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="G98" s="27"/>
+      <c r="G98" s="32"/>
     </row>
     <row r="99" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A99" s="14" t="s">
@@ -9148,7 +9148,7 @@
       <c r="F99" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="G99" s="27"/>
+      <c r="G99" s="32"/>
     </row>
     <row r="100" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A100" s="14" t="s">
@@ -9169,7 +9169,7 @@
       <c r="F100" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="G100" s="27"/>
+      <c r="G100" s="32"/>
     </row>
     <row r="101" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A101" s="14" t="s">
@@ -9190,7 +9190,7 @@
       <c r="F101" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="G101" s="27"/>
+      <c r="G101" s="32"/>
     </row>
     <row r="102" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A102" s="15" t="s">
@@ -9211,7 +9211,7 @@
       <c r="F102" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="G102" s="27"/>
+      <c r="G102" s="32"/>
     </row>
     <row r="103" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A103" s="14" t="s">
@@ -9232,7 +9232,7 @@
       <c r="F103" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G103" s="27" t="s">
+      <c r="G103" s="32" t="s">
         <v>372</v>
       </c>
     </row>
@@ -9255,7 +9255,7 @@
       <c r="F104" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G104" s="27"/>
+      <c r="G104" s="32"/>
     </row>
     <row r="105" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A105" s="14" t="s">
@@ -9276,7 +9276,7 @@
       <c r="F105" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G105" s="27"/>
+      <c r="G105" s="32"/>
     </row>
     <row r="106" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A106" s="14" t="s">
@@ -9297,7 +9297,7 @@
       <c r="F106" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G106" s="27"/>
+      <c r="G106" s="32"/>
     </row>
     <row r="107" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A107" s="14" t="s">
@@ -9318,7 +9318,7 @@
       <c r="F107" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G107" s="27"/>
+      <c r="G107" s="32"/>
     </row>
     <row r="108" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A108" s="15" t="s">
@@ -9339,7 +9339,7 @@
       <c r="F108" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="G108" s="27"/>
+      <c r="G108" s="32"/>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109" s="14" t="s">
@@ -9360,7 +9360,7 @@
       <c r="F109" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="G109" s="29" t="s">
+      <c r="G109" s="27" t="s">
         <v>382</v>
       </c>
     </row>
@@ -9383,7 +9383,7 @@
       <c r="F110" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="G110" s="30"/>
+      <c r="G110" s="28"/>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111" s="14" t="s">
@@ -9404,7 +9404,7 @@
       <c r="F111" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="G111" s="30"/>
+      <c r="G111" s="28"/>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112" s="14" t="s">
@@ -9425,7 +9425,7 @@
       <c r="F112" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="G112" s="30"/>
+      <c r="G112" s="28"/>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113" s="14" t="s">
@@ -9446,7 +9446,7 @@
       <c r="F113" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="G113" s="30"/>
+      <c r="G113" s="28"/>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114" s="14" t="s">
@@ -9467,7 +9467,7 @@
       <c r="F114" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="G114" s="30"/>
+      <c r="G114" s="28"/>
     </row>
     <row r="115" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A115" s="15" t="s">
@@ -9488,7 +9488,7 @@
       <c r="F115" s="12" t="s">
         <v>381</v>
       </c>
-      <c r="G115" s="30"/>
+      <c r="G115" s="28"/>
     </row>
     <row r="116" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A116" s="14" t="s">
@@ -9509,7 +9509,7 @@
       <c r="F116" s="3" t="s">
         <v>397</v>
       </c>
-      <c r="G116" s="32" t="s">
+      <c r="G116" s="30" t="s">
         <v>398</v>
       </c>
     </row>
@@ -9532,7 +9532,7 @@
       <c r="F117" s="3" t="s">
         <v>397</v>
       </c>
-      <c r="G117" s="32"/>
+      <c r="G117" s="30"/>
     </row>
     <row r="118" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A118" s="14" t="s">
@@ -9553,7 +9553,7 @@
       <c r="F118" s="3" t="s">
         <v>400</v>
       </c>
-      <c r="G118" s="32"/>
+      <c r="G118" s="30"/>
     </row>
     <row r="119" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A119" s="14" t="s">
@@ -9574,7 +9574,7 @@
       <c r="F119" s="3" t="s">
         <v>400</v>
       </c>
-      <c r="G119" s="32"/>
+      <c r="G119" s="30"/>
     </row>
     <row r="120" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A120" s="14" t="s">
@@ -9595,7 +9595,7 @@
       <c r="F120" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="G120" s="32"/>
+      <c r="G120" s="30"/>
     </row>
     <row r="121" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A121" s="14" t="s">
@@ -9616,7 +9616,7 @@
       <c r="F121" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="G121" s="32"/>
+      <c r="G121" s="30"/>
     </row>
     <row r="122" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A122" s="15" t="s">
@@ -9637,7 +9637,7 @@
       <c r="F122" s="12" t="s">
         <v>344</v>
       </c>
-      <c r="G122" s="32"/>
+      <c r="G122" s="30"/>
     </row>
     <row r="123" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A123" s="14" t="s">
@@ -9658,7 +9658,7 @@
       <c r="F123" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="G123" s="32" t="s">
+      <c r="G123" s="30" t="s">
         <v>402</v>
       </c>
     </row>
@@ -9681,7 +9681,7 @@
       <c r="F124" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="G124" s="32"/>
+      <c r="G124" s="30"/>
     </row>
     <row r="125" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A125" s="14" t="s">
@@ -9702,7 +9702,7 @@
       <c r="F125" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="G125" s="32"/>
+      <c r="G125" s="30"/>
     </row>
     <row r="126" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A126" s="14" t="s">
@@ -9723,7 +9723,7 @@
       <c r="F126" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="G126" s="32"/>
+      <c r="G126" s="30"/>
     </row>
     <row r="127" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A127" s="14" t="s">
@@ -9744,7 +9744,7 @@
       <c r="F127" s="3" t="s">
         <v>346</v>
       </c>
-      <c r="G127" s="32"/>
+      <c r="G127" s="30"/>
     </row>
     <row r="128" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A128" s="14" t="s">
@@ -9765,7 +9765,7 @@
       <c r="F128" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="G128" s="32"/>
+      <c r="G128" s="30"/>
     </row>
     <row r="129" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A129" s="15" t="s">
@@ -9786,7 +9786,7 @@
       <c r="F129" s="12" t="s">
         <v>351</v>
       </c>
-      <c r="G129" s="32"/>
+      <c r="G129" s="30"/>
     </row>
     <row r="130" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A130" s="14" t="s">
@@ -9807,7 +9807,7 @@
       <c r="F130" s="3" t="s">
         <v>353</v>
       </c>
-      <c r="G130" s="33" t="s">
+      <c r="G130" s="31" t="s">
         <v>410</v>
       </c>
     </row>
@@ -9830,7 +9830,7 @@
       <c r="F131" s="12" t="s">
         <v>355</v>
       </c>
-      <c r="G131" s="33"/>
+      <c r="G131" s="31"/>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132" s="14" t="s">
@@ -9851,7 +9851,7 @@
       <c r="F132" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="G132" s="29" t="s">
+      <c r="G132" s="27" t="s">
         <v>446</v>
       </c>
     </row>
@@ -9874,7 +9874,7 @@
       <c r="F133" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="G133" s="30"/>
+      <c r="G133" s="28"/>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A134" s="14" t="s">
@@ -9895,7 +9895,7 @@
       <c r="F134" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="G134" s="30"/>
+      <c r="G134" s="28"/>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A135" s="14" t="s">
@@ -9916,7 +9916,7 @@
       <c r="F135" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="G135" s="30"/>
+      <c r="G135" s="28"/>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A136" s="14" t="s">
@@ -9937,7 +9937,7 @@
       <c r="F136" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="G136" s="30"/>
+      <c r="G136" s="28"/>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A137" s="14" t="s">
@@ -9958,7 +9958,7 @@
       <c r="F137" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="G137" s="30"/>
+      <c r="G137" s="28"/>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A138" s="14" t="s">
@@ -9979,7 +9979,7 @@
       <c r="F138" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="G138" s="30"/>
+      <c r="G138" s="28"/>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A139" s="14" t="s">
@@ -10000,7 +10000,7 @@
       <c r="F139" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="G139" s="30"/>
+      <c r="G139" s="28"/>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A140" s="14" t="s">
@@ -10021,7 +10021,7 @@
       <c r="F140" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="G140" s="30"/>
+      <c r="G140" s="28"/>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A141" s="14" t="s">
@@ -10042,7 +10042,7 @@
       <c r="F141" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="G141" s="30"/>
+      <c r="G141" s="28"/>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A142" s="14" t="s">
@@ -10063,7 +10063,7 @@
       <c r="F142" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="G142" s="30"/>
+      <c r="G142" s="28"/>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A143" s="14" t="s">
@@ -10084,7 +10084,7 @@
       <c r="F143" s="3" t="s">
         <v>439</v>
       </c>
-      <c r="G143" s="30"/>
+      <c r="G143" s="28"/>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A144" s="14" t="s">
@@ -10105,7 +10105,7 @@
       <c r="F144" s="3" t="s">
         <v>439</v>
       </c>
-      <c r="G144" s="30"/>
+      <c r="G144" s="28"/>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A145" s="14" t="s">
@@ -10126,7 +10126,7 @@
       <c r="F145" s="3" t="s">
         <v>439</v>
       </c>
-      <c r="G145" s="30"/>
+      <c r="G145" s="28"/>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A146" s="14" t="s">
@@ -10147,7 +10147,7 @@
       <c r="F146" s="3" t="s">
         <v>439</v>
       </c>
-      <c r="G146" s="30"/>
+      <c r="G146" s="28"/>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A147" s="14" t="s">
@@ -10168,7 +10168,7 @@
       <c r="F147" s="3" t="s">
         <v>439</v>
       </c>
-      <c r="G147" s="30"/>
+      <c r="G147" s="28"/>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A148" s="14" t="s">
@@ -10189,7 +10189,7 @@
       <c r="F148" s="3" t="s">
         <v>439</v>
       </c>
-      <c r="G148" s="30"/>
+      <c r="G148" s="28"/>
     </row>
     <row r="149" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A149" s="15" t="s">
@@ -10210,7 +10210,7 @@
       <c r="F149" s="12" t="s">
         <v>439</v>
       </c>
-      <c r="G149" s="31"/>
+      <c r="G149" s="29"/>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A150" s="14" t="s">
@@ -10243,11 +10243,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="G132:G149"/>
-    <mergeCell ref="G109:G115"/>
-    <mergeCell ref="G116:G122"/>
-    <mergeCell ref="G123:G129"/>
-    <mergeCell ref="G130:G131"/>
     <mergeCell ref="G97:G102"/>
     <mergeCell ref="G103:G108"/>
     <mergeCell ref="G91:G96"/>
@@ -10262,6 +10257,11 @@
     <mergeCell ref="G73:G78"/>
     <mergeCell ref="G79:G84"/>
     <mergeCell ref="G85:G90"/>
+    <mergeCell ref="G132:G149"/>
+    <mergeCell ref="G109:G115"/>
+    <mergeCell ref="G116:G122"/>
+    <mergeCell ref="G123:G129"/>
+    <mergeCell ref="G130:G131"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>

</xml_diff>